<commit_message>
All Exploration Code Good 5/9
I have commented and run unit tests on all of the exploration code up to this point in the coding process.  Everything there is good and running properly and has been tested.  If I ever need to backtrack, this would be a solid starting point to regroup from.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6308551C-D16C-4915-AEF1-56187674C490}"/>
+  <xr:revisionPtr revIDLastSave="298" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0D97B76-23D3-43AB-8CE5-E5BF18ED12E2}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>Class</t>
   </si>
@@ -189,13 +189,52 @@
   </si>
   <si>
     <t>Checks whether the output values pass or fail the current set of output rules and adds this information to the discipline's dictionary of information</t>
+  </si>
+  <si>
+    <t>Calculates the normalized root mean square difference of calculated output points to each relevant rule of the discipline and returns those values as part of a numpy vector in the discipline's "Fail_Amount" key</t>
+  </si>
+  <si>
+    <t>A recursive function that calls itself until the rule being passed to it is a sympy inequality rather than an And or Or relational so that the normalized difference of a point to the base inequality can be calculated and evaluated further if it rests within a sympy relational before being returned for the root-mean square difference equation</t>
+  </si>
+  <si>
+    <t>EXPLORATION</t>
+  </si>
+  <si>
+    <t>SPACE REDUCTION / FRAGILITY</t>
+  </si>
+  <si>
+    <t>exploration_check</t>
+  </si>
+  <si>
+    <t>checkSpace</t>
+  </si>
+  <si>
+    <t>createClusters</t>
+  </si>
+  <si>
+    <t>getPartitions</t>
+  </si>
+  <si>
+    <t>merge_constraints</t>
+  </si>
+  <si>
+    <t>mergeConstraints</t>
+  </si>
+  <si>
+    <t>fragility_check</t>
+  </si>
+  <si>
+    <t>checkFragility</t>
+  </si>
+  <si>
+    <t>PROBLEM SETUP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,8 +242,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,12 +259,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -319,11 +371,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -331,11 +446,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -343,53 +479,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,6 +560,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -671,304 +829,404 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.9453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.20703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.89453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.9453125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.68359375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.89453125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.20703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1015625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.3125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="20"/>
+    <col min="5" max="5" width="18.1015625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.3125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83984375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="35" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="E3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="12" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="17" t="s">
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="25"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="19" t="s">
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="26"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3" t="s">
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="4"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="25"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="26"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1" t="s">
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1" t="s">
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="3" t="s">
+      <c r="E15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D16" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="20" t="s">
+      <c r="E16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="25"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="20" t="s">
+      <c r="D17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="26"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="9" t="s">
         <v>49</v>
       </c>
+      <c r="D18" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="29"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
+  <mergeCells count="9">
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
End of Day 5/12
Have organized and restructured a lot of the checkSpace class and I currently have methods (uncommented) that are able to use scikit learn's decision tree regressor to create a decision tree from the Input and Output data passed to it.  I think the way to go about it later will be to manipulate the output values of the decision tree being learned to involved failure amounts and such.  But currently the code works and the script gathers all of the inequalities of the decision tree in the irules_new list
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="298" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0D97B76-23D3-43AB-8CE5-E5BF18ED12E2}"/>
+  <xr:revisionPtr revIDLastSave="313" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBCA8745-F217-4C87-A3E6-4EAA373B2F05}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>Class</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Unittest necessary/complete?</t>
   </si>
   <si>
@@ -228,6 +225,12 @@
   </si>
   <si>
     <t>PROBLEM SETUP</t>
+  </si>
+  <si>
+    <t>Not necessary</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -473,6 +476,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -481,69 +547,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -832,389 +835,389 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.9453125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.9453125" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.68359375" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.89453125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.20703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1015625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.3125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.3125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.83984375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="19" t="s">
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="31"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="32"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="19" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="31"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="32"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="31"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="32"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="25"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="26"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="25"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="26"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="22"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="23"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="25"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="26"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="29"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
End of Day 5/24
Working code as of the end of the day on 5/24/23.  But definitely need to go back through commenting, reorganizing, old code and so forth and of course testing it all.  But the sortPoints function is complete moving failing points to an eliminated key of each disciplines dictionary and the new rules being added have had their signs flipped and organized in an Or relational.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBCA8745-F217-4C87-A3E6-4EAA373B2F05}"/>
+  <xr:revisionPtr revIDLastSave="366" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDAC8682-359F-4095-8A4E-9F9F69C872F0}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
   <si>
     <t>Class</t>
   </si>
@@ -206,24 +206,12 @@
     <t>checkSpace</t>
   </si>
   <si>
-    <t>createClusters</t>
-  </si>
-  <si>
-    <t>getPartitions</t>
-  </si>
-  <si>
     <t>merge_constraints</t>
   </si>
   <si>
     <t>mergeConstraints</t>
   </si>
   <si>
-    <t>fragility_check</t>
-  </si>
-  <si>
-    <t>checkFragility</t>
-  </si>
-  <si>
     <t>PROBLEM SETUP</t>
   </si>
   <si>
@@ -231,6 +219,66 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>uniform_grid</t>
+  </si>
+  <si>
+    <t>uniformGrid</t>
+  </si>
+  <si>
+    <t>exponential_reduction</t>
+  </si>
+  <si>
+    <t>calcExponential</t>
+  </si>
+  <si>
+    <t>plotExponential</t>
+  </si>
+  <si>
+    <t>point_sorter</t>
+  </si>
+  <si>
+    <t>sortPoints</t>
+  </si>
+  <si>
+    <t>goodBad</t>
+  </si>
+  <si>
+    <t>buildTree</t>
+  </si>
+  <si>
+    <t>extract_rules</t>
+  </si>
+  <si>
+    <t>tree_to_inequalities</t>
+  </si>
+  <si>
+    <t>recurse</t>
+  </si>
+  <si>
+    <t>remove_redundant_inequalities</t>
+  </si>
+  <si>
+    <t>review_partitions</t>
+  </si>
+  <si>
+    <t>filter_points_within_bounds</t>
+  </si>
+  <si>
+    <t>reduction_change</t>
+  </si>
+  <si>
+    <t>changeReduction</t>
+  </si>
+  <si>
+    <t>estimateSpace</t>
+  </si>
+  <si>
+    <t>forceReduction</t>
+  </si>
+  <si>
+    <t>AdjustCriteria</t>
   </si>
 </sst>
 </file>
@@ -441,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -547,6 +595,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -832,16 +910,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.9453125" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.62890625" style="21" customWidth="1"/>
     <col min="2" max="2" width="14.68359375" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.89453125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.20703125" style="2" bestFit="1" customWidth="1"/>
@@ -871,14 +949,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="A2" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="22" t="s">
@@ -897,339 +975,420 @@
         <v>9</v>
       </c>
       <c r="F3" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="29" t="s">
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="19" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="30" t="s">
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B11" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="31"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="9" t="s">
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="38"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="32"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="9" t="s">
+      <c r="E12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="39"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="30" t="s">
+      <c r="E13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B14" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="31"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="9" t="s">
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="31"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="32"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="9" t="s">
+      <c r="E15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="32"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="20" t="s">
+      <c r="E16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="20" t="s">
+      <c r="E17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="20" t="s">
+      <c r="E18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="20" t="s">
+      <c r="E19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="30" t="s">
+      <c r="E20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="31"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="9" t="s">
+      <c r="E21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="31"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="32"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="9" t="s">
+      <c r="E22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="32"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="29" t="s">
+      <c r="E23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="21" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B26" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C26" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="43"/>
+      <c r="C27" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="43"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C29" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C30" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C31" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C32" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C33" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="19" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="22"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13" t="s">
+      <c r="B34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="23"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="17"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C36" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C37" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A19:F19"/>
+  <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Middle of Day 6/2
Commenting and going through all of my code, mainly the checkSpace class right now.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDAC8682-359F-4095-8A4E-9F9F69C872F0}"/>
+  <xr:revisionPtr revIDLastSave="570" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF10E4CB-8C2F-4176-92B0-FAFF91D24FD7}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="102">
   <si>
     <t>Class</t>
   </si>
@@ -248,24 +248,12 @@
     <t>buildTree</t>
   </si>
   <si>
-    <t>extract_rules</t>
-  </si>
-  <si>
-    <t>tree_to_inequalities</t>
-  </si>
-  <si>
     <t>recurse</t>
   </si>
   <si>
-    <t>remove_redundant_inequalities</t>
-  </si>
-  <si>
     <t>review_partitions</t>
   </si>
   <si>
-    <t>filter_points_within_bounds</t>
-  </si>
-  <si>
     <t>reduction_change</t>
   </si>
   <si>
@@ -279,6 +267,81 @@
   </si>
   <si>
     <t>AdjustCriteria</t>
+  </si>
+  <si>
+    <t>Necessary</t>
+  </si>
+  <si>
+    <t>Creates an array of evenly spaced points based on the total number of points the user desires and the discipline's number of dimensions</t>
+  </si>
+  <si>
+    <t>Ensures parameters are within their required ranges and calculates the exponential function value for the given time elapsed (x-value)</t>
+  </si>
+  <si>
+    <t>Create a 2D-plot to allow the user to visualize how their chosen parameters will lead to any forced reductions</t>
+  </si>
+  <si>
+    <t>elimDicts</t>
+  </si>
+  <si>
+    <t>testPoints</t>
+  </si>
+  <si>
+    <t>checkPoints</t>
+  </si>
+  <si>
+    <t>updatePoints</t>
+  </si>
+  <si>
+    <t>Move previously established values from the necessary discipline keys to an eliminated key within the discipline based on the new input rule(s) being added</t>
+  </si>
+  <si>
+    <t>Creates an "eliminated" dictionary within a discipline's dictionary along with relevant keys within the nested dictionary if none of these things already exist within the discipline</t>
+  </si>
+  <si>
+    <t>Cycles through the tested input points and space remaining points within a discipline and moves values along with accompanying information to the nested "eliminated" dictionary based on the new input rule(s)</t>
+  </si>
+  <si>
+    <t>Check each point of the relevant array to see if they satisfy the new rule and collects the index of the point in a list if the point does not</t>
+  </si>
+  <si>
+    <t>Moves information from the indices of the relevant keys to the "eliminated" dictionary within the discipline</t>
+  </si>
+  <si>
+    <t>Create an array of "good" and "bad" labels based on the user-initialized cdf threshold amount for training the decision tree</t>
+  </si>
+  <si>
+    <t>Builds the decision tree with the data provided while also providing options to separate data into train and testing sets in case the decision tree needs to be tested as well as visualizing the decision tree with a tree diagram</t>
+  </si>
+  <si>
+    <t>prepareRule</t>
+  </si>
+  <si>
+    <t>extractRules</t>
+  </si>
+  <si>
+    <t>Gathers all of the inequalities for each path of the decision tree along with statistics on the total number and fraction of bad points within the space defined by each path</t>
+  </si>
+  <si>
+    <t>Cycles through the child nodes of the decision tree until the leaf nodes are reached and creates a list of inequalities defining each branch from the root node to the leaf node while also determing the amount of "bad" points within each branch</t>
+  </si>
+  <si>
+    <t>Create inequalities from the partitions of the decision tree encompassing the highest fraction of "bad" points without any redundancies that will be used to (potentially) propose a new rule</t>
+  </si>
+  <si>
+    <t>redundantIneqs</t>
+  </si>
+  <si>
+    <t>Checks if any inequalities of the decision tree's extracted rule describe any overlapping regions, and if so, simplifies those inequalities into a single inequality describing the redundant space</t>
+  </si>
+  <si>
+    <t>filterPoints</t>
+  </si>
+  <si>
+    <t>minMerge</t>
+  </si>
+  <si>
+    <t>Gather the input locations and failure amounts for all of the tested input points meeting all of the inequalities of the potential rule</t>
   </si>
 </sst>
 </file>
@@ -301,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +383,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -489,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -524,56 +593,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,35 +683,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,87 +1018,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.62890625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="18.62890625" style="20" customWidth="1"/>
     <col min="2" max="2" width="14.68359375" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.89453125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.20703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1015625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.3125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.3125" style="17" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.83984375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="46" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="48" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="21" t="s">
+      <c r="D4" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -999,396 +1116,546 @@
       <c r="C5" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="9" t="s">
+      <c r="D5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="21"/>
+      <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>60</v>
+      <c r="D6" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="54"/>
+      <c r="C9" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="54"/>
+      <c r="C10" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>60</v>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="38"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="39"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="31"/>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="9"/>
       <c r="B15" s="34"/>
       <c r="C15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C25" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="37"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="38"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="29"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D33" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="18" t="s">
+      <c r="E33" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="32"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="9" t="s">
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="30"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="18" t="s">
+      <c r="E34" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="20" t="s">
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="17" t="s">
+      <c r="E35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="20" t="s">
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="17" t="s">
+      <c r="E36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="20" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="17" t="s">
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="20" t="s">
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="17" t="s">
+      <c r="E38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="30" t="s">
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B39" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="17" t="s">
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="31"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="9" t="s">
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="29"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="18" t="s">
+      <c r="E40" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="32"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="9" t="s">
+    <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="30"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D41" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="18" t="s">
+      <c r="E41" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="17"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="43"/>
-      <c r="B28" s="45"/>
-      <c r="C28" s="43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C29" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C30" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C31" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C33" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="16"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C36" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
End of Day 6/2
Finished commenting all of the code in the exploration_check class.  Picking up with comments in merge_constraints next.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="570" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF10E4CB-8C2F-4176-92B0-FAFF91D24FD7}"/>
+  <xr:revisionPtr revIDLastSave="620" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74AAE5E1-CD17-4045-A51F-2E97E9DEA001}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="104">
   <si>
     <t>Class</t>
   </si>
@@ -251,9 +251,6 @@
     <t>recurse</t>
   </si>
   <si>
-    <t>review_partitions</t>
-  </si>
-  <si>
     <t>reduction_change</t>
   </si>
   <si>
@@ -342,6 +339,15 @@
   </si>
   <si>
     <t>Gather the input locations and failure amounts for all of the tested input points meeting all of the inequalities of the potential rule</t>
+  </si>
+  <si>
+    <t>reviewPartitions</t>
+  </si>
+  <si>
+    <t>Evaluate various criteria within the area of the discipline's design space to be reduced to ensure that area has been reasonably explored before committing to proposing the reduction</t>
+  </si>
+  <si>
+    <t>Flip signs of inequalities making up the potential rule and store the inequalities as arguments in an Or relational so that the rule describes the space still open to the discipline rather than the space being eliminated</t>
   </si>
 </sst>
 </file>
@@ -390,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -554,11 +560,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -659,8 +696,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -683,56 +738,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1021,8 +1049,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1057,85 +1085,83 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="51" t="s">
+      <c r="D4" s="35" t="s">
         <v>77</v>
       </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="53" t="s">
-        <v>77</v>
+      <c r="F5" s="38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="21"/>
-      <c r="B6" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="44"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="52" t="s">
-        <v>80</v>
+      <c r="D6" s="37" t="s">
+        <v>79</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>9</v>
@@ -1145,122 +1171,127 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="53"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="57" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="54"/>
-      <c r="C9" s="54" t="s">
+      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="53"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="54"/>
-      <c r="C10" s="54" t="s">
+      <c r="E10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="53"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="54"/>
-      <c r="C11" s="54" t="s">
+      <c r="E11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="54"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="21"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="58" t="s">
-        <v>77</v>
+      <c r="E12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="45" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="53"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="57" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="C14" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>91</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>9</v>
@@ -1270,82 +1301,117 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="9"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="9" t="s">
-        <v>93</v>
+      <c r="A15" s="53"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="49" t="s">
+        <v>92</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="53"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="53"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="53"/>
+      <c r="B18" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="53" t="s">
-        <v>77</v>
+      <c r="F18" s="38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="53"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="E19" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="53" t="s">
-        <v>77</v>
+      <c r="F19" s="38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="53"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="53" t="s">
-        <v>77</v>
+      <c r="F20" s="38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="54"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="53" t="s">
-        <v>77</v>
+      <c r="F21" s="38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1356,7 +1422,7 @@
         <v>57</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="7"/>
@@ -1364,34 +1430,34 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="18" t="s">
@@ -1414,10 +1480,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1434,8 +1500,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="37"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="9" t="s">
         <v>18</v>
       </c>
@@ -1450,8 +1516,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="38"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="9" t="s">
         <v>19</v>
       </c>
@@ -1639,7 +1705,7 @@
       <c r="C41" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="52" t="s">
+      <c r="D41" s="37" t="s">
         <v>51</v>
       </c>
       <c r="E41" s="13" t="s">
@@ -1650,13 +1716,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="12">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A27:F27"/>
     <mergeCell ref="A29:A31"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CODE RUNS TO COMPLETION
Everything is able to run to completion without the fragility framework.  Still need to comment and unit test stuff.  I have it set up for 100 time iterations and 5% of the space remaining by the end of the 100 time iterations.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="620" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74AAE5E1-CD17-4045-A51F-2E97E9DEA001}"/>
+  <xr:revisionPtr revIDLastSave="635" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{543373A4-FEFA-44D3-9308-4F5EB626A1AE}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
   <si>
     <t>Class</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>Flip signs of inequalities making up the potential rule and store the inequalities as arguments in an Or relational so that the rule describes the space still open to the discipline rather than the space being eliminated</t>
+  </si>
+  <si>
+    <t>Approximate the design space remaining in each discipline</t>
+  </si>
+  <si>
+    <t>Determine and indicate if any disciplines should force a space reduction depending on the space that has been eliminated thus far compared to the project time remaining</t>
   </si>
 </sst>
 </file>
@@ -595,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -717,6 +723,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,12 +753,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -758,9 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1050,7 +1053,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1085,14 +1088,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="21" t="s">
@@ -1135,10 +1138,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -1155,8 +1158,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="44"/>
-      <c r="B6" s="47"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
@@ -1171,20 +1174,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1202,7 +1205,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="53"/>
-      <c r="B9" s="46"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="9" t="s">
         <v>80</v>
       </c>
@@ -1218,7 +1221,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="53"/>
-      <c r="B10" s="46"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="9" t="s">
         <v>81</v>
       </c>
@@ -1234,7 +1237,7 @@
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="53"/>
-      <c r="B11" s="46"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="9" t="s">
         <v>82</v>
       </c>
@@ -1250,7 +1253,7 @@
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="54"/>
-      <c r="B12" s="46"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="9" t="s">
         <v>83</v>
       </c>
@@ -1268,7 +1271,7 @@
       <c r="A13" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="47" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1286,8 +1289,8 @@
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="53"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="49" t="s">
+      <c r="B14" s="48"/>
+      <c r="C14" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="11" t="s">
@@ -1302,8 +1305,8 @@
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="53"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="49" t="s">
+      <c r="B15" s="48"/>
+      <c r="C15" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -1318,8 +1321,8 @@
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="53"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="49" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -1335,10 +1338,10 @@
     <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17" s="53"/>
       <c r="B17" s="51"/>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="42" t="s">
         <v>103</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -1350,7 +1353,7 @@
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="53"/>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1368,7 +1371,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="53"/>
-      <c r="B19" s="46"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="9" t="s">
         <v>96</v>
       </c>
@@ -1384,7 +1387,7 @@
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="53"/>
-      <c r="B20" s="46"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="9" t="s">
         <v>70</v>
       </c>
@@ -1400,7 +1403,7 @@
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="54"/>
-      <c r="B21" s="47"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="9" t="s">
         <v>98</v>
       </c>
@@ -1438,10 +1441,28 @@
       <c r="C23" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="9" t="s">
         <v>74</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1450,14 +1471,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="18" t="s">
@@ -1480,10 +1501,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1500,8 +1521,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="43"/>
-      <c r="B30" s="46"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="9" t="s">
         <v>18</v>
       </c>
@@ -1516,8 +1537,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="44"/>
-      <c r="B31" s="47"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="9" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Working Code without Fragility
Everything is working cohesively and well commented without the fragility framework.  Worthwhile to mess around with the user input parameters in the script file as desired.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="635" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{543373A4-FEFA-44D3-9308-4F5EB626A1AE}"/>
+  <xr:revisionPtr revIDLastSave="664" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEC51766-9597-490B-8D7C-75502469358C}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
   <si>
     <t>Class</t>
   </si>
@@ -335,9 +335,6 @@
     <t>filterPoints</t>
   </si>
   <si>
-    <t>minMerge</t>
-  </si>
-  <si>
     <t>Gather the input locations and failure amounts for all of the tested input points meeting all of the inequalities of the potential rule</t>
   </si>
   <si>
@@ -354,6 +351,15 @@
   </si>
   <si>
     <t>Determine and indicate if any disciplines should force a space reduction depending on the space that has been eliminated thus far compared to the project time remaining</t>
+  </si>
+  <si>
+    <t>Cycles through the established criteria for allowing a space reduction that specifically pertain to the area of a discipline's design space being reduced and relaxes one criterion when a space reduction is being forced for the discipline</t>
+  </si>
+  <si>
+    <t>removeContradiction</t>
+  </si>
+  <si>
+    <t>Considers the independent rule (consisting of a single inequality or a sympy Or relational containing multiple inequalities) being proposed by one or more disciplines and merges them such that from the top-level, the rule(s) do not contradict each other</t>
   </si>
 </sst>
 </file>
@@ -1049,18 +1055,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="18.62890625" style="20" customWidth="1"/>
     <col min="2" max="2" width="14.68359375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.89453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.62890625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.20703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1015625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.3125" style="17" bestFit="1" customWidth="1"/>
@@ -1323,10 +1329,10 @@
       <c r="A16" s="53"/>
       <c r="B16" s="48"/>
       <c r="C16" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>9</v>
@@ -1342,7 +1348,7 @@
         <v>91</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>9</v>
@@ -1408,7 +1414,7 @@
         <v>98</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>9</v>
@@ -1417,7 +1423,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="18" t="s">
         <v>56</v>
       </c>
@@ -1425,11 +1431,17 @@
         <v>57</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="15"/>
+        <v>106</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="19" t="s">
@@ -1442,7 +1454,7 @@
         <v>73</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>9</v>
@@ -1456,7 +1468,7 @@
         <v>74</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>9</v>
@@ -1465,121 +1477,146 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="9" t="s">
         <v>75</v>
       </c>
+      <c r="D25" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="18" t="s">
+      <c r="A27" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="15" t="s">
+      <c r="E27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="47" t="s">
+      <c r="A29" s="45"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="46"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="45"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="46"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="17" t="s">
+      <c r="C31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="16" t="s">
+      <c r="A32" s="29"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="29"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>9</v>
@@ -1588,34 +1625,38 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="30"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>59</v>
+    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="19" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>9</v>
@@ -1624,58 +1665,58 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="19" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>16</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>9</v>
@@ -1684,64 +1725,44 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="16" t="s">
+    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="29"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="29"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="30"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="12" t="s">
+    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="30"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="D40" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="22" t="s">
+      <c r="E40" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="22" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B8:B12"/>

</xml_diff>

<commit_message>
End of Day 6/7
Finished commenting all code up to the fragility framework and am going through unittesting now.  This push has 2/5 functions in the point_sorter file properly unit tested and will be where I pick up again tomorrow.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="664" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEC51766-9597-490B-8D7C-75502469358C}"/>
+  <xr:revisionPtr revIDLastSave="752" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{569FA314-0671-4FAD-8651-61255B8B7051}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="110">
   <si>
     <t>Class</t>
   </si>
@@ -95,9 +96,6 @@
     <t>getInequalities</t>
   </si>
   <si>
-    <t>extract_inequality</t>
-  </si>
-  <si>
     <t>Gathers a list of constraints/rules that must be considered according to the variables passed along</t>
   </si>
   <si>
@@ -197,9 +195,6 @@
     <t>EXPLORATION</t>
   </si>
   <si>
-    <t>SPACE REDUCTION / FRAGILITY</t>
-  </si>
-  <si>
     <t>exploration_check</t>
   </si>
   <si>
@@ -360,6 +355,18 @@
   </si>
   <si>
     <t>Considers the independent rule (consisting of a single inequality or a sympy Or relational containing multiple inequalities) being proposed by one or more disciplines and merges them such that from the top-level, the rule(s) do not contradict each other</t>
+  </si>
+  <si>
+    <t>extractInequality</t>
+  </si>
+  <si>
+    <t>createNumpy2</t>
+  </si>
+  <si>
+    <t>Checks if a key is in the supplied dictionary and puts it there with an empty numpy array as the value if not</t>
+  </si>
+  <si>
+    <t>SPACE REDUCTION</t>
   </si>
 </sst>
 </file>
@@ -382,7 +389,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +414,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -607,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -618,18 +631,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -645,18 +652,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -672,9 +670,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -690,21 +685,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -734,6 +714,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1055,710 +1059,738 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.62890625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="14.68359375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.62890625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.62890625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="14.68359375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.62890625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.20703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1015625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.3125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="9"/>
+    <col min="5" max="5" width="18.1015625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.3125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83984375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="18" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="43"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="47" t="s">
+      <c r="E6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="50"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="46"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="37" t="s">
+      <c r="D9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="50"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="50" t="s">
+      <c r="D10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="50"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="51"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="52" t="s">
+      <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="D13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="50"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="50"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="50"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="50"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="50"/>
+      <c r="B18" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="53"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="53"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="53"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="54"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="52" t="s">
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="50"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="50"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="51"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B22" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="53"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="9" t="s">
+      <c r="C22" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="53"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="53"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="B23" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="53"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="42" t="s">
+      <c r="E23" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="42"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="53"/>
-      <c r="B18" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="53"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="53"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="54"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="E24" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="43"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="38" t="s">
-        <v>76</v>
+      <c r="E25" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="A26" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>60</v>
+      <c r="E27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="42"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="45"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="E29" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="43"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="46"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="11" t="s">
+      <c r="E30" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="28" t="s">
+      <c r="B31" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="50"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D32" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="29"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="9" t="s">
+      <c r="E32" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="50"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="30"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="11" t="s">
+      <c r="E33" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="51"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="19" t="s">
+      <c r="B35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D35" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E35" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="19" t="s">
+      <c r="B36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E36" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="19" t="s">
-        <v>41</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E38" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="28" t="s">
+      <c r="B39" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="C39" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D39" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A40" s="42"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D40" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="29"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="9" t="s">
+      <c r="E40" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="43"/>
+      <c r="B41" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D41" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="30"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>59</v>
+      <c r="E41" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A28:A30"/>

</xml_diff>

<commit_message>
End of Day 6/8
More unit testing...currently in the middle of the checkSpace class
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="752" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{569FA314-0671-4FAD-8651-61255B8B7051}"/>
+  <xr:revisionPtr revIDLastSave="766" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A54933A3-4D87-4493-BBEE-597605DCC786}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1062,8 +1062,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1241,8 +1241,8 @@
       <c r="E10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>74</v>
+      <c r="F10" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1257,8 +1257,8 @@
       <c r="E11" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="27" t="s">
-        <v>74</v>
+      <c r="F11" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1273,8 +1273,8 @@
       <c r="E12" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="29" t="s">
-        <v>74</v>
+      <c r="F12" s="39" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1293,8 +1293,8 @@
       <c r="E13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="28" t="s">
-        <v>74</v>
+      <c r="F13" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1357,8 +1357,8 @@
       <c r="E17" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="27" t="s">
-        <v>74</v>
+      <c r="F17" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
End of Day 6/9
Completed all unit tests for the exploration_check file (and even caught one small bug in extractRules).  Moving onto the mergeConstraints class next.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="766" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A54933A3-4D87-4493-BBEE-597605DCC786}"/>
+  <xr:revisionPtr revIDLastSave="778" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3743A61A-A8BB-45AF-B539-A7FE71685041}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -739,41 +738,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1062,8 +1061,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1098,14 +1097,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="16" t="s">
@@ -1148,10 +1147,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1168,8 +1167,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="43"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="10" t="s">
         <v>63</v>
       </c>
@@ -1184,20 +1183,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1214,8 +1213,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="50"/>
-      <c r="B9" s="45"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="7" t="s">
         <v>78</v>
       </c>
@@ -1230,8 +1229,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="50"/>
-      <c r="B10" s="45"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="7" t="s">
         <v>79</v>
       </c>
@@ -1246,8 +1245,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="50"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="7" t="s">
         <v>80</v>
       </c>
@@ -1262,8 +1261,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="51"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="7" t="s">
         <v>81</v>
       </c>
@@ -1278,10 +1277,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="40" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1298,8 +1297,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="50"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="7" t="s">
         <v>67</v>
       </c>
@@ -1314,8 +1313,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="50"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="7" t="s">
         <v>90</v>
       </c>
@@ -1325,13 +1324,13 @@
       <c r="E15" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="27" t="s">
-        <v>74</v>
+      <c r="F15" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="50"/>
-      <c r="B16" s="45"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="7" t="s">
         <v>98</v>
       </c>
@@ -1341,13 +1340,13 @@
       <c r="E16" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="27" t="s">
-        <v>74</v>
+      <c r="F16" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="50"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="30" t="s">
         <v>89</v>
       </c>
@@ -1362,8 +1361,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="50"/>
-      <c r="B18" s="45" t="s">
+      <c r="A18" s="45"/>
+      <c r="B18" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1375,13 +1374,13 @@
       <c r="E18" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="27" t="s">
-        <v>74</v>
+      <c r="F18" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="50"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="7" t="s">
         <v>94</v>
       </c>
@@ -1391,13 +1390,13 @@
       <c r="E19" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>74</v>
+      <c r="F19" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="50"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="7" t="s">
         <v>68</v>
       </c>
@@ -1407,13 +1406,13 @@
       <c r="E20" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="27" t="s">
-        <v>74</v>
+      <c r="F20" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="51"/>
-      <c r="B21" s="46"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="43"/>
       <c r="C21" s="7" t="s">
         <v>96</v>
       </c>
@@ -1423,8 +1422,8 @@
       <c r="E21" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="27" t="s">
-        <v>74</v>
+      <c r="F21" s="37" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1448,10 +1447,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="40" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1468,8 +1467,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="42"/>
-      <c r="B24" s="45"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="42"/>
       <c r="C24" s="7" t="s">
         <v>72</v>
       </c>
@@ -1484,8 +1483,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="43"/>
-      <c r="B25" s="46"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="43"/>
       <c r="C25" s="7" t="s">
         <v>73</v>
       </c>
@@ -1500,14 +1499,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="13" t="s">
@@ -1530,10 +1529,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1550,8 +1549,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="42"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
@@ -1566,8 +1565,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="43"/>
-      <c r="B30" s="46"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="7" t="s">
         <v>106</v>
       </c>
@@ -1582,10 +1581,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1602,8 +1601,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="50"/>
-      <c r="B32" s="45"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
@@ -1618,8 +1617,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="50"/>
-      <c r="B33" s="45"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="42"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
@@ -1634,8 +1633,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="51"/>
-      <c r="B34" s="46"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="7" t="s">
         <v>107</v>
       </c>
@@ -1730,10 +1729,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="40" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1750,8 +1749,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="42"/>
-      <c r="B40" s="48"/>
+      <c r="A40" s="48"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="30" t="s">
         <v>46</v>
       </c>
@@ -1766,7 +1765,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="43"/>
+      <c r="A41" s="49"/>
       <c r="B41" s="22" t="s">
         <v>16</v>
       </c>
@@ -1785,12 +1784,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A28:A30"/>
@@ -1803,6 +1796,12 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
End of Day 6/10
Finished unittests for merge constraints.  In the middle of unit tests for reduction_change.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="778" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3743A61A-A8BB-45AF-B539-A7FE71685041}"/>
+  <xr:revisionPtr revIDLastSave="782" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E249DBF-8C89-4E1C-AEF8-E18EFE336B09}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -693,9 +693,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -738,18 +735,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -758,21 +770,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1061,8 +1058,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1097,14 +1094,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="16" t="s">
@@ -1119,10 +1116,10 @@
       <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="39" t="s">
+      <c r="E3" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="38" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1139,18 +1136,18 @@
       <c r="D4" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="33" t="s">
+      <c r="E4" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1159,44 +1156,44 @@
       <c r="D5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="37" t="s">
+      <c r="E5" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="49"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1205,82 +1202,82 @@
       <c r="D8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="36" t="s">
+      <c r="E8" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="45"/>
-      <c r="B9" s="42"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="37" t="s">
+      <c r="E9" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="45"/>
-      <c r="B10" s="42"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="37" t="s">
+      <c r="E10" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="45"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="37" t="s">
+      <c r="E11" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="46"/>
-      <c r="B12" s="42"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="39" t="s">
+      <c r="E12" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="38" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="43" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1289,80 +1286,80 @@
       <c r="D13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="36" t="s">
+      <c r="E13" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="45"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="37" t="s">
+      <c r="E14" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="36" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="45"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="37" t="s">
+      <c r="E15" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="45"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="37" t="s">
+      <c r="E16" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="45"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="30" t="s">
+      <c r="A17" s="49"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="37" t="s">
+      <c r="E17" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="45"/>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="49"/>
+      <c r="B18" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1371,58 +1368,58 @@
       <c r="D18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="37" t="s">
+      <c r="E18" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="45"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="37" t="s">
+      <c r="E19" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="45"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="44"/>
       <c r="C20" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="37" t="s">
+      <c r="E20" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="46"/>
-      <c r="B21" s="43"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="7" t="s">
         <v>96</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="37" t="s">
+      <c r="E21" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="36" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1439,18 +1436,18 @@
       <c r="D22" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>74</v>
+      <c r="E22" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="43" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1459,54 +1456,54 @@
       <c r="D23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>74</v>
+      <c r="E23" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="48"/>
-      <c r="B24" s="42"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="27" t="s">
+      <c r="E24" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="26" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="49"/>
-      <c r="B25" s="43"/>
+      <c r="A25" s="42"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="27" t="s">
+      <c r="E25" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="26" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="13" t="s">
@@ -1521,18 +1518,18 @@
       <c r="D27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="33" t="s">
+      <c r="E27" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1541,50 +1538,50 @@
       <c r="D28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="28" t="s">
+      <c r="E28" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="48"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="44"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="27" t="s">
+      <c r="E29" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="26" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="49"/>
-      <c r="B30" s="43"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="27" t="s">
+      <c r="E30" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="26" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1593,58 +1590,58 @@
       <c r="D31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="36" t="s">
+      <c r="E31" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="35" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="45"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="37" t="s">
+      <c r="E32" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="36" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="45"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="37" t="s">
+      <c r="E33" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="36" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="46"/>
-      <c r="B34" s="43"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="7" t="s">
         <v>107</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="37" t="s">
+      <c r="E34" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="36" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1661,10 +1658,10 @@
       <c r="D35" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="36" t="s">
+      <c r="E35" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="35" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1681,10 +1678,10 @@
       <c r="D36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="36" t="s">
+      <c r="E36" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="35" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1701,10 +1698,10 @@
       <c r="D37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="28" t="s">
+      <c r="E37" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="27" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1721,18 +1718,18 @@
       <c r="D38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="36" t="s">
+      <c r="E38" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="43" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1741,49 +1738,55 @@
       <c r="D39" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="36" t="s">
+      <c r="E39" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="48"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="30" t="s">
+      <c r="A40" s="41"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="37" t="s">
+      <c r="E40" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="49"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D41" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="29" t="s">
+      <c r="E41" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="28" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A28:A30"/>
@@ -1796,12 +1799,6 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
End of Day 6/11
All unit tests done except for 2.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="782" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E249DBF-8C89-4E1C-AEF8-E18EFE336B09}"/>
+  <xr:revisionPtr revIDLastSave="792" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17500E3D-5BB0-4207-BE31-634CDDE59D96}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -696,9 +696,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -735,41 +732,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,8 +1055,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1094,14 +1091,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="16" t="s">
@@ -1116,10 +1113,10 @@
       <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1136,18 +1133,18 @@
       <c r="D4" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="32" t="s">
+      <c r="E4" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1156,44 +1153,44 @@
       <c r="D5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="36" t="s">
+      <c r="E5" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="38" t="s">
+      <c r="E6" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1202,82 +1199,82 @@
       <c r="D8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="35" t="s">
+      <c r="E8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="49"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="36" t="s">
+      <c r="E9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="49"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="36" t="s">
+      <c r="E10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="49"/>
-      <c r="B11" s="44"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="7" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="36" t="s">
+      <c r="E11" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="50"/>
-      <c r="B12" s="44"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="38" t="s">
+      <c r="E12" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="37" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="38" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1286,80 +1283,80 @@
       <c r="D13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="35" t="s">
+      <c r="E13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="49"/>
-      <c r="B14" s="44"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="7" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="36" t="s">
+      <c r="E14" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="35" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="49"/>
-      <c r="B15" s="44"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="7" t="s">
         <v>90</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="36" t="s">
+      <c r="E15" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="49"/>
-      <c r="B16" s="44"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="7" t="s">
         <v>98</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="36" t="s">
+      <c r="E16" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="49"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="29" t="s">
+      <c r="A17" s="43"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="36" t="s">
+      <c r="E17" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="49"/>
-      <c r="B18" s="44" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1368,58 +1365,58 @@
       <c r="D18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="36" t="s">
+      <c r="E18" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="49"/>
-      <c r="B19" s="44"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="7" t="s">
         <v>94</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="36" t="s">
+      <c r="E19" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="49"/>
-      <c r="B20" s="44"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="36" t="s">
+      <c r="E20" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="50"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="44"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="7" t="s">
         <v>96</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="36" t="s">
+      <c r="E21" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="35" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1436,18 +1433,18 @@
       <c r="D22" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="32" t="s">
+      <c r="E22" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="38" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1456,54 +1453,54 @@
       <c r="D23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="36" t="s">
+      <c r="E23" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="41"/>
-      <c r="B24" s="44"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>74</v>
+      <c r="E24" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="42"/>
-      <c r="B25" s="45"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="7" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>74</v>
+      <c r="E25" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="13" t="s">
@@ -1518,18 +1515,18 @@
       <c r="D27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="32" t="s">
+      <c r="E27" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1538,50 +1535,50 @@
       <c r="D28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>74</v>
+      <c r="E28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="41"/>
-      <c r="B29" s="44"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>74</v>
+      <c r="E29" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="42"/>
-      <c r="B30" s="45"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="7" t="s">
         <v>106</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>74</v>
+      <c r="E30" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1590,58 +1587,58 @@
       <c r="D31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="35" t="s">
+      <c r="E31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="49"/>
-      <c r="B32" s="44"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="36" t="s">
+      <c r="E32" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="35" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="49"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="36" t="s">
+      <c r="E33" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="35" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="50"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="7" t="s">
         <v>107</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="36" t="s">
+      <c r="E34" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="35" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1658,10 +1655,10 @@
       <c r="D35" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="35" t="s">
+      <c r="E35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="34" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1678,10 +1675,10 @@
       <c r="D36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="35" t="s">
+      <c r="E36" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="34" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1698,10 +1695,10 @@
       <c r="D37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="27" t="s">
+      <c r="E37" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="26" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1718,18 +1715,18 @@
       <c r="D38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="35" t="s">
+      <c r="E38" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="38" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1738,31 +1735,31 @@
       <c r="D39" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="35" t="s">
+      <c r="E39" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="41"/>
-      <c r="B40" s="47"/>
-      <c r="C40" s="29" t="s">
+      <c r="A40" s="46"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="36" t="s">
+      <c r="E40" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="35" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="42"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="22" t="s">
         <v>16</v>
       </c>
@@ -1772,21 +1769,15 @@
       <c r="D41" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="28" t="s">
+      <c r="E41" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="27" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A28:A30"/>
@@ -1799,6 +1790,12 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed all Unit Tests
Completed all unit tests and commenting for everything up until the fragility framework!  Code works!
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/joeyvan_umich_edu/Documents/DesignSpace_Fragility/Python Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="792" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17500E3D-5BB0-4207-BE31-634CDDE59D96}"/>
+  <xr:revisionPtr revIDLastSave="797" documentId="11_F25DC773A252ABDACC10482959995DA05ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B0D9A21-E80F-485F-BC6C-8837EC7BD0A5}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="109">
   <si>
     <t>Class</t>
   </si>
@@ -179,9 +179,6 @@
     <t>rmsFail</t>
   </si>
   <si>
-    <t>get_output_diff</t>
-  </si>
-  <si>
     <t>Checks whether the output values pass or fail the current set of output rules and adds this information to the discipline's dictionary of information</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>AdjustCriteria</t>
   </si>
   <si>
-    <t>Necessary</t>
-  </si>
-  <si>
     <t>Creates an array of evenly spaced points based on the total number of points the user desires and the discipline's number of dimensions</t>
   </si>
   <si>
@@ -366,6 +360,9 @@
   </si>
   <si>
     <t>SPACE REDUCTION</t>
+  </si>
+  <si>
+    <t>outputDiff</t>
   </si>
 </sst>
 </file>
@@ -388,7 +385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,12 +401,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -696,54 +687,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -752,21 +752,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1055,8 +1040,8 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1091,14 +1076,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="16" t="s">
@@ -1113,394 +1098,394 @@
       <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>57</v>
+      <c r="E3" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="B5" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="38" t="s">
+      <c r="E6" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="46"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="47"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="25" t="s">
+      <c r="D9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="46"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="46"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="47"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="43"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="43"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="43"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="44"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="E13" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="46"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="E14" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="46"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="46"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="46"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="43"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="43"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="43"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="7" t="s">
+      <c r="D17" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A17" s="43"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>58</v>
+      <c r="E17" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="43"/>
-      <c r="B18" s="40" t="s">
+      <c r="A18" s="46"/>
+      <c r="B18" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>58</v>
+        <v>89</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="43"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="46"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="47"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="43"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="44"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>58</v>
+      <c r="E21" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>58</v>
+        <v>103</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="C23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="38"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="39"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="46"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="47"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>58</v>
+      <c r="E25" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
+      <c r="A26" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="13" t="s">
@@ -1515,18 +1500,18 @@
       <c r="D27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="31" t="s">
-        <v>58</v>
+      <c r="E27" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1535,50 +1520,50 @@
       <c r="D28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="34" t="s">
-        <v>58</v>
+      <c r="E28" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="46"/>
-      <c r="B29" s="40"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>58</v>
+      <c r="E29" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="47"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E30" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="35" t="s">
-        <v>58</v>
+      <c r="E30" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1587,59 +1572,59 @@
       <c r="D31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>57</v>
+      <c r="E31" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="43"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="35" t="s">
-        <v>57</v>
+      <c r="E32" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="43"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="35" t="s">
-        <v>57</v>
+      <c r="E33" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="44"/>
-      <c r="B34" s="41"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="35" t="s">
-        <v>57</v>
+        <v>106</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="33" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1655,11 +1640,11 @@
       <c r="D35" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="34" t="s">
-        <v>58</v>
+      <c r="E35" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1675,11 +1660,11 @@
       <c r="D36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="34" t="s">
-        <v>58</v>
+      <c r="E36" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1695,11 +1680,11 @@
       <c r="D37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>74</v>
+      <c r="E37" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1715,69 +1700,75 @@
       <c r="D38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="34" t="s">
-        <v>58</v>
+      <c r="E38" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="40" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A40" s="38"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="46"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="35" t="s">
-        <v>58</v>
+      <c r="E40" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="47"/>
+      <c r="A41" s="39"/>
       <c r="B41" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>74</v>
+        <v>49</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A28:A30"/>
@@ -1790,12 +1781,6 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Slight adjustments made while writing 9/13
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ACBADB-2A69-4CA3-84E5-46FC15708AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6A1140-03F9-4F60-BF5E-2CB908BF10D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,10 +365,10 @@
     <t>outputDiff</t>
   </si>
   <si>
-    <t>Fragility</t>
-  </si>
-  <si>
     <t>fragility_check</t>
+  </si>
+  <si>
+    <t>FRAGILITY</t>
   </si>
 </sst>
 </file>
@@ -723,18 +723,27 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -748,15 +757,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,8 +1042,8 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,14 +1078,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1128,10 +1128,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1148,8 +1148,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1164,20 +1164,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
     </row>
     <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1194,8 +1194,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1210,8 +1210,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="46"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1226,8 +1226,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="46"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1242,8 +1242,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="47"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1258,10 +1258,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1278,8 +1278,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="46"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1294,8 +1294,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1310,8 +1310,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="46"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1326,8 +1326,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="46"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="26" t="s">
         <v>87</v>
       </c>
@@ -1342,8 +1342,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="46"/>
-      <c r="B18" s="41" t="s">
+      <c r="A18" s="37"/>
+      <c r="B18" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1360,8 +1360,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1376,8 +1376,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="46"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="44"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1392,8 +1392,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1428,10 +1428,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="43" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1448,8 +1448,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="38"/>
-      <c r="B24" s="41"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="7" t="s">
         <v>71</v>
       </c>
@@ -1464,8 +1464,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" s="39"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="7" t="s">
         <v>72</v>
       </c>
@@ -1480,14 +1480,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
@@ -1510,10 +1510,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1530,8 +1530,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="38"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="44"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
@@ -1546,8 +1546,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="39"/>
-      <c r="B30" s="42"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="7" t="s">
         <v>104</v>
       </c>
@@ -1562,10 +1562,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1582,8 +1582,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="46"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
@@ -1598,8 +1598,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="46"/>
-      <c r="B33" s="41"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
@@ -1614,8 +1614,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="47"/>
-      <c r="B34" s="42"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="7" t="s">
         <v>105</v>
       </c>
@@ -1710,10 +1710,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="43" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1730,8 +1730,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="38"/>
-      <c r="B40" s="44"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="26" t="s">
         <v>46</v>
       </c>
@@ -1746,7 +1746,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="39"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="22" t="s">
         <v>16</v>
       </c>
@@ -1764,22 +1764,25 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
+      <c r="A42" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B23:B25"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A39:A41"/>
@@ -1796,9 +1799,6 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B23:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
End of Day 9/14
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96301DF9-E563-4D39-92AD-29B5FC0FC026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF93B65-BEF0-442B-AA4C-ABF1FE69F823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="117">
   <si>
     <t>Class</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>Code at end</t>
+  </si>
+  <si>
+    <t>distribution_check</t>
+  </si>
+  <si>
+    <t>windfall_regret</t>
   </si>
 </sst>
 </file>
@@ -647,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -754,18 +760,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -774,39 +807,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,8 +1091,8 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,14 +1127,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1177,10 +1177,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1197,8 +1197,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1223,10 +1223,10 @@
       <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1243,40 +1243,40 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="41"/>
-      <c r="B9" s="38"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="36" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
-      <c r="B10" s="38"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="36" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1291,8 +1291,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="42"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1307,10 +1307,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1327,8 +1327,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
-      <c r="B14" s="38"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="41"/>
-      <c r="B15" s="38"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1359,8 +1359,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
-      <c r="B16" s="38"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1375,8 +1375,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="41"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1391,8 +1391,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="41"/>
-      <c r="B18" s="38" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1409,8 +1409,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="41"/>
-      <c r="B19" s="38"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1425,8 +1425,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="41"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1441,8 +1441,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="42"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="46"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1477,10 +1477,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1497,8 +1497,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="44"/>
-      <c r="B24" s="38"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="7" t="s">
         <v>71</v>
       </c>
@@ -1513,8 +1513,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" s="45"/>
-      <c r="B25" s="39"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="7" t="s">
         <v>72</v>
       </c>
@@ -1529,14 +1529,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
@@ -1559,10 +1559,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1579,8 +1579,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="44"/>
-      <c r="B29" s="38"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
@@ -1595,8 +1595,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="45"/>
-      <c r="B30" s="39"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="7" t="s">
         <v>104</v>
       </c>
@@ -1611,10 +1611,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1631,8 +1631,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="41"/>
-      <c r="B32" s="38"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
@@ -1647,8 +1647,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="38"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
@@ -1663,8 +1663,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="42"/>
-      <c r="B34" s="39"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="46"/>
       <c r="C34" s="7" t="s">
         <v>105</v>
       </c>
@@ -1759,10 +1759,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="44" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1779,33 +1779,33 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="44"/>
-      <c r="B40" s="37"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="25" t="s">
         <v>46</v>
       </c>
       <c r="D40" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F40" s="48" t="s">
+      <c r="F40" s="36" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="44"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="7" t="s">
         <v>108</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="53" t="s">
+      <c r="E41" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F41" s="32" t="s">
@@ -1813,29 +1813,39 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
         <v>109</v>
       </c>
     </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="50" t="s">
+      <c r="A62" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="46"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="51"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="40"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="15" t="s">
@@ -1844,6 +1854,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A42:F42"/>
     <mergeCell ref="A2:F2"/>
@@ -1860,10 +1874,6 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A39:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Temporary Unit test fixes
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF93B65-BEF0-442B-AA4C-ABF1FE69F823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF1D686-4099-4A08-92F6-02F616EFB996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -766,6 +766,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -775,37 +802,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
@@ -1127,14 +1127,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1177,10 +1177,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1197,8 +1197,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="43"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1213,20 +1213,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
     </row>
     <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1243,8 +1243,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="45"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1259,8 +1259,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="45"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1275,8 +1275,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1291,8 +1291,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="51"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1307,10 +1307,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="38" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1327,8 +1327,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="50"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1359,8 +1359,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="45"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1375,8 +1375,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="50"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1391,8 +1391,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="50"/>
-      <c r="B18" s="45" t="s">
+      <c r="A18" s="42"/>
+      <c r="B18" s="39" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1409,8 +1409,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="50"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1425,8 +1425,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="50"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1441,8 +1441,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="51"/>
-      <c r="B21" s="46"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1477,10 +1477,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1497,8 +1497,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="42"/>
-      <c r="B24" s="45"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="7" t="s">
         <v>71</v>
       </c>
@@ -1513,8 +1513,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" s="43"/>
-      <c r="B25" s="46"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="7" t="s">
         <v>72</v>
       </c>
@@ -1529,14 +1529,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
@@ -1559,10 +1559,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1579,8 +1579,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="42"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="39"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
@@ -1595,8 +1595,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="43"/>
-      <c r="B30" s="46"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="7" t="s">
         <v>104</v>
       </c>
@@ -1611,10 +1611,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="38" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1631,8 +1631,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="50"/>
-      <c r="B32" s="45"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="39"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
@@ -1647,8 +1647,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="50"/>
-      <c r="B33" s="45"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
@@ -1663,8 +1663,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="51"/>
-      <c r="B34" s="46"/>
+      <c r="A34" s="43"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="7" t="s">
         <v>105</v>
       </c>
@@ -1759,10 +1759,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="41" t="s">
+      <c r="A39" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="38" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1779,8 +1779,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="42"/>
-      <c r="B40" s="48"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="25" t="s">
         <v>46</v>
       </c>
@@ -1795,7 +1795,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="42"/>
+      <c r="A41" s="45"/>
       <c r="B41" s="35" t="s">
         <v>16</v>
       </c>
@@ -1813,14 +1813,14 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
@@ -1838,14 +1838,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="38" t="s">
+      <c r="A62" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="40"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="48"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="15" t="s">
@@ -1854,12 +1854,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A42:F42"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A28:A30"/>
@@ -1872,6 +1866,12 @@
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A42:F42"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B31:B34"/>
   </mergeCells>

</xml_diff>

<commit_message>
End of Day 11/9
Working through forming opinions on proposed space reduction(s)
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A449DF59-51D7-4841-B7C5-C724943428D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C779AD-B977-45DF-8753-2A52B98E988F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -766,21 +766,39 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -790,23 +808,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,8 +1097,8 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,14 +1133,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1177,10 +1183,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1197,8 +1203,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="41"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1213,20 +1219,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1243,8 +1249,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="48"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1259,8 +1265,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="48"/>
-      <c r="B10" s="43"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1275,8 +1281,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="48"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1291,8 +1297,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="49"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1307,10 +1313,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1327,8 +1333,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="48"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1343,8 +1349,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="48"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1359,8 +1365,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="48"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1375,8 +1381,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="48"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1391,8 +1397,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="48"/>
-      <c r="B18" s="43" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1409,8 +1415,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="48"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1425,8 +1431,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="48"/>
-      <c r="B20" s="43"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1441,8 +1447,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="49"/>
-      <c r="B21" s="44"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1469,18 +1475,18 @@
       <c r="D22" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>57</v>
+      <c r="E22" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="53" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="47" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1497,8 +1503,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="40"/>
-      <c r="B24" s="43"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="7" t="s">
         <v>71</v>
       </c>
@@ -1513,8 +1519,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A25" s="41"/>
-      <c r="B25" s="44"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="7" t="s">
         <v>72</v>
       </c>
@@ -1529,14 +1535,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
@@ -1559,10 +1565,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1579,8 +1585,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="40"/>
-      <c r="B29" s="43"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
@@ -1595,8 +1601,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="7" t="s">
         <v>104</v>
       </c>
@@ -1611,10 +1617,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1631,8 +1637,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="48"/>
-      <c r="B32" s="43"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="7" t="s">
         <v>24</v>
       </c>
@@ -1647,8 +1653,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="48"/>
-      <c r="B33" s="43"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="7" t="s">
         <v>25</v>
       </c>
@@ -1663,8 +1669,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="49"/>
-      <c r="B34" s="44"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="7" t="s">
         <v>105</v>
       </c>
@@ -1759,10 +1765,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="47" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1779,8 +1785,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="40"/>
-      <c r="B40" s="46"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="25" t="s">
         <v>46</v>
       </c>
@@ -1795,7 +1801,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="40"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="35" t="s">
         <v>16</v>
       </c>
@@ -1813,14 +1819,14 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
@@ -1838,14 +1844,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="50" t="s">
+      <c r="A62" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B62" s="38"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="51"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="46"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="15" t="s">
@@ -1854,13 +1860,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B31:B34"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A28:A30"/>
@@ -1874,6 +1873,13 @@
     <mergeCell ref="A13:A21"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B31:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Running unit tests on merge_constraints
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3FE18D-63E2-43C7-80A7-11CCADB26E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82F9742-DE4B-4803-BD4D-CD61E9666068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="132">
   <si>
     <t>Class</t>
   </si>
@@ -402,6 +402,36 @@
   </si>
   <si>
     <t>bezierPoint</t>
+  </si>
+  <si>
+    <t>Has each discipline form an opinion for a proposed rule.  A value of 0.0 means the discipline is not in favor of the rule at all.  A value of 1.0 means the discipline is totally in favor of the rule.  A value of nan means the discipline is not directly impacted by the rule.</t>
+  </si>
+  <si>
+    <t>Determines if any discipline has the grounds to throw out a rule being proposed.  Dominance is naturally included in every rule proposal as each discipline is given veto power.  Vetoing is much easier early on but becomes more difficult later.</t>
+  </si>
+  <si>
+    <t>Calculate the discipline's opinion of the rule by using a Gaussian process regressor to form perceptions of feasibility throughout the remaining design space and using perceived infeasibility and feasibility to produce two metrics.</t>
+  </si>
+  <si>
+    <t>Organize previously tested points into x and y training data for a Gaussian Process Regressor (GPR).</t>
+  </si>
+  <si>
+    <t>Fits a GPR from the training data.</t>
+  </si>
+  <si>
+    <t>Predicts pass or fail amounts for unexplored areas of the discretized space remaining from the trained GPR.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Calculate the range of each predicted point within 3 standard deviations (99.7%) and then determine the average fraction of that range that has a predicted pass or fail amount falling below 0.</t>
+  </si>
+  <si>
+    <t>Calculate the fraction of each point's normal distribution for predicted pass or fail value that is above 0 for the reduced and non-reduced design spaces.  Then sum those fractions and find the ratio of the reduced sum to the non-reduced sum.</t>
+  </si>
+  <si>
+    <t>Calculate the weighted contribution of the second metric (feasibility) based on the value of the first metric with a Quadratic Bezier curve.</t>
   </si>
 </sst>
 </file>
@@ -424,7 +454,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,6 +479,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -682,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -789,77 +825,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1144,8 +1171,8 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1153,7 +1180,7 @@
     <col min="1" max="1" width="19.81640625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6328125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.08984375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.81640625" style="7"/>
@@ -1180,14 +1207,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1230,10 +1257,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1250,8 +1277,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1266,20 +1293,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
     </row>
     <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1296,8 +1323,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1312,8 +1339,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="46"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="42"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1328,8 +1355,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="46"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1344,8 +1371,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="47"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1360,10 +1387,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="53" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1380,8 +1407,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="46"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="42"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1396,8 +1423,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1412,8 +1439,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="46"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1428,8 +1455,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="46"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1444,8 +1471,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="46"/>
-      <c r="B18" s="41" t="s">
+      <c r="A18" s="45"/>
+      <c r="B18" s="42" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1462,8 +1489,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1478,8 +1505,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="46"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1494,8 +1521,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="46"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1509,111 +1536,148 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="45" t="s">
+    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="E22" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="50"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="46"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="54" t="s">
+      <c r="F22" s="36"/>
+    </row>
+    <row r="23" spans="1:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="45"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="E23" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="52"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="46"/>
-      <c r="B24" s="41" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="45"/>
+      <c r="B24" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="52"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="46"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="54" t="s">
+      <c r="D24" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="45"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="52"/>
+      <c r="D25" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="46"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="54" t="s">
+      <c r="A26" s="45"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="52"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="46"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="54" t="s">
+      <c r="D26" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="45"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="52"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="46"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="54" t="s">
+      <c r="D27" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="45"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="52"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="46"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="54" t="s">
+      <c r="D28" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="45"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="52"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="47"/>
-      <c r="B30" s="42"/>
+      <c r="D29" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="46"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="56"/>
+      <c r="D30" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="53" t="s">
         <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1630,8 +1694,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="38"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="48"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="7" t="s">
         <v>71</v>
       </c>
@@ -1646,8 +1710,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="7" t="s">
         <v>72</v>
       </c>
@@ -1662,14 +1726,14 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
@@ -1692,10 +1756,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1712,8 +1776,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="48"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="7" t="s">
         <v>18</v>
       </c>
@@ -1728,8 +1792,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="39"/>
-      <c r="B38" s="42"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="7" t="s">
         <v>102</v>
       </c>
@@ -1744,10 +1808,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1764,8 +1828,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="46"/>
-      <c r="B40" s="41"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="42"/>
       <c r="C40" s="7" t="s">
         <v>24</v>
       </c>
@@ -1780,8 +1844,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="46"/>
-      <c r="B41" s="41"/>
+      <c r="A41" s="45"/>
+      <c r="B41" s="42"/>
       <c r="C41" s="7" t="s">
         <v>25</v>
       </c>
@@ -1796,8 +1860,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="42"/>
+      <c r="A42" s="46"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7" t="s">
         <v>103</v>
       </c>
@@ -1892,10 +1956,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="53" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -1912,23 +1976,23 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="38"/>
-      <c r="B48" s="44"/>
+      <c r="A48" s="48"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="25" t="s">
         <v>46</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="30" t="s">
-        <v>9</v>
+      <c r="E48" s="56" t="s">
+        <v>128</v>
       </c>
       <c r="F48" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="38"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="35" t="s">
         <v>16</v>
       </c>
@@ -1938,47 +2002,47 @@
       <c r="D49" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="30" t="s">
-        <v>9</v>
+      <c r="E49" s="56" t="s">
+        <v>128</v>
       </c>
       <c r="F49" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="15" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="15" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="48" t="s">
+      <c r="A70" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="49"/>
+      <c r="B70" s="51"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="51"/>
+      <c r="F70" s="52"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
@@ -1987,14 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B39:B42"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A36:A38"/>
@@ -2010,6 +2066,14 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B39:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Continued unit testing on merge_constraints
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82F9742-DE4B-4803-BD4D-CD61E9666068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257B0CAE-4912-4CB6-BD5E-7268F3E03840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="132">
   <si>
     <t>Class</t>
   </si>
@@ -718,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -834,21 +834,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -858,35 +879,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1171,8 +1168,8 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1207,14 +1204,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1257,10 +1254,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1277,8 +1274,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="49"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1293,20 +1290,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-    </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+    </row>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1323,8 +1320,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="45"/>
-      <c r="B9" s="42"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1339,8 +1336,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
-      <c r="B10" s="42"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1355,8 +1352,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1371,8 +1368,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="46"/>
-      <c r="B12" s="42"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1387,10 +1384,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="46" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1406,9 +1403,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
-      <c r="B14" s="42"/>
+    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="52"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1423,8 +1420,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="45"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1439,8 +1436,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1455,8 +1452,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="45"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1471,8 +1468,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="45"/>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1489,8 +1486,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1505,8 +1502,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="45"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1521,8 +1518,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="45"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1537,10 +1534,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="46" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="37" t="s">
@@ -1555,8 +1552,8 @@
       <c r="F22" s="36"/>
     </row>
     <row r="23" spans="1:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="45"/>
-      <c r="B23" s="54"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="38" t="s">
         <v>114</v>
       </c>
@@ -1568,14 +1565,14 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="45"/>
-      <c r="B24" s="42" t="s">
+      <c r="A24" s="52"/>
+      <c r="B24" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="40" t="s">
         <v>124</v>
       </c>
       <c r="E24" s="30" t="s">
@@ -1583,8 +1580,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="45"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="38" t="s">
         <v>116</v>
       </c>
@@ -1599,8 +1596,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="45"/>
-      <c r="B26" s="42"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="38" t="s">
         <v>117</v>
       </c>
@@ -1615,8 +1612,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="45"/>
-      <c r="B27" s="42"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="38" t="s">
         <v>118</v>
       </c>
@@ -1631,8 +1628,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="45"/>
-      <c r="B28" s="42"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="38" t="s">
         <v>119</v>
       </c>
@@ -1647,8 +1644,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="45"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="38" t="s">
         <v>120</v>
       </c>
@@ -1658,10 +1655,13 @@
       <c r="E29" s="30" t="s">
         <v>9</v>
       </c>
+      <c r="F29" s="32" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="46"/>
-      <c r="B30" s="43"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="10" t="s">
         <v>121</v>
       </c>
@@ -1671,13 +1671,15 @@
       <c r="E30" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="39"/>
+      <c r="F30" s="34" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="46" t="s">
         <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1694,8 +1696,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="48"/>
-      <c r="B32" s="42"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="7" t="s">
         <v>71</v>
       </c>
@@ -1709,9 +1711,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A33" s="49"/>
-      <c r="B33" s="43"/>
+    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="45"/>
+      <c r="B33" s="48"/>
       <c r="C33" s="7" t="s">
         <v>72</v>
       </c>
@@ -1726,14 +1728,14 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
@@ -1756,10 +1758,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1775,9 +1777,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="48"/>
-      <c r="B37" s="42"/>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="44"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="7" t="s">
         <v>18</v>
       </c>
@@ -1792,8 +1794,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="49"/>
-      <c r="B38" s="43"/>
+      <c r="A38" s="45"/>
+      <c r="B38" s="48"/>
       <c r="C38" s="7" t="s">
         <v>102</v>
       </c>
@@ -1808,10 +1810,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1828,8 +1830,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="45"/>
-      <c r="B40" s="42"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="7" t="s">
         <v>24</v>
       </c>
@@ -1844,8 +1846,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="45"/>
-      <c r="B41" s="42"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="7" t="s">
         <v>25</v>
       </c>
@@ -1860,8 +1862,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="46"/>
-      <c r="B42" s="43"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7" t="s">
         <v>103</v>
       </c>
@@ -1956,10 +1958,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="47" t="s">
+      <c r="A47" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="53" t="s">
+      <c r="B47" s="46" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -1976,15 +1978,15 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="48"/>
-      <c r="B48" s="54"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="50"/>
       <c r="C48" s="25" t="s">
         <v>46</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="56" t="s">
+      <c r="E48" s="41" t="s">
         <v>128</v>
       </c>
       <c r="F48" s="32" t="s">
@@ -1992,7 +1994,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="48"/>
+      <c r="A49" s="44"/>
       <c r="B49" s="35" t="s">
         <v>16</v>
       </c>
@@ -2002,7 +2004,7 @@
       <c r="D49" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="56" t="s">
+      <c r="E49" s="41" t="s">
         <v>128</v>
       </c>
       <c r="F49" s="32" t="s">
@@ -2010,14 +2012,14 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="51" t="s">
+      <c r="A50" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
@@ -2035,14 +2037,14 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="50" t="s">
+      <c r="A70" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="51"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="51"/>
-      <c r="F70" s="52"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="55"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
@@ -2051,6 +2053,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B39:B42"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A36:A38"/>
@@ -2067,13 +2076,6 @@
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B30"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B39:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed merge_constraints unit tests
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257B0CAE-4912-4CB6-BD5E-7268F3E03840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3C671C-2807-4355-A470-51BB10ACC552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="132">
   <si>
     <t>Class</t>
   </si>
@@ -718,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -825,9 +825,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -843,21 +840,39 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -865,24 +880,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1168,8 +1165,8 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1204,14 +1201,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1254,10 +1251,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="50" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1274,8 +1271,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1290,20 +1287,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="50" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1320,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1336,8 +1333,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="52"/>
-      <c r="B10" s="47"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1352,8 +1349,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1368,8 +1365,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1384,10 +1381,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="50" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1404,8 +1401,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="52"/>
-      <c r="B14" s="47"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1420,8 +1417,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="52"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1436,8 +1433,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1452,8 +1449,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="52"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1468,8 +1465,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="42"/>
+      <c r="B18" s="52" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1486,8 +1483,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="52"/>
-      <c r="B19" s="47"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1502,8 +1499,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
-      <c r="B20" s="47"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1518,8 +1515,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="52"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1534,13 +1531,13 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="36" t="s">
         <v>113</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -1549,12 +1546,14 @@
       <c r="E22" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="36"/>
+      <c r="F22" s="31" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="52"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="38" t="s">
+      <c r="A23" s="42"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="37" t="s">
         <v>114</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1563,26 +1562,32 @@
       <c r="E23" s="30" t="s">
         <v>9</v>
       </c>
+      <c r="F23" s="32" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="52"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="42"/>
+      <c r="B24" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="39" t="s">
         <v>124</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>9</v>
       </c>
+      <c r="F24" s="32" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="52"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="38" t="s">
+      <c r="A25" s="42"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="37" t="s">
         <v>116</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -1596,9 +1601,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="52"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="38" t="s">
+      <c r="A26" s="42"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="37" t="s">
         <v>117</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -1612,9 +1617,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="52"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="38" t="s">
+      <c r="A27" s="42"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="37" t="s">
         <v>118</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -1628,9 +1633,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="52"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="38" t="s">
+      <c r="A28" s="42"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="37" t="s">
         <v>119</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -1644,9 +1649,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="52"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="38" t="s">
+      <c r="A29" s="42"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="37" t="s">
         <v>120</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -1660,8 +1665,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="53"/>
-      <c r="B30" s="48"/>
+      <c r="A30" s="43"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="10" t="s">
         <v>121</v>
       </c>
@@ -1676,10 +1681,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="50" t="s">
         <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -1696,8 +1701,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="44"/>
-      <c r="B32" s="47"/>
+      <c r="A32" s="45"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="7" t="s">
         <v>71</v>
       </c>
@@ -1712,8 +1717,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="45"/>
-      <c r="B33" s="48"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="7" t="s">
         <v>72</v>
       </c>
@@ -1728,14 +1733,14 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
@@ -1758,10 +1763,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="50" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1778,8 +1783,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="44"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="52"/>
       <c r="C37" s="7" t="s">
         <v>18</v>
       </c>
@@ -1794,8 +1799,8 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="45"/>
-      <c r="B38" s="48"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="53"/>
       <c r="C38" s="7" t="s">
         <v>102</v>
       </c>
@@ -1810,10 +1815,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="46" t="s">
+      <c r="B39" s="50" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1830,8 +1835,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="52"/>
-      <c r="B40" s="47"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="52"/>
       <c r="C40" s="7" t="s">
         <v>24</v>
       </c>
@@ -1846,8 +1851,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="52"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="7" t="s">
         <v>25</v>
       </c>
@@ -1862,8 +1867,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="53"/>
-      <c r="B42" s="48"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="7" t="s">
         <v>103</v>
       </c>
@@ -1958,10 +1963,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="46" t="s">
+      <c r="B47" s="50" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -1978,15 +1983,15 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="44"/>
-      <c r="B48" s="50"/>
+      <c r="A48" s="45"/>
+      <c r="B48" s="51"/>
       <c r="C48" s="25" t="s">
         <v>46</v>
       </c>
       <c r="D48" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E48" s="41" t="s">
+      <c r="E48" s="40" t="s">
         <v>128</v>
       </c>
       <c r="F48" s="32" t="s">
@@ -1994,7 +1999,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="44"/>
+      <c r="A49" s="45"/>
       <c r="B49" s="35" t="s">
         <v>16</v>
       </c>
@@ -2004,7 +2009,7 @@
       <c r="D49" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="41" t="s">
+      <c r="E49" s="40" t="s">
         <v>128</v>
       </c>
       <c r="F49" s="32" t="s">
@@ -2012,14 +2017,14 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
@@ -2037,14 +2042,14 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
-      <c r="F70" s="55"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="49"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="15" t="s">
@@ -2053,13 +2058,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B39:B42"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="A36:A38"/>
@@ -2076,6 +2074,13 @@
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B30"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B39:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated passfail in merge_constraints
Updated this method so that passfail data is gathered for every combination of input rules proposed...working but need to unit test and recomment!
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1294BAD-56C7-421A-A041-6ABA4A41ACCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791E6CE3-7ADE-41D5-B3FD-8843BA86A779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +491,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -715,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -834,6 +840,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -843,38 +876,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,8 +1177,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1195,14 +1213,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1245,10 +1263,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1265,8 +1283,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1281,20 +1299,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1311,8 +1329,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="41"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1327,8 +1345,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1343,8 +1361,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1359,8 +1377,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="42"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1375,10 +1393,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1395,8 +1413,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1411,8 +1429,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="41"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1427,8 +1445,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1443,8 +1461,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="41"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1459,8 +1477,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="41"/>
-      <c r="B18" s="51" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1477,8 +1495,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="41"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1493,8 +1511,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="41"/>
-      <c r="B20" s="51"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1509,8 +1527,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="41"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1525,10 +1543,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="44" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1537,32 +1555,32 @@
       <c r="D22" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="31" t="s">
+      <c r="E22" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="55" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="41"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="39" t="s">
         <v>114</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="32" t="s">
+      <c r="E23" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="57" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="41"/>
-      <c r="B24" s="51" t="s">
+      <c r="A24" s="50"/>
+      <c r="B24" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1571,32 +1589,32 @@
       <c r="D24" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="32" t="s">
+      <c r="E24" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="57" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="41"/>
-      <c r="B25" s="51"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="37" t="s">
         <v>132</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="32" t="s">
+      <c r="E25" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="57" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="41"/>
-      <c r="B26" s="51"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="37" t="s">
         <v>115</v>
       </c>
@@ -1611,8 +1629,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="41"/>
-      <c r="B27" s="51"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="37" t="s">
         <v>128</v>
       </c>
@@ -1627,8 +1645,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="41"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="37" t="s">
         <v>116</v>
       </c>
@@ -1643,8 +1661,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="41"/>
-      <c r="B29" s="51"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="37" t="s">
         <v>117</v>
       </c>
@@ -1659,8 +1677,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="37" t="s">
         <v>118</v>
       </c>
@@ -1675,8 +1693,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="51"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="37" t="s">
         <v>119</v>
       </c>
@@ -1691,8 +1709,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="42"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="46"/>
       <c r="C32" s="10" t="s">
         <v>120</v>
       </c>
@@ -1707,10 +1725,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1727,8 +1745,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="44"/>
-      <c r="B34" s="51"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1743,8 +1761,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="45"/>
-      <c r="B35" s="52"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
@@ -1759,14 +1777,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1789,10 +1807,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1809,8 +1827,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="44"/>
-      <c r="B39" s="51"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="45"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1825,8 +1843,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="45"/>
-      <c r="B40" s="52"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="46"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1841,10 +1859,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1861,8 +1879,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="41"/>
-      <c r="B42" s="51"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1877,8 +1895,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="41"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1893,8 +1911,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="42"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="46"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -1989,10 +2007,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="44" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2009,8 +2027,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="44"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="42"/>
+      <c r="B50" s="48"/>
       <c r="C50" s="25" t="s">
         <v>46</v>
       </c>
@@ -2025,7 +2043,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="44"/>
+      <c r="A51" s="42"/>
       <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
@@ -2043,14 +2061,14 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
@@ -2074,14 +2092,14 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="46" t="s">
+      <c r="A72" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="48"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="53"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
@@ -2090,6 +2108,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2106,13 +2131,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed unit tests for exploration amount
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065B2AC7-F002-4AB0-BB85-481C6F7B8C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2666EFB-B8AA-431A-925F-9FDCC76ABBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -852,6 +852,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -861,37 +888,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1177,8 +1177,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J58" sqref="J58"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1213,14 +1213,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1263,10 +1263,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1283,8 +1283,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="49"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1299,20 +1299,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1329,8 +1329,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="45"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1345,8 +1345,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1361,8 +1361,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1377,8 +1377,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="46"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1393,10 +1393,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="48" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1413,8 +1413,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1429,8 +1429,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="45"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1445,8 +1445,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1461,8 +1461,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="45"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1477,8 +1477,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="45"/>
-      <c r="B18" s="55" t="s">
+      <c r="A18" s="54"/>
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1495,8 +1495,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1511,8 +1511,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="45"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1527,8 +1527,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="45"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1543,10 +1543,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="48" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1563,8 +1563,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="45"/>
-      <c r="B23" s="54"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="39" t="s">
         <v>114</v>
       </c>
@@ -1579,8 +1579,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="45"/>
-      <c r="B24" s="55" t="s">
+      <c r="A24" s="54"/>
+      <c r="B24" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1597,8 +1597,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="45"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="37" t="s">
         <v>132</v>
       </c>
@@ -1613,8 +1613,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="45"/>
-      <c r="B26" s="55"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="37" t="s">
         <v>115</v>
       </c>
@@ -1629,8 +1629,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="45"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="37" t="s">
         <v>128</v>
       </c>
@@ -1645,8 +1645,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="45"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="37" t="s">
         <v>116</v>
       </c>
@@ -1661,8 +1661,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="45"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="37" t="s">
         <v>117</v>
       </c>
@@ -1677,8 +1677,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="45"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="37" t="s">
         <v>118</v>
       </c>
@@ -1693,8 +1693,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="45"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="37" t="s">
         <v>119</v>
       </c>
@@ -1709,8 +1709,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="46"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="10" t="s">
         <v>120</v>
       </c>
@@ -1725,10 +1725,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="48" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1745,8 +1745,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="48"/>
-      <c r="B34" s="55"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1761,8 +1761,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="49"/>
-      <c r="B35" s="56"/>
+      <c r="A35" s="47"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
@@ -1777,14 +1777,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1807,10 +1807,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1827,8 +1827,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="48"/>
-      <c r="B39" s="55"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1843,8 +1843,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="49"/>
-      <c r="B40" s="56"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1859,10 +1859,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1879,8 +1879,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="45"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1895,8 +1895,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="45"/>
-      <c r="B43" s="55"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1911,8 +1911,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="46"/>
-      <c r="B44" s="56"/>
+      <c r="A44" s="55"/>
+      <c r="B44" s="50"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -2007,10 +2007,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="48" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2027,8 +2027,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="48"/>
-      <c r="B50" s="54"/>
+      <c r="A50" s="46"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="25" t="s">
         <v>46</v>
       </c>
@@ -2043,7 +2043,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="48"/>
+      <c r="A51" s="46"/>
       <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
@@ -2061,14 +2061,14 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
@@ -2092,14 +2092,14 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="50" t="s">
+      <c r="A72" s="56" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="51"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="52"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="57"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
@@ -2108,6 +2108,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2124,13 +2131,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix unit tests for adjustCriteria
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2666EFB-B8AA-431A-925F-9FDCC76ABBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811825B4-4B00-4DB6-827B-043A9183C7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -852,21 +852,39 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -874,24 +892,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1177,8 +1177,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1213,14 +1213,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1263,10 +1263,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1283,8 +1283,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1299,20 +1299,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1329,8 +1329,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="54"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1345,8 +1345,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="54"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1361,8 +1361,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="54"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1377,8 +1377,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1393,10 +1393,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="53" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1413,8 +1413,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="45"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1429,8 +1429,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="54"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1445,8 +1445,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="54"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1461,8 +1461,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="54"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1477,8 +1477,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="54"/>
-      <c r="B18" s="49" t="s">
+      <c r="A18" s="45"/>
+      <c r="B18" s="55" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1495,8 +1495,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="54"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1511,8 +1511,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="54"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1527,8 +1527,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="54"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1543,10 +1543,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="53" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1563,8 +1563,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="54"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="39" t="s">
         <v>114</v>
       </c>
@@ -1579,8 +1579,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="54"/>
-      <c r="B24" s="49" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="55" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1597,8 +1597,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="54"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="37" t="s">
         <v>132</v>
       </c>
@@ -1613,8 +1613,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="54"/>
-      <c r="B26" s="49"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="37" t="s">
         <v>115</v>
       </c>
@@ -1629,8 +1629,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="54"/>
-      <c r="B27" s="49"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="37" t="s">
         <v>128</v>
       </c>
@@ -1645,8 +1645,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="54"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="45"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="37" t="s">
         <v>116</v>
       </c>
@@ -1661,8 +1661,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="54"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="37" t="s">
         <v>117</v>
       </c>
@@ -1677,8 +1677,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="54"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="37" t="s">
         <v>118</v>
       </c>
@@ -1693,8 +1693,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="54"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="37" t="s">
         <v>119</v>
       </c>
@@ -1709,8 +1709,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="55"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="10" t="s">
         <v>120</v>
       </c>
@@ -1725,10 +1725,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="53" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1745,8 +1745,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="46"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1761,30 +1761,30 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="47"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="43" t="s">
+      <c r="E35" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1807,10 +1807,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1827,8 +1827,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1843,8 +1843,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="56"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1859,10 +1859,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="53" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1879,8 +1879,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="54"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="45"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1895,8 +1895,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="54"/>
-      <c r="B43" s="49"/>
+      <c r="A43" s="45"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1911,8 +1911,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="55"/>
-      <c r="B44" s="50"/>
+      <c r="A44" s="46"/>
+      <c r="B44" s="56"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -2007,10 +2007,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="48" t="s">
+      <c r="B49" s="53" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2027,8 +2027,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="46"/>
-      <c r="B50" s="52"/>
+      <c r="A50" s="48"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="25" t="s">
         <v>46</v>
       </c>
@@ -2043,7 +2043,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="46"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
@@ -2061,14 +2061,14 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
@@ -2092,14 +2092,14 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="56" t="s">
+      <c r="A72" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="57"/>
+      <c r="B72" s="51"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
+      <c r="E72" s="51"/>
+      <c r="F72" s="52"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
@@ -2108,13 +2108,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2131,6 +2124,13 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed old unit tests
Still need to go back through all of the comments
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811825B4-4B00-4DB6-827B-043A9183C7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77752779-C898-4911-9263-6203DCEEC1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -721,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -843,14 +843,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -861,37 +882,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1177,8 +1171,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1213,14 +1207,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1263,10 +1257,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1283,8 +1277,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="49"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1299,20 +1293,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1329,8 +1323,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="45"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1345,8 +1339,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="45"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1361,8 +1355,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="45"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1377,8 +1371,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="46"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1393,10 +1387,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="46" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1413,8 +1407,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="45"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1429,8 +1423,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="45"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1445,8 +1439,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1461,8 +1455,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="45"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1477,8 +1471,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="45"/>
-      <c r="B18" s="55" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1495,8 +1489,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1511,8 +1505,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="45"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1527,8 +1521,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="45"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1543,10 +1537,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="46" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1558,29 +1552,29 @@
       <c r="E22" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="41" t="s">
+      <c r="F22" s="31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="45"/>
-      <c r="B23" s="54"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="39" t="s">
         <v>114</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="43" t="s">
+      <c r="E23" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="45"/>
-      <c r="B24" s="55" t="s">
+      <c r="A24" s="52"/>
+      <c r="B24" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1589,32 +1583,32 @@
       <c r="D24" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="43" t="s">
+      <c r="E24" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="45"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="37" t="s">
         <v>132</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E25" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="43" t="s">
+      <c r="E25" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="45"/>
-      <c r="B26" s="55"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="37" t="s">
         <v>115</v>
       </c>
@@ -1629,8 +1623,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="45"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="37" t="s">
         <v>128</v>
       </c>
@@ -1645,8 +1639,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="45"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="37" t="s">
         <v>116</v>
       </c>
@@ -1661,8 +1655,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="45"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="37" t="s">
         <v>117</v>
       </c>
@@ -1677,8 +1671,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="45"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="37" t="s">
         <v>118</v>
       </c>
@@ -1693,8 +1687,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="45"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="37" t="s">
         <v>119</v>
       </c>
@@ -1709,8 +1703,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="46"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="48"/>
       <c r="C32" s="10" t="s">
         <v>120</v>
       </c>
@@ -1725,10 +1719,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="46" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1745,8 +1739,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="48"/>
-      <c r="B34" s="55"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1761,8 +1755,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="49"/>
-      <c r="B35" s="56"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="48"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
@@ -1777,14 +1771,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1807,10 +1801,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1827,8 +1821,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="48"/>
-      <c r="B39" s="55"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1843,8 +1837,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="49"/>
-      <c r="B40" s="56"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="48"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1859,10 +1853,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="46" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1879,8 +1873,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="45"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="52"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1895,8 +1889,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="45"/>
-      <c r="B43" s="55"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="47"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1911,8 +1905,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="46"/>
-      <c r="B44" s="56"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -2007,10 +2001,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="46" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2027,8 +2021,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="48"/>
-      <c r="B50" s="54"/>
+      <c r="A50" s="44"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="25" t="s">
         <v>46</v>
       </c>
@@ -2043,7 +2037,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="48"/>
+      <c r="A51" s="44"/>
       <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
@@ -2061,14 +2055,14 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
@@ -2092,14 +2086,14 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="50" t="s">
+      <c r="A72" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="51"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="51"/>
-      <c r="E72" s="51"/>
-      <c r="F72" s="52"/>
+      <c r="B72" s="42"/>
+      <c r="C72" s="42"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="55"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
@@ -2108,6 +2102,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2124,13 +2125,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Unit tests and comments before Fragility complete
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77752779-C898-4911-9263-6203DCEEC1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA65081-B1D2-4759-AB45-CCB3A118115D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,7 +466,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,12 +491,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -721,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -840,27 +834,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -868,24 +874,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1171,8 +1159,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1207,14 +1195,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1260,7 +1248,7 @@
       <c r="A5" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1278,7 +1266,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="45"/>
-      <c r="B6" s="48"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1293,20 +1281,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1323,8 +1311,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1339,8 +1327,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="52"/>
-      <c r="B10" s="47"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1355,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1371,8 +1359,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="53"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1387,10 +1375,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="49" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1407,8 +1395,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="52"/>
-      <c r="B14" s="47"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1423,8 +1411,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="52"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1439,8 +1427,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1455,7 +1443,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="52"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="50"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
@@ -1471,8 +1459,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="41"/>
+      <c r="B18" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1489,8 +1477,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="52"/>
-      <c r="B19" s="47"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1505,8 +1493,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
-      <c r="B20" s="47"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1521,8 +1509,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="52"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1537,10 +1525,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="51" t="s">
+      <c r="A22" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="49" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1549,7 +1537,7 @@
       <c r="D22" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="31" t="s">
@@ -1557,7 +1545,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="52"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="50"/>
       <c r="C23" s="39" t="s">
         <v>114</v>
@@ -1565,7 +1553,7 @@
       <c r="D23" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="32" t="s">
@@ -1573,8 +1561,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="52"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="41"/>
+      <c r="B24" s="51" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1583,7 +1571,7 @@
       <c r="D24" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="41" t="s">
+      <c r="E24" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="32" t="s">
@@ -1591,15 +1579,15 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="52"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="37" t="s">
         <v>132</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E25" s="41" t="s">
+      <c r="E25" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="32" t="s">
@@ -1607,8 +1595,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="52"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="37" t="s">
         <v>115</v>
       </c>
@@ -1623,8 +1611,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="52"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="37" t="s">
         <v>128</v>
       </c>
@@ -1639,8 +1627,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="52"/>
-      <c r="B28" s="47"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="37" t="s">
         <v>116</v>
       </c>
@@ -1655,8 +1643,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="52"/>
-      <c r="B29" s="47"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="37" t="s">
         <v>117</v>
       </c>
@@ -1671,8 +1659,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="52"/>
-      <c r="B30" s="47"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="37" t="s">
         <v>118</v>
       </c>
@@ -1687,8 +1675,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="52"/>
-      <c r="B31" s="47"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="37" t="s">
         <v>119</v>
       </c>
@@ -1703,8 +1691,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="53"/>
-      <c r="B32" s="48"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="52"/>
       <c r="C32" s="10" t="s">
         <v>120</v>
       </c>
@@ -1722,7 +1710,7 @@
       <c r="A33" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="49" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1740,7 +1728,7 @@
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="44"/>
-      <c r="B34" s="47"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1756,7 +1744,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="45"/>
-      <c r="B35" s="48"/>
+      <c r="B35" s="52"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
@@ -1771,14 +1759,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1804,7 +1792,7 @@
       <c r="A38" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1822,7 +1810,7 @@
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="44"/>
-      <c r="B39" s="47"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1838,7 +1826,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="45"/>
-      <c r="B40" s="48"/>
+      <c r="B40" s="52"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1853,10 +1841,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="51" t="s">
+      <c r="A41" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1873,8 +1861,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="52"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1889,8 +1877,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="52"/>
-      <c r="B43" s="47"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1905,8 +1893,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="53"/>
-      <c r="B44" s="48"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="52"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -2004,7 +1992,7 @@
       <c r="A49" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="49" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2055,14 +2043,14 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="42"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
@@ -2086,14 +2074,14 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="54" t="s">
+      <c r="A72" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="42"/>
-      <c r="C72" s="42"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="42"/>
-      <c r="F72" s="55"/>
+      <c r="B72" s="47"/>
+      <c r="C72" s="47"/>
+      <c r="D72" s="47"/>
+      <c r="E72" s="47"/>
+      <c r="F72" s="48"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
@@ -2102,13 +2090,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2125,6 +2106,13 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Getting read for unit testing and comments on windfall_regret and fragility_check
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA65081-B1D2-4759-AB45-CCB3A118115D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E41ECA-BEFD-4CBA-A417-767D662E0495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
   <si>
     <t>Class</t>
   </si>
@@ -369,9 +369,6 @@
   </si>
   <si>
     <t>Code at end</t>
-  </si>
-  <si>
-    <t>distribution_check</t>
   </si>
   <si>
     <t>windfall_regret</t>
@@ -834,6 +831,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -843,37 +867,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1159,8 +1156,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1195,14 +1192,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1245,10 +1242,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1265,8 +1262,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1281,20 +1278,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1311,8 +1308,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="41"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1327,8 +1324,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="41"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1343,8 +1340,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="41"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1359,8 +1356,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="42"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1375,10 +1372,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="44" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1395,8 +1392,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="41"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1411,8 +1408,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="41"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1427,8 +1424,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1443,8 +1440,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="41"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1459,8 +1456,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="41"/>
-      <c r="B18" s="51" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1477,8 +1474,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="41"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1493,8 +1490,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="41"/>
-      <c r="B20" s="51"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1509,8 +1506,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="41"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1525,34 +1522,34 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="44" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="50"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="41"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>122</v>
-      </c>
       <c r="E23" s="30" t="s">
         <v>9</v>
       </c>
@@ -1561,15 +1558,15 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="41"/>
-      <c r="B24" s="51" t="s">
+      <c r="A24" s="50"/>
+      <c r="B24" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>9</v>
@@ -1579,29 +1576,29 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="41"/>
-      <c r="B25" s="51"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="50"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="41"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>135</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>9</v>
@@ -1611,14 +1608,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="41"/>
-      <c r="B27" s="51"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="E27" s="30" t="s">
         <v>9</v>
       </c>
@@ -1627,29 +1624,29 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="41"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="50"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="41"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="37" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="E29" s="30" t="s">
         <v>9</v>
@@ -1659,46 +1656,46 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="50"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="37" t="s">
+      <c r="E31" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="51"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D32" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="42"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>127</v>
-      </c>
       <c r="E32" s="33" t="s">
         <v>9</v>
       </c>
@@ -1707,10 +1704,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
+      <c r="A33" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1727,8 +1724,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="44"/>
-      <c r="B34" s="51"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1743,8 +1740,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="45"/>
-      <c r="B35" s="52"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
@@ -1759,14 +1756,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1789,10 +1786,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="43" t="s">
+      <c r="A38" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1809,8 +1806,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="44"/>
-      <c r="B39" s="51"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="45"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1825,8 +1822,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="45"/>
-      <c r="B40" s="52"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="46"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1841,10 +1838,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1861,8 +1858,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="41"/>
-      <c r="B42" s="51"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="45"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1877,8 +1874,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="41"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="45"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1893,8 +1890,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="42"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="46"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -1989,10 +1986,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="43" t="s">
+      <c r="A49" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="44" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2009,8 +2006,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="44"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="42"/>
+      <c r="B50" s="48"/>
       <c r="C50" s="25" t="s">
         <v>46</v>
       </c>
@@ -2025,7 +2022,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="44"/>
+      <c r="A51" s="42"/>
       <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
@@ -2043,24 +2040,24 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2068,20 +2065,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="46" t="s">
+      <c r="A72" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="48"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="53"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="15" t="s">
@@ -2090,6 +2082,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2106,13 +2105,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Getting through comments in windfall_regret
Finished calcWindRegret comments
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E41ECA-BEFD-4CBA-A417-767D662E0495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1C6170-D13A-44D9-8F99-B226C073C89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="145">
   <si>
     <t>Class</t>
   </si>
@@ -365,12 +365,6 @@
     <t>FRAGILITY</t>
   </si>
   <si>
-    <t>PLOTTING</t>
-  </si>
-  <si>
-    <t>Code at end</t>
-  </si>
-  <si>
     <t>windfall_regret</t>
   </si>
   <si>
@@ -441,6 +435,42 @@
   </si>
   <si>
     <t>Calculate the discipline's opinion of the rule with passing and failure amount data and corresponding perceived infeasibility and feasibility to produce two metrics.</t>
+  </si>
+  <si>
+    <t>calcWindRegret</t>
+  </si>
+  <si>
+    <t>quantRisk</t>
+  </si>
+  <si>
+    <t>plotWindRegret</t>
+  </si>
+  <si>
+    <t>initializeWR</t>
+  </si>
+  <si>
+    <t>getIndices</t>
+  </si>
+  <si>
+    <t>complementProb</t>
+  </si>
+  <si>
+    <t>assignWR</t>
+  </si>
+  <si>
+    <t>checkFragility</t>
+  </si>
+  <si>
+    <t>newCombo</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Gathers windfall and regret data for non-reduced, reduced, and leftover design spaces.  The windreg data is used for plotting purposes.  The run_wind and run_reg data is used for risk quantification.</t>
   </si>
 </sst>
 </file>
@@ -463,7 +493,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,6 +518,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -685,23 +721,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="mediumDashed">
         <color indexed="64"/>
       </top>
@@ -712,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -825,27 +859,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -855,23 +901,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1153,11 +1199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1192,14 +1238,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1242,10 +1288,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1262,8 +1308,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="43"/>
-      <c r="B6" s="46"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1278,20 +1324,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1308,8 +1354,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="45"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1324,8 +1370,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="45"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1340,8 +1386,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1356,8 +1402,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="51"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1372,10 +1418,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1392,8 +1438,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="50"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1408,8 +1454,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
-      <c r="B15" s="45"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1424,8 +1470,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="45"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1440,7 +1486,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="50"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="48"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
@@ -1456,8 +1502,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="50"/>
-      <c r="B18" s="45" t="s">
+      <c r="A18" s="41"/>
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1474,8 +1520,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="50"/>
-      <c r="B19" s="45"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1490,8 +1536,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="50"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1506,8 +1552,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="50"/>
-      <c r="B21" s="45"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1522,17 +1568,17 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="47" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>9</v>
@@ -1542,13 +1588,13 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="50"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="48"/>
       <c r="C23" s="39" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E23" s="30" t="s">
         <v>9</v>
@@ -1558,15 +1604,15 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="45" t="s">
+      <c r="A24" s="41"/>
+      <c r="B24" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>130</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>132</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>9</v>
@@ -1576,14 +1622,14 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="50"/>
-      <c r="B25" s="45"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="E25" s="30" t="s">
         <v>9</v>
       </c>
@@ -1592,13 +1638,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="50"/>
-      <c r="B26" s="45"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>9</v>
@@ -1608,13 +1654,13 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="50"/>
-      <c r="B27" s="45"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="49"/>
       <c r="C27" s="37" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E27" s="30" t="s">
         <v>9</v>
@@ -1624,13 +1670,13 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="50"/>
-      <c r="B28" s="45"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>9</v>
@@ -1640,13 +1686,13 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="50"/>
-      <c r="B29" s="45"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E29" s="30" t="s">
         <v>9</v>
@@ -1656,46 +1702,46 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="50"/>
-      <c r="B30" s="45"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="41"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="42"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D32" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="50"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="51"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>126</v>
-      </c>
       <c r="E32" s="33" t="s">
         <v>9</v>
       </c>
@@ -1704,10 +1750,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="44" t="s">
+      <c r="B33" s="47" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1724,8 +1770,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1740,8 +1786,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="43"/>
-      <c r="B35" s="46"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="50"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
@@ -1756,14 +1802,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1786,10 +1832,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="44" t="s">
+      <c r="B38" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1806,8 +1852,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="42"/>
-      <c r="B39" s="45"/>
+      <c r="A39" s="44"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1822,8 +1868,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="43"/>
-      <c r="B40" s="46"/>
+      <c r="A40" s="45"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1838,10 +1884,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1858,8 +1904,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="50"/>
-      <c r="B42" s="45"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1874,8 +1920,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="50"/>
-      <c r="B43" s="45"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1890,8 +1936,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="51"/>
-      <c r="B44" s="46"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="50"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -1986,10 +2032,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="47" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2006,7 +2052,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="42"/>
+      <c r="A50" s="44"/>
       <c r="B50" s="48"/>
       <c r="C50" s="25" t="s">
         <v>46</v>
@@ -2022,7 +2068,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="42"/>
+      <c r="A51" s="44"/>
       <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
@@ -2040,55 +2086,155 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="40" t="s">
+      <c r="A52" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="40"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>115</v>
+      <c r="B52" s="51"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+    </row>
+    <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="44"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F54" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="44"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" s="26"/>
+      <c r="E55" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="44"/>
+      <c r="B56" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F56" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="44"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F57" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="44"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F58" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="45"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" s="24"/>
+      <c r="E59" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F59" s="57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="F60" s="55" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="40"/>
-      <c r="F72" s="53"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="15" t="s">
-        <v>110</v>
+      <c r="A61" s="45"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F61" s="57" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
+  <mergeCells count="27">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2105,6 +2251,17 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished comments on code before post-processing
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3D1FEC-AC68-40D0-B292-31AD82A60FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7944083B-02E2-4D4A-9F79-5D95E2533CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="154">
   <si>
     <t>Class</t>
   </si>
@@ -464,9 +464,6 @@
     <t>newCombo</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Incomplete</t>
   </si>
   <si>
@@ -495,6 +492,12 @@
   </si>
   <si>
     <t>Selects one rule combo to move forward from the all of the rule combo(s) not leading to any fragile design spaces while adding any rule(s) that only lead to fragile design spaces to the banned rule list.</t>
+  </si>
+  <si>
+    <t>POST-PROCESSING</t>
+  </si>
+  <si>
+    <t>load_data</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -889,62 +892,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1226,11 +1223,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1265,14 +1262,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1315,10 +1312,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1335,8 +1332,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="10" t="s">
         <v>62</v>
       </c>
@@ -1351,20 +1348,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1381,8 +1378,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="54"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="48"/>
       <c r="C9" s="7" t="s">
         <v>76</v>
       </c>
@@ -1397,8 +1394,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="54"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="48"/>
       <c r="C10" s="7" t="s">
         <v>77</v>
       </c>
@@ -1413,8 +1410,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="54"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="7" t="s">
         <v>78</v>
       </c>
@@ -1429,8 +1426,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1445,10 +1442,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1465,8 +1462,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1481,8 +1478,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="54"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
@@ -1497,8 +1494,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="54"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1513,8 +1510,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="54"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="25" t="s">
         <v>87</v>
       </c>
@@ -1529,8 +1526,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="54"/>
-      <c r="B18" s="49" t="s">
+      <c r="A18" s="53"/>
+      <c r="B18" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1547,8 +1544,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="54"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="7" t="s">
         <v>92</v>
       </c>
@@ -1563,8 +1560,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="54"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="48"/>
       <c r="C20" s="7" t="s">
         <v>67</v>
       </c>
@@ -1579,8 +1576,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="54"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="48"/>
       <c r="C21" s="7" t="s">
         <v>94</v>
       </c>
@@ -1595,10 +1592,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="47" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1615,8 +1612,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="54"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="39" t="s">
         <v>111</v>
       </c>
@@ -1631,8 +1628,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="54"/>
-      <c r="B24" s="49" t="s">
+      <c r="A24" s="53"/>
+      <c r="B24" s="48" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1649,8 +1646,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="54"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="48"/>
       <c r="C25" s="37" t="s">
         <v>129</v>
       </c>
@@ -1665,8 +1662,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="54"/>
-      <c r="B26" s="49"/>
+      <c r="A26" s="53"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="37" t="s">
         <v>112</v>
       </c>
@@ -1681,8 +1678,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="54"/>
-      <c r="B27" s="49"/>
+      <c r="A27" s="53"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="37" t="s">
         <v>125</v>
       </c>
@@ -1697,8 +1694,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="54"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="53"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="37" t="s">
         <v>113</v>
       </c>
@@ -1713,8 +1710,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="54"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="37" t="s">
         <v>114</v>
       </c>
@@ -1729,8 +1726,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="54"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="53"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="37" t="s">
         <v>115</v>
       </c>
@@ -1745,8 +1742,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="54"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="53"/>
+      <c r="B31" s="48"/>
       <c r="C31" s="37" t="s">
         <v>116</v>
       </c>
@@ -1761,8 +1758,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="55"/>
-      <c r="B32" s="50"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="51"/>
       <c r="C32" s="10" t="s">
         <v>117</v>
       </c>
@@ -1777,10 +1774,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="47" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1797,8 +1794,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="46"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="48"/>
       <c r="C34" s="7" t="s">
         <v>71</v>
       </c>
@@ -1813,8 +1810,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="47"/>
-      <c r="B35" s="50"/>
+      <c r="A35" s="46"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="7" t="s">
         <v>72</v>
       </c>
@@ -1829,14 +1826,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1859,10 +1856,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1879,8 +1876,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="45"/>
+      <c r="B39" s="48"/>
       <c r="C39" s="7" t="s">
         <v>18</v>
       </c>
@@ -1895,8 +1892,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="7" t="s">
         <v>102</v>
       </c>
@@ -1911,10 +1908,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1931,8 +1928,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="54"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7" t="s">
         <v>24</v>
       </c>
@@ -1947,8 +1944,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="54"/>
-      <c r="B43" s="49"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7" t="s">
         <v>25</v>
       </c>
@@ -1963,8 +1960,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="55"/>
-      <c r="B44" s="50"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="7" t="s">
         <v>103</v>
       </c>
@@ -2059,10 +2056,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="48" t="s">
+      <c r="B49" s="47" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2079,8 +2076,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="46"/>
-      <c r="B50" s="52"/>
+      <c r="A50" s="45"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="25" t="s">
         <v>46</v>
       </c>
@@ -2095,7 +2092,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="46"/>
+      <c r="A51" s="45"/>
       <c r="B51" s="35" t="s">
         <v>16</v>
       </c>
@@ -2113,59 +2110,59 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="B52" s="51"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="48" t="s">
+      <c r="B53" s="47" t="s">
         <v>127</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>133</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E53" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="41" t="s">
-        <v>143</v>
+      <c r="F53" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="46"/>
-      <c r="B54" s="49"/>
+      <c r="A54" s="45"/>
+      <c r="B54" s="48"/>
       <c r="C54" s="7" t="s">
         <v>134</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E54" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F54" s="41" t="s">
-        <v>143</v>
+      <c r="F54" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="46"/>
-      <c r="B55" s="52"/>
+      <c r="A55" s="45"/>
+      <c r="B55" s="49"/>
       <c r="C55" s="25" t="s">
         <v>135</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E55" s="30" t="s">
         <v>9</v>
@@ -2175,120 +2172,125 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="46"/>
-      <c r="B56" s="56" t="s">
+      <c r="A56" s="45"/>
+      <c r="B56" s="50" t="s">
         <v>16</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>136</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E56" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="41" t="s">
-        <v>143</v>
+      <c r="F56" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="46"/>
-      <c r="B57" s="49"/>
+      <c r="A57" s="45"/>
+      <c r="B57" s="48"/>
       <c r="C57" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E57" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F57" s="41" t="s">
-        <v>143</v>
+      <c r="F57" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="46"/>
-      <c r="B58" s="49"/>
+      <c r="A58" s="45"/>
+      <c r="B58" s="48"/>
       <c r="C58" s="7" t="s">
         <v>138</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E58" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="41" t="s">
-        <v>143</v>
+      <c r="F58" s="40" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="47"/>
-      <c r="B59" s="50"/>
+      <c r="A59" s="46"/>
+      <c r="B59" s="51"/>
       <c r="C59" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D59" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="E59" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="43" t="s">
-        <v>143</v>
+      <c r="D59" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E59" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="41" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="48" t="s">
+      <c r="B60" s="47" t="s">
         <v>140</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E60" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="F60" s="41" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="47"/>
-      <c r="B61" s="50"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="51"/>
       <c r="C61" s="10" t="s">
         <v>141</v>
       </c>
       <c r="D61" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="E61" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="F61" s="43" t="s">
-        <v>143</v>
+      <c r="B62" s="55"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="15" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
+  <mergeCells count="28">
+    <mergeCell ref="A62:F62"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2305,6 +2307,17 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Continuing to comment on code
Now in the post-processing section before getting to the unit tests
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7944083B-02E2-4D4A-9F79-5D95E2533CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE3481A-64CD-420C-90DA-08DF4A0E7D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="170">
   <si>
     <t>Class</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Unittest necessary/complete?</t>
-  </si>
-  <si>
     <t>exploration_amount</t>
   </si>
   <si>
@@ -498,6 +495,57 @@
   </si>
   <si>
     <t>load_data</t>
+  </si>
+  <si>
+    <t>loadSpaceRemaining</t>
+  </si>
+  <si>
+    <t>Loads space remaining data from all HDF5 files in a directory and reconstructs the original data structure.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>read_data</t>
+  </si>
+  <si>
+    <t>Reads all of the space remaining data from each test case and gathers passing and failing information of original space remaining arrays for each discipline from SBD1 problem.</t>
+  </si>
+  <si>
+    <t>organize_data</t>
+  </si>
+  <si>
+    <t>createTimeData</t>
+  </si>
+  <si>
+    <t>fillSpaceRemaining</t>
+  </si>
+  <si>
+    <t>findAverages</t>
+  </si>
+  <si>
+    <t>findPercentages</t>
+  </si>
+  <si>
+    <t>countBooleans</t>
+  </si>
+  <si>
+    <t>plot_data</t>
+  </si>
+  <si>
+    <t>Unittest complete?</t>
+  </si>
+  <si>
+    <t>Determine all of the times that data was collected for a test case by consulting the console output files.</t>
+  </si>
+  <si>
+    <t>Goes through all of the runs for a test case and organizes the total and feasible space remaining such that their are data points for every time iteration.</t>
+  </si>
+  <si>
+    <t>Finds the indices in the original space remaining array that still exist in the reduced space remaining array.</t>
+  </si>
+  <si>
+    <t>Counts the remaining number of passing data points for the reduced design space.</t>
   </si>
 </sst>
 </file>
@@ -552,7 +600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -769,11 +817,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -904,6 +961,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -919,29 +979,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1223,21 +1286,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="71.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.81640625" style="7"/>
   </cols>
   <sheetData>
@@ -1258,18 +1321,18 @@
         <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="A2" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1288,1008 +1351,1161 @@
         <v>9</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="B5" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="47"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="46"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="10" t="s">
+      <c r="E6" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+    </row>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="B8" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="54"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-    </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="54"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="54"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="55"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="53"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="54"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="47" t="s">
+      <c r="E13" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="54"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="54"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="54"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="54"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="54"/>
+      <c r="B18" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="54"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="54"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="54"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="53"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="53"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="53"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="53"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="26" t="s">
+      <c r="B22" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="54"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="54"/>
+      <c r="B24" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="54"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="54"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A27" s="54"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="54"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="54"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="54"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="55"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="53"/>
-      <c r="B18" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="53"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="53"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="53"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="53"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="53"/>
-      <c r="B24" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="53"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="53"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="53"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="53"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="53"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="53"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="53"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="54"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="E33" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="46"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E33" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="45"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="7" t="s">
+      <c r="E34" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="47"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D35" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="46"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>101</v>
-      </c>
       <c r="E35" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
+      <c r="A36" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E37" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="44" t="s">
+      <c r="B38" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="C38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="46"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="45"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="9" t="s">
+      <c r="E39" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="46"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="7" t="s">
+      <c r="E40" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="54"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="54"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="55"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="53"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="53"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="54"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="7" t="s">
+      <c r="D44" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>104</v>
-      </c>
       <c r="E44" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="C45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="E45" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F45" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="E46" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E47" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F47" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="D48" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="E48" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="E48" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="44" t="s">
+      <c r="B49" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="47" t="s">
+      <c r="C49" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="46"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D50" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E49" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="45"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D50" s="26" t="s">
+      <c r="E50" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="46"/>
+      <c r="B51" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E50" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="45"/>
-      <c r="B51" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="7" t="s">
+      <c r="E51" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" s="51"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+    </row>
+    <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A54" s="46"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="46"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="46"/>
+      <c r="B56" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="46"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="46"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="47"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="B52" s="56"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
-    </row>
-    <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E53" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="45"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="45"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D55" s="26" t="s">
+      <c r="B60" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E55" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="45"/>
-      <c r="B56" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="45"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E57" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="45"/>
-      <c r="B58" s="48"/>
-      <c r="C58" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E58" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="46"/>
-      <c r="B59" s="51"/>
-      <c r="C59" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D59" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="E59" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="41" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B60" s="47" t="s">
+      <c r="E60" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="47"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D60" s="6" t="s">
+      <c r="D61" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E60" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="46"/>
-      <c r="B61" s="51"/>
-      <c r="C61" s="10" t="s">
+      <c r="E61" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="D61" s="24" t="s">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="E61" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="41" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="55" t="s">
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+    </row>
+    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="15" t="s">
+      <c r="B63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>153</v>
       </c>
+      <c r="D63" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="E63" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="E64" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="46"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="46"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D67" s="9"/>
+      <c r="E67" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="F67" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="46"/>
+      <c r="B68" s="52"/>
+      <c r="C68" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D68" s="9"/>
+      <c r="E68" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="F68" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="46"/>
+      <c r="B69" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="47"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E70" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="15" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="31">
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
@@ -2306,18 +2522,6 @@
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working through unit tests
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35F32F-6948-4B4D-B0C3-41615A23A6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E44E48-1705-491E-B40C-1821B83F14DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -888,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1022,6 +1022,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1031,50 +1040,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1359,8 +1353,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1395,14 +1389,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1445,10 +1439,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1465,8 +1459,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1481,20 +1475,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1511,8 +1505,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="54"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1527,8 +1521,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="54"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1543,8 +1537,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="54"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1559,8 +1553,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1575,10 +1569,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="52" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1595,8 +1589,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1611,8 +1605,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="54"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1627,8 +1621,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="54"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1643,8 +1637,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="54"/>
-      <c r="B17" s="50"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1659,8 +1653,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="54"/>
-      <c r="B18" s="49" t="s">
+      <c r="A18" s="58"/>
+      <c r="B18" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1677,8 +1671,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="54"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1693,8 +1687,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="54"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1709,8 +1703,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="54"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1725,10 +1719,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="52" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1745,8 +1739,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="54"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1761,8 +1755,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="54"/>
-      <c r="B24" s="49" t="s">
+      <c r="A24" s="58"/>
+      <c r="B24" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1779,8 +1773,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="54"/>
-      <c r="B25" s="49"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1795,8 +1789,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="54"/>
-      <c r="B26" s="49"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1811,8 +1805,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="54"/>
-      <c r="B27" s="49"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1827,8 +1821,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="54"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1843,8 +1837,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="54"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1859,8 +1853,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="54"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1875,8 +1869,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="54"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1891,8 +1885,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="55"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="59"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1907,10 +1901,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="52" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1927,8 +1921,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="46"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1943,8 +1937,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="47"/>
-      <c r="B35" s="52"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -1959,14 +1953,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1989,10 +1983,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2009,8 +2003,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="49"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2025,8 +2019,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="52"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2041,10 +2035,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2061,8 +2055,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="54"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2077,8 +2071,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="54"/>
-      <c r="B43" s="49"/>
+      <c r="A43" s="58"/>
+      <c r="B43" s="53"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2093,8 +2087,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="55"/>
-      <c r="B44" s="52"/>
+      <c r="A44" s="59"/>
+      <c r="B44" s="54"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2189,10 +2183,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="48" t="s">
+      <c r="B49" s="52" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2209,8 +2203,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="46"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="49"/>
+      <c r="B50" s="56"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2225,7 +2219,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="46"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2243,20 +2237,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="48" t="s">
+      <c r="B53" s="52" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2273,8 +2267,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="46"/>
-      <c r="B54" s="49"/>
+      <c r="A54" s="49"/>
+      <c r="B54" s="53"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2289,8 +2283,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="46"/>
-      <c r="B55" s="50"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2305,8 +2299,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="46"/>
-      <c r="B56" s="51" t="s">
+      <c r="A56" s="49"/>
+      <c r="B56" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2323,8 +2317,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="46"/>
-      <c r="B57" s="49"/>
+      <c r="A57" s="49"/>
+      <c r="B57" s="53"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2339,8 +2333,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="46"/>
-      <c r="B58" s="49"/>
+      <c r="A58" s="49"/>
+      <c r="B58" s="53"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2355,8 +2349,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="47"/>
-      <c r="B59" s="52"/>
+      <c r="A59" s="50"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2371,10 +2365,10 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="48" t="s">
+      <c r="B60" s="52" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2391,8 +2385,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="47"/>
-      <c r="B61" s="52"/>
+      <c r="A61" s="50"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2407,14 +2401,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="56" t="s">
+      <c r="A62" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -2457,10 +2451,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="45" t="s">
+      <c r="A65" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="B65" s="48" t="s">
+      <c r="B65" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -2477,8 +2471,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="46"/>
-      <c r="B66" s="49"/>
+      <c r="A66" s="49"/>
+      <c r="B66" s="53"/>
       <c r="C66" s="7" t="s">
         <v>159</v>
       </c>
@@ -2493,8 +2487,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="46"/>
-      <c r="B67" s="49"/>
+      <c r="A67" s="49"/>
+      <c r="B67" s="53"/>
       <c r="C67" s="7" t="s">
         <v>160</v>
       </c>
@@ -2509,8 +2503,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="46"/>
-      <c r="B68" s="50"/>
+      <c r="A68" s="49"/>
+      <c r="B68" s="56"/>
       <c r="C68" s="7" t="s">
         <v>161</v>
       </c>
@@ -2525,8 +2519,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="46"/>
-      <c r="B69" s="51" t="s">
+      <c r="A69" s="49"/>
+      <c r="B69" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="44" t="s">
@@ -2543,8 +2537,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="47"/>
-      <c r="B70" s="52"/>
+      <c r="A70" s="50"/>
+      <c r="B70" s="54"/>
       <c r="C70" s="10" t="s">
         <v>162</v>
       </c>
@@ -2554,12 +2548,12 @@
       <c r="E70" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F70" s="41" t="s">
-        <v>141</v>
+      <c r="F70" s="34" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="45" t="s">
+      <c r="A71" s="48" t="s">
         <v>163</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -2579,15 +2573,14 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="46"/>
-      <c r="B72" s="58"/>
-      <c r="C72" s="58" t="s">
+      <c r="A72" s="49"/>
+      <c r="C72" s="7" t="s">
         <v>172</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E72" s="62" t="s">
+      <c r="E72" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F72" s="32" t="s">
@@ -2595,14 +2588,14 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="47"/>
-      <c r="B73" s="59" t="s">
+      <c r="A73" s="50"/>
+      <c r="B73" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="60" t="s">
+      <c r="C73" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="D73" s="61" t="s">
+      <c r="D73" s="47" t="s">
         <v>174</v>
       </c>
       <c r="E73" s="33" t="s">
@@ -2614,6 +2607,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A71:A73"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
@@ -2630,22 +2639,6 @@
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished unit tests for organize_data
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E44E48-1705-491E-B40C-1821B83F14DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1543337C-A971-4A17-98DD-0CFC481DD94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,35 +1040,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1352,9 +1352,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1389,14 +1389,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1442,7 +1442,7 @@
       <c r="A5" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1460,7 +1460,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="50"/>
-      <c r="B6" s="54"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1475,20 +1475,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1506,7 +1506,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="58"/>
-      <c r="B9" s="53"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="58"/>
-      <c r="B10" s="53"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="58"/>
-      <c r="B11" s="53"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
-      <c r="B12" s="53"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="A13" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="51" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1590,7 +1590,7 @@
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="58"/>
-      <c r="B14" s="53"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1606,7 +1606,7 @@
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="58"/>
-      <c r="B15" s="53"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="58"/>
-      <c r="B16" s="53"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="58"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="58"/>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1672,7 +1672,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="58"/>
-      <c r="B19" s="53"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="58"/>
-      <c r="B20" s="53"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="58"/>
-      <c r="B21" s="53"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="A22" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="51" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1740,7 +1740,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="58"/>
-      <c r="B23" s="56"/>
+      <c r="B23" s="53"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="58"/>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1774,7 +1774,7 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="58"/>
-      <c r="B25" s="53"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="58"/>
-      <c r="B26" s="53"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="58"/>
-      <c r="B27" s="53"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="58"/>
-      <c r="B28" s="53"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="58"/>
-      <c r="B29" s="53"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="58"/>
-      <c r="B30" s="53"/>
+      <c r="B30" s="52"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="58"/>
-      <c r="B31" s="53"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="59"/>
-      <c r="B32" s="54"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="A33" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="51" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1922,7 +1922,7 @@
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="49"/>
-      <c r="B34" s="53"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="50"/>
-      <c r="B35" s="54"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -1953,14 +1953,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1986,7 +1986,7 @@
       <c r="A38" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2004,7 +2004,7 @@
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="49"/>
-      <c r="B39" s="53"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="50"/>
-      <c r="B40" s="54"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="A41" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2056,7 +2056,7 @@
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="58"/>
-      <c r="B42" s="53"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="58"/>
-      <c r="B43" s="53"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="59"/>
-      <c r="B44" s="54"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="A49" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="52" t="s">
+      <c r="B49" s="51" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2204,7 +2204,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="49"/>
-      <c r="B50" s="56"/>
+      <c r="B50" s="53"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2237,20 +2237,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="55"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="52" t="s">
+      <c r="B53" s="51" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2268,7 +2268,7 @@
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A54" s="49"/>
-      <c r="B54" s="53"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="49"/>
-      <c r="B55" s="56"/>
+      <c r="B55" s="53"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="49"/>
-      <c r="B56" s="60" t="s">
+      <c r="B56" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2318,7 +2318,7 @@
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="49"/>
-      <c r="B57" s="53"/>
+      <c r="B57" s="52"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="49"/>
-      <c r="B58" s="53"/>
+      <c r="B58" s="52"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="50"/>
-      <c r="B59" s="54"/>
+      <c r="B59" s="55"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="A60" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="52" t="s">
+      <c r="B60" s="51" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2386,7 +2386,7 @@
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="50"/>
-      <c r="B61" s="54"/>
+      <c r="B61" s="55"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2401,14 +2401,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -2454,7 +2454,7 @@
       <c r="A65" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="B65" s="52" t="s">
+      <c r="B65" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -2472,7 +2472,7 @@
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="49"/>
-      <c r="B66" s="53"/>
+      <c r="B66" s="52"/>
       <c r="C66" s="7" t="s">
         <v>159</v>
       </c>
@@ -2482,13 +2482,13 @@
       <c r="E66" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="40" t="s">
-        <v>141</v>
+      <c r="F66" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="49"/>
-      <c r="B67" s="53"/>
+      <c r="B67" s="52"/>
       <c r="C67" s="7" t="s">
         <v>160</v>
       </c>
@@ -2498,13 +2498,13 @@
       <c r="E67" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F67" s="40" t="s">
-        <v>141</v>
+      <c r="F67" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="49"/>
-      <c r="B68" s="56"/>
+      <c r="B68" s="53"/>
       <c r="C68" s="7" t="s">
         <v>161</v>
       </c>
@@ -2514,13 +2514,13 @@
       <c r="E68" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="40" t="s">
-        <v>141</v>
+      <c r="F68" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="49"/>
-      <c r="B69" s="60" t="s">
+      <c r="B69" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="44" t="s">
@@ -2532,13 +2532,13 @@
       <c r="E69" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F69" s="40" t="s">
-        <v>141</v>
+      <c r="F69" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="50"/>
-      <c r="B70" s="54"/>
+      <c r="B70" s="55"/>
       <c r="C70" s="10" t="s">
         <v>162</v>
       </c>
@@ -2607,22 +2607,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A71:A73"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
@@ -2639,6 +2623,22 @@
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete Unit tests on fragility_check
Just have windfall_regret unit tests left to go
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1543337C-A971-4A17-98DD-0CFC481DD94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00175FD-F70D-4971-A7FC-4535C1D50B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,35 +1040,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1353,8 +1353,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G72" sqref="G72"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1389,14 +1389,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1442,7 +1442,7 @@
       <c r="A5" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1460,7 +1460,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="50"/>
-      <c r="B6" s="55"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1475,20 +1475,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1506,7 +1506,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="58"/>
-      <c r="B9" s="52"/>
+      <c r="B9" s="53"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="58"/>
-      <c r="B10" s="52"/>
+      <c r="B10" s="53"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="58"/>
-      <c r="B11" s="52"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="59"/>
-      <c r="B12" s="52"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="A13" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="52" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1590,7 +1590,7 @@
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="58"/>
-      <c r="B14" s="52"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1606,7 +1606,7 @@
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="58"/>
-      <c r="B15" s="52"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1622,7 +1622,7 @@
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="58"/>
-      <c r="B16" s="52"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="58"/>
-      <c r="B17" s="53"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="58"/>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1672,7 +1672,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="58"/>
-      <c r="B19" s="52"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="58"/>
-      <c r="B20" s="52"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="58"/>
-      <c r="B21" s="52"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="A22" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="52" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1740,7 +1740,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="58"/>
-      <c r="B23" s="53"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="58"/>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1774,7 +1774,7 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="58"/>
-      <c r="B25" s="52"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="58"/>
-      <c r="B26" s="52"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="58"/>
-      <c r="B27" s="52"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="58"/>
-      <c r="B28" s="52"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="58"/>
-      <c r="B29" s="52"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="58"/>
-      <c r="B30" s="52"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="58"/>
-      <c r="B31" s="52"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="59"/>
-      <c r="B32" s="55"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="A33" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="52" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1922,7 +1922,7 @@
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="49"/>
-      <c r="B34" s="52"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="50"/>
-      <c r="B35" s="55"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -1953,14 +1953,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1986,7 +1986,7 @@
       <c r="A38" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2004,7 +2004,7 @@
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="49"/>
-      <c r="B39" s="52"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="50"/>
-      <c r="B40" s="55"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="A41" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2056,7 +2056,7 @@
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="58"/>
-      <c r="B42" s="52"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="58"/>
-      <c r="B43" s="52"/>
+      <c r="B43" s="53"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="59"/>
-      <c r="B44" s="55"/>
+      <c r="B44" s="54"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2186,7 +2186,7 @@
       <c r="A49" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="51" t="s">
+      <c r="B49" s="52" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2204,7 +2204,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="49"/>
-      <c r="B50" s="53"/>
+      <c r="B50" s="56"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2237,20 +2237,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="56" t="s">
+      <c r="A52" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="60"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="51" t="s">
+      <c r="B53" s="52" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2268,7 +2268,7 @@
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A54" s="49"/>
-      <c r="B54" s="52"/>
+      <c r="B54" s="53"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="49"/>
-      <c r="B55" s="53"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="49"/>
-      <c r="B56" s="54" t="s">
+      <c r="B56" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2318,7 +2318,7 @@
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="49"/>
-      <c r="B57" s="52"/>
+      <c r="B57" s="53"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="49"/>
-      <c r="B58" s="52"/>
+      <c r="B58" s="53"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="50"/>
-      <c r="B59" s="55"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="A60" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="51" t="s">
+      <c r="B60" s="52" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2380,13 +2380,13 @@
       <c r="E60" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F60" s="40" t="s">
-        <v>141</v>
+      <c r="F60" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="50"/>
-      <c r="B61" s="55"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2396,19 +2396,19 @@
       <c r="E61" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F61" s="41" t="s">
-        <v>141</v>
+      <c r="F61" s="34" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="56" t="s">
+      <c r="A62" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
+      <c r="E62" s="51"/>
+      <c r="F62" s="51"/>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -2454,7 +2454,7 @@
       <c r="A65" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="B65" s="51" t="s">
+      <c r="B65" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -2472,7 +2472,7 @@
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="49"/>
-      <c r="B66" s="52"/>
+      <c r="B66" s="53"/>
       <c r="C66" s="7" t="s">
         <v>159</v>
       </c>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="49"/>
-      <c r="B67" s="52"/>
+      <c r="B67" s="53"/>
       <c r="C67" s="7" t="s">
         <v>160</v>
       </c>
@@ -2504,7 +2504,7 @@
     </row>
     <row r="68" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="49"/>
-      <c r="B68" s="53"/>
+      <c r="B68" s="56"/>
       <c r="C68" s="7" t="s">
         <v>161</v>
       </c>
@@ -2520,7 +2520,7 @@
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="49"/>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="44" t="s">
@@ -2538,7 +2538,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="50"/>
-      <c r="B70" s="55"/>
+      <c r="B70" s="54"/>
       <c r="C70" s="10" t="s">
         <v>162</v>
       </c>
@@ -2607,6 +2607,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A71:A73"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
@@ -2623,22 +2639,6 @@
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working through unittests for windfall_regret
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00175FD-F70D-4971-A7FC-4535C1D50B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B621FC-2A2C-4D09-986D-77D34AD93770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -888,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1010,9 +1010,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1040,35 +1037,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,7 +1351,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1389,14 +1386,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1439,10 +1436,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1459,7 +1456,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="54"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
@@ -1475,20 +1472,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1505,8 +1502,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="58"/>
-      <c r="B9" s="53"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1521,8 +1518,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="58"/>
-      <c r="B10" s="53"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1537,8 +1534,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="58"/>
-      <c r="B11" s="53"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1553,8 +1550,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="59"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1569,10 +1566,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1589,8 +1586,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="58"/>
-      <c r="B14" s="53"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1605,8 +1602,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="58"/>
-      <c r="B15" s="53"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1621,8 +1618,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="58"/>
-      <c r="B16" s="53"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1637,8 +1634,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="58"/>
-      <c r="B17" s="56"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1653,8 +1650,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="58"/>
-      <c r="B18" s="53" t="s">
+      <c r="A18" s="57"/>
+      <c r="B18" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1671,8 +1668,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="58"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1687,8 +1684,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="58"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1703,8 +1700,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="58"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1719,10 +1716,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="50" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1739,8 +1736,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="58"/>
-      <c r="B23" s="56"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1755,8 +1752,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="58"/>
-      <c r="B24" s="53" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1773,8 +1770,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="58"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1789,8 +1786,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="58"/>
-      <c r="B26" s="53"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1805,8 +1802,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="58"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1821,8 +1818,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="58"/>
-      <c r="B28" s="53"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1837,8 +1834,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="58"/>
-      <c r="B29" s="53"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1853,8 +1850,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="58"/>
-      <c r="B30" s="53"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1869,8 +1866,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
-      <c r="B31" s="53"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1885,7 +1882,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="59"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="54"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
@@ -1901,10 +1898,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="50" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1921,8 +1918,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="49"/>
-      <c r="B34" s="53"/>
+      <c r="A34" s="48"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1937,7 +1934,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="50"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="54"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
@@ -1953,14 +1950,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1983,10 +1980,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="48" t="s">
+      <c r="A38" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2003,8 +2000,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="49"/>
-      <c r="B39" s="53"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2019,7 +2016,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="50"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="54"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
@@ -2035,10 +2032,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="57" t="s">
+      <c r="A41" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="52" t="s">
+      <c r="B41" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2055,8 +2052,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="58"/>
-      <c r="B42" s="53"/>
+      <c r="A42" s="57"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2071,8 +2068,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="58"/>
-      <c r="B43" s="53"/>
+      <c r="A43" s="57"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2087,7 +2084,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="59"/>
+      <c r="A44" s="58"/>
       <c r="B44" s="54"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
@@ -2183,10 +2180,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="48" t="s">
+      <c r="A49" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="52" t="s">
+      <c r="B49" s="50" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2203,8 +2200,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="49"/>
-      <c r="B50" s="56"/>
+      <c r="A50" s="48"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2219,7 +2216,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="49"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2237,20 +2234,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="55"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="48" t="s">
+      <c r="A53" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="52" t="s">
+      <c r="B53" s="50" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2267,8 +2264,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="49"/>
-      <c r="B54" s="53"/>
+      <c r="A54" s="48"/>
+      <c r="B54" s="51"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2283,8 +2280,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="49"/>
-      <c r="B55" s="56"/>
+      <c r="A55" s="48"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2299,8 +2296,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="49"/>
-      <c r="B56" s="60" t="s">
+      <c r="A56" s="48"/>
+      <c r="B56" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2317,8 +2314,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="49"/>
-      <c r="B57" s="53"/>
+      <c r="A57" s="48"/>
+      <c r="B57" s="51"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2328,13 +2325,13 @@
       <c r="E57" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F57" s="40" t="s">
-        <v>141</v>
+      <c r="F57" s="32" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="49"/>
-      <c r="B58" s="53"/>
+      <c r="A58" s="48"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2344,31 +2341,31 @@
       <c r="E58" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="40" t="s">
-        <v>141</v>
+      <c r="F58" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="50"/>
+      <c r="A59" s="49"/>
       <c r="B59" s="54"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D59" s="42" t="s">
+      <c r="D59" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="E59" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="41" t="s">
-        <v>141</v>
+      <c r="E59" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="34" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="48" t="s">
+      <c r="A60" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="52" t="s">
+      <c r="B60" s="50" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2385,7 +2382,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="50"/>
+      <c r="A61" s="49"/>
       <c r="B61" s="54"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
@@ -2393,7 +2390,7 @@
       <c r="D61" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="E61" s="43" t="s">
+      <c r="E61" s="42" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="34" t="s">
@@ -2401,14 +2398,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="55" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="51"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -2451,10 +2448,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="48" t="s">
+      <c r="A65" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="B65" s="52" t="s">
+      <c r="B65" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -2471,8 +2468,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="49"/>
-      <c r="B66" s="53"/>
+      <c r="A66" s="48"/>
+      <c r="B66" s="51"/>
       <c r="C66" s="7" t="s">
         <v>159</v>
       </c>
@@ -2487,8 +2484,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="49"/>
-      <c r="B67" s="53"/>
+      <c r="A67" s="48"/>
+      <c r="B67" s="51"/>
       <c r="C67" s="7" t="s">
         <v>160</v>
       </c>
@@ -2503,8 +2500,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="49"/>
-      <c r="B68" s="56"/>
+      <c r="A68" s="48"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="7" t="s">
         <v>161</v>
       </c>
@@ -2519,11 +2516,11 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="49"/>
-      <c r="B69" s="60" t="s">
+      <c r="A69" s="48"/>
+      <c r="B69" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="44" t="s">
+      <c r="C69" s="43" t="s">
         <v>124</v>
       </c>
       <c r="D69" s="38" t="s">
@@ -2537,7 +2534,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="50"/>
+      <c r="A70" s="49"/>
       <c r="B70" s="54"/>
       <c r="C70" s="10" t="s">
         <v>162</v>
@@ -2553,7 +2550,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="48" t="s">
+      <c r="A71" s="47" t="s">
         <v>163</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -2573,7 +2570,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="49"/>
+      <c r="A72" s="48"/>
       <c r="C72" s="7" t="s">
         <v>172</v>
       </c>
@@ -2588,14 +2585,14 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="50"/>
-      <c r="B73" s="45" t="s">
+      <c r="A73" s="49"/>
+      <c r="B73" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="46" t="s">
+      <c r="C73" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="D73" s="47" t="s">
+      <c r="D73" s="46" t="s">
         <v>174</v>
       </c>
       <c r="E73" s="33" t="s">
@@ -2607,22 +2604,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A71:A73"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
@@ -2639,6 +2620,22 @@
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Two more unit tests to go in windfall_regret
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B621FC-2A2C-4D09-986D-77D34AD93770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A543714F-8C00-4BBF-B479-7CF4DEEEFCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1037,35 +1037,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1351,7 +1351,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1386,14 +1386,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1439,7 +1439,7 @@
       <c r="A5" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1457,7 +1457,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="49"/>
-      <c r="B6" s="54"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1472,20 +1472,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1503,7 +1503,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="57"/>
-      <c r="B9" s="51"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="57"/>
-      <c r="B10" s="51"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="57"/>
-      <c r="B11" s="51"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="58"/>
-      <c r="B12" s="51"/>
+      <c r="B12" s="52"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1569,7 +1569,7 @@
       <c r="A13" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="51" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1587,7 +1587,7 @@
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="57"/>
-      <c r="B14" s="51"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="57"/>
-      <c r="B15" s="51"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="57"/>
-      <c r="B16" s="51"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="57"/>
-      <c r="B17" s="52"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="57"/>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1669,7 +1669,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="57"/>
-      <c r="B19" s="51"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="57"/>
-      <c r="B20" s="51"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="57"/>
-      <c r="B21" s="51"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="A22" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="51" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1737,7 +1737,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="57"/>
-      <c r="B23" s="52"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="57"/>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1771,7 +1771,7 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="57"/>
-      <c r="B25" s="51"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="57"/>
-      <c r="B26" s="51"/>
+      <c r="B26" s="52"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="57"/>
-      <c r="B27" s="51"/>
+      <c r="B27" s="52"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="57"/>
-      <c r="B28" s="51"/>
+      <c r="B28" s="52"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="57"/>
-      <c r="B29" s="51"/>
+      <c r="B29" s="52"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="57"/>
-      <c r="B30" s="51"/>
+      <c r="B30" s="52"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="57"/>
-      <c r="B31" s="51"/>
+      <c r="B31" s="52"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1883,7 +1883,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="58"/>
-      <c r="B32" s="54"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="A33" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="51" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1919,7 +1919,7 @@
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="48"/>
-      <c r="B34" s="51"/>
+      <c r="B34" s="52"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="49"/>
-      <c r="B35" s="54"/>
+      <c r="B35" s="53"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -1950,14 +1950,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1983,7 +1983,7 @@
       <c r="A38" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2001,7 +2001,7 @@
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="48"/>
-      <c r="B39" s="51"/>
+      <c r="B39" s="52"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="49"/>
-      <c r="B40" s="54"/>
+      <c r="B40" s="53"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2035,7 +2035,7 @@
       <c r="A41" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2053,7 +2053,7 @@
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="57"/>
-      <c r="B42" s="51"/>
+      <c r="B42" s="52"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="57"/>
-      <c r="B43" s="51"/>
+      <c r="B43" s="52"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="58"/>
-      <c r="B44" s="54"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2183,7 +2183,7 @@
       <c r="A49" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="51" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2201,7 +2201,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="48"/>
-      <c r="B50" s="52"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2234,20 +2234,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="55" t="s">
+      <c r="A52" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="59"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="51" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2265,7 +2265,7 @@
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A54" s="48"/>
-      <c r="B54" s="51"/>
+      <c r="B54" s="52"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="48"/>
-      <c r="B55" s="52"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2297,7 +2297,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="48"/>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2309,13 +2309,13 @@
       <c r="E56" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="40" t="s">
-        <v>141</v>
+      <c r="F56" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="48"/>
-      <c r="B57" s="51"/>
+      <c r="B57" s="52"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="48"/>
-      <c r="B58" s="51"/>
+      <c r="B58" s="52"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="49"/>
-      <c r="B59" s="54"/>
+      <c r="B59" s="53"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="A60" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="51" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2383,7 +2383,7 @@
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="49"/>
-      <c r="B61" s="54"/>
+      <c r="B61" s="53"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2398,14 +2398,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="55" t="s">
+      <c r="A62" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -2451,7 +2451,7 @@
       <c r="A65" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="B65" s="50" t="s">
+      <c r="B65" s="51" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -2469,7 +2469,7 @@
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="48"/>
-      <c r="B66" s="51"/>
+      <c r="B66" s="52"/>
       <c r="C66" s="7" t="s">
         <v>159</v>
       </c>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="48"/>
-      <c r="B67" s="51"/>
+      <c r="B67" s="52"/>
       <c r="C67" s="7" t="s">
         <v>160</v>
       </c>
@@ -2501,7 +2501,7 @@
     </row>
     <row r="68" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="48"/>
-      <c r="B68" s="52"/>
+      <c r="B68" s="55"/>
       <c r="C68" s="7" t="s">
         <v>161</v>
       </c>
@@ -2517,7 +2517,7 @@
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="48"/>
-      <c r="B69" s="53" t="s">
+      <c r="B69" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="43" t="s">
@@ -2535,7 +2535,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="49"/>
-      <c r="B70" s="54"/>
+      <c r="B70" s="53"/>
       <c r="C70" s="10" t="s">
         <v>162</v>
       </c>
@@ -2604,6 +2604,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A71:A73"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
@@ -2620,22 +2636,6 @@
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working through new experimental results
Also fixed a bug in the merge_constraints class in the getPerceptions function.  No predictions to make if an array is empty
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7612075-8650-4BDB-9399-2F422E4835DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65112F8A-6E24-4363-B4B3-E296B9F28F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="186">
   <si>
     <t>Class</t>
   </si>
@@ -588,6 +588,12 @@
   </si>
   <si>
     <t>reevaluatePoints</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -635,6 +641,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -903,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1040,6 +1052,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1049,35 +1064,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,8 +1383,8 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1398,14 +1419,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1448,7 +1469,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="47" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="50" t="s">
@@ -1468,8 +1489,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="48"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1484,14 +1505,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="55" t="s">
@@ -1647,7 +1668,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="56"/>
-      <c r="B17" s="54"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1743,13 +1764,13 @@
       <c r="E22" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="31" t="s">
-        <v>56</v>
+      <c r="F22" s="61" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="56"/>
-      <c r="B23" s="54"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1774,11 +1795,11 @@
       <c r="D24" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>55</v>
+      <c r="E24" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="60" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -1895,7 +1916,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="57"/>
-      <c r="B32" s="52"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1910,7 +1931,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="47" t="s">
         <v>67</v>
       </c>
       <c r="B33" s="50" t="s">
@@ -1930,7 +1951,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="47"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="51"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
@@ -1946,8 +1967,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="48"/>
-      <c r="B35" s="52"/>
+      <c r="A35" s="49"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -1962,14 +1983,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -1992,7 +2013,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="50" t="s">
@@ -2012,7 +2033,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="51"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
@@ -2028,8 +2049,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="48"/>
-      <c r="B40" s="52"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2097,7 +2118,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="57"/>
-      <c r="B44" s="52"/>
+      <c r="B44" s="54"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2192,7 +2213,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="46" t="s">
+      <c r="A49" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="50" t="s">
@@ -2212,8 +2233,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="47"/>
-      <c r="B50" s="54"/>
+      <c r="A50" s="48"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2228,7 +2249,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2246,17 +2267,17 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="53"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="47" t="s">
         <v>108</v>
       </c>
       <c r="B53" s="50" t="s">
@@ -2276,7 +2297,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="51"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
@@ -2292,8 +2313,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="47"/>
-      <c r="B55" s="54"/>
+      <c r="A55" s="48"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2308,8 +2329,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="47"/>
-      <c r="B56" s="58" t="s">
+      <c r="A56" s="48"/>
+      <c r="B56" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2326,7 +2347,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="47"/>
+      <c r="A57" s="48"/>
       <c r="B57" s="51"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
@@ -2342,7 +2363,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="47"/>
+      <c r="A58" s="48"/>
       <c r="B58" s="51"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
@@ -2358,8 +2379,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="48"/>
-      <c r="B59" s="52"/>
+      <c r="A59" s="49"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2374,7 +2395,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="46" t="s">
+      <c r="A60" s="47" t="s">
         <v>106</v>
       </c>
       <c r="B60" s="50" t="s">
@@ -2394,8 +2415,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="48"/>
-      <c r="B61" s="52"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2410,14 +2431,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="49" t="s">
+      <c r="A62" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="49"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -2460,7 +2481,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="46" t="s">
+      <c r="A65" s="47" t="s">
         <v>156</v>
       </c>
       <c r="B65" s="50" t="s">
@@ -2480,7 +2501,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="47"/>
+      <c r="A66" s="48"/>
       <c r="B66" s="51"/>
       <c r="C66" s="7" t="s">
         <v>158</v>
@@ -2496,7 +2517,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="47"/>
+      <c r="A67" s="48"/>
       <c r="B67" s="51"/>
       <c r="C67" s="7" t="s">
         <v>159</v>
@@ -2512,8 +2533,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="47"/>
-      <c r="B68" s="54"/>
+      <c r="A68" s="48"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="7" t="s">
         <v>160</v>
       </c>
@@ -2528,8 +2549,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="47"/>
-      <c r="B69" s="58" t="s">
+      <c r="A69" s="48"/>
+      <c r="B69" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="42" t="s">
@@ -2546,8 +2567,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="48"/>
-      <c r="B70" s="52"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="54"/>
       <c r="C70" s="10" t="s">
         <v>161</v>
       </c>
@@ -2562,7 +2583,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="46" t="s">
+      <c r="A71" s="47" t="s">
         <v>162</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -2582,7 +2603,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="47"/>
+      <c r="A72" s="48"/>
       <c r="C72" s="7" t="s">
         <v>171</v>
       </c>
@@ -2597,7 +2618,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="48"/>
+      <c r="A73" s="49"/>
       <c r="B73" s="43" t="s">
         <v>15</v>
       </c>
@@ -2615,14 +2636,14 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="49" t="s">
+      <c r="A74" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="B74" s="49"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="49"/>
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="15" t="s">
@@ -2657,24 +2678,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A74:F74"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A71:A73"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2690,6 +2693,24 @@
     <mergeCell ref="B33:B35"/>
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A71:A73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Temporary plotting in merge_constraints
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242F405F-A165-4927-97CC-43DE65744F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4411C0-C62C-466C-8979-20E63CDEF100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="190">
   <si>
     <t>Class</t>
   </si>
@@ -600,6 +600,12 @@
   </si>
   <si>
     <t>fragility_script</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>incomplete</t>
   </si>
 </sst>
 </file>
@@ -622,7 +628,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -647,6 +653,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -915,7 +927,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1070,26 +1082,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1374,8 +1392,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1481,7 +1499,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="49"/>
-      <c r="B6" s="52"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1496,14 +1514,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="55" t="s">
@@ -1659,7 +1677,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="56"/>
-      <c r="B17" s="54"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1761,7 +1779,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="56"/>
-      <c r="B23" s="54"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1786,11 +1804,11 @@
       <c r="D24" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>56</v>
+      <c r="E24" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F24" s="60" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -1907,7 +1925,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="57"/>
-      <c r="B32" s="52"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1959,7 +1977,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="49"/>
-      <c r="B35" s="52"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2041,7 +2059,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="49"/>
-      <c r="B40" s="52"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2109,7 +2127,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="57"/>
-      <c r="B44" s="52"/>
+      <c r="B44" s="54"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2225,7 +2243,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="48"/>
-      <c r="B50" s="54"/>
+      <c r="B50" s="52"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2261,7 +2279,7 @@
       <c r="A52" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="53"/>
+      <c r="B52" s="58"/>
       <c r="C52" s="46"/>
       <c r="D52" s="46"/>
       <c r="E52" s="46"/>
@@ -2305,7 +2323,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="48"/>
-      <c r="B55" s="54"/>
+      <c r="B55" s="52"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2321,7 +2339,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="48"/>
-      <c r="B56" s="58" t="s">
+      <c r="B56" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2371,7 +2389,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="49"/>
-      <c r="B59" s="52"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2407,7 +2425,7 @@
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="49"/>
-      <c r="B61" s="52"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2525,7 +2543,7 @@
     </row>
     <row r="68" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="48"/>
-      <c r="B68" s="54"/>
+      <c r="B68" s="52"/>
       <c r="C68" s="7" t="s">
         <v>160</v>
       </c>
@@ -2541,7 +2559,7 @@
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="48"/>
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="42" t="s">
@@ -2578,7 +2596,7 @@
     </row>
     <row r="71" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="49"/>
-      <c r="B71" s="52"/>
+      <c r="B71" s="54"/>
       <c r="C71" s="10" t="s">
         <v>161</v>
       </c>
@@ -2693,23 +2711,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A65:A71"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2726,6 +2727,23 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A65:A71"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A72:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working through EFM bug
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4411C0-C62C-466C-8979-20E63CDEF100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A58779-6D91-44BC-82D7-4D920ABD624A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="192">
   <si>
     <t>Class</t>
   </si>
@@ -606,6 +606,12 @@
   </si>
   <si>
     <t>incomplete</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -927,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1064,6 +1070,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1102,12 +1120,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1392,8 +1404,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24:F24"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="E9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1428,14 +1440,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1470,18 +1482,18 @@
       <c r="D4" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>56</v>
+      <c r="E4" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1498,8 +1510,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="49"/>
-      <c r="B6" s="54"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1514,20 +1526,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1544,40 +1556,40 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="56"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>56</v>
+      <c r="E9" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="56"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>56</v>
+      <c r="E10" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1592,8 +1604,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="57"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1608,10 +1620,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="54" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1628,8 +1640,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="56"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1644,8 +1656,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="56"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1660,8 +1672,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1676,8 +1688,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="56"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1692,8 +1704,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="56"/>
-      <c r="B18" s="51" t="s">
+      <c r="A18" s="60"/>
+      <c r="B18" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1710,8 +1722,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="56"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1726,8 +1738,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="51"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1742,8 +1754,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="56"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1758,10 +1770,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="54" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1778,8 +1790,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="56"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1794,8 +1806,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="56"/>
-      <c r="B24" s="51" t="s">
+      <c r="A24" s="60"/>
+      <c r="B24" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1804,16 +1816,16 @@
       <c r="D24" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="47" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="56"/>
-      <c r="B25" s="51"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1828,8 +1840,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="56"/>
-      <c r="B26" s="51"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1844,8 +1856,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="56"/>
-      <c r="B27" s="51"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1860,8 +1872,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="56"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1876,8 +1888,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="56"/>
-      <c r="B29" s="51"/>
+      <c r="A29" s="60"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1892,8 +1904,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="56"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1908,8 +1920,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="56"/>
-      <c r="B31" s="51"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1924,8 +1936,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="57"/>
-      <c r="B32" s="54"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1940,10 +1952,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="54" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1960,8 +1972,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="48"/>
-      <c r="B34" s="51"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1976,8 +1988,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="49"/>
-      <c r="B35" s="54"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -1992,14 +2004,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="46"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2022,10 +2034,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2042,8 +2054,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="48"/>
-      <c r="B39" s="51"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2058,8 +2070,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="49"/>
-      <c r="B40" s="54"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2074,10 +2086,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="55" t="s">
+      <c r="A41" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2094,8 +2106,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="56"/>
-      <c r="B42" s="51"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2110,8 +2122,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="56"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="60"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2126,8 +2138,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="57"/>
-      <c r="B44" s="54"/>
+      <c r="A44" s="61"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2222,10 +2234,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="54" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2242,8 +2254,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="48"/>
-      <c r="B50" s="52"/>
+      <c r="A50" s="52"/>
+      <c r="B50" s="56"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2258,7 +2270,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="48"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2276,20 +2288,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="58"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="54" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2306,8 +2318,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="48"/>
-      <c r="B54" s="51"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="55"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2322,8 +2334,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="48"/>
-      <c r="B55" s="52"/>
+      <c r="A55" s="52"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2338,8 +2350,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="48"/>
-      <c r="B56" s="53" t="s">
+      <c r="A56" s="52"/>
+      <c r="B56" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2356,8 +2368,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="48"/>
-      <c r="B57" s="51"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2372,8 +2384,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="48"/>
-      <c r="B58" s="51"/>
+      <c r="A58" s="52"/>
+      <c r="B58" s="55"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2388,8 +2400,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="49"/>
-      <c r="B59" s="54"/>
+      <c r="A59" s="53"/>
+      <c r="B59" s="58"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2404,10 +2416,10 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="54" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2424,8 +2436,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="49"/>
-      <c r="B61" s="54"/>
+      <c r="A61" s="53"/>
+      <c r="B61" s="58"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2440,14 +2452,14 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="46" t="s">
+      <c r="A62" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="46"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
@@ -2469,7 +2481,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
         <v>154</v>
       </c>
@@ -2490,10 +2502,10 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="B65" s="50" t="s">
+      <c r="B65" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="7" t="s">
@@ -2510,8 +2522,8 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="48"/>
-      <c r="B66" s="51"/>
+      <c r="A66" s="52"/>
+      <c r="B66" s="55"/>
       <c r="C66" s="7" t="s">
         <v>158</v>
       </c>
@@ -2526,8 +2538,8 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="48"/>
-      <c r="B67" s="51"/>
+      <c r="A67" s="52"/>
+      <c r="B67" s="55"/>
       <c r="C67" s="7" t="s">
         <v>159</v>
       </c>
@@ -2542,8 +2554,8 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="48"/>
-      <c r="B68" s="52"/>
+      <c r="A68" s="52"/>
+      <c r="B68" s="56"/>
       <c r="C68" s="7" t="s">
         <v>160</v>
       </c>
@@ -2558,8 +2570,8 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="48"/>
-      <c r="B69" s="53" t="s">
+      <c r="A69" s="52"/>
+      <c r="B69" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="42" t="s">
@@ -2579,8 +2591,8 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="48"/>
-      <c r="B70" s="51"/>
+      <c r="A70" s="52"/>
+      <c r="B70" s="55"/>
       <c r="C70" s="7" t="s">
         <v>124</v>
       </c>
@@ -2595,8 +2607,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A71" s="49"/>
-      <c r="B71" s="54"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="58"/>
       <c r="C71" s="10" t="s">
         <v>161</v>
       </c>
@@ -2611,7 +2623,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="47" t="s">
+      <c r="A72" s="51" t="s">
         <v>162</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -2631,7 +2643,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="48"/>
+      <c r="A73" s="52"/>
       <c r="C73" s="7" t="s">
         <v>170</v>
       </c>
@@ -2646,7 +2658,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A74" s="49"/>
+      <c r="A74" s="53"/>
       <c r="B74" s="43" t="s">
         <v>15</v>
       </c>
@@ -2664,14 +2676,14 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A75" s="46" t="s">
+      <c r="A75" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="B75" s="46"/>
-      <c r="C75" s="46"/>
-      <c r="D75" s="46"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46"/>
+      <c r="B75" s="50"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="15" t="s">

</xml_diff>

<commit_message>
All PFM and EFM bugs are fixed!
Now just need to figure out what I want to do about the threshold....
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A58779-6D91-44BC-82D7-4D920ABD624A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BA2471-1563-46DC-AF37-9C77C1D8BDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1100,26 +1100,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1404,8 +1410,8 @@
   <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="E9:F9"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1511,7 +1517,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="53"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1526,14 +1532,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
@@ -1689,7 +1695,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="60"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1791,7 +1797,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="60"/>
-      <c r="B23" s="56"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1937,7 +1943,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="61"/>
-      <c r="B32" s="58"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1989,7 +1995,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="53"/>
-      <c r="B35" s="58"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2071,7 +2077,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="53"/>
-      <c r="B40" s="58"/>
+      <c r="B40" s="56"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2139,7 +2145,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="61"/>
-      <c r="B44" s="58"/>
+      <c r="B44" s="56"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2255,7 +2261,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="52"/>
-      <c r="B50" s="56"/>
+      <c r="B50" s="58"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2291,7 +2297,7 @@
       <c r="A52" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="62"/>
+      <c r="B52" s="57"/>
       <c r="C52" s="50"/>
       <c r="D52" s="50"/>
       <c r="E52" s="50"/>
@@ -2310,11 +2316,11 @@
       <c r="D53" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="32" t="s">
-        <v>56</v>
+      <c r="E53" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F53" s="47" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -2335,7 +2341,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="52"/>
-      <c r="B55" s="56"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2351,7 +2357,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="52"/>
-      <c r="B56" s="57" t="s">
+      <c r="B56" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2401,18 +2407,18 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="53"/>
-      <c r="B59" s="58"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D59" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="E59" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="34" t="s">
-        <v>56</v>
+      <c r="E59" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="F59" s="64" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -2437,7 +2443,7 @@
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="53"/>
-      <c r="B61" s="58"/>
+      <c r="B61" s="56"/>
       <c r="C61" s="10" t="s">
         <v>140</v>
       </c>
@@ -2555,7 +2561,7 @@
     </row>
     <row r="68" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="52"/>
-      <c r="B68" s="56"/>
+      <c r="B68" s="58"/>
       <c r="C68" s="7" t="s">
         <v>160</v>
       </c>
@@ -2571,7 +2577,7 @@
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="52"/>
-      <c r="B69" s="57" t="s">
+      <c r="B69" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C69" s="42" t="s">
@@ -2608,7 +2614,7 @@
     </row>
     <row r="71" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" s="53"/>
-      <c r="B71" s="58"/>
+      <c r="B71" s="56"/>
       <c r="C71" s="10" t="s">
         <v>161</v>
       </c>
@@ -2723,6 +2729,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A65:A71"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2739,23 +2762,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A65:A71"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A72:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EFM and PFM running smoothly
Needs unit tests and comments, but okay to start running some preliminary experiments!
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BA2471-1563-46DC-AF37-9C77C1D8BDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D9B1F7-142D-4A60-8479-3FE333BFFDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="193">
   <si>
     <t>Class</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>basicCheck2</t>
   </si>
 </sst>
 </file>
@@ -933,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1082,6 +1085,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1100,32 +1109,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1407,11 +1413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1446,14 +1452,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1496,10 +1502,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1516,8 +1522,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1532,20 +1538,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1562,8 +1568,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1578,8 +1584,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="60"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1594,8 +1600,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1610,8 +1616,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="61"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1626,10 +1632,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1646,8 +1652,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="60"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1662,8 +1668,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="60"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1678,8 +1684,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="60"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1694,7 +1700,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="60"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="58"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
@@ -1710,8 +1716,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="60"/>
-      <c r="B18" s="55" t="s">
+      <c r="A18" s="62"/>
+      <c r="B18" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1728,8 +1734,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="60"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1744,8 +1750,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="60"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1760,8 +1766,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1776,10 +1782,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="56" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1796,7 +1802,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="60"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="58"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
@@ -1812,8 +1818,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="60"/>
-      <c r="B24" s="55" t="s">
+      <c r="A24" s="62"/>
+      <c r="B24" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1830,8 +1836,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="60"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1846,8 +1852,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="60"/>
-      <c r="B26" s="55"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1862,8 +1868,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="60"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="62"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1878,8 +1884,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="60"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="57"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1894,8 +1900,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="60"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1910,8 +1916,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="60"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1926,8 +1932,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="60"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1942,8 +1948,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="61"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1958,10 +1964,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="56" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1978,8 +1984,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="52"/>
-      <c r="B34" s="55"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="57"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1994,8 +2000,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="53"/>
-      <c r="B35" s="56"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="60"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2010,14 +2016,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2040,10 +2046,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2060,8 +2066,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="52"/>
-      <c r="B39" s="55"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2076,8 +2082,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="53"/>
-      <c r="B40" s="56"/>
+      <c r="A40" s="55"/>
+      <c r="B40" s="60"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2092,10 +2098,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="59" t="s">
+      <c r="A41" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2112,8 +2118,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="60"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2128,8 +2134,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="60"/>
-      <c r="B43" s="55"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2144,8 +2150,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="61"/>
-      <c r="B44" s="56"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2240,10 +2246,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="56" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2260,7 +2266,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="52"/>
+      <c r="A50" s="54"/>
       <c r="B50" s="58"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
@@ -2276,7 +2282,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="52"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2294,20 +2300,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="56" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2324,8 +2330,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="52"/>
-      <c r="B54" s="55"/>
+      <c r="A54" s="54"/>
+      <c r="B54" s="57"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2340,7 +2346,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="52"/>
+      <c r="A55" s="54"/>
       <c r="B55" s="58"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
@@ -2356,8 +2362,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="52"/>
-      <c r="B56" s="62" t="s">
+      <c r="A56" s="54"/>
+      <c r="B56" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2374,8 +2380,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="52"/>
-      <c r="B57" s="55"/>
+      <c r="A57" s="54"/>
+      <c r="B57" s="57"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2390,8 +2396,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="52"/>
-      <c r="B58" s="55"/>
+      <c r="A58" s="54"/>
+      <c r="B58" s="57"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2406,26 +2412,26 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="53"/>
-      <c r="B59" s="56"/>
+      <c r="A59" s="55"/>
+      <c r="B59" s="60"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D59" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="E59" s="63" t="s">
+      <c r="E59" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="F59" s="64" t="s">
+      <c r="F59" s="51" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="51" t="s">
+      <c r="A60" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="54" t="s">
+      <c r="B60" s="56" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2441,64 +2447,58 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="53"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="10" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="54"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F61" s="47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="55"/>
+      <c r="B62" s="60"/>
+      <c r="C62" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D61" s="24" t="s">
+      <c r="D62" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="E61" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="50" t="s">
+      <c r="E62" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
-    </row>
-    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="13" t="s">
+      <c r="B63" s="52"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="52"/>
+    </row>
+    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="13" t="s">
         <v>151</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D63" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="E63" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="13" t="s">
-        <v>154</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>15</v>
+        <v>152</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E64" s="27" t="s">
         <v>9</v>
@@ -2507,245 +2507,248 @@
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="51" t="s">
+    <row r="65" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="B65" s="54" t="s">
+      <c r="B66" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C66" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D66" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E65" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="32" t="s">
+      <c r="E66" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="52"/>
-      <c r="B66" s="55"/>
-      <c r="C66" s="7" t="s">
+    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="54"/>
+      <c r="B67" s="57"/>
+      <c r="C67" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D67" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E66" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="52"/>
-      <c r="B67" s="55"/>
-      <c r="C67" s="7" t="s">
+      <c r="E67" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="54"/>
+      <c r="B68" s="57"/>
+      <c r="C68" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D68" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E67" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="52"/>
-      <c r="B68" s="58"/>
-      <c r="C68" s="7" t="s">
+      <c r="E68" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="54"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E68" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="52"/>
-      <c r="B69" s="62" t="s">
+      <c r="E69" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="54"/>
+      <c r="B70" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="42" t="s">
+      <c r="C70" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="D69" s="38" t="s">
+      <c r="D70" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="E69" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="J69" s="7" t="s">
+      <c r="E70" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J70" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="52"/>
-      <c r="B70" s="55"/>
-      <c r="C70" s="7" t="s">
+    <row r="71" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="54"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D71" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E70" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A71" s="53"/>
-      <c r="B71" s="56"/>
-      <c r="C71" s="10" t="s">
+      <c r="E71" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A72" s="55"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D71" s="24" t="s">
+      <c r="D72" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E71" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="51" t="s">
+      <c r="E72" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D73" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E72" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="31" t="s">
+      <c r="E73" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="52"/>
-      <c r="C73" s="7" t="s">
+    <row r="74" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="54"/>
+      <c r="C74" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D74" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="E73" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="32" t="s">
+      <c r="E74" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A74" s="53"/>
-      <c r="B74" s="43" t="s">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A75" s="55"/>
+      <c r="B75" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="44" t="s">
+      <c r="C75" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="D74" s="45" t="s">
+      <c r="D75" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="E74" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="34" t="s">
+      <c r="E75" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A75" s="50" t="s">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A76" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="B75" s="50"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" s="15" t="s">
+      <c r="B76" s="52"/>
+      <c r="C76" s="52"/>
+      <c r="D76" s="52"/>
+      <c r="E76" s="52"/>
+      <c r="F76" s="52"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A77" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B77" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C77" s="7" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C77" s="7" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C78" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C79" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C80" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C81" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="15" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="15" t="s">
         <v>187</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A65:A71"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2762,6 +2765,23 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A73:A75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed reduction change bug
Criteria now reset if a discipline is no longer trying to force a space reduction
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D9B1F7-142D-4A60-8479-3FE333BFFDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6928648C-9143-4E2C-B02E-E41F9B7C33E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -936,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1109,29 +1109,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,8 +1413,8 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1523,7 +1520,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="55"/>
-      <c r="B6" s="60"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1538,14 +1535,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="61" t="s">
@@ -1701,7 +1698,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="62"/>
-      <c r="B17" s="58"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1803,7 +1800,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="62"/>
-      <c r="B23" s="58"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1949,7 +1946,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="63"/>
-      <c r="B32" s="60"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1992,16 +1989,16 @@
       <c r="D34" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>56</v>
+      <c r="E34" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="47" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="55"/>
-      <c r="B35" s="60"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2083,7 +2080,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="55"/>
-      <c r="B40" s="60"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2151,7 +2148,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="63"/>
-      <c r="B44" s="60"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2267,7 +2264,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="54"/>
-      <c r="B50" s="58"/>
+      <c r="B50" s="60"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2303,7 +2300,7 @@
       <c r="A52" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="64"/>
+      <c r="B52" s="59"/>
       <c r="C52" s="52"/>
       <c r="D52" s="52"/>
       <c r="E52" s="52"/>
@@ -2347,7 +2344,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="54"/>
-      <c r="B55" s="58"/>
+      <c r="B55" s="60"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2363,7 +2360,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="54"/>
-      <c r="B56" s="59" t="s">
+      <c r="B56" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2413,7 +2410,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="55"/>
-      <c r="B59" s="60"/>
+      <c r="B59" s="58"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2450,7 +2447,7 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="54"/>
       <c r="B61" s="57"/>
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="7" t="s">
         <v>192</v>
       </c>
       <c r="D61" s="9"/>
@@ -2463,7 +2460,7 @@
     </row>
     <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="55"/>
-      <c r="B62" s="60"/>
+      <c r="B62" s="58"/>
       <c r="C62" s="10" t="s">
         <v>140</v>
       </c>
@@ -2581,7 +2578,7 @@
     </row>
     <row r="69" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="54"/>
-      <c r="B69" s="58"/>
+      <c r="B69" s="60"/>
       <c r="C69" s="7" t="s">
         <v>160</v>
       </c>
@@ -2597,7 +2594,7 @@
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="54"/>
-      <c r="B70" s="59" t="s">
+      <c r="B70" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C70" s="42" t="s">
@@ -2634,7 +2631,7 @@
     </row>
     <row r="72" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="55"/>
-      <c r="B72" s="60"/>
+      <c r="B72" s="58"/>
       <c r="C72" s="10" t="s">
         <v>161</v>
       </c>
@@ -2749,6 +2746,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2765,23 +2779,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A73:A75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commented and unit tested uniform_grid
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD93FC7-105B-496E-9207-31D1A9841CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E91D00-898C-4A39-B747-E1876DC2ECA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -936,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1079,12 +1079,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1109,26 +1103,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1413,8 +1407,8 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1449,14 +1443,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1491,18 +1485,18 @@
       <c r="D4" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="48" t="s">
-        <v>188</v>
-      </c>
-      <c r="F4" s="49" t="s">
-        <v>190</v>
+      <c r="E4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1519,8 +1513,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="60"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1535,20 +1529,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1565,8 +1559,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="62"/>
-      <c r="B9" s="57"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1581,8 +1575,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="62"/>
-      <c r="B10" s="57"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1597,8 +1591,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1613,8 +1607,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="63"/>
-      <c r="B12" s="57"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1629,10 +1623,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="54" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1649,8 +1643,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="62"/>
-      <c r="B14" s="57"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1665,8 +1659,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="62"/>
-      <c r="B15" s="57"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1681,8 +1675,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="62"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1697,7 +1691,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="62"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="58"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
@@ -1713,8 +1707,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
-      <c r="B18" s="57" t="s">
+      <c r="A18" s="60"/>
+      <c r="B18" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1731,8 +1725,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="62"/>
-      <c r="B19" s="57"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1747,8 +1741,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="62"/>
-      <c r="B20" s="57"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1763,8 +1757,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="62"/>
-      <c r="B21" s="57"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1779,10 +1773,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="54" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1799,7 +1793,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="62"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="58"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
@@ -1815,8 +1809,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="62"/>
-      <c r="B24" s="57" t="s">
+      <c r="A24" s="60"/>
+      <c r="B24" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1833,8 +1827,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="62"/>
-      <c r="B25" s="57"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1849,8 +1843,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="62"/>
-      <c r="B26" s="57"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1865,8 +1859,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="62"/>
-      <c r="B27" s="57"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1881,8 +1875,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="62"/>
-      <c r="B28" s="57"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1897,8 +1891,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="62"/>
-      <c r="B29" s="57"/>
+      <c r="A29" s="60"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1913,8 +1907,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="62"/>
-      <c r="B30" s="57"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1929,8 +1923,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="62"/>
-      <c r="B31" s="57"/>
+      <c r="A31" s="60"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1945,8 +1939,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="63"/>
-      <c r="B32" s="60"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1961,10 +1955,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="53" t="s">
+      <c r="A33" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="54" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1981,8 +1975,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="54"/>
-      <c r="B34" s="57"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1997,8 +1991,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="55"/>
-      <c r="B35" s="60"/>
+      <c r="A35" s="53"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2013,14 +2007,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2043,10 +2037,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2063,8 +2057,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="54"/>
-      <c r="B39" s="57"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2079,8 +2073,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="55"/>
-      <c r="B40" s="60"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="56"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2095,10 +2089,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="61" t="s">
+      <c r="A41" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2115,8 +2109,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="62"/>
-      <c r="B42" s="57"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2131,8 +2125,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="62"/>
-      <c r="B43" s="57"/>
+      <c r="A43" s="60"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2147,8 +2141,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="63"/>
-      <c r="B44" s="60"/>
+      <c r="A44" s="61"/>
+      <c r="B44" s="56"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2243,10 +2237,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="54" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2263,7 +2257,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="54"/>
+      <c r="A50" s="52"/>
       <c r="B50" s="58"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
@@ -2279,7 +2273,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="54"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2297,20 +2291,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="52" t="s">
+      <c r="A52" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="64"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="53" t="s">
+      <c r="A53" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="56" t="s">
+      <c r="B53" s="54" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2327,8 +2321,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="54"/>
-      <c r="B54" s="57"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="55"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2343,7 +2337,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="54"/>
+      <c r="A55" s="52"/>
       <c r="B55" s="58"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
@@ -2359,8 +2353,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="54"/>
-      <c r="B56" s="59" t="s">
+      <c r="A56" s="52"/>
+      <c r="B56" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2377,8 +2371,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="54"/>
-      <c r="B57" s="57"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2393,8 +2387,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="54"/>
-      <c r="B58" s="57"/>
+      <c r="A58" s="52"/>
+      <c r="B58" s="55"/>
       <c r="C58" s="7" t="s">
         <v>137</v>
       </c>
@@ -2409,26 +2403,26 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="55"/>
-      <c r="B59" s="60"/>
+      <c r="A59" s="53"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D59" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="E59" s="50" t="s">
+      <c r="E59" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="F59" s="51" t="s">
+      <c r="F59" s="49" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="53" t="s">
+      <c r="A60" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="54" t="s">
         <v>139</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -2445,8 +2439,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="54"/>
-      <c r="B61" s="57"/>
+      <c r="A61" s="52"/>
+      <c r="B61" s="55"/>
       <c r="C61" s="7" t="s">
         <v>192</v>
       </c>
@@ -2459,8 +2453,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="55"/>
-      <c r="B62" s="60"/>
+      <c r="A62" s="53"/>
+      <c r="B62" s="56"/>
       <c r="C62" s="10" t="s">
         <v>140</v>
       </c>
@@ -2475,14 +2469,14 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="52" t="s">
+      <c r="A63" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
@@ -2525,10 +2519,10 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="53" t="s">
+      <c r="A66" s="51" t="s">
         <v>156</v>
       </c>
-      <c r="B66" s="56" t="s">
+      <c r="B66" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="7" t="s">
@@ -2545,8 +2539,8 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="54"/>
-      <c r="B67" s="57"/>
+      <c r="A67" s="52"/>
+      <c r="B67" s="55"/>
       <c r="C67" s="7" t="s">
         <v>158</v>
       </c>
@@ -2561,8 +2555,8 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="54"/>
-      <c r="B68" s="57"/>
+      <c r="A68" s="52"/>
+      <c r="B68" s="55"/>
       <c r="C68" s="7" t="s">
         <v>159</v>
       </c>
@@ -2577,7 +2571,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="54"/>
+      <c r="A69" s="52"/>
       <c r="B69" s="58"/>
       <c r="C69" s="7" t="s">
         <v>160</v>
@@ -2593,8 +2587,8 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="54"/>
-      <c r="B70" s="59" t="s">
+      <c r="A70" s="52"/>
+      <c r="B70" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C70" s="42" t="s">
@@ -2614,8 +2608,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="54"/>
-      <c r="B71" s="57"/>
+      <c r="A71" s="52"/>
+      <c r="B71" s="55"/>
       <c r="C71" s="7" t="s">
         <v>124</v>
       </c>
@@ -2630,8 +2624,8 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A72" s="55"/>
-      <c r="B72" s="60"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="56"/>
       <c r="C72" s="10" t="s">
         <v>161</v>
       </c>
@@ -2646,7 +2640,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="53" t="s">
+      <c r="A73" s="51" t="s">
         <v>162</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -2666,7 +2660,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="54"/>
+      <c r="A74" s="52"/>
       <c r="C74" s="7" t="s">
         <v>170</v>
       </c>
@@ -2681,7 +2675,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A75" s="55"/>
+      <c r="A75" s="53"/>
       <c r="B75" s="43" t="s">
         <v>15</v>
       </c>
@@ -2699,14 +2693,14 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" s="52" t="s">
+      <c r="A76" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="B76" s="52"/>
-      <c r="C76" s="52"/>
-      <c r="D76" s="52"/>
-      <c r="E76" s="52"/>
-      <c r="F76" s="52"/>
+      <c r="B76" s="50"/>
+      <c r="C76" s="50"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="15" t="s">
@@ -2746,6 +2740,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2762,23 +2773,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A73:A75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commented and unit tested point_sorter
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E91D00-898C-4A39-B747-E1876DC2ECA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD1684C-8E03-48F1-8EA5-5BBF06574D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,26 +1103,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1407,8 +1407,8 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="53"/>
-      <c r="B6" s="56"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1529,14 +1529,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
@@ -1567,11 +1567,11 @@
       <c r="D9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F9" s="47" t="s">
-        <v>190</v>
+      <c r="E9" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
@@ -1583,11 +1583,11 @@
       <c r="D10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F10" s="47" t="s">
-        <v>190</v>
+      <c r="E10" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1692,7 +1692,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="60"/>
-      <c r="B17" s="58"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="60"/>
-      <c r="B23" s="58"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="61"/>
-      <c r="B32" s="56"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1992,7 +1992,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="53"/>
-      <c r="B35" s="56"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="53"/>
-      <c r="B40" s="56"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="61"/>
-      <c r="B44" s="56"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="52"/>
-      <c r="B50" s="58"/>
+      <c r="B50" s="56"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2294,7 +2294,7 @@
       <c r="A52" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="57"/>
+      <c r="B52" s="62"/>
       <c r="C52" s="50"/>
       <c r="D52" s="50"/>
       <c r="E52" s="50"/>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="52"/>
-      <c r="B55" s="58"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="52"/>
-      <c r="B56" s="62" t="s">
+      <c r="B56" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2404,7 +2404,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="53"/>
-      <c r="B59" s="56"/>
+      <c r="B59" s="58"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="53"/>
-      <c r="B62" s="56"/>
+      <c r="B62" s="58"/>
       <c r="C62" s="10" t="s">
         <v>140</v>
       </c>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="69" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="52"/>
-      <c r="B69" s="58"/>
+      <c r="B69" s="56"/>
       <c r="C69" s="7" t="s">
         <v>160</v>
       </c>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="52"/>
-      <c r="B70" s="62" t="s">
+      <c r="B70" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C70" s="42" t="s">
@@ -2625,7 +2625,7 @@
     </row>
     <row r="72" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="53"/>
-      <c r="B72" s="56"/>
+      <c r="B72" s="58"/>
       <c r="C72" s="10" t="s">
         <v>161</v>
       </c>
@@ -2740,23 +2740,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2773,6 +2756,23 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A73:A75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Comments and unit tests for force_reduction
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD1684C-8E03-48F1-8EA5-5BBF06574D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9104ACD8-4825-403A-B735-32B5E354CD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,26 +1103,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1407,8 +1407,8 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="53"/>
-      <c r="B6" s="58"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1529,14 +1529,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
@@ -1692,7 +1692,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="60"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="60"/>
-      <c r="B23" s="56"/>
+      <c r="B23" s="58"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="61"/>
-      <c r="B32" s="58"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1983,16 +1983,16 @@
       <c r="D34" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F34" s="47" t="s">
-        <v>190</v>
+      <c r="E34" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="53"/>
-      <c r="B35" s="58"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="53"/>
-      <c r="B40" s="58"/>
+      <c r="B40" s="56"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="61"/>
-      <c r="B44" s="58"/>
+      <c r="B44" s="56"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="52"/>
-      <c r="B50" s="56"/>
+      <c r="B50" s="58"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2294,7 +2294,7 @@
       <c r="A52" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="62"/>
+      <c r="B52" s="57"/>
       <c r="C52" s="50"/>
       <c r="D52" s="50"/>
       <c r="E52" s="50"/>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="52"/>
-      <c r="B55" s="56"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="52"/>
-      <c r="B56" s="57" t="s">
+      <c r="B56" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2404,7 +2404,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="53"/>
-      <c r="B59" s="58"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="10" t="s">
         <v>138</v>
       </c>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="53"/>
-      <c r="B62" s="58"/>
+      <c r="B62" s="56"/>
       <c r="C62" s="10" t="s">
         <v>140</v>
       </c>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="69" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="52"/>
-      <c r="B69" s="56"/>
+      <c r="B69" s="58"/>
       <c r="C69" s="7" t="s">
         <v>160</v>
       </c>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="52"/>
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C70" s="42" t="s">
@@ -2625,7 +2625,7 @@
     </row>
     <row r="72" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="53"/>
-      <c r="B72" s="58"/>
+      <c r="B72" s="56"/>
       <c r="C72" s="10" t="s">
         <v>161</v>
       </c>
@@ -2740,6 +2740,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2756,23 +2773,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A73:A75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More comments and unit tests
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9104ACD8-4825-403A-B735-32B5E354CD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275F658F-8EB9-4C5A-B3E6-7B354E58EA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="194">
   <si>
     <t>Class</t>
   </si>
@@ -615,6 +615,9 @@
   </si>
   <si>
     <t>basicCheck2</t>
+  </si>
+  <si>
+    <t>minmaxNormalize</t>
   </si>
 </sst>
 </file>
@@ -936,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1079,11 +1082,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1103,26 +1103,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1404,11 +1413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1443,14 +1452,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1493,10 +1502,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1513,8 +1522,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1529,20 +1538,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1559,8 +1568,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="60"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1575,8 +1584,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="60"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1591,8 +1600,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1607,8 +1616,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="61"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1623,10 +1632,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="53" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1643,8 +1652,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="60"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1659,8 +1668,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="60"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1675,8 +1684,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="60"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1691,8 +1700,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="60"/>
-      <c r="B17" s="58"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1707,8 +1716,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="60"/>
-      <c r="B18" s="55" t="s">
+      <c r="A18" s="59"/>
+      <c r="B18" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1725,8 +1734,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="60"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1741,8 +1750,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="60"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1757,8 +1766,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1773,10 +1782,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="53" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1793,8 +1802,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="60"/>
-      <c r="B23" s="58"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1809,8 +1818,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="60"/>
-      <c r="B24" s="55" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1827,8 +1836,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="60"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1843,8 +1852,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="60"/>
-      <c r="B26" s="55"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1859,8 +1868,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="60"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1875,8 +1884,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="60"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1891,8 +1900,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="60"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1907,8 +1916,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="60"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1923,8 +1932,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="60"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1939,8 +1948,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="61"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="57"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1955,10 +1964,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="53" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1975,8 +1984,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="52"/>
-      <c r="B34" s="55"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1991,8 +2000,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="53"/>
-      <c r="B35" s="56"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="57"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2007,14 +2016,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="50" t="s">
+      <c r="A36" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2037,10 +2046,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2057,8 +2066,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="52"/>
-      <c r="B39" s="55"/>
+      <c r="A39" s="51"/>
+      <c r="B39" s="54"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2073,8 +2082,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="53"/>
-      <c r="B40" s="56"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2089,10 +2098,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="59" t="s">
+      <c r="A41" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2109,8 +2118,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="60"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="59"/>
+      <c r="B42" s="54"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2125,8 +2134,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="60"/>
-      <c r="B43" s="55"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2141,8 +2150,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="61"/>
-      <c r="B44" s="56"/>
+      <c r="A44" s="60"/>
+      <c r="B44" s="57"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2237,10 +2246,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="51" t="s">
+      <c r="A49" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="53" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2257,8 +2266,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="52"/>
-      <c r="B50" s="58"/>
+      <c r="A50" s="51"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2273,7 +2282,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="52"/>
+      <c r="A51" s="51"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2291,20 +2300,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="53" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2313,16 +2322,16 @@
       <c r="D53" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F53" s="47" t="s">
-        <v>190</v>
+      <c r="E53" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="52"/>
-      <c r="B54" s="55"/>
+      <c r="A54" s="51"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2337,8 +2346,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="52"/>
-      <c r="B55" s="58"/>
+      <c r="A55" s="51"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2353,8 +2362,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="52"/>
-      <c r="B56" s="62" t="s">
+      <c r="A56" s="51"/>
+      <c r="B56" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2371,8 +2380,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="52"/>
-      <c r="B57" s="55"/>
+      <c r="A57" s="51"/>
+      <c r="B57" s="54"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2386,377 +2395,382 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="52"/>
-      <c r="B58" s="55"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="51"/>
+      <c r="B58" s="54"/>
       <c r="C58" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F58" s="47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="51"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D59" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E58" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="53"/>
-      <c r="B59" s="56"/>
-      <c r="C59" s="10" t="s">
+      <c r="E59" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="52"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D59" s="40" t="s">
+      <c r="D60" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="E59" s="48" t="s">
+      <c r="E60" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="48"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="63"/>
+      <c r="F61" s="64"/>
+    </row>
+    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="51"/>
+      <c r="B63" s="54"/>
+      <c r="C63" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D63" s="9"/>
+      <c r="E63" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="F59" s="49" t="s">
+      <c r="F63" s="47" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" s="54" t="s">
-        <v>139</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E60" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="52"/>
-      <c r="B61" s="55"/>
-      <c r="C61" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D61" s="9"/>
-      <c r="E61" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F61" s="47" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="53"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="10" t="s">
+    <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="52"/>
+      <c r="B64" s="57"/>
+      <c r="C64" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D62" s="24" t="s">
+      <c r="D64" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="E62" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="50" t="s">
+      <c r="E64" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A65" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
-    </row>
-    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="13" t="s">
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+    </row>
+    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B66" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D64" s="23" t="s">
+      <c r="D66" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="E64" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="28" t="s">
+      <c r="E66" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A65" s="13" t="s">
+    <row r="67" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B67" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="23" t="s">
+      <c r="D67" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="E65" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="28" t="s">
+      <c r="E67" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="51" t="s">
+    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="B66" s="54" t="s">
+      <c r="B68" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C68" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D68" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E66" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="32" t="s">
+      <c r="E68" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="52"/>
-      <c r="B67" s="55"/>
-      <c r="C67" s="7" t="s">
+    <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="51"/>
+      <c r="B69" s="54"/>
+      <c r="C69" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E67" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="52"/>
-      <c r="B68" s="55"/>
-      <c r="C68" s="7" t="s">
+      <c r="E69" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="51"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D70" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E68" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="52"/>
-      <c r="B69" s="58"/>
-      <c r="C69" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D69" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E69" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="52"/>
-      <c r="B70" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="D70" s="38" t="s">
-        <v>185</v>
-      </c>
       <c r="E70" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F70" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="J70" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="52"/>
+    </row>
+    <row r="71" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="51"/>
       <c r="B71" s="55"/>
       <c r="C71" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="51"/>
+      <c r="B72" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="D72" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="51"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D73" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E71" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A72" s="53"/>
-      <c r="B72" s="56"/>
-      <c r="C72" s="10" t="s">
+      <c r="E73" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A74" s="52"/>
+      <c r="B74" s="57"/>
+      <c r="C74" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D72" s="24" t="s">
+      <c r="D74" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E72" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="51" t="s">
+      <c r="E74" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="D75" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E73" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="31" t="s">
+      <c r="E75" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="52"/>
-      <c r="C74" s="7" t="s">
+    <row r="76" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="51"/>
+      <c r="C76" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D76" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="E74" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="32" t="s">
+      <c r="E76" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A75" s="53"/>
-      <c r="B75" s="43" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A77" s="52"/>
+      <c r="B77" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C75" s="44" t="s">
+      <c r="C77" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="D75" s="45" t="s">
+      <c r="D77" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="E75" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="34" t="s">
+      <c r="E77" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" s="50" t="s">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A78" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="B76" s="50"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="50"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" s="15" t="s">
+      <c r="B78" s="49"/>
+      <c r="C78" s="49"/>
+      <c r="D78" s="49"/>
+      <c r="E78" s="49"/>
+      <c r="F78" s="49"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A79" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B79" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C78" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C79" s="7" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C80" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C81" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C82" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C83" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="15" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="15" t="s">
         <v>187</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2773,6 +2787,23 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A75:A77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished windfall_regret comments and unit tests
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275F658F-8EB9-4C5A-B3E6-7B354E58EA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137C232B-8B36-46F1-8618-9557A531F96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="195">
   <si>
     <t>Class</t>
   </si>
@@ -618,6 +618,9 @@
   </si>
   <si>
     <t>minmaxNormalize</t>
+  </si>
+  <si>
+    <t>Normalizes data between 0 and 1.</t>
   </si>
 </sst>
 </file>
@@ -939,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1085,6 +1088,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1103,35 +1112,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,8 +1416,8 @@
   <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1452,14 +1452,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1502,10 +1502,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1522,7 +1522,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="52"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="57"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
@@ -1538,20 +1538,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1568,8 +1568,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
-      <c r="B9" s="54"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1584,8 +1584,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="59"/>
-      <c r="B10" s="54"/>
+      <c r="A10" s="61"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1600,8 +1600,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1616,8 +1616,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
-      <c r="B12" s="54"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1632,10 +1632,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="55" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1652,8 +1652,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
-      <c r="B14" s="54"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1668,8 +1668,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1684,8 +1684,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="59"/>
-      <c r="B16" s="54"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1700,8 +1700,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="59"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="59"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1716,8 +1716,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="59"/>
-      <c r="B18" s="54" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1734,8 +1734,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="59"/>
-      <c r="B19" s="54"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1750,8 +1750,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="59"/>
-      <c r="B20" s="54"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1766,8 +1766,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="59"/>
-      <c r="B21" s="54"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1782,10 +1782,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="55" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1802,8 +1802,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="59"/>
-      <c r="B23" s="55"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1818,8 +1818,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="59"/>
-      <c r="B24" s="54" t="s">
+      <c r="A24" s="61"/>
+      <c r="B24" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1836,8 +1836,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="59"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="56"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1852,8 +1852,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="59"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="56"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1868,8 +1868,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="59"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1884,8 +1884,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="59"/>
-      <c r="B28" s="54"/>
+      <c r="A28" s="61"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1900,8 +1900,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="59"/>
-      <c r="B29" s="54"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1916,8 +1916,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="59"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1932,8 +1932,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="59"/>
-      <c r="B31" s="54"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1948,7 +1948,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="60"/>
+      <c r="A32" s="62"/>
       <c r="B32" s="57"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
@@ -1964,10 +1964,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="55" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1984,8 +1984,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="51"/>
-      <c r="B34" s="54"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2000,7 +2000,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="52"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="57"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
@@ -2016,14 +2016,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2046,10 +2046,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2066,8 +2066,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="51"/>
-      <c r="B39" s="54"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="56"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2082,7 +2082,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="52"/>
+      <c r="A40" s="54"/>
       <c r="B40" s="57"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
@@ -2098,10 +2098,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="58" t="s">
+      <c r="A41" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2118,8 +2118,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="59"/>
-      <c r="B42" s="54"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="56"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2134,8 +2134,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="59"/>
-      <c r="B43" s="54"/>
+      <c r="A43" s="61"/>
+      <c r="B43" s="56"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="60"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="57"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
@@ -2246,10 +2246,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="55" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2266,8 +2266,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="51"/>
-      <c r="B50" s="55"/>
+      <c r="A50" s="53"/>
+      <c r="B50" s="59"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2282,7 +2282,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="51"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2300,20 +2300,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="61"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="50" t="s">
+      <c r="A53" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="55" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2330,8 +2330,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="51"/>
-      <c r="B54" s="54"/>
+      <c r="A54" s="53"/>
+      <c r="B54" s="56"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2346,8 +2346,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="51"/>
-      <c r="B55" s="55"/>
+      <c r="A55" s="53"/>
+      <c r="B55" s="59"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2362,8 +2362,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="51"/>
-      <c r="B56" s="56" t="s">
+      <c r="A56" s="53"/>
+      <c r="B56" s="63" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2380,8 +2380,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="51"/>
-      <c r="B57" s="54"/>
+      <c r="A57" s="53"/>
+      <c r="B57" s="56"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2396,22 +2396,24 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="51"/>
-      <c r="B58" s="54"/>
+      <c r="A58" s="53"/>
+      <c r="B58" s="56"/>
       <c r="C58" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D58" s="9"/>
-      <c r="E58" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F58" s="47" t="s">
-        <v>189</v>
+      <c r="D58" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E58" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="51"/>
-      <c r="B59" s="54"/>
+      <c r="A59" s="53"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2426,7 +2428,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="52"/>
+      <c r="A60" s="54"/>
       <c r="B60" s="57"/>
       <c r="C60" s="10" t="s">
         <v>138</v>
@@ -2444,16 +2446,15 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="48"/>
       <c r="B61" s="35"/>
-      <c r="C61" s="62"/>
       <c r="D61" s="40"/>
-      <c r="E61" s="63"/>
-      <c r="F61" s="64"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="50"/>
     </row>
     <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="50" t="s">
+      <c r="A62" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="53" t="s">
+      <c r="B62" s="55" t="s">
         <v>139</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -2470,8 +2471,8 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="51"/>
-      <c r="B63" s="54"/>
+      <c r="A63" s="53"/>
+      <c r="B63" s="56"/>
       <c r="C63" s="7" t="s">
         <v>192</v>
       </c>
@@ -2484,7 +2485,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="52"/>
+      <c r="A64" s="54"/>
       <c r="B64" s="57"/>
       <c r="C64" s="10" t="s">
         <v>140</v>
@@ -2500,14 +2501,14 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A65" s="49" t="s">
+      <c r="A65" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="B65" s="49"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
+      <c r="B65" s="51"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="51"/>
+      <c r="F65" s="51"/>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
@@ -2550,10 +2551,10 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="50" t="s">
+      <c r="A68" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="B68" s="53" t="s">
+      <c r="B68" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="7" t="s">
@@ -2570,8 +2571,8 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="51"/>
-      <c r="B69" s="54"/>
+      <c r="A69" s="53"/>
+      <c r="B69" s="56"/>
       <c r="C69" s="7" t="s">
         <v>158</v>
       </c>
@@ -2586,8 +2587,8 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="51"/>
-      <c r="B70" s="54"/>
+      <c r="A70" s="53"/>
+      <c r="B70" s="56"/>
       <c r="C70" s="7" t="s">
         <v>159</v>
       </c>
@@ -2602,8 +2603,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="51"/>
-      <c r="B71" s="55"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="59"/>
       <c r="C71" s="7" t="s">
         <v>160</v>
       </c>
@@ -2618,8 +2619,8 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="51"/>
-      <c r="B72" s="56" t="s">
+      <c r="A72" s="53"/>
+      <c r="B72" s="63" t="s">
         <v>15</v>
       </c>
       <c r="C72" s="42" t="s">
@@ -2639,8 +2640,8 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="51"/>
-      <c r="B73" s="54"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="56"/>
       <c r="C73" s="7" t="s">
         <v>124</v>
       </c>
@@ -2655,7 +2656,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A74" s="52"/>
+      <c r="A74" s="54"/>
       <c r="B74" s="57"/>
       <c r="C74" s="10" t="s">
         <v>161</v>
@@ -2671,7 +2672,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="50" t="s">
+      <c r="A75" s="52" t="s">
         <v>162</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -2691,7 +2692,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="51"/>
+      <c r="A76" s="53"/>
       <c r="C76" s="7" t="s">
         <v>170</v>
       </c>
@@ -2706,7 +2707,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" s="52"/>
+      <c r="A77" s="54"/>
       <c r="B77" s="43" t="s">
         <v>15</v>
       </c>
@@ -2724,14 +2725,14 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" s="49" t="s">
+      <c r="A78" s="51" t="s">
         <v>175</v>
       </c>
-      <c r="B78" s="49"/>
-      <c r="C78" s="49"/>
-      <c r="D78" s="49"/>
-      <c r="E78" s="49"/>
-      <c r="F78" s="49"/>
+      <c r="B78" s="51"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="51"/>
+      <c r="E78" s="51"/>
+      <c r="F78" s="51"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="15" t="s">
@@ -2771,6 +2772,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2787,23 +2805,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A75:A77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished comments and unit tests for fragility_check
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137C232B-8B36-46F1-8618-9557A531F96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCD0FBE-ED0F-44A2-84BB-5132E0A8E884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="194">
   <si>
     <t>Class</t>
   </si>
@@ -608,12 +608,6 @@
     <t>incomplete</t>
   </si>
   <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>basicCheck2</t>
   </si>
   <si>
@@ -621,6 +615,9 @@
   </si>
   <si>
     <t>Normalizes data between 0 and 1.</t>
+  </si>
+  <si>
+    <t>Asymptotic method for setting maximum risk threshold that adjusts according to time remaining and amount of each discipline's design space that has already been reduced.</t>
   </si>
 </sst>
 </file>
@@ -1112,26 +1109,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,7 +1413,7 @@
   <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
@@ -1523,7 +1520,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="54"/>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1538,14 +1535,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="60" t="s">
@@ -1701,7 +1698,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="61"/>
-      <c r="B17" s="59"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1803,7 +1800,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="61"/>
-      <c r="B23" s="59"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1949,7 +1946,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="62"/>
-      <c r="B32" s="57"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2001,7 +1998,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="54"/>
-      <c r="B35" s="57"/>
+      <c r="B35" s="59"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2083,7 +2080,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="54"/>
-      <c r="B40" s="57"/>
+      <c r="B40" s="59"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2151,7 +2148,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="62"/>
-      <c r="B44" s="57"/>
+      <c r="B44" s="59"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2267,7 +2264,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="53"/>
-      <c r="B50" s="59"/>
+      <c r="B50" s="57"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2303,7 +2300,7 @@
       <c r="A52" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="58"/>
+      <c r="B52" s="63"/>
       <c r="C52" s="51"/>
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
@@ -2347,7 +2344,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="53"/>
-      <c r="B55" s="59"/>
+      <c r="B55" s="57"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2363,7 +2360,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="53"/>
-      <c r="B56" s="63" t="s">
+      <c r="B56" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2399,10 +2396,10 @@
       <c r="A58" s="53"/>
       <c r="B58" s="56"/>
       <c r="C58" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E58" s="30" t="s">
         <v>9</v>
@@ -2429,7 +2426,7 @@
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="54"/>
-      <c r="B60" s="57"/>
+      <c r="B60" s="59"/>
       <c r="C60" s="10" t="s">
         <v>138</v>
       </c>
@@ -2470,23 +2467,25 @@
         <v>56</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="53"/>
       <c r="B63" s="56"/>
       <c r="C63" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D63" s="9"/>
-      <c r="E63" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="F63" s="47" t="s">
         <v>190</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="54"/>
-      <c r="B64" s="57"/>
+      <c r="B64" s="59"/>
       <c r="C64" s="10" t="s">
         <v>140</v>
       </c>
@@ -2604,7 +2603,7 @@
     </row>
     <row r="71" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="53"/>
-      <c r="B71" s="59"/>
+      <c r="B71" s="57"/>
       <c r="C71" s="7" t="s">
         <v>160</v>
       </c>
@@ -2620,7 +2619,7 @@
     </row>
     <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="53"/>
-      <c r="B72" s="63" t="s">
+      <c r="B72" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C72" s="42" t="s">
@@ -2657,7 +2656,7 @@
     </row>
     <row r="74" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A74" s="54"/>
-      <c r="B74" s="57"/>
+      <c r="B74" s="59"/>
       <c r="C74" s="10" t="s">
         <v>161</v>
       </c>
@@ -2772,23 +2771,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2805,6 +2787,23 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A75:A77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished comments and unit tests on merge_constraints
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCD0FBE-ED0F-44A2-84BB-5132E0A8E884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5410DD-CA7B-4651-B34A-01EC49AB4B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="192">
   <si>
     <t>Class</t>
   </si>
@@ -600,12 +600,6 @@
   </si>
   <si>
     <t>fragility_script</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>incomplete</t>
   </si>
   <si>
     <t>basicCheck2</t>
@@ -939,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1076,12 +1070,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1109,26 +1097,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1413,8 +1401,8 @@
   <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1449,14 +1437,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1499,10 +1487,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1519,8 +1507,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="54"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1535,20 +1523,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1565,8 +1553,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="61"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1581,8 +1569,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="61"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1597,8 +1585,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="61"/>
-      <c r="B11" s="56"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1613,8 +1601,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="62"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1629,10 +1617,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="53" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1649,8 +1637,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="61"/>
-      <c r="B14" s="56"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1665,8 +1653,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="61"/>
-      <c r="B15" s="56"/>
+      <c r="A15" s="59"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1681,8 +1669,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="61"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="59"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1697,7 +1685,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="61"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="57"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
@@ -1713,8 +1701,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="61"/>
-      <c r="B18" s="56" t="s">
+      <c r="A18" s="59"/>
+      <c r="B18" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1731,8 +1719,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="61"/>
-      <c r="B19" s="56"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1747,8 +1735,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="61"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1763,8 +1751,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
-      <c r="B21" s="56"/>
+      <c r="A21" s="59"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1779,10 +1767,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="53" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1799,7 +1787,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="61"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="57"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
@@ -1815,8 +1803,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="56" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1825,16 +1813,16 @@
       <c r="D24" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="F24" s="47" t="s">
-        <v>189</v>
+      <c r="E24" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="56"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1849,8 +1837,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="56"/>
+      <c r="A26" s="59"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1865,8 +1853,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="56"/>
+      <c r="A27" s="59"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1881,8 +1869,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="61"/>
-      <c r="B28" s="56"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1897,8 +1885,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="61"/>
-      <c r="B29" s="56"/>
+      <c r="A29" s="59"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1913,8 +1901,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="61"/>
-      <c r="B30" s="56"/>
+      <c r="A30" s="59"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1929,8 +1917,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="61"/>
-      <c r="B31" s="56"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1945,8 +1933,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="62"/>
-      <c r="B32" s="59"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1961,10 +1949,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="53" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1981,8 +1969,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="53"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1997,8 +1985,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="54"/>
-      <c r="B35" s="59"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2013,14 +2001,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="51" t="s">
+      <c r="A36" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="51"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2043,10 +2031,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2063,8 +2051,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="53"/>
-      <c r="B39" s="56"/>
+      <c r="A39" s="51"/>
+      <c r="B39" s="54"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2079,8 +2067,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="54"/>
-      <c r="B40" s="59"/>
+      <c r="A40" s="52"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2095,10 +2083,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="60" t="s">
+      <c r="A41" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2115,8 +2103,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="61"/>
-      <c r="B42" s="56"/>
+      <c r="A42" s="59"/>
+      <c r="B42" s="54"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2131,8 +2119,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="61"/>
-      <c r="B43" s="56"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2147,8 +2135,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="62"/>
-      <c r="B44" s="59"/>
+      <c r="A44" s="60"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2243,10 +2231,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="52" t="s">
+      <c r="A49" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="55" t="s">
+      <c r="B49" s="53" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2263,7 +2251,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="53"/>
+      <c r="A50" s="51"/>
       <c r="B50" s="57"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
@@ -2279,7 +2267,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="53"/>
+      <c r="A51" s="51"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2297,20 +2285,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="51" t="s">
+      <c r="A52" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="63"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
+      <c r="B52" s="56"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="52" t="s">
+      <c r="A53" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="55" t="s">
+      <c r="B53" s="53" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2327,8 +2315,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="53"/>
-      <c r="B54" s="56"/>
+      <c r="A54" s="51"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2343,7 +2331,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="53"/>
+      <c r="A55" s="51"/>
       <c r="B55" s="57"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
@@ -2359,8 +2347,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="53"/>
-      <c r="B56" s="58" t="s">
+      <c r="A56" s="51"/>
+      <c r="B56" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2377,8 +2365,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="53"/>
-      <c r="B57" s="56"/>
+      <c r="A57" s="51"/>
+      <c r="B57" s="54"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2393,13 +2381,13 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="53"/>
-      <c r="B58" s="56"/>
+      <c r="A58" s="51"/>
+      <c r="B58" s="54"/>
       <c r="C58" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E58" s="30" t="s">
         <v>9</v>
@@ -2409,8 +2397,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="53"/>
-      <c r="B59" s="56"/>
+      <c r="A59" s="51"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2425,8 +2413,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="54"/>
-      <c r="B60" s="59"/>
+      <c r="A60" s="52"/>
+      <c r="B60" s="55"/>
       <c r="C60" s="10" t="s">
         <v>138</v>
       </c>
@@ -2441,17 +2429,17 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="48"/>
+      <c r="A61" s="46"/>
       <c r="B61" s="35"/>
       <c r="D61" s="40"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="50"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="48"/>
     </row>
     <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="55" t="s">
+      <c r="B62" s="53" t="s">
         <v>139</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -2468,13 +2456,13 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="53"/>
-      <c r="B63" s="56"/>
+      <c r="A63" s="51"/>
+      <c r="B63" s="54"/>
       <c r="C63" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E63" s="30" t="s">
         <v>9</v>
@@ -2484,8 +2472,8 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="54"/>
-      <c r="B64" s="59"/>
+      <c r="A64" s="52"/>
+      <c r="B64" s="55"/>
       <c r="C64" s="10" t="s">
         <v>140</v>
       </c>
@@ -2500,14 +2488,14 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A65" s="51" t="s">
+      <c r="A65" s="49" t="s">
         <v>150</v>
       </c>
-      <c r="B65" s="51"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="51"/>
-      <c r="F65" s="51"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
@@ -2550,10 +2538,10 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="52" t="s">
+      <c r="A68" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="7" t="s">
@@ -2570,8 +2558,8 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="53"/>
-      <c r="B69" s="56"/>
+      <c r="A69" s="51"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="7" t="s">
         <v>158</v>
       </c>
@@ -2586,8 +2574,8 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="53"/>
-      <c r="B70" s="56"/>
+      <c r="A70" s="51"/>
+      <c r="B70" s="54"/>
       <c r="C70" s="7" t="s">
         <v>159</v>
       </c>
@@ -2602,7 +2590,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="53"/>
+      <c r="A71" s="51"/>
       <c r="B71" s="57"/>
       <c r="C71" s="7" t="s">
         <v>160</v>
@@ -2618,8 +2606,8 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="53"/>
-      <c r="B72" s="58" t="s">
+      <c r="A72" s="51"/>
+      <c r="B72" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C72" s="42" t="s">
@@ -2639,8 +2627,8 @@
       </c>
     </row>
     <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="53"/>
-      <c r="B73" s="56"/>
+      <c r="A73" s="51"/>
+      <c r="B73" s="54"/>
       <c r="C73" s="7" t="s">
         <v>124</v>
       </c>
@@ -2655,8 +2643,8 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A74" s="54"/>
-      <c r="B74" s="59"/>
+      <c r="A74" s="52"/>
+      <c r="B74" s="55"/>
       <c r="C74" s="10" t="s">
         <v>161</v>
       </c>
@@ -2671,7 +2659,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="52" t="s">
+      <c r="A75" s="50" t="s">
         <v>162</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -2691,7 +2679,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="53"/>
+      <c r="A76" s="51"/>
       <c r="C76" s="7" t="s">
         <v>170</v>
       </c>
@@ -2706,7 +2694,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" s="54"/>
+      <c r="A77" s="52"/>
       <c r="B77" s="43" t="s">
         <v>15</v>
       </c>
@@ -2724,14 +2712,14 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" s="51" t="s">
+      <c r="A78" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="B78" s="51"/>
-      <c r="C78" s="51"/>
-      <c r="D78" s="51"/>
-      <c r="E78" s="51"/>
-      <c r="F78" s="51"/>
+      <c r="B78" s="49"/>
+      <c r="C78" s="49"/>
+      <c r="D78" s="49"/>
+      <c r="E78" s="49"/>
+      <c r="F78" s="49"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="15" t="s">
@@ -2771,6 +2759,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A62:A64"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2787,23 +2792,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A75:A77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on new unit tests and comments
Will need to revisit getPerceptions and making sure that the discipline proposing a space reduction has an opinion
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5410DD-CA7B-4651-B34A-01EC49AB4B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8262249B-63E3-4DC6-8437-05577C4BEE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="203">
   <si>
     <t>Class</t>
   </si>
@@ -612,6 +612,39 @@
   </si>
   <si>
     <t>Asymptotic method for setting maximum risk threshold that adjusts according to time remaining and amount of each discipline's design space that has already been reduced.</t>
+  </si>
+  <si>
+    <t>entropy_tracker</t>
+  </si>
+  <si>
+    <t>fragilityCommands</t>
+  </si>
+  <si>
+    <t>PFM</t>
+  </si>
+  <si>
+    <t>EFM</t>
+  </si>
+  <si>
+    <t>assessRisk</t>
+  </si>
+  <si>
+    <t>entropyTracker</t>
+  </si>
+  <si>
+    <t>prepEntropy</t>
+  </si>
+  <si>
+    <t>evalEntropy</t>
+  </si>
+  <si>
+    <t>initializePF</t>
+  </si>
+  <si>
+    <t>timeHistory</t>
+  </si>
+  <si>
+    <t>reassignPF</t>
   </si>
 </sst>
 </file>
@@ -933,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1052,9 +1085,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1070,24 +1100,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1097,26 +1118,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1398,17 +1455,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7265625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="73.1796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.08984375" style="8" bestFit="1" customWidth="1"/>
@@ -1437,14 +1494,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1487,10 +1544,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1507,8 +1564,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="52"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1523,20 +1580,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1553,8 +1610,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="59"/>
-      <c r="B9" s="54"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1569,8 +1626,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="59"/>
-      <c r="B10" s="54"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1585,8 +1642,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="59"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1601,8 +1658,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
-      <c r="B12" s="54"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1617,10 +1674,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="49" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1637,8 +1694,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="59"/>
-      <c r="B14" s="54"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1653,8 +1710,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1669,8 +1726,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="59"/>
-      <c r="B16" s="54"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1685,8 +1742,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="59"/>
-      <c r="B17" s="57"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1701,8 +1758,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="59"/>
-      <c r="B18" s="54" t="s">
+      <c r="A18" s="55"/>
+      <c r="B18" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1719,8 +1776,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="59"/>
-      <c r="B19" s="54"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1735,8 +1792,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="59"/>
-      <c r="B20" s="54"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1751,8 +1808,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="59"/>
-      <c r="B21" s="54"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1767,10 +1824,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="49" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1787,8 +1844,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="59"/>
-      <c r="B23" s="57"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1803,8 +1860,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="59"/>
-      <c r="B24" s="54" t="s">
+      <c r="A24" s="55"/>
+      <c r="B24" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1813,16 +1870,16 @@
       <c r="D24" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="32" t="s">
+      <c r="E24" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="69" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="59"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1837,8 +1894,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="59"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1853,8 +1910,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="59"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1869,8 +1926,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="59"/>
-      <c r="B28" s="54"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1885,8 +1942,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="59"/>
-      <c r="B29" s="54"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="50"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1901,8 +1958,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="59"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1917,8 +1974,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="59"/>
-      <c r="B31" s="54"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="50"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1933,8 +1990,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="60"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="56"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -1949,10 +2006,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1969,8 +2026,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="51"/>
-      <c r="B34" s="54"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="50"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -1985,8 +2042,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="52"/>
-      <c r="B35" s="55"/>
+      <c r="A35" s="48"/>
+      <c r="B35" s="53"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2001,14 +2058,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2031,10 +2088,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2051,8 +2108,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="51"/>
-      <c r="B39" s="54"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2067,8 +2124,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="52"/>
-      <c r="B40" s="55"/>
+      <c r="A40" s="48"/>
+      <c r="B40" s="53"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2083,10 +2140,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="58" t="s">
+      <c r="A41" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2103,8 +2160,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="59"/>
-      <c r="B42" s="54"/>
+      <c r="A42" s="55"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2119,8 +2176,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="59"/>
-      <c r="B43" s="54"/>
+      <c r="A43" s="55"/>
+      <c r="B43" s="50"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2135,8 +2192,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="60"/>
-      <c r="B44" s="55"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2231,10 +2288,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="50" t="s">
+      <c r="A49" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="49" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2251,8 +2308,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="51"/>
-      <c r="B50" s="57"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="51"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2267,7 +2324,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="51"/>
+      <c r="A51" s="47"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2285,20 +2342,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="56"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="50" t="s">
+      <c r="A53" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="49" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2315,8 +2372,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="51"/>
-      <c r="B54" s="54"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2331,8 +2388,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="51"/>
-      <c r="B55" s="57"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="51"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2347,8 +2404,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="51"/>
-      <c r="B56" s="61" t="s">
+      <c r="A56" s="47"/>
+      <c r="B56" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2365,8 +2422,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="51"/>
-      <c r="B57" s="54"/>
+      <c r="A57" s="47"/>
+      <c r="B57" s="50"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2381,8 +2438,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="51"/>
-      <c r="B58" s="54"/>
+      <c r="A58" s="47"/>
+      <c r="B58" s="50"/>
       <c r="C58" s="7" t="s">
         <v>189</v>
       </c>
@@ -2397,8 +2454,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="51"/>
-      <c r="B59" s="54"/>
+      <c r="A59" s="47"/>
+      <c r="B59" s="50"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2413,369 +2470,490 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="52"/>
-      <c r="B60" s="55"/>
+      <c r="A60" s="48"/>
+      <c r="B60" s="53"/>
       <c r="C60" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="E60" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="34" t="s">
+      <c r="E60" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="46"/>
-      <c r="B61" s="35"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="48"/>
-    </row>
-    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="50" t="s">
+      <c r="A61" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="B61" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="C61" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="D61" s="59"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="65"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="47"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="59"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="62"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="47"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="59"/>
+      <c r="E63" s="62"/>
+      <c r="F63" s="62"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="47"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="D64" s="59"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+    </row>
+    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="47"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="D65" s="67"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="62"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="47"/>
+      <c r="B66" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" s="59"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="47"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" s="59"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="62"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="47"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" s="59"/>
+      <c r="E68" s="62"/>
+      <c r="F68" s="62"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" s="47"/>
+      <c r="B69" s="50"/>
+      <c r="C69" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="D69" s="59"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="47"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="D70" s="59"/>
+      <c r="E70" s="62"/>
+      <c r="F70" s="62"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="47"/>
+      <c r="B71" s="53"/>
+      <c r="C71" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" s="59"/>
+      <c r="E71" s="62"/>
+      <c r="F71" s="62"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="47" t="s">
+        <v>187</v>
+      </c>
+      <c r="B72" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D72" s="64"/>
+      <c r="E72" s="65"/>
+      <c r="F72" s="65"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" s="47"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="D73" s="59"/>
+      <c r="E73" s="62"/>
+      <c r="F73" s="62"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" s="48"/>
+      <c r="B74" s="53"/>
+      <c r="C74" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D74" s="66"/>
+      <c r="E74" s="60"/>
+      <c r="F74" s="60"/>
+    </row>
+    <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="53" t="s">
+      <c r="B75" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D75" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E62" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="51"/>
-      <c r="B63" s="54"/>
-      <c r="C63" s="7" t="s">
+      <c r="E75" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="47"/>
+      <c r="B76" s="50"/>
+      <c r="C76" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D76" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E63" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A64" s="52"/>
-      <c r="B64" s="55"/>
-      <c r="C64" s="10" t="s">
+      <c r="E76" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="48"/>
+      <c r="B77" s="53"/>
+      <c r="C77" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D64" s="24" t="s">
+      <c r="D77" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="E64" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A65" s="49" t="s">
+      <c r="E77" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="B65" s="49"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-    </row>
-    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="13" t="s">
+      <c r="B78" s="45"/>
+      <c r="C78" s="45"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="F78" s="45"/>
+    </row>
+    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B79" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C79" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D66" s="23" t="s">
+      <c r="D79" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="E66" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="28" t="s">
+      <c r="E79" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A67" s="13" t="s">
+    <row r="80" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="23" t="s">
+      <c r="D80" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="E67" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="28" t="s">
+      <c r="E80" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="50" t="s">
+    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="B68" s="53" t="s">
+      <c r="B81" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C81" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D81" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E68" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="32" t="s">
+      <c r="E81" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="51"/>
-      <c r="B69" s="54"/>
-      <c r="C69" s="7" t="s">
+    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="47"/>
+      <c r="B82" s="50"/>
+      <c r="C82" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D82" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E69" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="51"/>
-      <c r="B70" s="54"/>
-      <c r="C70" s="7" t="s">
+      <c r="E82" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="47"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D83" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E70" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="51"/>
-      <c r="B71" s="57"/>
-      <c r="C71" s="7" t="s">
+      <c r="E83" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="47"/>
+      <c r="B84" s="51"/>
+      <c r="C84" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D84" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E71" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="51"/>
-      <c r="B72" s="61" t="s">
+      <c r="E84" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="47"/>
+      <c r="B85" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="42" t="s">
+      <c r="C85" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="D72" s="38" t="s">
+      <c r="D85" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="E72" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="J72" s="7" t="s">
+      <c r="E85" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J85" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="51"/>
-      <c r="B73" s="54"/>
-      <c r="C73" s="7" t="s">
+    <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="47"/>
+      <c r="B86" s="50"/>
+      <c r="C86" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D86" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E73" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A74" s="52"/>
-      <c r="B74" s="55"/>
-      <c r="C74" s="10" t="s">
+      <c r="E86" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A87" s="48"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D74" s="24" t="s">
+      <c r="D87" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E74" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="50" t="s">
+      <c r="E87" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A88" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D75" s="6" t="s">
+      <c r="D88" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="E75" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="31" t="s">
+      <c r="E88" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="51"/>
-      <c r="C76" s="7" t="s">
+    <row r="89" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="47"/>
+      <c r="C89" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D89" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="E76" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="32" t="s">
+      <c r="E89" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" s="52"/>
-      <c r="B77" s="43" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" s="48"/>
+      <c r="B90" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="44" t="s">
+      <c r="C90" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="D77" s="45" t="s">
+      <c r="D90" s="44" t="s">
         <v>172</v>
       </c>
-      <c r="E77" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="34" t="s">
+      <c r="E90" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" s="49" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="B78" s="49"/>
-      <c r="C78" s="49"/>
-      <c r="D78" s="49"/>
-      <c r="E78" s="49"/>
-      <c r="F78" s="49"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A79" s="15" t="s">
+      <c r="B91" s="45"/>
+      <c r="C91" s="45"/>
+      <c r="D91" s="45"/>
+      <c r="E91" s="45"/>
+      <c r="F91" s="45"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A92" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B92" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C92" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C80" s="7" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C93" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C81" s="7" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C94" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C82" s="7" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C95" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C83" s="7" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C96" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A62:A64"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
+  <mergeCells count="38">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2792,6 +2970,28 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A81:A87"/>
+    <mergeCell ref="B81:B84"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A61:A71"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B66:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished commenting for fragility_script
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8262249B-63E3-4DC6-8437-05577C4BEE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FAE2E7-3E84-436E-AB95-C91BBB279F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="206">
   <si>
     <t>Class</t>
   </si>
@@ -645,6 +645,15 @@
   </si>
   <si>
     <t>reassignPF</t>
+  </si>
+  <si>
+    <t>Performs the necessary commands to evaluate each design space's fragility with the probabilistic fragility model approach.</t>
+  </si>
+  <si>
+    <t>Performs the necessary commands to evaluate each design space's fragility with the entropic fragility model approach.</t>
+  </si>
+  <si>
+    <t>Assesses whether or not any design spaces are too fragile for the current set of input rule(s) being proposed in combination with any rules accepted already and then organizes rules and accompanying data that went into making the decision.</t>
   </si>
 </sst>
 </file>
@@ -966,7 +975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1100,6 +1109,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1118,62 +1154,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1458,8 +1458,8 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1494,14 +1494,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1544,10 +1544,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1564,8 +1564,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="48"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1580,20 +1580,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1610,8 +1610,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="55"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1626,8 +1626,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="55"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1642,8 +1642,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1658,8 +1658,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="56"/>
-      <c r="B12" s="50"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1674,10 +1674,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="58" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1694,8 +1694,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="50"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1710,8 +1710,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="50"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1726,8 +1726,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
-      <c r="B16" s="50"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1742,8 +1742,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="55"/>
-      <c r="B17" s="51"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1758,8 +1758,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="55"/>
-      <c r="B18" s="50" t="s">
+      <c r="A18" s="64"/>
+      <c r="B18" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1776,8 +1776,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="55"/>
-      <c r="B19" s="50"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1792,8 +1792,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="55"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1808,8 +1808,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="55"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1824,10 +1824,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="58" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1844,8 +1844,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="55"/>
-      <c r="B23" s="51"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="62"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1860,8 +1860,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="55"/>
-      <c r="B24" s="50" t="s">
+      <c r="A24" s="64"/>
+      <c r="B24" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1870,16 +1870,16 @@
       <c r="D24" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="69" t="s">
+      <c r="E24" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="53" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="55"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1894,8 +1894,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="55"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="64"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1910,8 +1910,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="55"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1926,8 +1926,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="55"/>
-      <c r="B28" s="50"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1942,8 +1942,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="55"/>
-      <c r="B29" s="50"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1958,8 +1958,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="55"/>
-      <c r="B30" s="50"/>
+      <c r="A30" s="64"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1974,8 +1974,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="55"/>
-      <c r="B31" s="50"/>
+      <c r="A31" s="64"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -1990,8 +1990,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
-      <c r="B32" s="53"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2006,10 +2006,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="58" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2026,8 +2026,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="47"/>
-      <c r="B34" s="50"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="59"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2042,8 +2042,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="48"/>
-      <c r="B35" s="53"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="60"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2058,14 +2058,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2088,10 +2088,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2108,8 +2108,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="56"/>
+      <c r="B39" s="59"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2124,8 +2124,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="48"/>
-      <c r="B40" s="53"/>
+      <c r="A40" s="57"/>
+      <c r="B40" s="60"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2140,10 +2140,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="54" t="s">
+      <c r="A41" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2160,8 +2160,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="55"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="64"/>
+      <c r="B42" s="59"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2176,8 +2176,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="55"/>
-      <c r="B43" s="50"/>
+      <c r="A43" s="64"/>
+      <c r="B43" s="59"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2192,8 +2192,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="56"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="65"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2288,10 +2288,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="46" t="s">
+      <c r="A49" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="58" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2308,8 +2308,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="47"/>
-      <c r="B50" s="51"/>
+      <c r="A50" s="56"/>
+      <c r="B50" s="62"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2324,7 +2324,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2342,20 +2342,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="54"/>
     </row>
     <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="49" t="s">
+      <c r="B53" s="58" t="s">
         <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2372,8 +2372,8 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="50"/>
+      <c r="A54" s="56"/>
+      <c r="B54" s="59"/>
       <c r="C54" s="7" t="s">
         <v>133</v>
       </c>
@@ -2388,8 +2388,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="47"/>
-      <c r="B55" s="51"/>
+      <c r="A55" s="56"/>
+      <c r="B55" s="62"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2404,8 +2404,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="47"/>
-      <c r="B56" s="52" t="s">
+      <c r="A56" s="56"/>
+      <c r="B56" s="66" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2422,8 +2422,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="47"/>
-      <c r="B57" s="50"/>
+      <c r="A57" s="56"/>
+      <c r="B57" s="59"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2438,8 +2438,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="47"/>
-      <c r="B58" s="50"/>
+      <c r="A58" s="56"/>
+      <c r="B58" s="59"/>
       <c r="C58" s="7" t="s">
         <v>189</v>
       </c>
@@ -2454,8 +2454,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="47"/>
-      <c r="B59" s="50"/>
+      <c r="A59" s="56"/>
+      <c r="B59" s="59"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2470,15 +2470,15 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="48"/>
-      <c r="B60" s="53"/>
+      <c r="A60" s="57"/>
+      <c r="B60" s="60"/>
       <c r="C60" s="10" t="s">
         <v>138</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="E60" s="61" t="s">
+      <c r="E60" s="46" t="s">
         <v>9</v>
       </c>
       <c r="F60" s="32" t="s">
@@ -2486,160 +2486,178 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="46" t="s">
+      <c r="A61" s="55" t="s">
         <v>192</v>
       </c>
-      <c r="B61" s="49" t="s">
+      <c r="B61" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="C61" s="58" t="s">
+      <c r="C61" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D61" s="59"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="65"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="47"/>
-      <c r="B62" s="50"/>
-      <c r="C62" s="58" t="s">
+      <c r="A62" s="56"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D62" s="59"/>
-      <c r="E62" s="62"/>
-      <c r="F62" s="62"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="47"/>
-      <c r="B63" s="50"/>
-      <c r="C63" s="58" t="s">
+      <c r="A63" s="56"/>
+      <c r="B63" s="59"/>
+      <c r="C63" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="59"/>
-      <c r="E63" s="62"/>
-      <c r="F63" s="62"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="47"/>
-      <c r="B64" s="50"/>
-      <c r="C64" s="58" t="s">
+      <c r="A64" s="56"/>
+      <c r="B64" s="59"/>
+      <c r="C64" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D64" s="59"/>
-      <c r="E64" s="62"/>
-      <c r="F64" s="62"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
     </row>
     <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="47"/>
-      <c r="B65" s="50"/>
-      <c r="C65" s="58" t="s">
+      <c r="A65" s="56"/>
+      <c r="B65" s="59"/>
+      <c r="C65" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="67"/>
-      <c r="E65" s="62"/>
-      <c r="F65" s="62"/>
+      <c r="D65" s="52"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="47"/>
-      <c r="B66" s="52" t="s">
+      <c r="A66" s="56"/>
+      <c r="B66" s="66" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="D66" s="59"/>
-      <c r="E66" s="62"/>
-      <c r="F66" s="62"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="47"/>
-      <c r="B67" s="50"/>
-      <c r="C67" s="58" t="s">
+      <c r="A67" s="56"/>
+      <c r="B67" s="59"/>
+      <c r="C67" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D67" s="59"/>
-      <c r="E67" s="62"/>
-      <c r="F67" s="62"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="47"/>
-      <c r="B68" s="50"/>
-      <c r="C68" s="58" t="s">
+      <c r="A68" s="56"/>
+      <c r="B68" s="59"/>
+      <c r="C68" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D68" s="59"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="47"/>
-      <c r="B69" s="50"/>
-      <c r="C69" s="58" t="s">
+      <c r="A69" s="56"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D69" s="59"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="62"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="47"/>
-      <c r="B70" s="50"/>
-      <c r="C70" s="58" t="s">
+      <c r="A70" s="56"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D70" s="59"/>
-      <c r="E70" s="62"/>
-      <c r="F70" s="62"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="47"/>
-      <c r="B71" s="53"/>
-      <c r="C71" s="58" t="s">
+      <c r="A71" s="56"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D71" s="59"/>
-      <c r="E71" s="62"/>
-      <c r="F71" s="62"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="47" t="s">
+      <c r="D71" s="45"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="47"/>
+    </row>
+    <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="55" t="s">
         <v>187</v>
       </c>
-      <c r="B72" s="49" t="s">
+      <c r="B72" s="58" t="s">
         <v>193</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D72" s="64"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="65"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="47"/>
-      <c r="B73" s="50"/>
-      <c r="C73" s="58" t="s">
+      <c r="D72" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="56"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D73" s="59"/>
-      <c r="E73" s="62"/>
-      <c r="F73" s="62"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="48"/>
-      <c r="B74" s="53"/>
+      <c r="D73" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="57"/>
+      <c r="B74" s="60"/>
       <c r="C74" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="D74" s="66"/>
-      <c r="E74" s="60"/>
-      <c r="F74" s="60"/>
+      <c r="D74" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="E74" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="33" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="46" t="s">
+      <c r="A75" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="B75" s="49" t="s">
+      <c r="B75" s="58" t="s">
         <v>139</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -2648,7 +2666,7 @@
       <c r="D75" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E75" s="63" t="s">
+      <c r="E75" s="48" t="s">
         <v>9</v>
       </c>
       <c r="F75" s="31" t="s">
@@ -2656,8 +2674,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="47"/>
-      <c r="B76" s="50"/>
+      <c r="A76" s="56"/>
+      <c r="B76" s="59"/>
       <c r="C76" s="7" t="s">
         <v>188</v>
       </c>
@@ -2672,8 +2690,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="48"/>
-      <c r="B77" s="53"/>
+      <c r="A77" s="57"/>
+      <c r="B77" s="60"/>
       <c r="C77" s="10" t="s">
         <v>140</v>
       </c>
@@ -2688,14 +2706,14 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="45" t="s">
+      <c r="A78" s="54" t="s">
         <v>150</v>
       </c>
-      <c r="B78" s="45"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="54"/>
+      <c r="D78" s="54"/>
+      <c r="E78" s="54"/>
+      <c r="F78" s="54"/>
     </row>
     <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
@@ -2738,10 +2756,10 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="46" t="s">
+      <c r="A81" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="B81" s="49" t="s">
+      <c r="B81" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C81" s="7" t="s">
@@ -2758,8 +2776,8 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="47"/>
-      <c r="B82" s="50"/>
+      <c r="A82" s="56"/>
+      <c r="B82" s="59"/>
       <c r="C82" s="7" t="s">
         <v>158</v>
       </c>
@@ -2774,8 +2792,8 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="47"/>
-      <c r="B83" s="50"/>
+      <c r="A83" s="56"/>
+      <c r="B83" s="59"/>
       <c r="C83" s="7" t="s">
         <v>159</v>
       </c>
@@ -2790,8 +2808,8 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="47"/>
-      <c r="B84" s="51"/>
+      <c r="A84" s="56"/>
+      <c r="B84" s="62"/>
       <c r="C84" s="7" t="s">
         <v>160</v>
       </c>
@@ -2806,8 +2824,8 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="47"/>
-      <c r="B85" s="52" t="s">
+      <c r="A85" s="56"/>
+      <c r="B85" s="66" t="s">
         <v>15</v>
       </c>
       <c r="C85" s="41" t="s">
@@ -2827,8 +2845,8 @@
       </c>
     </row>
     <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="47"/>
-      <c r="B86" s="50"/>
+      <c r="A86" s="56"/>
+      <c r="B86" s="59"/>
       <c r="C86" s="7" t="s">
         <v>124</v>
       </c>
@@ -2843,8 +2861,8 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A87" s="48"/>
-      <c r="B87" s="53"/>
+      <c r="A87" s="57"/>
+      <c r="B87" s="60"/>
       <c r="C87" s="10" t="s">
         <v>161</v>
       </c>
@@ -2859,7 +2877,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="46" t="s">
+      <c r="A88" s="55" t="s">
         <v>162</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -2879,7 +2897,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="47"/>
+      <c r="A89" s="56"/>
       <c r="C89" s="7" t="s">
         <v>170</v>
       </c>
@@ -2894,7 +2912,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="48"/>
+      <c r="A90" s="57"/>
       <c r="B90" s="42" t="s">
         <v>15</v>
       </c>
@@ -2912,14 +2930,14 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="45" t="s">
+      <c r="A91" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="B91" s="45"/>
-      <c r="C91" s="45"/>
-      <c r="D91" s="45"/>
-      <c r="E91" s="45"/>
-      <c r="F91" s="45"/>
+      <c r="B91" s="54"/>
+      <c r="C91" s="54"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="54"/>
+      <c r="F91" s="54"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="15" t="s">
@@ -2954,6 +2972,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A81:A87"/>
+    <mergeCell ref="B81:B84"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A88:A90"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A61:A71"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B66:B71"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2970,28 +3010,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A81:A87"/>
-    <mergeCell ref="B81:B84"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A61:A71"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B66:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working through entropy_tracker comments
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FAE2E7-3E84-436E-AB95-C91BBB279F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C1E703-D3C4-4F63-9B95-1C3EA776A181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="211">
   <si>
     <t>Class</t>
   </si>
@@ -654,6 +654,21 @@
   </si>
   <si>
     <t>Assesses whether or not any design spaces are too fragile for the current set of input rule(s) being proposed in combination with any rules accepted already and then organizes rules and accompanying data that went into making the decision.</t>
+  </si>
+  <si>
+    <t>Initializes empty numpy arrays for the space remaining points in each discipline to be able to track their history of pass-fail predictions.</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Gathers the pass-fail data pertinent to each discipline's remaining potential design solutions for eventual sorting of the history of a point's predictions.</t>
+  </si>
+  <si>
+    <t>Fill the numpy arrays with history of pass-fail predictions for each space remaining point in a discipline.</t>
+  </si>
+  <si>
+    <t>Prepares calculated TVE and DTVE values for assignment to windfall and regret dictionaries based on presently formed perceptions of feasibility and design spaces in which a point falls.</t>
   </si>
 </sst>
 </file>
@@ -1154,26 +1169,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1458,8 +1473,8 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1565,7 +1580,7 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="57"/>
-      <c r="B6" s="60"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1580,14 +1595,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="63" t="s">
@@ -1743,7 +1758,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="64"/>
-      <c r="B17" s="62"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1845,7 +1860,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="64"/>
-      <c r="B23" s="62"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1991,7 +2006,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="65"/>
-      <c r="B32" s="60"/>
+      <c r="B32" s="62"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2043,7 +2058,7 @@
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="57"/>
-      <c r="B35" s="60"/>
+      <c r="B35" s="62"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2125,7 +2140,7 @@
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="57"/>
-      <c r="B40" s="60"/>
+      <c r="B40" s="62"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2193,7 +2208,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="65"/>
-      <c r="B44" s="60"/>
+      <c r="B44" s="62"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2309,7 +2324,7 @@
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="56"/>
-      <c r="B50" s="62"/>
+      <c r="B50" s="60"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2345,7 +2360,7 @@
       <c r="A52" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="61"/>
+      <c r="B52" s="66"/>
       <c r="C52" s="54"/>
       <c r="D52" s="54"/>
       <c r="E52" s="54"/>
@@ -2389,7 +2404,7 @@
     </row>
     <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="56"/>
-      <c r="B55" s="62"/>
+      <c r="B55" s="60"/>
       <c r="C55" s="25" t="s">
         <v>134</v>
       </c>
@@ -2405,7 +2420,7 @@
     </row>
     <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="56"/>
-      <c r="B56" s="66" t="s">
+      <c r="B56" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -2471,7 +2486,7 @@
     </row>
     <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="57"/>
-      <c r="B60" s="60"/>
+      <c r="B60" s="62"/>
       <c r="C60" s="10" t="s">
         <v>138</v>
       </c>
@@ -2539,37 +2554,55 @@
       <c r="E65" s="47"/>
       <c r="F65" s="47"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="56"/>
-      <c r="B66" s="66" t="s">
+      <c r="B66" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="D66" s="45"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D66" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="56"/>
       <c r="B67" s="59"/>
       <c r="C67" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D67" s="45"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D67" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="56"/>
       <c r="B68" s="59"/>
       <c r="C68" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D68" s="45"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
+      <c r="D68" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E68" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="47" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="56"/>
@@ -2577,29 +2610,47 @@
       <c r="C69" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D69" s="45"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D69" s="45" t="s">
+        <v>190</v>
+      </c>
+      <c r="E69" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="56"/>
       <c r="B70" s="59"/>
       <c r="C70" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D70" s="45"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D70" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="56"/>
-      <c r="B71" s="60"/>
+      <c r="B71" s="62"/>
       <c r="C71" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D71" s="45"/>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
+      <c r="D71" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="47" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="55" t="s">
@@ -2639,7 +2690,7 @@
     </row>
     <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="57"/>
-      <c r="B74" s="60"/>
+      <c r="B74" s="62"/>
       <c r="C74" s="10" t="s">
         <v>196</v>
       </c>
@@ -2691,7 +2742,7 @@
     </row>
     <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="57"/>
-      <c r="B77" s="60"/>
+      <c r="B77" s="62"/>
       <c r="C77" s="10" t="s">
         <v>140</v>
       </c>
@@ -2809,7 +2860,7 @@
     </row>
     <row r="84" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="56"/>
-      <c r="B84" s="62"/>
+      <c r="B84" s="60"/>
       <c r="C84" s="7" t="s">
         <v>160</v>
       </c>
@@ -2825,7 +2876,7 @@
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="56"/>
-      <c r="B85" s="66" t="s">
+      <c r="B85" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C85" s="41" t="s">
@@ -2862,7 +2913,7 @@
     </row>
     <row r="87" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A87" s="57"/>
-      <c r="B87" s="60"/>
+      <c r="B87" s="62"/>
       <c r="C87" s="10" t="s">
         <v>161</v>
       </c>
@@ -2972,6 +3023,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A22:A32"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A91:F91"/>
     <mergeCell ref="A81:A87"/>
     <mergeCell ref="B81:B84"/>
@@ -2988,28 +3061,6 @@
     <mergeCell ref="A61:A71"/>
     <mergeCell ref="B61:B65"/>
     <mergeCell ref="B66:B71"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="A22:A32"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Consolidating EFM and PFM code
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C1E703-D3C4-4F63-9B95-1C3EA776A181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F78EB96-DC19-4CBA-BEAE-0D050488EC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="212">
   <si>
     <t>Class</t>
   </si>
@@ -669,6 +669,9 @@
   </si>
   <si>
     <t>Prepares calculated TVE and DTVE values for assignment to windfall and regret dictionaries based on presently formed perceptions of feasibility and design spaces in which a point falls.</t>
+  </si>
+  <si>
+    <t>Goes through steps to organize history of each discipline's space remaining points pass-fail predictions for TVE and DTVE calculations.</t>
   </si>
 </sst>
 </file>
@@ -723,7 +726,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -986,11 +989,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1139,15 +1153,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1169,26 +1177,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1470,11 +1499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1509,14 +1538,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1559,10 +1588,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1579,8 +1608,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="57"/>
-      <c r="B6" s="62"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1595,20 +1624,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1625,8 +1654,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="64"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1641,8 +1670,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="64"/>
-      <c r="B10" s="59"/>
+      <c r="A10" s="62"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1657,8 +1686,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="64"/>
-      <c r="B11" s="59"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1673,8 +1702,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="65"/>
-      <c r="B12" s="59"/>
+      <c r="A12" s="63"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1689,10 +1718,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1709,8 +1738,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="64"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1725,8 +1754,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="64"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1741,8 +1770,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="64"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1757,7 +1786,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="64"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="60"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
@@ -1773,8 +1802,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="64"/>
-      <c r="B18" s="59" t="s">
+      <c r="A18" s="62"/>
+      <c r="B18" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1791,8 +1820,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="64"/>
-      <c r="B19" s="59"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1807,8 +1836,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="64"/>
-      <c r="B20" s="59"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1823,8 +1852,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="64"/>
-      <c r="B21" s="59"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1839,10 +1868,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="56" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1859,7 +1888,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="64"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="60"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
@@ -1875,8 +1904,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="64"/>
-      <c r="B24" s="59" t="s">
+      <c r="A24" s="62"/>
+      <c r="B24" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1888,13 +1917,13 @@
       <c r="E24" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="F24" s="51" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="64"/>
-      <c r="B25" s="59"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1909,8 +1938,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="64"/>
-      <c r="B26" s="59"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1925,8 +1954,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="64"/>
-      <c r="B27" s="59"/>
+      <c r="A27" s="62"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1941,8 +1970,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="64"/>
-      <c r="B28" s="59"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="57"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1957,8 +1986,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="64"/>
-      <c r="B29" s="59"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1973,8 +2002,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="64"/>
-      <c r="B30" s="59"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1989,8 +2018,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="64"/>
-      <c r="B31" s="59"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -2005,8 +2034,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="65"/>
-      <c r="B32" s="62"/>
+      <c r="A32" s="63"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2021,10 +2050,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="55" t="s">
+      <c r="A33" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="56" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2041,8 +2070,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="56"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="57"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2057,8 +2086,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="57"/>
-      <c r="B35" s="62"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2073,14 +2102,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2103,10 +2132,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2123,8 +2152,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="56"/>
-      <c r="B39" s="59"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2139,8 +2168,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="57"/>
-      <c r="B40" s="62"/>
+      <c r="A40" s="55"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2155,10 +2184,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="63" t="s">
+      <c r="A41" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2175,8 +2204,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="64"/>
-      <c r="B42" s="59"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2191,8 +2220,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="64"/>
-      <c r="B43" s="59"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2207,8 +2236,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="65"/>
-      <c r="B44" s="62"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2303,10 +2332,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="56" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2323,7 +2352,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="56"/>
+      <c r="A50" s="54"/>
       <c r="B50" s="60"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
@@ -2339,7 +2368,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="56"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2357,23 +2386,23 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="66"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
-      <c r="E52" s="54"/>
-      <c r="F52" s="54"/>
-    </row>
-    <row r="53" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="55" t="s">
+      <c r="B52" s="59"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+    </row>
+    <row r="53" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="70" t="s">
         <v>132</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2386,14 +2415,16 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="56"/>
-      <c r="B54" s="59"/>
+    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A54" s="62"/>
+      <c r="B54" s="64" t="s">
+        <v>15</v>
+      </c>
       <c r="C54" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>146</v>
+        <v>135</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>142</v>
       </c>
       <c r="E54" s="30" t="s">
         <v>9</v>
@@ -2402,14 +2433,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="56"/>
-      <c r="B55" s="60"/>
-      <c r="C55" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>147</v>
+    <row r="55" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="62"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="E55" s="30" t="s">
         <v>9</v>
@@ -2418,152 +2449,168 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A56" s="56"/>
-      <c r="B56" s="61" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="62"/>
+      <c r="B56" s="57"/>
+      <c r="C56" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="62"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E57" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="62"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A59" s="62"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="68" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="63"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="B61" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D61" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="54"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="67"/>
+      <c r="E62" s="69"/>
+      <c r="F62" s="69"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="54"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="67"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="69"/>
+    </row>
+    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="54"/>
+      <c r="B64" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E56" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="56"/>
-      <c r="B57" s="59"/>
-      <c r="C57" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E57" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="56"/>
-      <c r="B58" s="59"/>
-      <c r="C58" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E58" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="56"/>
-      <c r="B59" s="59"/>
-      <c r="C59" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="57"/>
-      <c r="B60" s="62"/>
-      <c r="C60" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D60" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="E60" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="55" t="s">
-        <v>192</v>
-      </c>
-      <c r="B61" s="58" t="s">
-        <v>197</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D61" s="45"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="56"/>
-      <c r="B62" s="59"/>
-      <c r="C62" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="56"/>
-      <c r="B63" s="59"/>
-      <c r="C63" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="45"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="56"/>
-      <c r="B64" s="59"/>
-      <c r="C64" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D64" s="45"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-    </row>
-    <row r="65" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="56"/>
-      <c r="B65" s="59"/>
+      <c r="C64" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="E64" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="54"/>
+      <c r="B65" s="57"/>
       <c r="C65" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D65" s="52"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
+        <v>201</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="E65" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="47" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="56"/>
-      <c r="B66" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="C66" s="41" t="s">
-        <v>200</v>
+      <c r="A66" s="54"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="7" t="s">
+        <v>202</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E66" s="30" t="s">
         <v>9</v>
@@ -2572,14 +2619,14 @@
         <v>207</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="56"/>
-      <c r="B67" s="59"/>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="54"/>
+      <c r="B67" s="57"/>
       <c r="C67" s="7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D67" s="45" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E67" s="30" t="s">
         <v>9</v>
@@ -2588,14 +2635,14 @@
         <v>207</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="56"/>
-      <c r="B68" s="59"/>
+    <row r="68" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="55"/>
+      <c r="B68" s="58"/>
       <c r="C68" s="7" t="s">
-        <v>202</v>
+        <v>138</v>
       </c>
       <c r="D68" s="45" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E68" s="30" t="s">
         <v>9</v>
@@ -2604,425 +2651,398 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="56"/>
-      <c r="B69" s="59"/>
-      <c r="C69" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D69" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="E69" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="47" t="s">
-        <v>207</v>
+    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="B69" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D69" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="56"/>
-      <c r="B70" s="59"/>
+      <c r="A70" s="54"/>
+      <c r="B70" s="57"/>
       <c r="C70" s="7" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="D70" s="45" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="E70" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F70" s="47" t="s">
-        <v>207</v>
+      <c r="F70" s="30" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="56"/>
-      <c r="B71" s="62"/>
-      <c r="C71" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D71" s="45" t="s">
-        <v>210</v>
-      </c>
-      <c r="E71" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="47" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="55" t="s">
-        <v>187</v>
-      </c>
-      <c r="B72" s="58" t="s">
-        <v>193</v>
+      <c r="A71" s="55"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="E71" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B72" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D72" s="49" t="s">
-        <v>203</v>
-      </c>
-      <c r="E72" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E72" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="54"/>
+      <c r="B73" s="57"/>
+      <c r="C73" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="55"/>
+      <c r="B74" s="58"/>
+      <c r="C74" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E74" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" s="52"/>
+      <c r="C75" s="52"/>
+      <c r="D75" s="52"/>
+      <c r="E75" s="52"/>
+      <c r="F75" s="52"/>
+    </row>
+    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D76" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="E76" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="56"/>
-      <c r="B73" s="59"/>
-      <c r="C73" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D73" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="E73" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="30" t="s">
+    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="E77" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="57"/>
-      <c r="B74" s="62"/>
-      <c r="C74" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D74" s="51" t="s">
-        <v>205</v>
-      </c>
-      <c r="E74" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="33" t="s">
+    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="B75" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E75" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="56"/>
-      <c r="B76" s="59"/>
-      <c r="C76" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="57"/>
-      <c r="B77" s="62"/>
-      <c r="C77" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D77" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="E77" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="54" t="s">
-        <v>150</v>
-      </c>
-      <c r="B78" s="54"/>
-      <c r="C78" s="54"/>
-      <c r="D78" s="54"/>
-      <c r="E78" s="54"/>
-      <c r="F78" s="54"/>
-    </row>
     <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B79" s="5" t="s">
+      <c r="A79" s="54"/>
+      <c r="B79" s="57"/>
+      <c r="C79" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A80" s="54"/>
+      <c r="B80" s="57"/>
+      <c r="C80" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="54"/>
+      <c r="B81" s="60"/>
+      <c r="C81" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="54"/>
+      <c r="B82" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D79" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="E79" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="28" t="s">
+      <c r="C82" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D82" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J82" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="54"/>
+      <c r="B83" s="57"/>
+      <c r="C83" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A84" s="55"/>
+      <c r="B84" s="58"/>
+      <c r="C84" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D84" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E84" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="53" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E85" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B80" s="5" t="s">
+    <row r="86" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="54"/>
+      <c r="C86" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E86" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" s="55"/>
+      <c r="B87" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="E80" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="28" t="s">
+      <c r="C87" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="D87" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E87" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="55" t="s">
-        <v>156</v>
-      </c>
-      <c r="B81" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E81" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="56"/>
-      <c r="B82" s="59"/>
-      <c r="C82" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="56"/>
-      <c r="B83" s="59"/>
-      <c r="C83" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="56"/>
-      <c r="B84" s="60"/>
-      <c r="C84" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E84" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="56"/>
-      <c r="B85" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="D85" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="E85" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="J85" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="56"/>
-      <c r="B86" s="59"/>
-      <c r="C86" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E86" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A87" s="57"/>
-      <c r="B87" s="62"/>
-      <c r="C87" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D87" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="E87" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E88" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F88" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="56"/>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="B88" s="52"/>
+      <c r="C88" s="52"/>
+      <c r="D88" s="52"/>
+      <c r="E88" s="52"/>
+      <c r="F88" s="52"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="C89" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D89" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E89" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F89" s="32" t="s">
-        <v>55</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="57"/>
-      <c r="B90" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="D90" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="E90" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="34" t="s">
-        <v>55</v>
+      <c r="C90" s="7" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="54" t="s">
-        <v>175</v>
-      </c>
-      <c r="B91" s="54"/>
-      <c r="C91" s="54"/>
-      <c r="D91" s="54"/>
-      <c r="E91" s="54"/>
-      <c r="F91" s="54"/>
+      <c r="C91" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A92" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>177</v>
-      </c>
       <c r="C92" s="7" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C93" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C94" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C95" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C96" s="7" t="s">
         <v>182</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="37">
+    <mergeCell ref="B54:B60"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="A61:A68"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -3039,28 +3059,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A81:A87"/>
-    <mergeCell ref="B81:B84"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A61:A71"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B66:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reorganizing and Consolidating EFM and PFM code
Still need to go back and recomment and unit test everything
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F78EB96-DC19-4CBA-BEAE-0D050488EC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BE11AA-0E40-4E3F-8F70-BFDD761423B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="211">
   <si>
     <t>Class</t>
   </si>
@@ -666,9 +666,6 @@
   </si>
   <si>
     <t>Fill the numpy arrays with history of pass-fail predictions for each space remaining point in a discipline.</t>
-  </si>
-  <si>
-    <t>Prepares calculated TVE and DTVE values for assignment to windfall and regret dictionaries based on presently formed perceptions of feasibility and design spaces in which a point falls.</t>
   </si>
   <si>
     <t>Goes through steps to organize history of each discipline's space remaining points pass-fail predictions for TVE and DTVE calculations.</t>
@@ -1141,9 +1138,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1159,65 +1153,68 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1499,11 +1496,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1538,14 +1535,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1588,10 +1585,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1608,8 +1605,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
-      <c r="B6" s="58"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1624,20 +1621,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1654,8 +1651,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="62"/>
-      <c r="B9" s="57"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1670,8 +1667,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="62"/>
-      <c r="B10" s="57"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1686,8 +1683,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1702,8 +1699,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="63"/>
-      <c r="B12" s="57"/>
+      <c r="A12" s="58"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1718,10 +1715,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="62" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1738,8 +1735,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="62"/>
-      <c r="B14" s="57"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1754,8 +1751,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="62"/>
-      <c r="B15" s="57"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1770,8 +1767,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="62"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1786,8 +1783,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="62"/>
-      <c r="B17" s="60"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1802,8 +1799,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
-      <c r="B18" s="57" t="s">
+      <c r="A18" s="57"/>
+      <c r="B18" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1820,8 +1817,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="62"/>
-      <c r="B19" s="57"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1836,8 +1833,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="62"/>
-      <c r="B20" s="57"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1852,8 +1849,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="62"/>
-      <c r="B21" s="57"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1868,10 +1865,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="62" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1888,8 +1885,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="62"/>
-      <c r="B23" s="60"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="63"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1904,8 +1901,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="62"/>
-      <c r="B24" s="57" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1914,16 +1911,16 @@
       <c r="D24" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="51" t="s">
+      <c r="E24" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="62"/>
-      <c r="B25" s="57"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="37" t="s">
         <v>128</v>
       </c>
@@ -1938,8 +1935,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="62"/>
-      <c r="B26" s="57"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="55"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1954,8 +1951,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="62"/>
-      <c r="B27" s="57"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1970,8 +1967,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="62"/>
-      <c r="B28" s="57"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1986,8 +1983,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="62"/>
-      <c r="B29" s="57"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -2002,8 +1999,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="62"/>
-      <c r="B30" s="57"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -2018,8 +2015,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="62"/>
-      <c r="B31" s="57"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -2034,8 +2031,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="63"/>
-      <c r="B32" s="58"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2050,10 +2047,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="53" t="s">
+      <c r="A33" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="62" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2070,8 +2067,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="54"/>
-      <c r="B34" s="57"/>
+      <c r="A34" s="60"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2086,8 +2083,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="55"/>
-      <c r="B35" s="58"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="64"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2102,14 +2099,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2132,10 +2129,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2152,8 +2149,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="54"/>
-      <c r="B39" s="57"/>
+      <c r="A39" s="60"/>
+      <c r="B39" s="55"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2168,8 +2165,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="55"/>
-      <c r="B40" s="58"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2184,10 +2181,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="61" t="s">
+      <c r="A41" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="62" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2204,8 +2201,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="62"/>
-      <c r="B42" s="57"/>
+      <c r="A42" s="57"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2220,8 +2217,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="62"/>
-      <c r="B43" s="57"/>
+      <c r="A43" s="57"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2236,8 +2233,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="63"/>
-      <c r="B44" s="58"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="64"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2332,10 +2329,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="62" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2352,8 +2349,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="54"/>
-      <c r="B50" s="60"/>
+      <c r="A50" s="60"/>
+      <c r="B50" s="63"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2368,7 +2365,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="54"/>
+      <c r="A51" s="60"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2386,38 +2383,38 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="52" t="s">
+      <c r="A52" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="59"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
     </row>
     <row r="53" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="61" t="s">
+      <c r="A53" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C53" s="70" t="s">
+      <c r="C53" s="52" t="s">
         <v>132</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="32" t="s">
+      <c r="E53" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="62"/>
-      <c r="B54" s="64" t="s">
+      <c r="A54" s="57"/>
+      <c r="B54" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -2426,357 +2423,355 @@
       <c r="D54" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="E54" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="32" t="s">
+      <c r="E54" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="62"/>
-      <c r="B55" s="57"/>
+      <c r="A55" s="57"/>
+      <c r="B55" s="55"/>
       <c r="C55" s="7" t="s">
         <v>136</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E55" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="32" t="s">
+      <c r="E55" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="50" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="62"/>
-      <c r="B56" s="57"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="55"/>
       <c r="C56" s="7" t="s">
         <v>189</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="E56" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="32" t="s">
+      <c r="E56" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="62"/>
-      <c r="B57" s="57"/>
+      <c r="A57" s="57"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E57" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="32" t="s">
+      <c r="E57" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="62"/>
-      <c r="B58" s="57"/>
-      <c r="C58" s="66" t="s">
+      <c r="A58" s="57"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="7" t="s">
         <v>138</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E58" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="32" t="s">
+      <c r="E58" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="50" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A59" s="62"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="66" t="s">
+      <c r="A59" s="57"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="7" t="s">
         <v>133</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E59" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="68" t="s">
+      <c r="E59" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="46" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="63"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="66" t="s">
+      <c r="A60" s="58"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="7" t="s">
         <v>134</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="E60" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="32" t="s">
+      <c r="E60" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="50" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="53" t="s">
+      <c r="A61" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="B61" s="56" t="s">
+      <c r="B61" s="62" t="s">
         <v>197</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D61" s="49" t="s">
-        <v>211</v>
-      </c>
-      <c r="E61" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="29" t="s">
+      <c r="D61" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="E61" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="70" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="54"/>
-      <c r="B62" s="57"/>
-      <c r="C62" s="66" t="s">
+      <c r="B62" s="55"/>
+      <c r="C62" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D62" s="67"/>
-      <c r="E62" s="69"/>
-      <c r="F62" s="69"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
     </row>
     <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="54"/>
-      <c r="B63" s="60"/>
-      <c r="C63" s="66" t="s">
+      <c r="B63" s="63"/>
+      <c r="C63" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="67"/>
-      <c r="E63" s="69"/>
-      <c r="F63" s="69"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="54"/>
-      <c r="B64" s="64" t="s">
+      <c r="B64" s="67" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="D64" s="71" t="s">
+      <c r="D64" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="E64" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="47" t="s">
+      <c r="E64" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="46" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="54"/>
-      <c r="B65" s="57"/>
+      <c r="B65" s="68"/>
       <c r="C65" s="7" t="s">
         <v>201</v>
       </c>
       <c r="D65" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="E65" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="47" t="s">
+      <c r="E65" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="46" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="54"/>
-      <c r="B66" s="57"/>
+      <c r="B66" s="68"/>
       <c r="C66" s="7" t="s">
         <v>202</v>
       </c>
       <c r="D66" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="E66" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="47" t="s">
+      <c r="E66" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="46" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" s="54"/>
-      <c r="B67" s="57"/>
+      <c r="B67" s="68"/>
       <c r="C67" s="7" t="s">
         <v>189</v>
       </c>
       <c r="D67" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="E67" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="47" t="s">
+      <c r="E67" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="46" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="55"/>
-      <c r="B68" s="58"/>
-      <c r="C68" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D68" s="45" t="s">
-        <v>210</v>
-      </c>
-      <c r="E68" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="47" t="s">
-        <v>207</v>
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="B68" s="62" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D68" s="48" t="s">
+        <v>203</v>
+      </c>
+      <c r="E68" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="53" t="s">
-        <v>187</v>
-      </c>
-      <c r="B69" s="56" t="s">
-        <v>193</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D69" s="49" t="s">
-        <v>203</v>
-      </c>
-      <c r="E69" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="29" t="s">
+      <c r="A69" s="60"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D69" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="E69" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="54"/>
-      <c r="B70" s="57"/>
-      <c r="C70" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D70" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="E70" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="30" t="s">
+    <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="61"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D70" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="E70" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="33" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="55"/>
-      <c r="B71" s="58"/>
-      <c r="C71" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D71" s="50" t="s">
-        <v>205</v>
-      </c>
-      <c r="E71" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="33" t="s">
+      <c r="A71" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="60"/>
+      <c r="B72" s="55"/>
+      <c r="C72" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="61"/>
+      <c r="B73" s="64"/>
+      <c r="C73" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E73" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" s="65"/>
+      <c r="C74" s="65"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="65"/>
+      <c r="F74" s="65"/>
+    </row>
+    <row r="75" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D75" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" s="56" t="s">
-        <v>139</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E72" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="54"/>
-      <c r="B73" s="57"/>
-      <c r="C73" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E73" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="55"/>
-      <c r="B74" s="58"/>
-      <c r="C74" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D74" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="E74" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="B75" s="52"/>
-      <c r="C75" s="52"/>
-      <c r="D75" s="52"/>
-      <c r="E75" s="52"/>
-      <c r="F75" s="52"/>
-    </row>
-    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>152</v>
+        <v>15</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E76" s="27" t="s">
         <v>9</v>
@@ -2785,264 +2780,223 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B77" s="5" t="s">
+    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="60"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="60"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="60"/>
+      <c r="B80" s="63"/>
+      <c r="C80" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="60"/>
+      <c r="B81" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D77" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="E77" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="28" t="s">
+      <c r="C81" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D81" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J81" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="60"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A83" s="61"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E83" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E84" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="B78" s="56" t="s">
+    <row r="85" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A85" s="60"/>
+      <c r="C85" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" s="61"/>
+      <c r="B86" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E78" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" s="32" t="s">
+      <c r="C86" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="D86" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E86" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="54"/>
-      <c r="B79" s="57"/>
-      <c r="C79" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="54"/>
-      <c r="B80" s="57"/>
-      <c r="C80" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E80" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="54"/>
-      <c r="B81" s="60"/>
-      <c r="C81" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E81" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="54"/>
-      <c r="B82" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="D82" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="J82" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="54"/>
-      <c r="B83" s="57"/>
-      <c r="C83" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D83" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A84" s="55"/>
-      <c r="B84" s="58"/>
-      <c r="C84" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D84" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="E84" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="53" t="s">
-        <v>162</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E85" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="54"/>
-      <c r="C86" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="E86" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A87" s="55"/>
-      <c r="B87" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C87" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="D87" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="E87" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" s="34" t="s">
-        <v>55</v>
-      </c>
+      <c r="A87" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="65"/>
+      <c r="C87" s="65"/>
+      <c r="D87" s="65"/>
+      <c r="E87" s="65"/>
+      <c r="F87" s="65"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="52" t="s">
-        <v>175</v>
-      </c>
-      <c r="B88" s="52"/>
-      <c r="C88" s="52"/>
-      <c r="D88" s="52"/>
-      <c r="E88" s="52"/>
-      <c r="F88" s="52"/>
+      <c r="A88" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>177</v>
-      </c>
       <c r="C89" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C90" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C91" s="7" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C92" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C93" s="7" t="s">
         <v>182</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B54:B60"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="A61:A68"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
+  <mergeCells count="35">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -3059,6 +3013,25 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="A74:F74"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="B54:B60"/>
+    <mergeCell ref="A53:A60"/>
+    <mergeCell ref="B61:B63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished windfall_regret unit tests
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BE11AA-0E40-4E3F-8F70-BFDD761423B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5B39B0-4C52-4ACE-AFD4-4DB58983183A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="211">
   <si>
     <t>Class</t>
   </si>
@@ -416,9 +416,6 @@
     <t>Analyzes a discipline without a proposed space reduction (A) and a discipline with a proposed space reduction (B) and organizes the indices of the points in the space remaining into lists for the non-reduced, reduced, and leftover (eliminated) areas of the design space.</t>
   </si>
   <si>
-    <t>windfallRegret</t>
-  </si>
-  <si>
     <t>getPerceptions</t>
   </si>
   <si>
@@ -467,15 +464,9 @@
     <t>Initializes empty dictionaries for windfall and regret data-tracking that will be filled up later.</t>
   </si>
   <si>
-    <t>Collects a list of indices for rows of space remaining data that would be found in the non-reduced, reduced, and leftover design spaces for a particular combination of input rule(s)</t>
-  </si>
-  <si>
     <t>Calculates the complementary probability of feasibility from a predicted point's pass-fail value.</t>
   </si>
   <si>
-    <t>Prepares complementary probability of feasiblity for assignment to windfall and regret dictionaries based on initially formed perceptions of feasiblity and design spaces in which a point falls.</t>
-  </si>
-  <si>
     <t>Determines the amount of space that would remaing in each discipline if they were to move forward with the new rule combo(s) being considered for the current time stamp and calculates the entire design spaces' added potentials for regret and windfall.</t>
   </si>
   <si>
@@ -629,9 +620,6 @@
     <t>assessRisk</t>
   </si>
   <si>
-    <t>entropyTracker</t>
-  </si>
-  <si>
     <t>prepEntropy</t>
   </si>
   <si>
@@ -669,6 +657,18 @@
   </si>
   <si>
     <t>Goes through steps to organize history of each discipline's space remaining points pass-fail predictions for TVE and DTVE calculations.</t>
+  </si>
+  <si>
+    <t>evalCompProb</t>
+  </si>
+  <si>
+    <t>Collects a list of indices for rows of space remaining data that would be found in the non-reduced, reduced, and leftover design spaces for a particular combination of input rule(s).</t>
+  </si>
+  <si>
+    <t>Prepares complementary probability of feasiblity or TVE for assignment to windfall and regret dictionaries based on initially formed perceptions of feasiblity and design spaces in which a point falls.</t>
+  </si>
+  <si>
+    <t>Calculates and normalizes the complementary probabilities of feasibility for remaining design solutions in each discipline's non-reduced design space.</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -986,22 +986,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1153,67 +1142,55 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1496,11 +1473,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1531,18 +1508,18 @@
         <v>3</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1585,10 +1562,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1605,8 +1582,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="61"/>
-      <c r="B6" s="64"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1621,20 +1598,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1651,8 +1628,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="57"/>
-      <c r="B9" s="55"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1667,8 +1644,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="57"/>
-      <c r="B10" s="55"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1683,8 +1660,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="57"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1699,8 +1676,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="58"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1715,10 +1692,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="57" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1735,8 +1712,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="57"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1751,8 +1728,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="57"/>
-      <c r="B15" s="55"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1767,8 +1744,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="57"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1783,8 +1760,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="57"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1799,8 +1776,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="57"/>
-      <c r="B18" s="55" t="s">
+      <c r="A18" s="63"/>
+      <c r="B18" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1817,8 +1794,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="57"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1833,8 +1810,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="57"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1849,8 +1826,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="57"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1865,10 +1842,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="57" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1885,8 +1862,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="57"/>
-      <c r="B23" s="63"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1901,32 +1878,32 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="57"/>
-      <c r="B24" s="55" t="s">
+      <c r="A24" s="63"/>
+      <c r="B24" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="63"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D25" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E24" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="57"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>130</v>
-      </c>
       <c r="E25" s="30" t="s">
         <v>9</v>
       </c>
@@ -1935,13 +1912,13 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="57"/>
-      <c r="B26" s="55"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>9</v>
@@ -1951,8 +1928,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="57"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="63"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1967,8 +1944,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="57"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="63"/>
+      <c r="B28" s="58"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1983,8 +1960,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="57"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1999,8 +1976,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="57"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -2015,8 +1992,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="57"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="58"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -2031,8 +2008,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="58"/>
-      <c r="B32" s="64"/>
+      <c r="A32" s="64"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2047,10 +2024,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="57" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2067,8 +2044,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="60"/>
-      <c r="B34" s="55"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2083,8 +2060,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="61"/>
-      <c r="B35" s="64"/>
+      <c r="A35" s="56"/>
+      <c r="B35" s="59"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2099,14 +2076,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="65" t="s">
+      <c r="A36" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2129,10 +2106,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="59" t="s">
+      <c r="A38" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2149,8 +2126,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="60"/>
-      <c r="B39" s="55"/>
+      <c r="A39" s="55"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2165,8 +2142,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="61"/>
-      <c r="B40" s="64"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="59"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2181,10 +2158,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="62" t="s">
+      <c r="B41" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2201,8 +2178,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="57"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2217,8 +2194,8 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="57"/>
-      <c r="B43" s="55"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2233,8 +2210,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="58"/>
-      <c r="B44" s="64"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="59"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2329,10 +2306,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="59" t="s">
+      <c r="A49" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="62" t="s">
+      <c r="B49" s="57" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2349,8 +2326,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="60"/>
-      <c r="B50" s="63"/>
+      <c r="A50" s="55"/>
+      <c r="B50" s="61"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2365,7 +2342,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="60"/>
+      <c r="A51" s="55"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2383,364 +2360,380 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="65" t="s">
+      <c r="A52" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="66"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="65"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="65"/>
-    </row>
-    <row r="53" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="56" t="s">
+      <c r="B52" s="60"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+    </row>
+    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="C53" s="52" t="s">
-        <v>132</v>
+      <c r="B53" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="57"/>
-      <c r="B54" s="54" t="s">
-        <v>15</v>
-      </c>
+      <c r="E53" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="63"/>
+      <c r="B54" s="58"/>
       <c r="C54" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D54" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="E54" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="57"/>
-      <c r="B55" s="55"/>
+      <c r="D54" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="63"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="7" t="s">
         <v>136</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E55" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="50" t="s">
-        <v>55</v>
+        <v>142</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="57"/>
-      <c r="B56" s="55"/>
+      <c r="A56" s="63"/>
+      <c r="B56" s="58"/>
       <c r="C56" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E56" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="57"/>
-      <c r="B57" s="55"/>
+        <v>187</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="63"/>
+      <c r="B57" s="58"/>
       <c r="C57" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D57" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E57" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="63"/>
+      <c r="B58" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="E58" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="63"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A60" s="63"/>
+      <c r="B60" s="58"/>
+      <c r="C60" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="64"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E57" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="57"/>
-      <c r="B58" s="55"/>
-      <c r="C58" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="50" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A59" s="57"/>
-      <c r="B59" s="55"/>
-      <c r="C59" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E59" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="46" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="58"/>
-      <c r="B60" s="55"/>
-      <c r="C60" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E60" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="50" t="s">
+      <c r="E61" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="B61" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D61" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="E61" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="70" t="s">
+    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="B62" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D62" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="E62" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B62" s="55"/>
-      <c r="C62" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-    </row>
     <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="63"/>
+      <c r="A63" s="55"/>
+      <c r="B63" s="61"/>
       <c r="C63" s="7" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="D63" s="45"/>
       <c r="E63" s="46"/>
       <c r="F63" s="46"/>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B64" s="67" t="s">
+      <c r="A64" s="55"/>
+      <c r="B64" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="E64" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="55"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="E65" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="56"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D66" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E66" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="54" t="s">
+        <v>184</v>
+      </c>
+      <c r="B67" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="48" t="s">
+        <v>199</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="55"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D68" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="D64" s="53" t="s">
-        <v>208</v>
-      </c>
-      <c r="E64" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="46" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B65" s="68"/>
-      <c r="C65" s="7" t="s">
+      <c r="E68" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="56"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="D65" s="45" t="s">
-        <v>206</v>
-      </c>
-      <c r="E65" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="46" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B66" s="68"/>
-      <c r="C66" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D66" s="45" t="s">
-        <v>209</v>
-      </c>
-      <c r="E66" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="46" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B67" s="68"/>
-      <c r="C67" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D67" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="E67" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="46" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="59" t="s">
-        <v>187</v>
-      </c>
-      <c r="B68" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D68" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="E68" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="29" t="s">
+      <c r="E69" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="60"/>
-      <c r="B69" s="55"/>
-      <c r="C69" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D69" s="45" t="s">
-        <v>204</v>
-      </c>
-      <c r="E69" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="30" t="s">
+    <row r="70" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="55"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E71" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="56"/>
+      <c r="B72" s="59"/>
+      <c r="C72" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="E72" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A73" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="53"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53"/>
+    </row>
+    <row r="74" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A74" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E74" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="61"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D70" s="49" t="s">
-        <v>205</v>
-      </c>
-      <c r="E70" s="71" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="B71" s="62" t="s">
-        <v>139</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E71" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="60"/>
-      <c r="B72" s="55"/>
-      <c r="C72" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E72" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="61"/>
-      <c r="B73" s="64"/>
-      <c r="C73" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="D73" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="E73" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="B74" s="65"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="65"/>
-      <c r="E74" s="65"/>
-      <c r="F74" s="65"/>
-    </row>
-    <row r="75" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="13" t="s">
         <v>151</v>
       </c>
@@ -2748,10 +2741,10 @@
         <v>15</v>
       </c>
       <c r="C75" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="23" t="s">
         <v>152</v>
-      </c>
-      <c r="D75" s="23" t="s">
-        <v>153</v>
       </c>
       <c r="E75" s="27" t="s">
         <v>9</v>
@@ -2760,243 +2753,245 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="13" t="s">
+    <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="D76" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="55"/>
+      <c r="B77" s="58"/>
+      <c r="C77" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="55"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E78" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="55"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E79" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A80" s="55"/>
+      <c r="B80" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C80" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D80" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="J80" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="55"/>
+      <c r="B81" s="58"/>
+      <c r="C81" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A82" s="56"/>
+      <c r="B82" s="59"/>
+      <c r="C82" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D82" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="E82" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D76" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="E76" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="28" t="s">
+      <c r="C83" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E83" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="59" t="s">
-        <v>156</v>
-      </c>
-      <c r="B77" s="62" t="s">
+    <row r="84" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A84" s="55"/>
+      <c r="C84" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="56"/>
+      <c r="B85" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E77" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="32" t="s">
+      <c r="C85" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="D85" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="E85" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="60"/>
-      <c r="B78" s="55"/>
-      <c r="C78" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E78" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="60"/>
-      <c r="B79" s="55"/>
-      <c r="C79" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="60"/>
-      <c r="B80" s="63"/>
-      <c r="C80" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E80" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="60"/>
-      <c r="B81" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="D81" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="E81" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="J81" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="60"/>
-      <c r="B82" s="55"/>
-      <c r="C82" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A83" s="61"/>
-      <c r="B83" s="64"/>
-      <c r="C83" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D83" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="E83" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D84" s="6" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" s="53"/>
+      <c r="C86" s="53"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="53"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="E84" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="60"/>
-      <c r="C85" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D85" s="9" t="s">
+      <c r="B87" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E85" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A86" s="61"/>
-      <c r="B86" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C86" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="D86" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="E86" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A87" s="65" t="s">
+      <c r="C87" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B87" s="65"/>
-      <c r="C87" s="65"/>
-      <c r="D87" s="65"/>
-      <c r="E87" s="65"/>
-      <c r="F87" s="65"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="15" t="s">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C88" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B88" s="7" t="s">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C89" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C88" s="7" t="s">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C90" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C89" s="7" t="s">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C91" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C90" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C91" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C92" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="38">
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A53:A61"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B64:B66"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -3013,25 +3008,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="A74:F74"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="B54:B60"/>
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="B61:B63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Need to finish unit tests on EFM
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5B39B0-4C52-4ACE-AFD4-4DB58983183A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8082F67A-9131-4083-8189-87371A8CE879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="212">
   <si>
     <t>Class</t>
   </si>
@@ -669,6 +669,9 @@
   </si>
   <si>
     <t>Calculates and normalizes the complementary probabilities of feasibility for remaining design solutions in each discipline's non-reduced design space.</t>
+  </si>
+  <si>
+    <t>Calculates normalized TVE values from history of passfail predictions for potential design solutions remaining in each discipline's non-reduced design space.</t>
   </si>
 </sst>
 </file>
@@ -990,7 +993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1145,8 +1148,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1160,38 +1169,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1476,8 +1473,8 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L60" sqref="L60"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1512,14 +1509,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1562,10 +1559,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1582,8 +1579,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="56"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1598,20 +1595,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1629,7 +1626,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="63"/>
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1645,7 +1642,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="63"/>
-      <c r="B10" s="58"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1661,7 +1658,7 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="63"/>
-      <c r="B11" s="58"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1677,7 +1674,7 @@
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="64"/>
-      <c r="B12" s="58"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1695,7 +1692,7 @@
       <c r="A13" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="53" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1713,7 +1710,7 @@
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="63"/>
-      <c r="B14" s="58"/>
+      <c r="B14" s="59"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1729,7 +1726,7 @@
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="63"/>
-      <c r="B15" s="58"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1745,7 +1742,7 @@
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="63"/>
-      <c r="B16" s="58"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1761,7 +1758,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="63"/>
-      <c r="B17" s="61"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1777,7 +1774,7 @@
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="63"/>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1795,7 +1792,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="63"/>
-      <c r="B19" s="58"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1811,7 +1808,7 @@
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="63"/>
-      <c r="B20" s="58"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1827,7 +1824,7 @@
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="63"/>
-      <c r="B21" s="58"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1845,7 +1842,7 @@
       <c r="A22" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="53" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1863,7 +1860,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="63"/>
-      <c r="B23" s="61"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1879,7 +1876,7 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="63"/>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1897,7 +1894,7 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="63"/>
-      <c r="B25" s="58"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="37" t="s">
         <v>127</v>
       </c>
@@ -1913,7 +1910,7 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="63"/>
-      <c r="B26" s="58"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1929,7 +1926,7 @@
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="63"/>
-      <c r="B27" s="58"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1945,7 +1942,7 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="63"/>
-      <c r="B28" s="58"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1961,7 +1958,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="63"/>
-      <c r="B29" s="58"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1977,7 +1974,7 @@
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="63"/>
-      <c r="B30" s="58"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1993,7 +1990,7 @@
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="63"/>
-      <c r="B31" s="58"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -2009,7 +2006,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="64"/>
-      <c r="B32" s="59"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2024,10 +2021,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="57" t="s">
+      <c r="B33" s="53" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2044,8 +2041,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="55"/>
-      <c r="B34" s="58"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="59"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2060,8 +2057,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="56"/>
-      <c r="B35" s="59"/>
+      <c r="A35" s="58"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2076,14 +2073,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="53" t="s">
+      <c r="A36" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2106,10 +2103,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2126,8 +2123,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="55"/>
-      <c r="B39" s="58"/>
+      <c r="A39" s="57"/>
+      <c r="B39" s="59"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2142,8 +2139,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="56"/>
-      <c r="B40" s="59"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="61"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2161,7 +2158,7 @@
       <c r="A41" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="57" t="s">
+      <c r="B41" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2179,7 +2176,7 @@
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="63"/>
-      <c r="B42" s="58"/>
+      <c r="B42" s="59"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2195,7 +2192,7 @@
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="63"/>
-      <c r="B43" s="58"/>
+      <c r="B43" s="59"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2211,7 +2208,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="64"/>
-      <c r="B44" s="59"/>
+      <c r="B44" s="61"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2306,10 +2303,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="54" t="s">
+      <c r="A49" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="53" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2326,8 +2323,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="55"/>
-      <c r="B50" s="61"/>
+      <c r="A50" s="57"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2342,7 +2339,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="55"/>
+      <c r="A51" s="57"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2360,20 +2357,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="53" t="s">
+      <c r="A52" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="60"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
     </row>
     <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -2391,7 +2388,7 @@
     </row>
     <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="63"/>
-      <c r="B54" s="58"/>
+      <c r="B54" s="59"/>
       <c r="C54" s="7" t="s">
         <v>135</v>
       </c>
@@ -2407,7 +2404,7 @@
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="63"/>
-      <c r="B55" s="58"/>
+      <c r="B55" s="59"/>
       <c r="C55" s="7" t="s">
         <v>136</v>
       </c>
@@ -2423,7 +2420,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="63"/>
-      <c r="B56" s="58"/>
+      <c r="B56" s="59"/>
       <c r="C56" s="7" t="s">
         <v>186</v>
       </c>
@@ -2439,14 +2436,14 @@
     </row>
     <row r="57" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="63"/>
-      <c r="B57" s="58"/>
+      <c r="B57" s="59"/>
       <c r="C57" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="E57" s="66" t="s">
+      <c r="E57" s="52" t="s">
         <v>9</v>
       </c>
       <c r="F57" s="32" t="s">
@@ -2455,7 +2452,7 @@
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="63"/>
-      <c r="B58" s="65" t="s">
+      <c r="B58" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="41" t="s">
@@ -2464,7 +2461,7 @@
       <c r="D58" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="E58" s="67" t="s">
+      <c r="E58" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F58" s="32" t="s">
@@ -2473,14 +2470,14 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="63"/>
-      <c r="B59" s="58"/>
+      <c r="B59" s="59"/>
       <c r="C59" s="7" t="s">
         <v>131</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E59" s="67" t="s">
+      <c r="E59" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F59" s="32" t="s">
@@ -2489,7 +2486,7 @@
     </row>
     <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="63"/>
-      <c r="B60" s="58"/>
+      <c r="B60" s="59"/>
       <c r="C60" s="7" t="s">
         <v>132</v>
       </c>
@@ -2505,7 +2502,7 @@
     </row>
     <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="64"/>
-      <c r="B61" s="59"/>
+      <c r="B61" s="61"/>
       <c r="C61" s="7" t="s">
         <v>133</v>
       </c>
@@ -2520,10 +2517,10 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="54" t="s">
+      <c r="A62" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="57" t="s">
+      <c r="B62" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -2532,26 +2529,30 @@
       <c r="D62" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="E62" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="52" t="s">
+      <c r="E62" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="55"/>
-      <c r="B63" s="61"/>
+    <row r="63" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="57"/>
+      <c r="B63" s="54"/>
       <c r="C63" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D63" s="45"/>
-      <c r="E63" s="46"/>
+      <c r="D63" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>9</v>
+      </c>
       <c r="F63" s="46"/>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="55"/>
-      <c r="B64" s="65" t="s">
+      <c r="A64" s="57"/>
+      <c r="B64" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="41" t="s">
@@ -2560,7 +2561,7 @@
       <c r="D64" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="E64" s="46" t="s">
+      <c r="E64" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F64" s="46" t="s">
@@ -2568,15 +2569,15 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="55"/>
-      <c r="B65" s="58"/>
+      <c r="A65" s="57"/>
+      <c r="B65" s="59"/>
       <c r="C65" s="7" t="s">
         <v>197</v>
       </c>
       <c r="D65" s="45" t="s">
         <v>202</v>
       </c>
-      <c r="E65" s="46" t="s">
+      <c r="E65" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F65" s="46" t="s">
@@ -2584,15 +2585,15 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="56"/>
-      <c r="B66" s="59"/>
+      <c r="A66" s="58"/>
+      <c r="B66" s="61"/>
       <c r="C66" s="7" t="s">
         <v>198</v>
       </c>
       <c r="D66" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="E66" s="46" t="s">
+      <c r="E66" s="30" t="s">
         <v>9</v>
       </c>
       <c r="F66" s="46" t="s">
@@ -2600,10 +2601,10 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="56" t="s">
         <v>184</v>
       </c>
-      <c r="B67" s="57" t="s">
+      <c r="B67" s="53" t="s">
         <v>190</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2620,8 +2621,8 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="55"/>
-      <c r="B68" s="58"/>
+      <c r="A68" s="57"/>
+      <c r="B68" s="59"/>
       <c r="C68" s="7" t="s">
         <v>192</v>
       </c>
@@ -2636,8 +2637,8 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="56"/>
-      <c r="B69" s="59"/>
+      <c r="A69" s="58"/>
+      <c r="B69" s="61"/>
       <c r="C69" s="10" t="s">
         <v>193</v>
       </c>
@@ -2652,10 +2653,10 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="53" t="s">
         <v>138</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -2672,8 +2673,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="55"/>
-      <c r="B71" s="58"/>
+      <c r="A71" s="57"/>
+      <c r="B71" s="59"/>
       <c r="C71" s="7" t="s">
         <v>185</v>
       </c>
@@ -2688,8 +2689,8 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="56"/>
-      <c r="B72" s="59"/>
+      <c r="A72" s="58"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="10" t="s">
         <v>139</v>
       </c>
@@ -2704,14 +2705,14 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" s="53" t="s">
+      <c r="A73" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="B73" s="53"/>
-      <c r="C73" s="53"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="53"/>
+      <c r="B73" s="55"/>
+      <c r="C73" s="55"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="55"/>
+      <c r="F73" s="55"/>
     </row>
     <row r="74" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
@@ -2754,10 +2755,10 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="54" t="s">
+      <c r="A76" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="B76" s="57" t="s">
+      <c r="B76" s="53" t="s">
         <v>15</v>
       </c>
       <c r="C76" s="7" t="s">
@@ -2774,8 +2775,8 @@
       </c>
     </row>
     <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="55"/>
-      <c r="B77" s="58"/>
+      <c r="A77" s="57"/>
+      <c r="B77" s="59"/>
       <c r="C77" s="7" t="s">
         <v>155</v>
       </c>
@@ -2790,8 +2791,8 @@
       </c>
     </row>
     <row r="78" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="55"/>
-      <c r="B78" s="58"/>
+      <c r="A78" s="57"/>
+      <c r="B78" s="59"/>
       <c r="C78" s="7" t="s">
         <v>156</v>
       </c>
@@ -2806,8 +2807,8 @@
       </c>
     </row>
     <row r="79" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="55"/>
-      <c r="B79" s="61"/>
+      <c r="A79" s="57"/>
+      <c r="B79" s="54"/>
       <c r="C79" s="7" t="s">
         <v>157</v>
       </c>
@@ -2822,8 +2823,8 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="55"/>
-      <c r="B80" s="65" t="s">
+      <c r="A80" s="57"/>
+      <c r="B80" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C80" s="41" t="s">
@@ -2843,8 +2844,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="55"/>
-      <c r="B81" s="58"/>
+      <c r="A81" s="57"/>
+      <c r="B81" s="59"/>
       <c r="C81" s="7" t="s">
         <v>124</v>
       </c>
@@ -2859,8 +2860,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A82" s="56"/>
-      <c r="B82" s="59"/>
+      <c r="A82" s="58"/>
+      <c r="B82" s="61"/>
       <c r="C82" s="10" t="s">
         <v>158</v>
       </c>
@@ -2875,7 +2876,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="54" t="s">
+      <c r="A83" s="56" t="s">
         <v>159</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -2895,7 +2896,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="55"/>
+      <c r="A84" s="57"/>
       <c r="C84" s="7" t="s">
         <v>167</v>
       </c>
@@ -2910,7 +2911,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="56"/>
+      <c r="A85" s="58"/>
       <c r="B85" s="42" t="s">
         <v>15</v>
       </c>
@@ -2928,14 +2929,14 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="53" t="s">
+      <c r="A86" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="B86" s="53"/>
-      <c r="C86" s="53"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="53"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="55"/>
+      <c r="D86" s="55"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="55"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="15" t="s">
@@ -2970,28 +2971,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A86:F86"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A53:A61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="B64:B66"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -3008,6 +2987,28 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A53:A61"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working through EFM unit tests
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8082F67A-9131-4083-8189-87371A8CE879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4693FE5F-AE0B-4999-9901-0E2CA3B839D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="212">
   <si>
     <t>Class</t>
   </si>
@@ -1151,44 +1151,44 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1474,7 +1474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L67" sqref="L67"/>
+      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1509,14 +1509,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1559,10 +1559,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1579,8 +1579,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="58"/>
-      <c r="B6" s="61"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1595,20 +1595,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1626,7 +1626,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="63"/>
-      <c r="B9" s="59"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="63"/>
-      <c r="B10" s="59"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="63"/>
-      <c r="B11" s="59"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1674,7 +1674,7 @@
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="64"/>
-      <c r="B12" s="59"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1692,7 +1692,7 @@
       <c r="A13" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="57" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1710,7 +1710,7 @@
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="63"/>
-      <c r="B14" s="59"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="63"/>
-      <c r="B15" s="59"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="63"/>
-      <c r="B16" s="59"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="63"/>
-      <c r="B17" s="54"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="63"/>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1792,7 +1792,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="63"/>
-      <c r="B19" s="59"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="63"/>
-      <c r="B20" s="59"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="63"/>
-      <c r="B21" s="59"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1842,7 +1842,7 @@
       <c r="A22" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="57" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1860,7 +1860,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="63"/>
-      <c r="B23" s="54"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="63"/>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1894,7 +1894,7 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="63"/>
-      <c r="B25" s="59"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="37" t="s">
         <v>127</v>
       </c>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="63"/>
-      <c r="B26" s="59"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="63"/>
-      <c r="B27" s="59"/>
+      <c r="B27" s="58"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="63"/>
-      <c r="B28" s="59"/>
+      <c r="B28" s="58"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="63"/>
-      <c r="B29" s="59"/>
+      <c r="B29" s="58"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="63"/>
-      <c r="B30" s="59"/>
+      <c r="B30" s="58"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="63"/>
-      <c r="B31" s="59"/>
+      <c r="B31" s="58"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="64"/>
-      <c r="B32" s="61"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2021,10 +2021,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="57" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2041,8 +2041,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="57"/>
-      <c r="B34" s="59"/>
+      <c r="A34" s="55"/>
+      <c r="B34" s="58"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2057,8 +2057,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="58"/>
-      <c r="B35" s="61"/>
+      <c r="A35" s="56"/>
+      <c r="B35" s="59"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2073,14 +2073,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2103,10 +2103,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2123,8 +2123,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="57"/>
-      <c r="B39" s="59"/>
+      <c r="A39" s="55"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2139,8 +2139,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="58"/>
-      <c r="B40" s="61"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="59"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="A41" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2176,7 +2176,7 @@
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="63"/>
-      <c r="B42" s="59"/>
+      <c r="B42" s="58"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="63"/>
-      <c r="B43" s="59"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="64"/>
-      <c r="B44" s="61"/>
+      <c r="B44" s="59"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2303,10 +2303,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="53" t="s">
+      <c r="B49" s="57" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2323,8 +2323,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="57"/>
-      <c r="B50" s="54"/>
+      <c r="A50" s="55"/>
+      <c r="B50" s="61"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2339,7 +2339,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="57"/>
+      <c r="A51" s="55"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2357,20 +2357,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="55" t="s">
+      <c r="A52" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="65"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="65"/>
-      <c r="E52" s="55"/>
-      <c r="F52" s="55"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
     </row>
     <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -2388,7 +2388,7 @@
     </row>
     <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="63"/>
-      <c r="B54" s="59"/>
+      <c r="B54" s="58"/>
       <c r="C54" s="7" t="s">
         <v>135</v>
       </c>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="63"/>
-      <c r="B55" s="59"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="7" t="s">
         <v>136</v>
       </c>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="63"/>
-      <c r="B56" s="59"/>
+      <c r="B56" s="58"/>
       <c r="C56" s="7" t="s">
         <v>186</v>
       </c>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="57" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="63"/>
-      <c r="B57" s="59"/>
+      <c r="B57" s="58"/>
       <c r="C57" s="7" t="s">
         <v>137</v>
       </c>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="63"/>
-      <c r="B58" s="60" t="s">
+      <c r="B58" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="41" t="s">
@@ -2470,7 +2470,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="63"/>
-      <c r="B59" s="59"/>
+      <c r="B59" s="58"/>
       <c r="C59" s="7" t="s">
         <v>131</v>
       </c>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="63"/>
-      <c r="B60" s="59"/>
+      <c r="B60" s="58"/>
       <c r="C60" s="7" t="s">
         <v>132</v>
       </c>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="64"/>
-      <c r="B61" s="61"/>
+      <c r="B61" s="59"/>
       <c r="C61" s="7" t="s">
         <v>133</v>
       </c>
@@ -2517,10 +2517,10 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="56" t="s">
+      <c r="A62" s="54" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="53" t="s">
+      <c r="B62" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -2537,8 +2537,8 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="57"/>
-      <c r="B63" s="54"/>
+      <c r="A63" s="55"/>
+      <c r="B63" s="61"/>
       <c r="C63" s="7" t="s">
         <v>195</v>
       </c>
@@ -2548,11 +2548,13 @@
       <c r="E63" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F63" s="46"/>
+      <c r="F63" s="46" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="57"/>
-      <c r="B64" s="60" t="s">
+      <c r="A64" s="55"/>
+      <c r="B64" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="41" t="s">
@@ -2564,13 +2566,13 @@
       <c r="E64" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="46" t="s">
-        <v>203</v>
+      <c r="F64" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="57"/>
-      <c r="B65" s="59"/>
+      <c r="A65" s="55"/>
+      <c r="B65" s="58"/>
       <c r="C65" s="7" t="s">
         <v>197</v>
       </c>
@@ -2585,8 +2587,8 @@
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="58"/>
-      <c r="B66" s="61"/>
+      <c r="A66" s="56"/>
+      <c r="B66" s="59"/>
       <c r="C66" s="7" t="s">
         <v>198</v>
       </c>
@@ -2601,10 +2603,10 @@
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="56" t="s">
+      <c r="A67" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="B67" s="53" t="s">
+      <c r="B67" s="57" t="s">
         <v>190</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2621,8 +2623,8 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="57"/>
-      <c r="B68" s="59"/>
+      <c r="A68" s="55"/>
+      <c r="B68" s="58"/>
       <c r="C68" s="7" t="s">
         <v>192</v>
       </c>
@@ -2637,8 +2639,8 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="58"/>
-      <c r="B69" s="61"/>
+      <c r="A69" s="56"/>
+      <c r="B69" s="59"/>
       <c r="C69" s="10" t="s">
         <v>193</v>
       </c>
@@ -2653,10 +2655,10 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="56" t="s">
+      <c r="A70" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="B70" s="53" t="s">
+      <c r="B70" s="57" t="s">
         <v>138</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -2673,8 +2675,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="57"/>
-      <c r="B71" s="59"/>
+      <c r="A71" s="55"/>
+      <c r="B71" s="58"/>
       <c r="C71" s="7" t="s">
         <v>185</v>
       </c>
@@ -2689,8 +2691,8 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="58"/>
-      <c r="B72" s="61"/>
+      <c r="A72" s="56"/>
+      <c r="B72" s="59"/>
       <c r="C72" s="10" t="s">
         <v>139</v>
       </c>
@@ -2705,14 +2707,14 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" s="55" t="s">
+      <c r="A73" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="B73" s="55"/>
-      <c r="C73" s="55"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="55"/>
+      <c r="B73" s="53"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="53"/>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53"/>
     </row>
     <row r="74" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
@@ -2755,10 +2757,10 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="56" t="s">
+      <c r="A76" s="54" t="s">
         <v>153</v>
       </c>
-      <c r="B76" s="53" t="s">
+      <c r="B76" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C76" s="7" t="s">
@@ -2775,8 +2777,8 @@
       </c>
     </row>
     <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="57"/>
-      <c r="B77" s="59"/>
+      <c r="A77" s="55"/>
+      <c r="B77" s="58"/>
       <c r="C77" s="7" t="s">
         <v>155</v>
       </c>
@@ -2791,8 +2793,8 @@
       </c>
     </row>
     <row r="78" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="57"/>
-      <c r="B78" s="59"/>
+      <c r="A78" s="55"/>
+      <c r="B78" s="58"/>
       <c r="C78" s="7" t="s">
         <v>156</v>
       </c>
@@ -2807,8 +2809,8 @@
       </c>
     </row>
     <row r="79" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="57"/>
-      <c r="B79" s="54"/>
+      <c r="A79" s="55"/>
+      <c r="B79" s="61"/>
       <c r="C79" s="7" t="s">
         <v>157</v>
       </c>
@@ -2823,8 +2825,8 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="57"/>
-      <c r="B80" s="60" t="s">
+      <c r="A80" s="55"/>
+      <c r="B80" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C80" s="41" t="s">
@@ -2844,8 +2846,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="57"/>
-      <c r="B81" s="59"/>
+      <c r="A81" s="55"/>
+      <c r="B81" s="58"/>
       <c r="C81" s="7" t="s">
         <v>124</v>
       </c>
@@ -2860,8 +2862,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A82" s="58"/>
-      <c r="B82" s="61"/>
+      <c r="A82" s="56"/>
+      <c r="B82" s="59"/>
       <c r="C82" s="10" t="s">
         <v>158</v>
       </c>
@@ -2876,7 +2878,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="56" t="s">
+      <c r="A83" s="54" t="s">
         <v>159</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -2896,7 +2898,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="57"/>
+      <c r="A84" s="55"/>
       <c r="C84" s="7" t="s">
         <v>167</v>
       </c>
@@ -2911,7 +2913,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="58"/>
+      <c r="A85" s="56"/>
       <c r="B85" s="42" t="s">
         <v>15</v>
       </c>
@@ -2929,14 +2931,14 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="55" t="s">
+      <c r="A86" s="53" t="s">
         <v>172</v>
       </c>
-      <c r="B86" s="55"/>
-      <c r="C86" s="55"/>
-      <c r="D86" s="55"/>
-      <c r="E86" s="55"/>
-      <c r="F86" s="55"/>
+      <c r="B86" s="53"/>
+      <c r="C86" s="53"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="53"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="15" t="s">
@@ -2971,6 +2973,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A53:A61"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B62:B63"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -2987,28 +3011,6 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A53:A61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A86:F86"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished all unit tests and comments
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4693FE5F-AE0B-4999-9901-0E2CA3B839D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454B5330-EB47-4E87-8C62-520B856E9CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="211">
   <si>
     <t>Class</t>
   </si>
@@ -645,9 +645,6 @@
   </si>
   <si>
     <t>Initializes empty numpy arrays for the space remaining points in each discipline to be able to track their history of pass-fail predictions.</t>
-  </si>
-  <si>
-    <t>Incomplete</t>
   </si>
   <si>
     <t>Gathers the pass-fail data pertinent to each discipline's remaining potential design solutions for eventual sorting of the history of a point's predictions.</t>
@@ -1151,44 +1148,44 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1473,8 +1470,8 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1509,14 +1506,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
@@ -1559,10 +1556,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1579,8 +1576,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="56"/>
-      <c r="B6" s="59"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
       <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
@@ -1595,20 +1592,20 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1626,7 +1623,7 @@
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="63"/>
-      <c r="B9" s="58"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1642,7 +1639,7 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="63"/>
-      <c r="B10" s="58"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
@@ -1658,7 +1655,7 @@
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="63"/>
-      <c r="B11" s="58"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="7" t="s">
         <v>77</v>
       </c>
@@ -1674,7 +1671,7 @@
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="64"/>
-      <c r="B12" s="58"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="7" t="s">
         <v>78</v>
       </c>
@@ -1692,7 +1689,7 @@
       <c r="A13" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1710,7 +1707,7 @@
     </row>
     <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="63"/>
-      <c r="B14" s="58"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
@@ -1726,7 +1723,7 @@
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="63"/>
-      <c r="B15" s="58"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="7" t="s">
         <v>87</v>
       </c>
@@ -1742,7 +1739,7 @@
     </row>
     <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="63"/>
-      <c r="B16" s="58"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="7" t="s">
         <v>95</v>
       </c>
@@ -1758,7 +1755,7 @@
     </row>
     <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="63"/>
-      <c r="B17" s="61"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="25" t="s">
         <v>86</v>
       </c>
@@ -1774,7 +1771,7 @@
     </row>
     <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="63"/>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1792,7 +1789,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="63"/>
-      <c r="B19" s="58"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="7" t="s">
         <v>91</v>
       </c>
@@ -1808,7 +1805,7 @@
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="63"/>
-      <c r="B20" s="58"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="7" t="s">
         <v>66</v>
       </c>
@@ -1824,7 +1821,7 @@
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="63"/>
-      <c r="B21" s="58"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="7" t="s">
         <v>93</v>
       </c>
@@ -1842,7 +1839,7 @@
       <c r="A22" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="56" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -1860,7 +1857,7 @@
     </row>
     <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="63"/>
-      <c r="B23" s="61"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="39" t="s">
         <v>110</v>
       </c>
@@ -1876,7 +1873,7 @@
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="63"/>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -1894,7 +1891,7 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="63"/>
-      <c r="B25" s="58"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="37" t="s">
         <v>127</v>
       </c>
@@ -1910,7 +1907,7 @@
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="63"/>
-      <c r="B26" s="58"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="37" t="s">
         <v>111</v>
       </c>
@@ -1926,7 +1923,7 @@
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="63"/>
-      <c r="B27" s="58"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="37" t="s">
         <v>124</v>
       </c>
@@ -1942,7 +1939,7 @@
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="63"/>
-      <c r="B28" s="58"/>
+      <c r="B28" s="57"/>
       <c r="C28" s="37" t="s">
         <v>112</v>
       </c>
@@ -1958,7 +1955,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="63"/>
-      <c r="B29" s="58"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="37" t="s">
         <v>113</v>
       </c>
@@ -1974,7 +1971,7 @@
     </row>
     <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="63"/>
-      <c r="B30" s="58"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="37" t="s">
         <v>114</v>
       </c>
@@ -1990,7 +1987,7 @@
     </row>
     <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="63"/>
-      <c r="B31" s="58"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="37" t="s">
         <v>115</v>
       </c>
@@ -2006,7 +2003,7 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="64"/>
-      <c r="B32" s="59"/>
+      <c r="B32" s="58"/>
       <c r="C32" s="10" t="s">
         <v>116</v>
       </c>
@@ -2021,10 +2018,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="57" t="s">
+      <c r="B33" s="56" t="s">
         <v>68</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2041,8 +2038,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="55"/>
-      <c r="B34" s="58"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="57"/>
       <c r="C34" s="7" t="s">
         <v>70</v>
       </c>
@@ -2057,8 +2054,8 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="56"/>
-      <c r="B35" s="59"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="58"/>
       <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
@@ -2073,14 +2070,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="53" t="s">
+      <c r="A36" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
@@ -2103,10 +2100,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="54" t="s">
+      <c r="A38" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2123,8 +2120,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="55"/>
-      <c r="B39" s="58"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="7" t="s">
         <v>17</v>
       </c>
@@ -2139,8 +2136,8 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="56"/>
-      <c r="B40" s="59"/>
+      <c r="A40" s="55"/>
+      <c r="B40" s="58"/>
       <c r="C40" s="7" t="s">
         <v>101</v>
       </c>
@@ -2158,7 +2155,7 @@
       <c r="A41" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="57" t="s">
+      <c r="B41" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2176,7 +2173,7 @@
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="63"/>
-      <c r="B42" s="58"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
@@ -2192,7 +2189,7 @@
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="63"/>
-      <c r="B43" s="58"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="7" t="s">
         <v>24</v>
       </c>
@@ -2208,7 +2205,7 @@
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="64"/>
-      <c r="B44" s="59"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
@@ -2303,10 +2300,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="54" t="s">
+      <c r="A49" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="56" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2323,8 +2320,8 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="55"/>
-      <c r="B50" s="61"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="60"/>
       <c r="C50" s="25" t="s">
         <v>45</v>
       </c>
@@ -2339,7 +2336,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="55"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="35" t="s">
         <v>15</v>
       </c>
@@ -2357,20 +2354,20 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="53" t="s">
+      <c r="A52" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="60"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
     </row>
     <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -2388,12 +2385,12 @@
     </row>
     <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="63"/>
-      <c r="B54" s="58"/>
+      <c r="B54" s="57"/>
       <c r="C54" s="7" t="s">
         <v>135</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E54" s="30" t="s">
         <v>9</v>
@@ -2404,7 +2401,7 @@
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="63"/>
-      <c r="B55" s="58"/>
+      <c r="B55" s="57"/>
       <c r="C55" s="7" t="s">
         <v>136</v>
       </c>
@@ -2420,7 +2417,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="63"/>
-      <c r="B56" s="58"/>
+      <c r="B56" s="57"/>
       <c r="C56" s="7" t="s">
         <v>186</v>
       </c>
@@ -2436,12 +2433,12 @@
     </row>
     <row r="57" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="63"/>
-      <c r="B57" s="58"/>
+      <c r="B57" s="57"/>
       <c r="C57" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E57" s="52" t="s">
         <v>9</v>
@@ -2452,14 +2449,14 @@
     </row>
     <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="63"/>
-      <c r="B58" s="65" t="s">
+      <c r="B58" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E58" s="30" t="s">
         <v>9</v>
@@ -2470,7 +2467,7 @@
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="63"/>
-      <c r="B59" s="58"/>
+      <c r="B59" s="57"/>
       <c r="C59" s="7" t="s">
         <v>131</v>
       </c>
@@ -2486,7 +2483,7 @@
     </row>
     <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A60" s="63"/>
-      <c r="B60" s="58"/>
+      <c r="B60" s="57"/>
       <c r="C60" s="7" t="s">
         <v>132</v>
       </c>
@@ -2502,7 +2499,7 @@
     </row>
     <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="64"/>
-      <c r="B61" s="59"/>
+      <c r="B61" s="58"/>
       <c r="C61" s="7" t="s">
         <v>133</v>
       </c>
@@ -2517,17 +2514,17 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="54" t="s">
+      <c r="A62" s="53" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="57" t="s">
+      <c r="B62" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>194</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E62" s="29" t="s">
         <v>9</v>
@@ -2537,31 +2534,31 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="55"/>
-      <c r="B63" s="61"/>
+      <c r="A63" s="54"/>
+      <c r="B63" s="60"/>
       <c r="C63" s="7" t="s">
         <v>195</v>
       </c>
       <c r="D63" s="45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E63" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F63" s="46" t="s">
-        <v>203</v>
+      <c r="F63" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="55"/>
-      <c r="B64" s="65" t="s">
+      <c r="A64" s="54"/>
+      <c r="B64" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="41" t="s">
         <v>196</v>
       </c>
       <c r="D64" s="51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E64" s="30" t="s">
         <v>9</v>
@@ -2571,8 +2568,8 @@
       </c>
     </row>
     <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="55"/>
-      <c r="B65" s="58"/>
+      <c r="A65" s="54"/>
+      <c r="B65" s="57"/>
       <c r="C65" s="7" t="s">
         <v>197</v>
       </c>
@@ -2582,31 +2579,31 @@
       <c r="E65" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="46" t="s">
-        <v>203</v>
+      <c r="F65" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="56"/>
-      <c r="B66" s="59"/>
+      <c r="A66" s="55"/>
+      <c r="B66" s="58"/>
       <c r="C66" s="7" t="s">
         <v>198</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E66" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="46" t="s">
-        <v>203</v>
+      <c r="F66" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="B67" s="57" t="s">
+      <c r="B67" s="56" t="s">
         <v>190</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2623,8 +2620,8 @@
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="55"/>
-      <c r="B68" s="58"/>
+      <c r="A68" s="54"/>
+      <c r="B68" s="57"/>
       <c r="C68" s="7" t="s">
         <v>192</v>
       </c>
@@ -2639,8 +2636,8 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="56"/>
-      <c r="B69" s="59"/>
+      <c r="A69" s="55"/>
+      <c r="B69" s="58"/>
       <c r="C69" s="10" t="s">
         <v>193</v>
       </c>
@@ -2655,10 +2652,10 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="56" t="s">
         <v>138</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -2675,8 +2672,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="55"/>
-      <c r="B71" s="58"/>
+      <c r="A71" s="54"/>
+      <c r="B71" s="57"/>
       <c r="C71" s="7" t="s">
         <v>185</v>
       </c>
@@ -2691,8 +2688,8 @@
       </c>
     </row>
     <row r="72" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="56"/>
-      <c r="B72" s="59"/>
+      <c r="A72" s="55"/>
+      <c r="B72" s="58"/>
       <c r="C72" s="10" t="s">
         <v>139</v>
       </c>
@@ -2707,14 +2704,14 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" s="53" t="s">
+      <c r="A73" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="B73" s="53"/>
-      <c r="C73" s="53"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="53"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
     </row>
     <row r="74" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="13" t="s">
@@ -2757,10 +2754,10 @@
       </c>
     </row>
     <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="54" t="s">
+      <c r="A76" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="B76" s="57" t="s">
+      <c r="B76" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C76" s="7" t="s">
@@ -2777,8 +2774,8 @@
       </c>
     </row>
     <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="55"/>
-      <c r="B77" s="58"/>
+      <c r="A77" s="54"/>
+      <c r="B77" s="57"/>
       <c r="C77" s="7" t="s">
         <v>155</v>
       </c>
@@ -2793,8 +2790,8 @@
       </c>
     </row>
     <row r="78" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="55"/>
-      <c r="B78" s="58"/>
+      <c r="A78" s="54"/>
+      <c r="B78" s="57"/>
       <c r="C78" s="7" t="s">
         <v>156</v>
       </c>
@@ -2809,8 +2806,8 @@
       </c>
     </row>
     <row r="79" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="55"/>
-      <c r="B79" s="61"/>
+      <c r="A79" s="54"/>
+      <c r="B79" s="60"/>
       <c r="C79" s="7" t="s">
         <v>157</v>
       </c>
@@ -2825,8 +2822,8 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="55"/>
-      <c r="B80" s="65" t="s">
+      <c r="A80" s="54"/>
+      <c r="B80" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C80" s="41" t="s">
@@ -2846,8 +2843,8 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="55"/>
-      <c r="B81" s="58"/>
+      <c r="A81" s="54"/>
+      <c r="B81" s="57"/>
       <c r="C81" s="7" t="s">
         <v>124</v>
       </c>
@@ -2862,8 +2859,8 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A82" s="56"/>
-      <c r="B82" s="59"/>
+      <c r="A82" s="55"/>
+      <c r="B82" s="58"/>
       <c r="C82" s="10" t="s">
         <v>158</v>
       </c>
@@ -2878,7 +2875,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="54" t="s">
+      <c r="A83" s="53" t="s">
         <v>159</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -2898,7 +2895,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="55"/>
+      <c r="A84" s="54"/>
       <c r="C84" s="7" t="s">
         <v>167</v>
       </c>
@@ -2913,7 +2910,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" s="56"/>
+      <c r="A85" s="55"/>
       <c r="B85" s="42" t="s">
         <v>15</v>
       </c>
@@ -2931,14 +2928,14 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="53" t="s">
+      <c r="A86" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="B86" s="53"/>
-      <c r="C86" s="53"/>
-      <c r="D86" s="53"/>
-      <c r="E86" s="53"/>
-      <c r="F86" s="53"/>
+      <c r="B86" s="59"/>
+      <c r="C86" s="59"/>
+      <c r="D86" s="59"/>
+      <c r="E86" s="59"/>
+      <c r="F86" s="59"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="15" t="s">
@@ -2973,28 +2970,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="A86:F86"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A53:A61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B62:B63"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A38:A40"/>
@@ -3011,6 +2986,28 @@
     <mergeCell ref="A22:A32"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B32"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A53:A61"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B80:B82"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A83:A85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Getting through unit tests again
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABAC88C-9B18-4968-BEC8-7C3469D90A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EB7B5F-9F3A-42CD-AF90-DCE4A2101F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="217">
   <si>
     <t>Class</t>
   </si>
@@ -675,6 +675,18 @@
   </si>
   <si>
     <t>Plots data points for a single dataset within a given discipline.</t>
+  </si>
+  <si>
+    <t>Sen Yang</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Creates the list of dictionaries and set of rules for Sen and Yang Bulk Carrier problem.</t>
+  </si>
+  <si>
+    <t>Creates an expression that denormalizes an input variable.</t>
   </si>
 </sst>
 </file>
@@ -697,7 +709,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -722,6 +734,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -990,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1037,9 +1055,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1142,6 +1157,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1160,31 +1178,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1467,11 +1515,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1485,27 +1533,27 @@
     <col min="7" max="16384" width="8.81640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
         <v>54</v>
       </c>
@@ -1515,1517 +1563,1554 @@
       <c r="E2" s="57"/>
       <c r="F2" s="57"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="34" t="s">
+      <c r="E3" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="30" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="G3" s="64"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="60"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="64"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="61"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="64"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="51" t="s">
+      <c r="E6" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B7" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="10" t="s">
+      <c r="E7" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="53"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="34" t="s">
+      <c r="E8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="63" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-    </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="60" t="s">
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B10" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="61"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="61"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="61"/>
+      <c r="E10" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="60"/>
       <c r="B11" s="55"/>
       <c r="C11" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="62"/>
+        <v>80</v>
+      </c>
+      <c r="E11" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="60"/>
       <c r="B12" s="55"/>
       <c r="C12" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="E12" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="60"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="61"/>
       <c r="B14" s="55"/>
       <c r="C14" s="7" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="61"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="61"/>
+        <v>83</v>
+      </c>
+      <c r="E14" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="60"/>
       <c r="B16" s="55"/>
       <c r="C16" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="60"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="60"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="61"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="25" t="s">
+      <c r="E18" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="60"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="61"/>
-      <c r="B18" s="55" t="s">
+      <c r="E19" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="60"/>
+      <c r="B20" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="61"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="61"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
+      <c r="E20" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="60"/>
       <c r="B21" s="55"/>
       <c r="C21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="60"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="60"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="60" t="s">
+      <c r="E23" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B24" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C24" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="61"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="39" t="s">
+      <c r="E24" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="60"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="55" t="s">
+      <c r="E25" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="60"/>
+      <c r="B26" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D26" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="37" t="s">
+      <c r="E26" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="60"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="37" t="s">
+      <c r="E27" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="60"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="32" t="s">
+      <c r="E28" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="74" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="37" t="s">
+    <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="60"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="61"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="37" t="s">
+      <c r="E29" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="60"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="61"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="37" t="s">
+      <c r="E30" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="60"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="32" t="s">
+      <c r="E31" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="74" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="61"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="37" t="s">
+    <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="60"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D32" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="61"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="37" t="s">
+      <c r="E32" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="60"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D33" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="62"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="10" t="s">
+      <c r="E33" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="61"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D34" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="51" t="s">
+      <c r="E34" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B35" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="52"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="7" t="s">
+      <c r="E35" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="52"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E34" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="53"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="7" t="s">
+      <c r="E36" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="53"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D37" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="57" t="s">
+      <c r="E37" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="51" t="s">
+      <c r="E39" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B40" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="52"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="7" t="s">
+      <c r="E40" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="52"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="53"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="7" t="s">
+      <c r="E41" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="53"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E40" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="60" t="s">
+      <c r="E42" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B43" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="31" t="s">
+      <c r="E43" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="65" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="61"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="7" t="s">
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="60"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D44" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="32" t="s">
+      <c r="E44" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="74" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="61"/>
-      <c r="B43" s="55"/>
-      <c r="C43" s="7" t="s">
+    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="60"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="32" t="s">
+      <c r="E45" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="74" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="62"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="7" t="s">
+    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="61"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="32" t="s">
+      <c r="E46" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="74" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
+    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B47" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="14" t="s">
+      <c r="E47" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="14" t="s">
+      <c r="E48" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="s">
+      <c r="E49" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="51" t="s">
+      <c r="E50" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="54" t="s">
+      <c r="B51" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="52"/>
-      <c r="B50" s="58"/>
-      <c r="C50" s="25" t="s">
+      <c r="E51" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="52"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D50" s="26" t="s">
+      <c r="D52" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E50" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="52"/>
-      <c r="B51" s="35" t="s">
+      <c r="E52" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A53" s="52"/>
+      <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C53" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D53" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E51" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="57" t="s">
+      <c r="E53" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="63"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-    </row>
-    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="60" t="s">
+      <c r="B54" s="57"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+    </row>
+    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B55" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D55" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="61"/>
-      <c r="B54" s="55"/>
-      <c r="C54" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E54" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="61"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E55" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="61"/>
+      <c r="E55" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="60"/>
       <c r="B56" s="55"/>
       <c r="C56" s="7" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="E56" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="61"/>
+        <v>207</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="60"/>
       <c r="B57" s="55"/>
       <c r="C57" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="E57" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="61"/>
-      <c r="B58" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="41" t="s">
-        <v>206</v>
-      </c>
-      <c r="D58" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="E58" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="61"/>
+        <v>142</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="60"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="60"/>
       <c r="B59" s="55"/>
       <c r="C59" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E59" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="60"/>
+      <c r="B60" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="D60" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="60"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D61" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E59" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A60" s="61"/>
-      <c r="B60" s="55"/>
-      <c r="C60" s="7" t="s">
+      <c r="E61" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A62" s="60"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D62" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E60" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="62"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="7" t="s">
+      <c r="E62" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" s="61"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D63" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E61" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="32" t="s">
+      <c r="E63" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="51" t="s">
+    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="B62" s="54" t="s">
+      <c r="B64" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D62" s="47" t="s">
+      <c r="D64" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="E62" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="29" t="s">
+      <c r="E64" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="52"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="7" t="s">
+    <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="52"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D63" s="45" t="s">
+      <c r="D65" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="E63" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="52"/>
-      <c r="B64" s="59" t="s">
+      <c r="E65" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="52"/>
+      <c r="B66" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="C66" s="40" t="s">
         <v>196</v>
       </c>
-      <c r="D64" s="49" t="s">
+      <c r="D66" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="E64" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="52"/>
-      <c r="B65" s="55"/>
-      <c r="C65" s="7" t="s">
+      <c r="E66" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="52"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D65" s="45" t="s">
+      <c r="D67" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="E65" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="53"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="7" t="s">
+      <c r="E67" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="53"/>
+      <c r="B68" s="56"/>
+      <c r="C68" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D66" s="45" t="s">
+      <c r="D68" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="E66" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="51" t="s">
+      <c r="E68" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="B67" s="54" t="s">
+      <c r="B69" s="54" t="s">
         <v>190</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D67" s="47" t="s">
+      <c r="D69" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="E67" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="29" t="s">
+      <c r="E69" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="52"/>
-      <c r="B68" s="55"/>
-      <c r="C68" s="7" t="s">
+    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="52"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D68" s="45" t="s">
+      <c r="D70" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="E68" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="30" t="s">
+      <c r="E70" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="53"/>
-      <c r="B69" s="56"/>
-      <c r="C69" s="10" t="s">
+    <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="53"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D69" s="48" t="s">
+      <c r="D71" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="E69" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="33" t="s">
+      <c r="E71" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="51" t="s">
+    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B70" s="54" t="s">
+      <c r="B72" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E70" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="52"/>
-      <c r="B71" s="55"/>
-      <c r="C71" s="7" t="s">
+      <c r="E72" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="52"/>
+      <c r="B73" s="55"/>
+      <c r="C73" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D73" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E71" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="53"/>
-      <c r="B72" s="56"/>
-      <c r="C72" s="10" t="s">
+      <c r="E73" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="53"/>
+      <c r="B74" s="56"/>
+      <c r="C74" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D72" s="24" t="s">
+      <c r="D74" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E72" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" s="57" t="s">
+      <c r="E74" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B73" s="57"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="57"/>
-      <c r="F73" s="57"/>
-    </row>
-    <row r="74" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A74" s="13" t="s">
+      <c r="B75" s="50"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+    </row>
+    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B76" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C76" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D74" s="23" t="s">
+      <c r="D76" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E74" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="28" t="s">
+      <c r="E76" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="13" t="s">
+    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B77" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C77" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D75" s="23" t="s">
+      <c r="D77" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="E75" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="28" t="s">
+      <c r="E77" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="51" t="s">
+    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="B76" s="54" t="s">
+      <c r="B78" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C78" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D76" s="9" t="s">
+      <c r="D78" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E76" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="32" t="s">
+      <c r="E78" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="52"/>
-      <c r="B77" s="55"/>
-      <c r="C77" s="7" t="s">
+    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="52"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D77" s="9" t="s">
+      <c r="D79" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="E77" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="52"/>
-      <c r="B78" s="55"/>
-      <c r="C78" s="7" t="s">
+      <c r="E79" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A80" s="52"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D80" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E78" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="52"/>
-      <c r="B79" s="58"/>
-      <c r="C79" s="7" t="s">
+      <c r="E80" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="52"/>
+      <c r="B81" s="58"/>
+      <c r="C81" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D81" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E79" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="52"/>
-      <c r="B80" s="59" t="s">
+      <c r="E81" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="52"/>
+      <c r="B82" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C80" s="41" t="s">
+      <c r="C82" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="D80" s="38" t="s">
+      <c r="D82" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="E80" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="J80" s="7" t="s">
+      <c r="E82" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J82" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="52"/>
-      <c r="B81" s="55"/>
-      <c r="C81" s="7" t="s">
+    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="52"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D83" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E81" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A82" s="53"/>
-      <c r="B82" s="56"/>
-      <c r="C82" s="10" t="s">
+      <c r="E83" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A84" s="53"/>
+      <c r="B84" s="56"/>
+      <c r="C84" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D82" s="24" t="s">
+      <c r="D84" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="E82" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="51" t="s">
+      <c r="E84" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="B83" s="54" t="s">
+      <c r="B85" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D85" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E83" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="31" t="s">
+      <c r="E85" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" s="52"/>
-      <c r="B84" s="55"/>
-      <c r="C84" s="64" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A86" s="52"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="D84" s="9" t="s">
+      <c r="D86" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E84" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="32" t="s">
+      <c r="E86" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A85" s="52"/>
-      <c r="B85" s="58"/>
-      <c r="C85" s="7" t="s">
+    <row r="87" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="52"/>
+      <c r="B87" s="58"/>
+      <c r="C87" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D85" s="9" t="s">
+      <c r="D87" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="E85" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="32" t="s">
+      <c r="E87" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="53"/>
-      <c r="B86" s="42" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" s="53"/>
+      <c r="B88" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C86" s="43" t="s">
+      <c r="C88" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="D86" s="44" t="s">
+      <c r="D88" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="E86" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="34" t="s">
+      <c r="E88" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="57" t="s">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" s="50" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="57"/>
-      <c r="C87" s="57"/>
-      <c r="D87" s="57"/>
-      <c r="E87" s="57"/>
-      <c r="F87" s="57"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" s="15" t="s">
+      <c r="B89" s="50"/>
+      <c r="C89" s="50"/>
+      <c r="D89" s="50"/>
+      <c r="E89" s="50"/>
+      <c r="F89" s="50"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B90" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C89" s="7" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C91" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C90" s="7" t="s">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C92" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C91" s="7" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C93" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C92" s="7" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C94" s="7" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="41">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A55:A63"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B64:B65"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="A22:A32"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A53:A61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="B80:B82"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A73:F73"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Almost through all of the unit testing
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EB7B5F-9F3A-42CD-AF90-DCE4A2101F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D558DD-0BFF-402F-B24C-722AD56B0D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1157,83 +1157,77 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1519,7 +1513,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1554,20 +1548,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="64" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1582,41 +1576,41 @@
       <c r="F3" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="60"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="63" t="s">
+      <c r="A4" s="62"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="67" t="s">
+      <c r="E4" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="64"/>
+      <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="61"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="10" t="s">
         <v>214</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="69" t="s">
+      <c r="E5" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="64"/>
+      <c r="G5" s="50"/>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
@@ -1631,18 +1625,18 @@
       <c r="D6" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="71" t="s">
+      <c r="E6" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="57" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1659,8 +1653,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1675,20 +1669,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1697,82 +1691,82 @@
       <c r="D10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="65" t="s">
+      <c r="E10" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="51" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="60"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="74" t="s">
+      <c r="E11" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="60"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="74" t="s">
+      <c r="E12" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
-      <c r="B13" s="55"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="74" t="s">
+      <c r="E13" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="61"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="75" t="s">
+      <c r="E14" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="60" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="64" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1781,80 +1775,80 @@
       <c r="D15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="65" t="s">
+      <c r="E15" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="51" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="60"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="74" t="s">
+      <c r="E16" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="59" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="60"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="74" t="s">
+      <c r="E17" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="60"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="74" t="s">
+      <c r="E18" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="60"/>
-      <c r="B19" s="58"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="74" t="s">
+      <c r="E19" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="60"/>
-      <c r="B20" s="55" t="s">
+      <c r="A20" s="62"/>
+      <c r="B20" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1863,66 +1857,66 @@
       <c r="D20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="74" t="s">
+      <c r="E20" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="60"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="74" t="s">
+      <c r="E21" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="60"/>
-      <c r="B22" s="55"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="74" t="s">
+      <c r="E22" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="60"/>
-      <c r="B23" s="55"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="74" t="s">
+      <c r="E23" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="59" t="s">
+      <c r="A24" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="64" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="35" t="s">
@@ -1931,32 +1925,32 @@
       <c r="D24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="65" t="s">
+      <c r="E24" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="51" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="60"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="74" t="s">
+      <c r="E25" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="60"/>
-      <c r="B26" s="55" t="s">
+      <c r="A26" s="62"/>
+      <c r="B26" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1965,146 +1959,146 @@
       <c r="D26" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="74" t="s">
+      <c r="E26" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="60"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="62"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E27" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="74" t="s">
+      <c r="E27" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="60"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="74" t="s">
+      <c r="E28" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="59" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="60"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="74" t="s">
+      <c r="E29" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="60"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="74" t="s">
+      <c r="E30" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="60"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="65"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E31" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="74" t="s">
+      <c r="E31" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="59" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="60"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="65"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E32" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="74" t="s">
+      <c r="E32" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="60"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E33" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="74" t="s">
+      <c r="E33" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="61"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="63"/>
+      <c r="B34" s="66"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="E34" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="75" t="s">
+      <c r="E34" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="60" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="64" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2113,54 +2107,54 @@
       <c r="D35" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="74" t="s">
+      <c r="E35" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="52"/>
-      <c r="B36" s="55"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="65"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="74" t="s">
+      <c r="E36" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="53"/>
-      <c r="B37" s="56"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="74" t="s">
+      <c r="E37" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="70"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="70"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2175,18 +2169,18 @@
       <c r="D39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="71" t="s">
+      <c r="E39" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="57" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2195,50 +2189,50 @@
       <c r="D40" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="65" t="s">
+      <c r="E40" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="51" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="52"/>
-      <c r="B41" s="55"/>
+      <c r="A41" s="68"/>
+      <c r="B41" s="65"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="74" t="s">
+      <c r="E41" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="53"/>
-      <c r="B42" s="56"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="66"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="74" t="s">
+      <c r="E42" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="59" t="s">
+      <c r="A43" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2247,58 +2241,58 @@
       <c r="D43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="65" t="s">
+      <c r="E43" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="51" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="60"/>
-      <c r="B44" s="55"/>
+      <c r="A44" s="62"/>
+      <c r="B44" s="65"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="74" t="s">
+      <c r="E44" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="59" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="60"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="62"/>
+      <c r="B45" s="65"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="74" t="s">
+      <c r="E45" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="59" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="61"/>
-      <c r="B46" s="56"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="66"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E46" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="74" t="s">
+      <c r="E46" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="59" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2315,10 +2309,10 @@
       <c r="D47" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="65" t="s">
+      <c r="E47" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="51" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2335,10 +2329,10 @@
       <c r="D48" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E48" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="65" t="s">
+      <c r="E48" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="51" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2355,10 +2349,10 @@
       <c r="D49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="65" t="s">
+      <c r="E49" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="51" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2375,18 +2369,18 @@
       <c r="D50" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="30" t="s">
+      <c r="E50" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="51" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="64" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2403,8 +2397,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="52"/>
-      <c r="B52" s="58"/>
+      <c r="A52" s="68"/>
+      <c r="B52" s="71"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2419,7 +2413,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="52"/>
+      <c r="A53" s="68"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2437,20 +2431,20 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="50" t="s">
+      <c r="A54" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="57"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
+      <c r="B54" s="73"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="70"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="59" t="s">
+      <c r="A55" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="54" t="s">
+      <c r="B55" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -2467,8 +2461,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="60"/>
-      <c r="B56" s="55"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="65"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
@@ -2483,8 +2477,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="60"/>
-      <c r="B57" s="55"/>
+      <c r="A57" s="62"/>
+      <c r="B57" s="65"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2499,8 +2493,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="60"/>
-      <c r="B58" s="55"/>
+      <c r="A58" s="62"/>
+      <c r="B58" s="65"/>
       <c r="C58" s="7" t="s">
         <v>186</v>
       </c>
@@ -2515,8 +2509,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="60"/>
-      <c r="B59" s="55"/>
+      <c r="A59" s="62"/>
+      <c r="B59" s="65"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2531,8 +2525,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="60"/>
-      <c r="B60" s="62" t="s">
+      <c r="A60" s="62"/>
+      <c r="B60" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C60" s="40" t="s">
@@ -2549,8 +2543,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="60"/>
-      <c r="B61" s="55"/>
+      <c r="A61" s="62"/>
+      <c r="B61" s="65"/>
       <c r="C61" s="7" t="s">
         <v>131</v>
       </c>
@@ -2565,8 +2559,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="60"/>
-      <c r="B62" s="55"/>
+      <c r="A62" s="62"/>
+      <c r="B62" s="65"/>
       <c r="C62" s="7" t="s">
         <v>132</v>
       </c>
@@ -2581,8 +2575,8 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="61"/>
-      <c r="B63" s="56"/>
+      <c r="A63" s="63"/>
+      <c r="B63" s="66"/>
       <c r="C63" s="7" t="s">
         <v>133</v>
       </c>
@@ -2597,10 +2591,10 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="51" t="s">
+      <c r="A64" s="67" t="s">
         <v>189</v>
       </c>
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -2617,8 +2611,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="52"/>
-      <c r="B65" s="58"/>
+      <c r="A65" s="68"/>
+      <c r="B65" s="71"/>
       <c r="C65" s="7" t="s">
         <v>195</v>
       </c>
@@ -2633,8 +2627,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="52"/>
-      <c r="B66" s="62" t="s">
+      <c r="A66" s="68"/>
+      <c r="B66" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="40" t="s">
@@ -2651,8 +2645,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="52"/>
-      <c r="B67" s="55"/>
+      <c r="A67" s="68"/>
+      <c r="B67" s="65"/>
       <c r="C67" s="7" t="s">
         <v>197</v>
       </c>
@@ -2667,8 +2661,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="53"/>
-      <c r="B68" s="56"/>
+      <c r="A68" s="69"/>
+      <c r="B68" s="66"/>
       <c r="C68" s="7" t="s">
         <v>198</v>
       </c>
@@ -2683,10 +2677,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="51" t="s">
+      <c r="A69" s="67" t="s">
         <v>184</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="64" t="s">
         <v>190</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -2703,8 +2697,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="52"/>
-      <c r="B70" s="55"/>
+      <c r="A70" s="68"/>
+      <c r="B70" s="65"/>
       <c r="C70" s="7" t="s">
         <v>192</v>
       </c>
@@ -2719,8 +2713,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="53"/>
-      <c r="B71" s="56"/>
+      <c r="A71" s="69"/>
+      <c r="B71" s="66"/>
       <c r="C71" s="10" t="s">
         <v>193</v>
       </c>
@@ -2735,10 +2729,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="B72" s="54" t="s">
+      <c r="B72" s="64" t="s">
         <v>138</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -2755,8 +2749,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="52"/>
-      <c r="B73" s="55"/>
+      <c r="A73" s="68"/>
+      <c r="B73" s="65"/>
       <c r="C73" s="7" t="s">
         <v>185</v>
       </c>
@@ -2771,8 +2765,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="53"/>
-      <c r="B74" s="56"/>
+      <c r="A74" s="69"/>
+      <c r="B74" s="66"/>
       <c r="C74" s="10" t="s">
         <v>139</v>
       </c>
@@ -2787,14 +2781,14 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="50" t="s">
+      <c r="A75" s="70" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="50"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
+      <c r="B75" s="70"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="70"/>
+      <c r="F75" s="70"/>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
@@ -2837,10 +2831,10 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="51" t="s">
+      <c r="A78" s="67" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="54" t="s">
+      <c r="B78" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C78" s="7" t="s">
@@ -2857,8 +2851,8 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="52"/>
-      <c r="B79" s="55"/>
+      <c r="A79" s="68"/>
+      <c r="B79" s="65"/>
       <c r="C79" s="7" t="s">
         <v>155</v>
       </c>
@@ -2873,8 +2867,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="52"/>
-      <c r="B80" s="55"/>
+      <c r="A80" s="68"/>
+      <c r="B80" s="65"/>
       <c r="C80" s="7" t="s">
         <v>156</v>
       </c>
@@ -2889,8 +2883,8 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="52"/>
-      <c r="B81" s="58"/>
+      <c r="A81" s="68"/>
+      <c r="B81" s="71"/>
       <c r="C81" s="7" t="s">
         <v>157</v>
       </c>
@@ -2905,8 +2899,8 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="52"/>
-      <c r="B82" s="62" t="s">
+      <c r="A82" s="68"/>
+      <c r="B82" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C82" s="40" t="s">
@@ -2926,8 +2920,8 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="52"/>
-      <c r="B83" s="55"/>
+      <c r="A83" s="68"/>
+      <c r="B83" s="65"/>
       <c r="C83" s="7" t="s">
         <v>124</v>
       </c>
@@ -2942,8 +2936,8 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A84" s="53"/>
-      <c r="B84" s="56"/>
+      <c r="A84" s="69"/>
+      <c r="B84" s="66"/>
       <c r="C84" s="10" t="s">
         <v>158</v>
       </c>
@@ -2958,10 +2952,10 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="51" t="s">
+      <c r="A85" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="B85" s="54" t="s">
+      <c r="B85" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -2978,8 +2972,8 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A86" s="52"/>
-      <c r="B86" s="55"/>
+      <c r="A86" s="68"/>
+      <c r="B86" s="65"/>
       <c r="C86" s="7" t="s">
         <v>211</v>
       </c>
@@ -2994,8 +2988,8 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="52"/>
-      <c r="B87" s="58"/>
+      <c r="A87" s="68"/>
+      <c r="B87" s="71"/>
       <c r="C87" s="7" t="s">
         <v>167</v>
       </c>
@@ -3010,7 +3004,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="53"/>
+      <c r="A88" s="69"/>
       <c r="B88" s="41" t="s">
         <v>15</v>
       </c>
@@ -3028,14 +3022,14 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="50" t="s">
+      <c r="A89" s="70" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="50"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="50"/>
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
+      <c r="D89" s="70"/>
+      <c r="E89" s="70"/>
+      <c r="F89" s="70"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -3070,6 +3064,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A55:A63"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A69:A71"/>
@@ -3086,31 +3105,6 @@
     <mergeCell ref="A43:A46"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed all of the unit tests
Not including newest post-processing though
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D558DD-0BFF-402F-B24C-722AD56B0D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610BAD0D-3A18-4BCC-85C0-FB461C3F48FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,7 +709,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,12 +734,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -1008,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1160,36 +1154,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1202,6 +1166,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1217,16 +1184,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1512,8 +1476,8 @@
   <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1548,20 +1512,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="54" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1579,35 +1543,35 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="62"/>
-      <c r="B4" s="65"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="7" t="s">
         <v>213</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="E4" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="53" t="s">
+      <c r="E4" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="29" t="s">
         <v>55</v>
       </c>
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="63"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="10" t="s">
         <v>214</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="E5" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="55" t="s">
+      <c r="E5" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="32" t="s">
         <v>55</v>
       </c>
       <c r="G5" s="50"/>
@@ -1625,18 +1589,18 @@
       <c r="D6" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="57" t="s">
+      <c r="E6" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1653,8 +1617,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="69"/>
-      <c r="B8" s="66"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1669,20 +1633,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1691,82 +1655,82 @@
       <c r="D10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="51" t="s">
+      <c r="E10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
-      <c r="B11" s="65"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="59" t="s">
+      <c r="E11" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="62"/>
-      <c r="B12" s="65"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="59" t="s">
+      <c r="E12" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="62"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="59" t="s">
+      <c r="E13" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="63"/>
-      <c r="B14" s="65"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="60" t="s">
+      <c r="E14" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="54" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1775,80 +1739,80 @@
       <c r="D15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="51" t="s">
+      <c r="E15" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="62"/>
-      <c r="B16" s="65"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="59" t="s">
+      <c r="E16" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="62"/>
-      <c r="B17" s="65"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="59" t="s">
+      <c r="E17" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
-      <c r="B18" s="65"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="59" t="s">
+      <c r="E18" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="62"/>
-      <c r="B19" s="71"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="59" t="s">
+      <c r="E19" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="62"/>
-      <c r="B20" s="65" t="s">
+      <c r="A20" s="52"/>
+      <c r="B20" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1857,66 +1821,66 @@
       <c r="D20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="59" t="s">
+      <c r="E20" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="62"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="59" t="s">
+      <c r="E21" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="62"/>
-      <c r="B22" s="65"/>
+      <c r="A22" s="52"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="59" t="s">
+      <c r="E22" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="62"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="52"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="59" t="s">
+      <c r="E23" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="54" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="35" t="s">
@@ -1925,32 +1889,32 @@
       <c r="D24" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="51" t="s">
+      <c r="E24" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="62"/>
-      <c r="B25" s="71"/>
+      <c r="A25" s="52"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="59" t="s">
+      <c r="E25" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="62"/>
-      <c r="B26" s="65" t="s">
+      <c r="A26" s="52"/>
+      <c r="B26" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1959,146 +1923,146 @@
       <c r="D26" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="59" t="s">
+      <c r="E26" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="62"/>
-      <c r="B27" s="65"/>
+      <c r="A27" s="52"/>
+      <c r="B27" s="56"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E27" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="59" t="s">
+      <c r="E27" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="62"/>
-      <c r="B28" s="65"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="56"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="59" t="s">
+      <c r="E28" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="62"/>
-      <c r="B29" s="65"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="56"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="59" t="s">
+      <c r="E29" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="62"/>
-      <c r="B30" s="65"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="E30" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="59" t="s">
+      <c r="E30" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="62"/>
-      <c r="B31" s="65"/>
+      <c r="A31" s="52"/>
+      <c r="B31" s="56"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E31" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="59" t="s">
+      <c r="E31" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="62"/>
-      <c r="B32" s="65"/>
+      <c r="A32" s="52"/>
+      <c r="B32" s="56"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E32" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="59" t="s">
+      <c r="E32" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="62"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="56"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E33" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="59" t="s">
+      <c r="E33" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="63"/>
-      <c r="B34" s="66"/>
+      <c r="A34" s="53"/>
+      <c r="B34" s="57"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="E34" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="60" t="s">
+      <c r="E34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="33" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="54" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2107,54 +2071,54 @@
       <c r="D35" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="59" t="s">
+      <c r="E35" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="68"/>
-      <c r="B36" s="65"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="56"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="59" t="s">
+      <c r="E36" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="69"/>
-      <c r="B37" s="66"/>
+      <c r="A37" s="60"/>
+      <c r="B37" s="57"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="59" t="s">
+      <c r="E37" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="70" t="s">
+      <c r="A38" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2169,18 +2133,18 @@
       <c r="D39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="56" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="57" t="s">
+      <c r="E39" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="64" t="s">
+      <c r="B40" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2189,50 +2153,50 @@
       <c r="D40" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="51" t="s">
+      <c r="E40" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="68"/>
-      <c r="B41" s="65"/>
+      <c r="A41" s="59"/>
+      <c r="B41" s="56"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="59" t="s">
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="69"/>
-      <c r="B42" s="66"/>
+      <c r="A42" s="60"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="59" t="s">
+      <c r="E42" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="61" t="s">
+      <c r="A43" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2241,58 +2205,58 @@
       <c r="D43" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="51" t="s">
+      <c r="E43" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="62"/>
-      <c r="B44" s="65"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="56"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="59" t="s">
+      <c r="E44" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="62"/>
-      <c r="B45" s="65"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="56"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="59" t="s">
+      <c r="E45" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="63"/>
-      <c r="B46" s="66"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E46" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="59" t="s">
+      <c r="E46" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="31" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2309,10 +2273,10 @@
       <c r="D47" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="51" t="s">
+      <c r="E47" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="30" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2329,10 +2293,10 @@
       <c r="D48" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E48" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="51" t="s">
+      <c r="E48" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="30" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2349,10 +2313,10 @@
       <c r="D49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="51" t="s">
+      <c r="E49" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="30" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2369,18 +2333,18 @@
       <c r="D50" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="51" t="s">
+      <c r="E50" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="30" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="67" t="s">
+      <c r="A51" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="64" t="s">
+      <c r="B51" s="54" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2397,8 +2361,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="68"/>
-      <c r="B52" s="71"/>
+      <c r="A52" s="59"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2413,7 +2377,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="68"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2431,20 +2395,20 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="70" t="s">
+      <c r="A54" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="73"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="73"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="62"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="61" t="s">
+      <c r="A55" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="64" t="s">
+      <c r="B55" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -2461,8 +2425,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="62"/>
-      <c r="B56" s="65"/>
+      <c r="A56" s="52"/>
+      <c r="B56" s="56"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
@@ -2477,8 +2441,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="62"/>
-      <c r="B57" s="65"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="56"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2493,8 +2457,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="62"/>
-      <c r="B58" s="65"/>
+      <c r="A58" s="52"/>
+      <c r="B58" s="56"/>
       <c r="C58" s="7" t="s">
         <v>186</v>
       </c>
@@ -2509,8 +2473,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="62"/>
-      <c r="B59" s="65"/>
+      <c r="A59" s="52"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2525,8 +2489,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="62"/>
-      <c r="B60" s="72" t="s">
+      <c r="A60" s="52"/>
+      <c r="B60" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C60" s="40" t="s">
@@ -2543,8 +2507,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="62"/>
-      <c r="B61" s="65"/>
+      <c r="A61" s="52"/>
+      <c r="B61" s="56"/>
       <c r="C61" s="7" t="s">
         <v>131</v>
       </c>
@@ -2559,8 +2523,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="62"/>
-      <c r="B62" s="65"/>
+      <c r="A62" s="52"/>
+      <c r="B62" s="56"/>
       <c r="C62" s="7" t="s">
         <v>132</v>
       </c>
@@ -2575,8 +2539,8 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="63"/>
-      <c r="B63" s="66"/>
+      <c r="A63" s="53"/>
+      <c r="B63" s="57"/>
       <c r="C63" s="7" t="s">
         <v>133</v>
       </c>
@@ -2591,10 +2555,10 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="67" t="s">
+      <c r="A64" s="58" t="s">
         <v>189</v>
       </c>
-      <c r="B64" s="64" t="s">
+      <c r="B64" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -2611,8 +2575,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="68"/>
-      <c r="B65" s="71"/>
+      <c r="A65" s="59"/>
+      <c r="B65" s="55"/>
       <c r="C65" s="7" t="s">
         <v>195</v>
       </c>
@@ -2627,8 +2591,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="68"/>
-      <c r="B66" s="72" t="s">
+      <c r="A66" s="59"/>
+      <c r="B66" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="40" t="s">
@@ -2645,8 +2609,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="68"/>
-      <c r="B67" s="65"/>
+      <c r="A67" s="59"/>
+      <c r="B67" s="56"/>
       <c r="C67" s="7" t="s">
         <v>197</v>
       </c>
@@ -2661,8 +2625,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="69"/>
-      <c r="B68" s="66"/>
+      <c r="A68" s="60"/>
+      <c r="B68" s="57"/>
       <c r="C68" s="7" t="s">
         <v>198</v>
       </c>
@@ -2677,10 +2641,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="67" t="s">
+      <c r="A69" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="B69" s="64" t="s">
+      <c r="B69" s="54" t="s">
         <v>190</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -2697,8 +2661,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="68"/>
-      <c r="B70" s="65"/>
+      <c r="A70" s="59"/>
+      <c r="B70" s="56"/>
       <c r="C70" s="7" t="s">
         <v>192</v>
       </c>
@@ -2713,8 +2677,8 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="69"/>
-      <c r="B71" s="66"/>
+      <c r="A71" s="60"/>
+      <c r="B71" s="57"/>
       <c r="C71" s="10" t="s">
         <v>193</v>
       </c>
@@ -2729,10 +2693,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="67" t="s">
+      <c r="A72" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B72" s="64" t="s">
+      <c r="B72" s="54" t="s">
         <v>138</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -2749,8 +2713,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="68"/>
-      <c r="B73" s="65"/>
+      <c r="A73" s="59"/>
+      <c r="B73" s="56"/>
       <c r="C73" s="7" t="s">
         <v>185</v>
       </c>
@@ -2765,8 +2729,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="69"/>
-      <c r="B74" s="66"/>
+      <c r="A74" s="60"/>
+      <c r="B74" s="57"/>
       <c r="C74" s="10" t="s">
         <v>139</v>
       </c>
@@ -2781,14 +2745,14 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="70" t="s">
+      <c r="A75" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="70"/>
-      <c r="C75" s="70"/>
-      <c r="D75" s="70"/>
-      <c r="E75" s="70"/>
-      <c r="F75" s="70"/>
+      <c r="B75" s="63"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="63"/>
+      <c r="E75" s="63"/>
+      <c r="F75" s="63"/>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
@@ -2831,10 +2795,10 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="67" t="s">
+      <c r="A78" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="64" t="s">
+      <c r="B78" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C78" s="7" t="s">
@@ -2851,8 +2815,8 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="68"/>
-      <c r="B79" s="65"/>
+      <c r="A79" s="59"/>
+      <c r="B79" s="56"/>
       <c r="C79" s="7" t="s">
         <v>155</v>
       </c>
@@ -2867,8 +2831,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="68"/>
-      <c r="B80" s="65"/>
+      <c r="A80" s="59"/>
+      <c r="B80" s="56"/>
       <c r="C80" s="7" t="s">
         <v>156</v>
       </c>
@@ -2883,8 +2847,8 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="68"/>
-      <c r="B81" s="71"/>
+      <c r="A81" s="59"/>
+      <c r="B81" s="55"/>
       <c r="C81" s="7" t="s">
         <v>157</v>
       </c>
@@ -2899,8 +2863,8 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="68"/>
-      <c r="B82" s="72" t="s">
+      <c r="A82" s="59"/>
+      <c r="B82" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C82" s="40" t="s">
@@ -2920,8 +2884,8 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="68"/>
-      <c r="B83" s="65"/>
+      <c r="A83" s="59"/>
+      <c r="B83" s="56"/>
       <c r="C83" s="7" t="s">
         <v>124</v>
       </c>
@@ -2936,8 +2900,8 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A84" s="69"/>
-      <c r="B84" s="66"/>
+      <c r="A84" s="60"/>
+      <c r="B84" s="57"/>
       <c r="C84" s="10" t="s">
         <v>158</v>
       </c>
@@ -2952,10 +2916,10 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="67" t="s">
+      <c r="A85" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="B85" s="64" t="s">
+      <c r="B85" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -2972,8 +2936,8 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A86" s="68"/>
-      <c r="B86" s="65"/>
+      <c r="A86" s="59"/>
+      <c r="B86" s="56"/>
       <c r="C86" s="7" t="s">
         <v>211</v>
       </c>
@@ -2988,8 +2952,8 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="68"/>
-      <c r="B87" s="71"/>
+      <c r="A87" s="59"/>
+      <c r="B87" s="55"/>
       <c r="C87" s="7" t="s">
         <v>167</v>
       </c>
@@ -3004,7 +2968,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="69"/>
+      <c r="A88" s="60"/>
       <c r="B88" s="41" t="s">
         <v>15</v>
       </c>
@@ -3022,14 +2986,14 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="70" t="s">
+      <c r="A89" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
-      <c r="D89" s="70"/>
-      <c r="E89" s="70"/>
-      <c r="F89" s="70"/>
+      <c r="B89" s="63"/>
+      <c r="C89" s="63"/>
+      <c r="D89" s="63"/>
+      <c r="E89" s="63"/>
+      <c r="F89" s="63"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -3064,12 +3028,17 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="B85:B87"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A40:A42"/>
@@ -3083,27 +3052,22 @@
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B64:B65"/>
     <mergeCell ref="A54:F54"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B43:B46"/>
     <mergeCell ref="B55:B59"/>
     <mergeCell ref="B60:B63"/>
     <mergeCell ref="A55:A63"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="B85:B87"/>
     <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A35:A37"/>
     <mergeCell ref="A51:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gradually adding variable combinations
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610BAD0D-3A18-4BCC-85C0-FB461C3F48FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FA334B-4F12-4803-BCD7-EB4176A3C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,7 +709,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,6 +734,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -1002,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1154,6 +1160,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1163,35 +1199,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1476,8 +1494,8 @@
   <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K84" sqref="K84"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1512,17 +1530,17 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="61" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="54" t="s">
@@ -1543,8 +1561,8 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="52"/>
-      <c r="B4" s="56"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="7" t="s">
         <v>213</v>
       </c>
@@ -1560,8 +1578,8 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="53"/>
-      <c r="B5" s="57"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="10" t="s">
         <v>214</v>
       </c>
@@ -1597,7 +1615,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="51" t="s">
         <v>59</v>
       </c>
       <c r="B7" s="54" t="s">
@@ -1617,8 +1635,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="60"/>
-      <c r="B8" s="57"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1633,17 +1651,17 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="61" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="54" t="s">
@@ -1663,8 +1681,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="56"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
@@ -1679,8 +1697,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="52"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="62"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1695,8 +1713,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="52"/>
-      <c r="B13" s="56"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
@@ -1711,8 +1729,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="53"/>
-      <c r="B14" s="56"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
@@ -1727,7 +1745,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="51" t="s">
+      <c r="A15" s="61" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="54" t="s">
@@ -1747,8 +1765,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="52"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1763,8 +1781,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="52"/>
-      <c r="B17" s="56"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
@@ -1779,8 +1797,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="52"/>
-      <c r="B18" s="56"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
@@ -1795,8 +1813,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="52"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1811,8 +1829,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="52"/>
-      <c r="B20" s="56" t="s">
+      <c r="A20" s="62"/>
+      <c r="B20" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1829,8 +1847,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="52"/>
-      <c r="B21" s="56"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
@@ -1845,8 +1863,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="52"/>
-      <c r="B22" s="56"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
@@ -1861,8 +1879,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="52"/>
-      <c r="B23" s="56"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="55"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
@@ -1877,7 +1895,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="51" t="s">
+      <c r="A24" s="61" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="54" t="s">
@@ -1897,8 +1915,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="52"/>
-      <c r="B25" s="55"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1913,8 +1931,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="52"/>
-      <c r="B26" s="56" t="s">
+      <c r="A26" s="62"/>
+      <c r="B26" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1931,8 +1949,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="52"/>
-      <c r="B27" s="56"/>
+      <c r="A27" s="62"/>
+      <c r="B27" s="55"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
@@ -1947,8 +1965,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="52"/>
-      <c r="B28" s="56"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
@@ -1963,8 +1981,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="52"/>
-      <c r="B29" s="56"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
@@ -1979,8 +1997,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="52"/>
-      <c r="B30" s="56"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
@@ -1995,8 +2013,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="52"/>
-      <c r="B31" s="56"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
@@ -2011,8 +2029,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="52"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="62"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
@@ -2027,8 +2045,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="52"/>
-      <c r="B33" s="56"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
@@ -2043,8 +2061,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="53"/>
-      <c r="B34" s="57"/>
+      <c r="A34" s="63"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
@@ -2059,7 +2077,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="51" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="54" t="s">
@@ -2079,8 +2097,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="59"/>
-      <c r="B36" s="56"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2095,8 +2113,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="60"/>
-      <c r="B37" s="57"/>
+      <c r="A37" s="53"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
@@ -2111,14 +2129,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2141,7 +2159,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="58" t="s">
+      <c r="A40" s="51" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="54" t="s">
@@ -2161,8 +2179,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="59"/>
-      <c r="B41" s="56"/>
+      <c r="A41" s="52"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
@@ -2177,8 +2195,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="60"/>
-      <c r="B42" s="57"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="56"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
@@ -2193,7 +2211,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="51" t="s">
+      <c r="A43" s="61" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="54" t="s">
@@ -2213,8 +2231,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="52"/>
-      <c r="B44" s="56"/>
+      <c r="A44" s="62"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
@@ -2229,8 +2247,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="52"/>
-      <c r="B45" s="56"/>
+      <c r="A45" s="62"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
@@ -2245,8 +2263,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="53"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="56"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
@@ -2341,7 +2359,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="58" t="s">
+      <c r="A51" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="54" t="s">
@@ -2361,8 +2379,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="59"/>
-      <c r="B52" s="55"/>
+      <c r="A52" s="52"/>
+      <c r="B52" s="58"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2377,7 +2395,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="59"/>
+      <c r="A53" s="52"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2395,17 +2413,17 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="63" t="s">
+      <c r="A54" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="62"/>
-      <c r="C54" s="63"/>
-      <c r="D54" s="62"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="63"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="57"/>
+      <c r="F54" s="57"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="51" t="s">
+      <c r="A55" s="61" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="54" t="s">
@@ -2417,16 +2435,16 @@
       <c r="D55" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="31" t="s">
+      <c r="E55" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="67" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="52"/>
-      <c r="B56" s="56"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="55"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
@@ -2441,8 +2459,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="52"/>
-      <c r="B57" s="56"/>
+      <c r="A57" s="62"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2457,8 +2475,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="52"/>
-      <c r="B58" s="56"/>
+      <c r="A58" s="62"/>
+      <c r="B58" s="55"/>
       <c r="C58" s="7" t="s">
         <v>186</v>
       </c>
@@ -2473,8 +2491,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="52"/>
-      <c r="B59" s="56"/>
+      <c r="A59" s="62"/>
+      <c r="B59" s="55"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2489,8 +2507,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="52"/>
-      <c r="B60" s="61" t="s">
+      <c r="A60" s="62"/>
+      <c r="B60" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C60" s="40" t="s">
@@ -2507,40 +2525,40 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="52"/>
-      <c r="B61" s="56"/>
+      <c r="A61" s="62"/>
+      <c r="B61" s="55"/>
       <c r="C61" s="7" t="s">
         <v>131</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E61" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="31" t="s">
+      <c r="E61" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="67" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="52"/>
-      <c r="B62" s="56"/>
+      <c r="A62" s="62"/>
+      <c r="B62" s="55"/>
       <c r="C62" s="7" t="s">
         <v>132</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E62" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="31" t="s">
+      <c r="E62" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="67" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="53"/>
-      <c r="B63" s="57"/>
+      <c r="A63" s="63"/>
+      <c r="B63" s="56"/>
       <c r="C63" s="7" t="s">
         <v>133</v>
       </c>
@@ -2555,7 +2573,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="58" t="s">
+      <c r="A64" s="51" t="s">
         <v>189</v>
       </c>
       <c r="B64" s="54" t="s">
@@ -2575,8 +2593,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="59"/>
-      <c r="B65" s="55"/>
+      <c r="A65" s="52"/>
+      <c r="B65" s="58"/>
       <c r="C65" s="7" t="s">
         <v>195</v>
       </c>
@@ -2591,8 +2609,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="59"/>
-      <c r="B66" s="61" t="s">
+      <c r="A66" s="52"/>
+      <c r="B66" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="40" t="s">
@@ -2609,8 +2627,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="59"/>
-      <c r="B67" s="56"/>
+      <c r="A67" s="52"/>
+      <c r="B67" s="55"/>
       <c r="C67" s="7" t="s">
         <v>197</v>
       </c>
@@ -2625,8 +2643,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="60"/>
-      <c r="B68" s="57"/>
+      <c r="A68" s="53"/>
+      <c r="B68" s="56"/>
       <c r="C68" s="7" t="s">
         <v>198</v>
       </c>
@@ -2641,7 +2659,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="58" t="s">
+      <c r="A69" s="51" t="s">
         <v>184</v>
       </c>
       <c r="B69" s="54" t="s">
@@ -2653,7 +2671,7 @@
       <c r="D69" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="E69" s="28" t="s">
+      <c r="E69" s="64" t="s">
         <v>9</v>
       </c>
       <c r="F69" s="28" t="s">
@@ -2661,15 +2679,15 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="59"/>
-      <c r="B70" s="56"/>
+      <c r="A70" s="52"/>
+      <c r="B70" s="55"/>
       <c r="C70" s="7" t="s">
         <v>192</v>
       </c>
       <c r="D70" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="E70" s="29" t="s">
+      <c r="E70" s="65" t="s">
         <v>9</v>
       </c>
       <c r="F70" s="29" t="s">
@@ -2677,15 +2695,15 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="60"/>
-      <c r="B71" s="57"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="56"/>
       <c r="C71" s="10" t="s">
         <v>193</v>
       </c>
       <c r="D71" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="E71" s="32" t="s">
+      <c r="E71" s="66" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="32" t="s">
@@ -2693,7 +2711,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="58" t="s">
+      <c r="A72" s="51" t="s">
         <v>106</v>
       </c>
       <c r="B72" s="54" t="s">
@@ -2713,8 +2731,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="59"/>
-      <c r="B73" s="56"/>
+      <c r="A73" s="52"/>
+      <c r="B73" s="55"/>
       <c r="C73" s="7" t="s">
         <v>185</v>
       </c>
@@ -2729,8 +2747,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="60"/>
-      <c r="B74" s="57"/>
+      <c r="A74" s="53"/>
+      <c r="B74" s="56"/>
       <c r="C74" s="10" t="s">
         <v>139</v>
       </c>
@@ -2745,14 +2763,14 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="63" t="s">
+      <c r="A75" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="63"/>
-      <c r="C75" s="63"/>
-      <c r="D75" s="63"/>
-      <c r="E75" s="63"/>
-      <c r="F75" s="63"/>
+      <c r="B75" s="57"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="57"/>
+      <c r="F75" s="57"/>
     </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="13" t="s">
@@ -2795,7 +2813,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="58" t="s">
+      <c r="A78" s="51" t="s">
         <v>153</v>
       </c>
       <c r="B78" s="54" t="s">
@@ -2815,8 +2833,8 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="59"/>
-      <c r="B79" s="56"/>
+      <c r="A79" s="52"/>
+      <c r="B79" s="55"/>
       <c r="C79" s="7" t="s">
         <v>155</v>
       </c>
@@ -2831,8 +2849,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="59"/>
-      <c r="B80" s="56"/>
+      <c r="A80" s="52"/>
+      <c r="B80" s="55"/>
       <c r="C80" s="7" t="s">
         <v>156</v>
       </c>
@@ -2847,8 +2865,8 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="59"/>
-      <c r="B81" s="55"/>
+      <c r="A81" s="52"/>
+      <c r="B81" s="58"/>
       <c r="C81" s="7" t="s">
         <v>157</v>
       </c>
@@ -2863,8 +2881,8 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="59"/>
-      <c r="B82" s="61" t="s">
+      <c r="A82" s="52"/>
+      <c r="B82" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C82" s="40" t="s">
@@ -2884,8 +2902,8 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="59"/>
-      <c r="B83" s="56"/>
+      <c r="A83" s="52"/>
+      <c r="B83" s="55"/>
       <c r="C83" s="7" t="s">
         <v>124</v>
       </c>
@@ -2900,8 +2918,8 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A84" s="60"/>
-      <c r="B84" s="57"/>
+      <c r="A84" s="53"/>
+      <c r="B84" s="56"/>
       <c r="C84" s="10" t="s">
         <v>158</v>
       </c>
@@ -2916,7 +2934,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="58" t="s">
+      <c r="A85" s="51" t="s">
         <v>159</v>
       </c>
       <c r="B85" s="54" t="s">
@@ -2936,8 +2954,8 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A86" s="59"/>
-      <c r="B86" s="56"/>
+      <c r="A86" s="52"/>
+      <c r="B86" s="55"/>
       <c r="C86" s="7" t="s">
         <v>211</v>
       </c>
@@ -2952,8 +2970,8 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="59"/>
-      <c r="B87" s="55"/>
+      <c r="A87" s="52"/>
+      <c r="B87" s="58"/>
       <c r="C87" s="7" t="s">
         <v>167</v>
       </c>
@@ -2968,7 +2986,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="60"/>
+      <c r="A88" s="53"/>
       <c r="B88" s="41" t="s">
         <v>15</v>
       </c>
@@ -2986,14 +3004,14 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="63" t="s">
+      <c r="A89" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="63"/>
-      <c r="C89" s="63"/>
-      <c r="D89" s="63"/>
-      <c r="E89" s="63"/>
-      <c r="F89" s="63"/>
+      <c r="B89" s="57"/>
+      <c r="C89" s="57"/>
+      <c r="D89" s="57"/>
+      <c r="E89" s="57"/>
+      <c r="F89" s="57"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="15" t="s">
@@ -3028,17 +3046,20 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="A55:A63"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A40:A42"/>
@@ -3055,20 +3076,17 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A78:A84"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="B85:B87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Gathered more results and editting code
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FA334B-4F12-4803-BCD7-EB4176A3C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043E4A22-466F-46F8-B841-A648109A6953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="219">
   <si>
     <t>Class</t>
   </si>
@@ -687,6 +687,12 @@
   </si>
   <si>
     <t>Creates an expression that denormalizes an input variable.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1160,6 +1166,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1169,47 +1211,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1491,11 +1500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M62" sqref="M62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1530,20 +1539,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="59" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1561,8 +1570,8 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="62"/>
-      <c r="B4" s="55"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="7" t="s">
         <v>213</v>
       </c>
@@ -1578,8 +1587,8 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="63"/>
-      <c r="B5" s="56"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="10" t="s">
         <v>214</v>
       </c>
@@ -1615,10 +1624,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1635,8 +1644,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="53"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1651,20 +1660,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1681,8 +1690,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="62"/>
-      <c r="B11" s="55"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
@@ -1697,8 +1706,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="62"/>
-      <c r="B12" s="55"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1713,8 +1722,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="62"/>
-      <c r="B13" s="55"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
@@ -1729,8 +1738,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="63"/>
-      <c r="B14" s="55"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
@@ -1745,10 +1754,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="59" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1765,8 +1774,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="62"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1781,8 +1790,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="62"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
@@ -1797,8 +1806,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="62"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
@@ -1813,8 +1822,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="62"/>
-      <c r="B19" s="58"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1829,8 +1838,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="62"/>
-      <c r="B20" s="55" t="s">
+      <c r="A20" s="57"/>
+      <c r="B20" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1847,8 +1856,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="62"/>
-      <c r="B21" s="55"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
@@ -1863,8 +1872,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="62"/>
-      <c r="B22" s="55"/>
+      <c r="A22" s="57"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
@@ -1879,8 +1888,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="62"/>
-      <c r="B23" s="55"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
@@ -1895,10 +1904,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="59" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="35" t="s">
@@ -1915,8 +1924,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="62"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1931,8 +1940,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="62"/>
-      <c r="B26" s="55" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1949,8 +1958,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="62"/>
-      <c r="B27" s="55"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
@@ -1965,8 +1974,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="62"/>
-      <c r="B28" s="55"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
@@ -1981,8 +1990,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="62"/>
-      <c r="B29" s="55"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
@@ -1997,8 +2006,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="62"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
@@ -2013,8 +2022,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="62"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
@@ -2029,8 +2038,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="62"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
@@ -2045,8 +2054,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="62"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="57"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
@@ -2061,8 +2070,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="63"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="62"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
@@ -2077,10 +2086,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="51" t="s">
+      <c r="A35" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="59" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2097,8 +2106,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="52"/>
-      <c r="B36" s="55"/>
+      <c r="A36" s="64"/>
+      <c r="B36" s="61"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2113,8 +2122,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="53"/>
-      <c r="B37" s="56"/>
+      <c r="A37" s="65"/>
+      <c r="B37" s="62"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
@@ -2129,14 +2138,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2159,10 +2168,10 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2179,8 +2188,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="52"/>
-      <c r="B41" s="55"/>
+      <c r="A41" s="64"/>
+      <c r="B41" s="61"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
@@ -2195,8 +2204,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="53"/>
-      <c r="B42" s="56"/>
+      <c r="A42" s="65"/>
+      <c r="B42" s="62"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
@@ -2211,10 +2220,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="61" t="s">
+      <c r="A43" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2231,8 +2240,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="62"/>
-      <c r="B44" s="55"/>
+      <c r="A44" s="57"/>
+      <c r="B44" s="61"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
@@ -2247,8 +2256,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="62"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="57"/>
+      <c r="B45" s="61"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
@@ -2263,8 +2272,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="63"/>
-      <c r="B46" s="56"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="62"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
@@ -2359,10 +2368,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="59" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2379,8 +2388,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="52"/>
-      <c r="B52" s="58"/>
+      <c r="A52" s="64"/>
+      <c r="B52" s="60"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2395,7 +2404,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="52"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2413,20 +2422,20 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="57" t="s">
+      <c r="A54" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="60"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="57"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="67"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="61" t="s">
+      <c r="A55" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="54" t="s">
+      <c r="B55" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -2435,16 +2444,16 @@
       <c r="D55" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="67" t="s">
+      <c r="E55" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="54" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="62"/>
-      <c r="B56" s="55"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="61"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
@@ -2459,8 +2468,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="62"/>
-      <c r="B57" s="55"/>
+      <c r="A57" s="57"/>
+      <c r="B57" s="61"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2475,8 +2484,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="62"/>
-      <c r="B58" s="55"/>
+      <c r="A58" s="57"/>
+      <c r="B58" s="61"/>
       <c r="C58" s="7" t="s">
         <v>186</v>
       </c>
@@ -2490,320 +2499,311 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="62"/>
-      <c r="B59" s="55"/>
+    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="57"/>
+      <c r="B59" s="61"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E59" s="49" t="s">
+      <c r="E59" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F59" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="62"/>
-      <c r="B60" s="59" t="s">
+    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="57"/>
+      <c r="B60" s="61"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="55" t="s">
+        <v>217</v>
+      </c>
+      <c r="F60" s="54" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="57"/>
+      <c r="B61" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="40" t="s">
+      <c r="C61" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="D60" s="37" t="s">
+      <c r="D61" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="E60" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="62"/>
-      <c r="B61" s="55"/>
-      <c r="C61" s="7" t="s">
+      <c r="E61" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="57"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D62" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E61" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="67" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="62"/>
-      <c r="B62" s="55"/>
-      <c r="C62" s="7" t="s">
+      <c r="E62" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A63" s="57"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D63" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E62" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="67" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="63"/>
-      <c r="B63" s="56"/>
-      <c r="C63" s="7" t="s">
+      <c r="E63" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="58"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D64" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E63" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="31" t="s">
+      <c r="E64" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="51" t="s">
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="63" t="s">
         <v>189</v>
       </c>
-      <c r="B64" s="54" t="s">
+      <c r="B65" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D64" s="46" t="s">
+      <c r="D65" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="E64" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="28" t="s">
+      <c r="E65" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="52"/>
-      <c r="B65" s="58"/>
-      <c r="C65" s="7" t="s">
+    <row r="66" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="64"/>
+      <c r="B66" s="60"/>
+      <c r="C66" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D65" s="44" t="s">
+      <c r="D66" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="E65" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="52"/>
-      <c r="B66" s="59" t="s">
+      <c r="E66" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="64"/>
+      <c r="B67" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="40" t="s">
+      <c r="C67" s="40" t="s">
         <v>196</v>
       </c>
-      <c r="D66" s="48" t="s">
+      <c r="D67" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="E66" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="52"/>
-      <c r="B67" s="55"/>
-      <c r="C67" s="7" t="s">
+      <c r="E67" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="64"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D67" s="44" t="s">
+      <c r="D68" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="E67" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="53"/>
-      <c r="B68" s="56"/>
-      <c r="C68" s="7" t="s">
+      <c r="E68" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="65"/>
+      <c r="B69" s="62"/>
+      <c r="C69" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D68" s="44" t="s">
+      <c r="D69" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="E68" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="51" t="s">
+      <c r="E69" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B70" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D69" s="46" t="s">
+      <c r="D70" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="E69" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="28" t="s">
+      <c r="E70" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="52"/>
-      <c r="B70" s="55"/>
-      <c r="C70" s="7" t="s">
+    <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="64"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D70" s="44" t="s">
+      <c r="D71" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="E70" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="29" t="s">
+      <c r="E71" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="53"/>
-      <c r="B71" s="56"/>
-      <c r="C71" s="10" t="s">
+    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="65"/>
+      <c r="B72" s="62"/>
+      <c r="C72" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="D71" s="47" t="s">
+      <c r="D72" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="E71" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="32" t="s">
+      <c r="E72" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="51" t="s">
+    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="B72" s="54" t="s">
+      <c r="B73" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D73" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E72" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="52"/>
-      <c r="B73" s="55"/>
-      <c r="C73" s="7" t="s">
+      <c r="E73" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="64"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D74" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E73" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="53"/>
-      <c r="B74" s="56"/>
-      <c r="C74" s="10" t="s">
+      <c r="E74" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="65"/>
+      <c r="B75" s="62"/>
+      <c r="C75" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D74" s="23" t="s">
+      <c r="D75" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E74" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="57" t="s">
+      <c r="E75" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="57"/>
-      <c r="C75" s="57"/>
-      <c r="D75" s="57"/>
-      <c r="E75" s="57"/>
-      <c r="F75" s="57"/>
-    </row>
-    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="13" t="s">
+      <c r="B76" s="67"/>
+      <c r="C76" s="67"/>
+      <c r="D76" s="67"/>
+      <c r="E76" s="67"/>
+      <c r="F76" s="67"/>
+    </row>
+    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="E76" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="13" t="s">
-        <v>151</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>9</v>
@@ -2812,171 +2812,175 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="51" t="s">
+    <row r="78" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E78" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="54" t="s">
+      <c r="B79" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D78" s="9" t="s">
+      <c r="D79" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E78" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" s="31" t="s">
+      <c r="E79" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="52"/>
-      <c r="B79" s="55"/>
-      <c r="C79" s="7" t="s">
+    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A80" s="64"/>
+      <c r="B80" s="61"/>
+      <c r="C80" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D80" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="E79" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="52"/>
-      <c r="B80" s="55"/>
-      <c r="C80" s="7" t="s">
+      <c r="E80" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="64"/>
+      <c r="B81" s="61"/>
+      <c r="C81" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D81" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E80" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="52"/>
-      <c r="B81" s="58"/>
-      <c r="C81" s="7" t="s">
+      <c r="E81" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="64"/>
+      <c r="B82" s="60"/>
+      <c r="C82" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D82" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E81" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="52"/>
-      <c r="B82" s="59" t="s">
+      <c r="E82" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="64"/>
+      <c r="B83" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C82" s="40" t="s">
+      <c r="C83" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="D82" s="37" t="s">
+      <c r="D83" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="E82" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J82" s="7" t="s">
+      <c r="E83" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J83" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="52"/>
-      <c r="B83" s="55"/>
-      <c r="C83" s="7" t="s">
+    <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="64"/>
+      <c r="B84" s="61"/>
+      <c r="C84" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D83" s="9" t="s">
+      <c r="D84" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E83" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A84" s="53"/>
-      <c r="B84" s="56"/>
-      <c r="C84" s="10" t="s">
+      <c r="E84" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A85" s="65"/>
+      <c r="B85" s="62"/>
+      <c r="C85" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D84" s="23" t="s">
+      <c r="D85" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="E84" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="51" t="s">
+      <c r="E85" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="B85" s="54" t="s">
+      <c r="B86" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D86" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E85" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="30" t="s">
+      <c r="E86" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A86" s="52"/>
-      <c r="B86" s="55"/>
-      <c r="C86" s="7" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A87" s="64"/>
+      <c r="B87" s="61"/>
+      <c r="C87" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="D86" s="9" t="s">
+      <c r="D87" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="E86" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="52"/>
-      <c r="B87" s="58"/>
-      <c r="C87" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="E87" s="29" t="s">
         <v>9</v>
@@ -2985,81 +2989,94 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="53"/>
-      <c r="B88" s="41" t="s">
+    <row r="88" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="64"/>
+      <c r="B88" s="60"/>
+      <c r="C88" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A89" s="65"/>
+      <c r="B89" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="42" t="s">
+      <c r="C89" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="D88" s="43" t="s">
+      <c r="D89" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="E88" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F88" s="33" t="s">
+      <c r="E89" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="57" t="s">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" s="67" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="57"/>
-      <c r="C89" s="57"/>
-      <c r="D89" s="57"/>
-      <c r="E89" s="57"/>
-      <c r="F89" s="57"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="15" t="s">
+      <c r="B90" s="67"/>
+      <c r="C90" s="67"/>
+      <c r="D90" s="67"/>
+      <c r="E90" s="67"/>
+      <c r="F90" s="67"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B90" s="7" t="s">
+      <c r="B91" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C91" s="7" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C91" s="7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C92" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C93" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C94" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C95" s="7" t="s">
         <v>179</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="A55:A63"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="B86:B88"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A40:A42"/>
@@ -3076,17 +3093,20 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A78:A84"/>
-    <mergeCell ref="B78:B81"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A51:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Still working on subspaces
Midday 8/26
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043E4A22-466F-46F8-B841-A648109A6953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B392D22B-3976-4032-BA22-09B135D6FCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="220">
   <si>
     <t>Class</t>
   </si>
@@ -467,9 +467,6 @@
     <t>Calculates the complementary probability of feasibility from a predicted point's pass-fail value.</t>
   </si>
   <si>
-    <t>Determines the amount of space that would remaing in each discipline if they were to move forward with the new rule combo(s) being considered for the current time stamp and calculates the entire design spaces' added potentials for regret and windfall.</t>
-  </si>
-  <si>
     <t>Visualizes the windfall and regret potentials of remaining design points for each design space of each discipline specifically for the SBD1 problem.</t>
   </si>
   <si>
@@ -693,6 +690,12 @@
   </si>
   <si>
     <t>Incomplete</t>
+  </si>
+  <si>
+    <t>averageWR</t>
+  </si>
+  <si>
+    <t>Determines the amount of space that would remain in each discipline if they were to move forward with the new rule combo(s) being considered for the current time stamp and calculates the entire design spaces' added potentials for regret and windfall.</t>
   </si>
 </sst>
 </file>
@@ -1181,6 +1184,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1189,36 +1222,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1503,8 +1506,8 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1535,21 +1538,21 @@
         <v>3</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="59" t="s">
@@ -1570,13 +1573,13 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="57"/>
-      <c r="B4" s="61"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" s="49" t="s">
         <v>9</v>
@@ -1587,13 +1590,13 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="58"/>
-      <c r="B5" s="62"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>9</v>
@@ -1624,7 +1627,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="56" t="s">
         <v>59</v>
       </c>
       <c r="B7" s="59" t="s">
@@ -1644,8 +1647,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="65"/>
-      <c r="B8" s="62"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1660,17 +1663,17 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="66" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="59" t="s">
@@ -1690,8 +1693,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="57"/>
-      <c r="B11" s="61"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
@@ -1706,8 +1709,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="57"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1722,8 +1725,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="57"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
@@ -1738,8 +1741,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="58"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
@@ -1754,7 +1757,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="66" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="59" t="s">
@@ -1774,8 +1777,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="57"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1790,8 +1793,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="57"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
@@ -1806,8 +1809,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="57"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
@@ -1822,8 +1825,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="57"/>
-      <c r="B19" s="60"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1838,8 +1841,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="57"/>
-      <c r="B20" s="61" t="s">
+      <c r="A20" s="67"/>
+      <c r="B20" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1856,8 +1859,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="57"/>
-      <c r="B21" s="61"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
@@ -1872,8 +1875,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="57"/>
-      <c r="B22" s="61"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
@@ -1888,8 +1891,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="57"/>
-      <c r="B23" s="61"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
@@ -1904,7 +1907,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="66" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="59" t="s">
@@ -1924,8 +1927,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="57"/>
-      <c r="B25" s="60"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1940,8 +1943,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="57"/>
-      <c r="B26" s="61" t="s">
+      <c r="A26" s="67"/>
+      <c r="B26" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1958,8 +1961,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="57"/>
-      <c r="B27" s="61"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="60"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
@@ -1974,8 +1977,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="57"/>
-      <c r="B28" s="61"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
@@ -1990,8 +1993,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="57"/>
-      <c r="B29" s="61"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="60"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
@@ -2006,8 +2009,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="57"/>
-      <c r="B30" s="61"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
@@ -2022,8 +2025,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="57"/>
-      <c r="B31" s="61"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="60"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
@@ -2038,8 +2041,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="57"/>
-      <c r="B32" s="61"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
@@ -2054,8 +2057,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="57"/>
-      <c r="B33" s="61"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
@@ -2070,8 +2073,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="58"/>
-      <c r="B34" s="62"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
@@ -2086,7 +2089,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="56" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="59" t="s">
@@ -2106,8 +2109,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="64"/>
-      <c r="B36" s="61"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2122,8 +2125,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="65"/>
-      <c r="B37" s="62"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="61"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
@@ -2138,14 +2141,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
-      <c r="F38" s="67"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2168,7 +2171,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="63" t="s">
+      <c r="A40" s="56" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="59" t="s">
@@ -2188,8 +2191,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="64"/>
-      <c r="B41" s="61"/>
+      <c r="A41" s="57"/>
+      <c r="B41" s="60"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
@@ -2204,8 +2207,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="65"/>
-      <c r="B42" s="62"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="61"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
@@ -2220,7 +2223,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="66" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="59" t="s">
@@ -2240,8 +2243,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="57"/>
-      <c r="B44" s="61"/>
+      <c r="A44" s="67"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
@@ -2256,8 +2259,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="57"/>
-      <c r="B45" s="61"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="60"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
@@ -2272,8 +2275,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="62"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="61"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
@@ -2368,7 +2371,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="63" t="s">
+      <c r="A51" s="56" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="59" t="s">
@@ -2388,8 +2391,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="64"/>
-      <c r="B52" s="60"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="63"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2404,7 +2407,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="64"/>
+      <c r="A53" s="57"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2422,17 +2425,17 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="67" t="s">
+      <c r="A54" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="68"/>
-      <c r="C54" s="67"/>
-      <c r="D54" s="68"/>
-      <c r="E54" s="67"/>
-      <c r="F54" s="67"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="62"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="66" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="59" t="s">
@@ -2452,13 +2455,13 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="57"/>
-      <c r="B56" s="61"/>
+      <c r="A56" s="67"/>
+      <c r="B56" s="60"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E56" s="29" t="s">
         <v>9</v>
@@ -2468,8 +2471,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="57"/>
-      <c r="B57" s="61"/>
+      <c r="A57" s="67"/>
+      <c r="B57" s="60"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2484,14 +2487,14 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="57"/>
-      <c r="B58" s="61"/>
+      <c r="A58" s="67"/>
+      <c r="B58" s="60"/>
       <c r="C58" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>187</v>
-      </c>
       <c r="E58" s="29" t="s">
         <v>9</v>
       </c>
@@ -2500,42 +2503,45 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="57"/>
-      <c r="B59" s="61"/>
+      <c r="A59" s="67"/>
+      <c r="B59" s="60"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="E59" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="E59" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="54" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="57"/>
-      <c r="B60" s="61"/>
+      <c r="A60" s="67"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="7" t="s">
+        <v>218</v>
+      </c>
       <c r="D60" s="9"/>
       <c r="E60" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="F60" s="54" t="s">
         <v>217</v>
       </c>
-      <c r="F60" s="54" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="57"/>
-      <c r="B61" s="66" t="s">
+      <c r="A61" s="67"/>
+      <c r="B61" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C61" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E61" s="29" t="s">
         <v>9</v>
@@ -2545,8 +2551,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="57"/>
-      <c r="B62" s="61"/>
+      <c r="A62" s="67"/>
+      <c r="B62" s="60"/>
       <c r="C62" s="7" t="s">
         <v>131</v>
       </c>
@@ -2561,13 +2567,13 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A63" s="57"/>
-      <c r="B63" s="61"/>
+      <c r="A63" s="67"/>
+      <c r="B63" s="60"/>
       <c r="C63" s="7" t="s">
         <v>132</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>143</v>
+        <v>219</v>
       </c>
       <c r="E63" s="52" t="s">
         <v>9</v>
@@ -2577,13 +2583,13 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="58"/>
-      <c r="B64" s="62"/>
+      <c r="A64" s="68"/>
+      <c r="B64" s="61"/>
       <c r="C64" s="7" t="s">
         <v>133</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E64" s="29" t="s">
         <v>9</v>
@@ -2593,17 +2599,17 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="63" t="s">
-        <v>189</v>
+      <c r="A65" s="56" t="s">
+        <v>188</v>
       </c>
       <c r="B65" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D65" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E65" s="28" t="s">
         <v>9</v>
@@ -2613,83 +2619,83 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="64"/>
-      <c r="B66" s="60"/>
+      <c r="A66" s="57"/>
+      <c r="B66" s="63"/>
       <c r="C66" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="57"/>
+      <c r="B67" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="40" t="s">
         <v>195</v>
       </c>
-      <c r="D66" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="E66" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="64"/>
-      <c r="B67" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" s="40" t="s">
+      <c r="D67" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="57"/>
+      <c r="B68" s="60"/>
+      <c r="C68" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D67" s="48" t="s">
+      <c r="D68" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="E68" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="58"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D69" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="E67" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="64"/>
-      <c r="B68" s="61"/>
-      <c r="C68" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D68" s="44" t="s">
-        <v>202</v>
-      </c>
-      <c r="E68" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="65"/>
-      <c r="B69" s="62"/>
-      <c r="C69" s="7" t="s">
+      <c r="E69" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="B70" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D70" s="46" t="s">
         <v>198</v>
-      </c>
-      <c r="D69" s="44" t="s">
-        <v>204</v>
-      </c>
-      <c r="E69" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="B70" s="59" t="s">
-        <v>190</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D70" s="46" t="s">
-        <v>199</v>
       </c>
       <c r="E70" s="51" t="s">
         <v>9</v>
@@ -2699,13 +2705,13 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="64"/>
-      <c r="B71" s="61"/>
+      <c r="A71" s="57"/>
+      <c r="B71" s="60"/>
       <c r="C71" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D71" s="44" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E71" s="52" t="s">
         <v>9</v>
@@ -2715,13 +2721,13 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="65"/>
-      <c r="B72" s="62"/>
+      <c r="A72" s="58"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D72" s="47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E72" s="53" t="s">
         <v>9</v>
@@ -2731,7 +2737,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="63" t="s">
+      <c r="A73" s="56" t="s">
         <v>106</v>
       </c>
       <c r="B73" s="59" t="s">
@@ -2741,7 +2747,7 @@
         <v>44</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E73" s="45" t="s">
         <v>9</v>
@@ -2751,13 +2757,13 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="64"/>
-      <c r="B74" s="61"/>
+      <c r="A74" s="57"/>
+      <c r="B74" s="60"/>
       <c r="C74" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E74" s="29" t="s">
         <v>9</v>
@@ -2767,43 +2773,43 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="65"/>
-      <c r="B75" s="62"/>
+      <c r="A75" s="58"/>
+      <c r="B75" s="61"/>
       <c r="C75" s="10" t="s">
         <v>139</v>
       </c>
       <c r="D75" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="E75" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="67" t="s">
-        <v>147</v>
-      </c>
-      <c r="B76" s="67"/>
-      <c r="C76" s="67"/>
-      <c r="D76" s="67"/>
-      <c r="E76" s="67"/>
-      <c r="F76" s="67"/>
+      <c r="B76" s="62"/>
+      <c r="C76" s="62"/>
+      <c r="D76" s="62"/>
+      <c r="E76" s="62"/>
+      <c r="F76" s="62"/>
     </row>
     <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C77" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>149</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>150</v>
       </c>
       <c r="E77" s="26" t="s">
         <v>9</v>
@@ -2814,7 +2820,7 @@
     </row>
     <row r="78" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>15</v>
@@ -2823,7 +2829,7 @@
         <v>15</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E78" s="26" t="s">
         <v>9</v>
@@ -2833,17 +2839,17 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="63" t="s">
-        <v>153</v>
+      <c r="A79" s="56" t="s">
+        <v>152</v>
       </c>
       <c r="B79" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E79" s="29" t="s">
         <v>9</v>
@@ -2853,46 +2859,46 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="64"/>
-      <c r="B80" s="61"/>
+      <c r="A80" s="57"/>
+      <c r="B80" s="60"/>
       <c r="C80" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E80" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="57"/>
+      <c r="B81" s="60"/>
+      <c r="C81" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E80" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="64"/>
-      <c r="B81" s="61"/>
-      <c r="C81" s="7" t="s">
+      <c r="D81" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E81" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="57"/>
+      <c r="B82" s="63"/>
+      <c r="C82" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D82" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E81" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="64"/>
-      <c r="B82" s="60"/>
-      <c r="C82" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>165</v>
-      </c>
       <c r="E82" s="29" t="s">
         <v>9</v>
       </c>
@@ -2901,34 +2907,34 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="64"/>
-      <c r="B83" s="66" t="s">
+      <c r="A83" s="57"/>
+      <c r="B83" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C83" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="E83" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J83" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D83" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="E83" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J83" s="7" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84" s="64"/>
-      <c r="B84" s="61"/>
+      <c r="A84" s="57"/>
+      <c r="B84" s="60"/>
       <c r="C84" s="7" t="s">
         <v>124</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E84" s="29" t="s">
         <v>9</v>
@@ -2938,33 +2944,33 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A85" s="65"/>
-      <c r="B85" s="62"/>
+      <c r="A85" s="58"/>
+      <c r="B85" s="61"/>
       <c r="C85" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D85" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E85" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="56" t="s">
         <v>158</v>
-      </c>
-      <c r="D85" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E85" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="63" t="s">
-        <v>159</v>
       </c>
       <c r="B86" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E86" s="28" t="s">
         <v>9</v>
@@ -2974,13 +2980,13 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A87" s="64"/>
-      <c r="B87" s="61"/>
+      <c r="A87" s="57"/>
+      <c r="B87" s="60"/>
       <c r="C87" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D87" s="9" t="s">
         <v>211</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>212</v>
       </c>
       <c r="E87" s="29" t="s">
         <v>9</v>
@@ -2990,13 +2996,13 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="64"/>
-      <c r="B88" s="60"/>
+      <c r="A88" s="57"/>
+      <c r="B88" s="63"/>
       <c r="C88" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E88" s="29" t="s">
         <v>9</v>
@@ -3006,15 +3012,15 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="65"/>
+      <c r="A89" s="58"/>
       <c r="B89" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C89" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D89" s="43" t="s">
         <v>168</v>
-      </c>
-      <c r="D89" s="43" t="s">
-        <v>169</v>
       </c>
       <c r="E89" s="32" t="s">
         <v>9</v>
@@ -3024,59 +3030,62 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="67" t="s">
-        <v>172</v>
-      </c>
-      <c r="B90" s="67"/>
-      <c r="C90" s="67"/>
-      <c r="D90" s="67"/>
-      <c r="E90" s="67"/>
-      <c r="F90" s="67"/>
+      <c r="A90" s="62" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90" s="62"/>
+      <c r="C90" s="62"/>
+      <c r="D90" s="62"/>
+      <c r="E90" s="62"/>
+      <c r="F90" s="62"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="C91" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C92" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C93" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C94" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C95" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A40:A42"/>
@@ -3093,20 +3102,17 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="A55:A64"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="A76:F76"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="B86:B88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working through subspaces still
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B392D22B-3976-4032-BA22-09B135D6FCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C04B55A-204A-437F-B530-10BECB7A7325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="221">
   <si>
     <t>Class</t>
   </si>
@@ -696,6 +696,9 @@
   </si>
   <si>
     <t>Determines the amount of space that would remain in each discipline if they were to move forward with the new rule combo(s) being considered for the current time stamp and calculates the entire design spaces' added potentials for regret and windfall.</t>
+  </si>
+  <si>
+    <t>subspaceConsolidate</t>
   </si>
 </sst>
 </file>
@@ -1184,6 +1187,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1193,35 +1217,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1503,11 +1506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1542,17 +1545,17 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="56" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="59" t="s">
@@ -1573,8 +1576,8 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="67"/>
-      <c r="B4" s="60"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="7" t="s">
         <v>212</v>
       </c>
@@ -1590,8 +1593,8 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="61"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="10" t="s">
         <v>213</v>
       </c>
@@ -1627,7 +1630,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="63" t="s">
         <v>59</v>
       </c>
       <c r="B7" s="59" t="s">
@@ -1647,8 +1650,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="58"/>
-      <c r="B8" s="61"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1663,17 +1666,17 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="56" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="59" t="s">
@@ -1693,8 +1696,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="67"/>
-      <c r="B11" s="60"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
@@ -1709,8 +1712,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="67"/>
-      <c r="B12" s="60"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1725,8 +1728,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="67"/>
-      <c r="B13" s="60"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
@@ -1741,8 +1744,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="68"/>
-      <c r="B14" s="60"/>
+      <c r="A14" s="58"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
@@ -1757,7 +1760,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="56" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="59" t="s">
@@ -1777,8 +1780,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="67"/>
-      <c r="B16" s="60"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1793,8 +1796,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="67"/>
-      <c r="B17" s="60"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
@@ -1809,8 +1812,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="67"/>
-      <c r="B18" s="60"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
@@ -1825,8 +1828,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="67"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1841,8 +1844,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="67"/>
-      <c r="B20" s="60" t="s">
+      <c r="A20" s="57"/>
+      <c r="B20" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1859,8 +1862,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="67"/>
-      <c r="B21" s="60"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
@@ -1875,8 +1878,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="67"/>
-      <c r="B22" s="60"/>
+      <c r="A22" s="57"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
@@ -1891,8 +1894,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="67"/>
-      <c r="B23" s="60"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
@@ -1907,7 +1910,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="56" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="59" t="s">
@@ -1927,8 +1930,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="67"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1943,8 +1946,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="67"/>
-      <c r="B26" s="60" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1961,8 +1964,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="67"/>
-      <c r="B27" s="60"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
@@ -1977,8 +1980,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="67"/>
-      <c r="B28" s="60"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
@@ -1993,8 +1996,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="67"/>
-      <c r="B29" s="60"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
@@ -2009,8 +2012,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="67"/>
-      <c r="B30" s="60"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
@@ -2025,8 +2028,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="67"/>
-      <c r="B31" s="60"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
@@ -2041,8 +2044,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="67"/>
-      <c r="B32" s="60"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="61"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
@@ -2057,8 +2060,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="67"/>
-      <c r="B33" s="60"/>
+      <c r="A33" s="57"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
@@ -2073,8 +2076,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="68"/>
-      <c r="B34" s="61"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="62"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
@@ -2089,7 +2092,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="63" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="59" t="s">
@@ -2109,8 +2112,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="57"/>
-      <c r="B36" s="60"/>
+      <c r="A36" s="64"/>
+      <c r="B36" s="61"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2125,8 +2128,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="58"/>
-      <c r="B37" s="61"/>
+      <c r="A37" s="65"/>
+      <c r="B37" s="62"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
@@ -2141,14 +2144,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="62" t="s">
+      <c r="A38" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
+      <c r="B38" s="67"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="67"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2171,7 +2174,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="63" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="59" t="s">
@@ -2191,8 +2194,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="57"/>
-      <c r="B41" s="60"/>
+      <c r="A41" s="64"/>
+      <c r="B41" s="61"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
@@ -2207,8 +2210,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="58"/>
-      <c r="B42" s="61"/>
+      <c r="A42" s="65"/>
+      <c r="B42" s="62"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
@@ -2223,7 +2226,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="56" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="59" t="s">
@@ -2243,8 +2246,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="67"/>
-      <c r="B44" s="60"/>
+      <c r="A44" s="57"/>
+      <c r="B44" s="61"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
@@ -2259,8 +2262,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="67"/>
-      <c r="B45" s="60"/>
+      <c r="A45" s="57"/>
+      <c r="B45" s="61"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
@@ -2275,8 +2278,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="68"/>
-      <c r="B46" s="61"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="62"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
@@ -2371,7 +2374,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="63" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="59" t="s">
@@ -2391,8 +2394,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="57"/>
-      <c r="B52" s="63"/>
+      <c r="A52" s="64"/>
+      <c r="B52" s="60"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2407,7 +2410,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="57"/>
+      <c r="A53" s="64"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2425,17 +2428,17 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="62" t="s">
+      <c r="A54" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="65"/>
-      <c r="C54" s="62"/>
-      <c r="D54" s="65"/>
-      <c r="E54" s="62"/>
-      <c r="F54" s="62"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="67"/>
+      <c r="D54" s="68"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="56" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="59" t="s">
@@ -2455,8 +2458,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="67"/>
-      <c r="B56" s="60"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="61"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
@@ -2471,8 +2474,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="67"/>
-      <c r="B57" s="60"/>
+      <c r="A57" s="57"/>
+      <c r="B57" s="61"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2487,8 +2490,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="67"/>
-      <c r="B58" s="60"/>
+      <c r="A58" s="57"/>
+      <c r="B58" s="61"/>
       <c r="C58" s="7" t="s">
         <v>185</v>
       </c>
@@ -2503,8 +2506,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="67"/>
-      <c r="B59" s="60"/>
+      <c r="A59" s="57"/>
+      <c r="B59" s="61"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2518,63 +2521,61 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="67"/>
-      <c r="B60" s="60"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="57"/>
+      <c r="B60" s="61"/>
       <c r="C60" s="7" t="s">
         <v>218</v>
       </c>
       <c r="D60" s="9"/>
-      <c r="E60" s="55" t="s">
+      <c r="E60" s="52" t="s">
         <v>216</v>
       </c>
       <c r="F60" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="57"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="55" t="s">
+        <v>216</v>
+      </c>
+      <c r="F61" s="54" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="67"/>
-      <c r="B61" s="64" t="s">
+    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="57"/>
+      <c r="B62" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C61" s="40" t="s">
+      <c r="C62" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="D61" s="37" t="s">
+      <c r="D62" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="E61" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="67"/>
-      <c r="B62" s="60"/>
-      <c r="C62" s="7" t="s">
+      <c r="E62" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="57"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D63" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E62" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A63" s="67"/>
-      <c r="B63" s="60"/>
-      <c r="C63" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D63" s="9" t="s">
-        <v>219</v>
-      </c>
       <c r="E63" s="52" t="s">
         <v>9</v>
       </c>
@@ -2582,85 +2583,85 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="68"/>
+    <row r="64" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A64" s="57"/>
       <c r="B64" s="61"/>
       <c r="C64" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E64" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="58"/>
+      <c r="B65" s="62"/>
+      <c r="C65" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D65" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E64" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="31" t="s">
+      <c r="E65" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="56" t="s">
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="63" t="s">
         <v>188</v>
       </c>
-      <c r="B65" s="59" t="s">
+      <c r="B66" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D65" s="46" t="s">
+      <c r="D66" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="E65" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="28" t="s">
+      <c r="E66" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="57"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="7" t="s">
+    <row r="67" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="64"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D66" s="44" t="s">
+      <c r="D67" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="E66" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="57"/>
-      <c r="B67" s="64" t="s">
+      <c r="E67" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="64"/>
+      <c r="B68" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="C68" s="40" t="s">
         <v>195</v>
       </c>
-      <c r="D67" s="48" t="s">
+      <c r="D68" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="E67" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="57"/>
-      <c r="B68" s="60"/>
-      <c r="C68" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D68" s="44" t="s">
-        <v>201</v>
-      </c>
       <c r="E68" s="29" t="s">
         <v>9</v>
       </c>
@@ -2669,167 +2670,163 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="58"/>
+      <c r="A69" s="64"/>
       <c r="B69" s="61"/>
       <c r="C69" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D69" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="65"/>
+      <c r="B70" s="62"/>
+      <c r="C70" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D69" s="44" t="s">
+      <c r="D70" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="E69" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="56" t="s">
+      <c r="E70" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A71" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="B70" s="59" t="s">
+      <c r="B71" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D70" s="46" t="s">
+      <c r="D71" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="E70" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="28" t="s">
+      <c r="E71" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="57"/>
-      <c r="B71" s="60"/>
-      <c r="C71" s="7" t="s">
+    <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="64"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D71" s="44" t="s">
+      <c r="D72" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="E71" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="29" t="s">
+      <c r="E72" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="58"/>
-      <c r="B72" s="61"/>
-      <c r="C72" s="10" t="s">
+    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="65"/>
+      <c r="B73" s="62"/>
+      <c r="C73" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="D72" s="47" t="s">
+      <c r="D73" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="E72" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="32" t="s">
+      <c r="E73" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="56" t="s">
+    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="59" t="s">
+      <c r="B74" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="D74" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E73" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="57"/>
-      <c r="B74" s="60"/>
-      <c r="C74" s="7" t="s">
+      <c r="E74" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="64"/>
+      <c r="B75" s="61"/>
+      <c r="C75" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="E74" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="58"/>
-      <c r="B75" s="61"/>
-      <c r="C75" s="10" t="s">
+      <c r="E75" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="65"/>
+      <c r="B76" s="62"/>
+      <c r="C76" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D75" s="23" t="s">
+      <c r="D76" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E75" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="62" t="s">
+      <c r="E76" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="B76" s="62"/>
-      <c r="C76" s="62"/>
-      <c r="D76" s="62"/>
-      <c r="E76" s="62"/>
-      <c r="F76" s="62"/>
-    </row>
-    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="13" t="s">
+      <c r="B77" s="67"/>
+      <c r="C77" s="67"/>
+      <c r="D77" s="67"/>
+      <c r="E77" s="67"/>
+      <c r="F77" s="67"/>
+    </row>
+    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="13" t="s">
         <v>147</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="E77" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="13" t="s">
-        <v>150</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E78" s="26" t="s">
         <v>9</v>
@@ -2838,171 +2835,175 @@
         <v>55</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="56" t="s">
+    <row r="79" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E79" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A80" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="B79" s="59" t="s">
+      <c r="B80" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D80" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="E79" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="31" t="s">
+      <c r="E80" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="57"/>
-      <c r="B80" s="60"/>
-      <c r="C80" s="7" t="s">
+    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="64"/>
+      <c r="B81" s="61"/>
+      <c r="C81" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D81" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E80" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="57"/>
-      <c r="B81" s="60"/>
-      <c r="C81" s="7" t="s">
+      <c r="E81" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="64"/>
+      <c r="B82" s="61"/>
+      <c r="C82" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D82" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E81" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="57"/>
-      <c r="B82" s="63"/>
-      <c r="C82" s="7" t="s">
+      <c r="E82" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="64"/>
+      <c r="B83" s="60"/>
+      <c r="C83" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="D83" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E82" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="57"/>
-      <c r="B83" s="64" t="s">
+      <c r="E83" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="64"/>
+      <c r="B84" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="40" t="s">
+      <c r="C84" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="D83" s="37" t="s">
+      <c r="D84" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="E83" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J83" s="7" t="s">
+      <c r="E84" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J84" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84" s="57"/>
-      <c r="B84" s="60"/>
-      <c r="C84" s="7" t="s">
+    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="64"/>
+      <c r="B85" s="61"/>
+      <c r="C85" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D84" s="9" t="s">
+      <c r="D85" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="E84" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A85" s="58"/>
-      <c r="B85" s="61"/>
-      <c r="C85" s="10" t="s">
+      <c r="E85" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A86" s="65"/>
+      <c r="B86" s="62"/>
+      <c r="C86" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="D85" s="23" t="s">
+      <c r="D86" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="E85" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="56" t="s">
+      <c r="E86" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A87" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="B86" s="59" t="s">
+      <c r="B87" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D87" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E86" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="30" t="s">
+      <c r="E87" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A87" s="57"/>
-      <c r="B87" s="60"/>
-      <c r="C87" s="7" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A88" s="64"/>
+      <c r="B88" s="61"/>
+      <c r="C88" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="D87" s="9" t="s">
+      <c r="D88" s="9" t="s">
         <v>211</v>
-      </c>
-      <c r="E87" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="57"/>
-      <c r="B88" s="63"/>
-      <c r="C88" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="E88" s="29" t="s">
         <v>9</v>
@@ -3011,81 +3012,94 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="58"/>
-      <c r="B89" s="41" t="s">
+    <row r="89" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="64"/>
+      <c r="B89" s="60"/>
+      <c r="C89" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E89" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" s="65"/>
+      <c r="B90" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="42" t="s">
+      <c r="C90" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="D89" s="43" t="s">
+      <c r="D90" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="E89" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F89" s="33" t="s">
+      <c r="E90" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="62" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A91" s="67" t="s">
         <v>171</v>
       </c>
-      <c r="B90" s="62"/>
-      <c r="C90" s="62"/>
-      <c r="D90" s="62"/>
-      <c r="E90" s="62"/>
-      <c r="F90" s="62"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="15" t="s">
+      <c r="B91" s="67"/>
+      <c r="C91" s="67"/>
+      <c r="D91" s="67"/>
+      <c r="E91" s="67"/>
+      <c r="F91" s="67"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A92" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="B92" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C92" s="7" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C92" s="7" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C93" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C94" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C95" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C96" s="7" t="s">
         <v>178</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="A55:A64"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="A77:F77"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B89"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A40:A42"/>
@@ -3102,17 +3116,20 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="A76:F76"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="A66:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B55:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="A55:A65"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A51:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made it to the quantRisk method for subspaces
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C04B55A-204A-437F-B530-10BECB7A7325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F50BC8-2D5E-4AD7-A950-4BE710C14A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -698,7 +698,7 @@
     <t>Determines the amount of space that would remain in each discipline if they were to move forward with the new rule combo(s) being considered for the current time stamp and calculates the entire design spaces' added potentials for regret and windfall.</t>
   </si>
   <si>
-    <t>subspaceConsolidate</t>
+    <t>createBins</t>
   </si>
 </sst>
 </file>
@@ -1187,6 +1187,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1195,36 +1225,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1509,8 +1509,8 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1545,17 +1545,17 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="59" t="s">
@@ -1576,8 +1576,8 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="57"/>
-      <c r="B4" s="61"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="7" t="s">
         <v>212</v>
       </c>
@@ -1593,8 +1593,8 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="58"/>
-      <c r="B5" s="62"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="10" t="s">
         <v>213</v>
       </c>
@@ -1630,7 +1630,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="56" t="s">
         <v>59</v>
       </c>
       <c r="B7" s="59" t="s">
@@ -1650,8 +1650,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="65"/>
-      <c r="B8" s="62"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1666,17 +1666,17 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="66" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="59" t="s">
@@ -1696,8 +1696,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="57"/>
-      <c r="B11" s="61"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
@@ -1712,8 +1712,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="57"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1728,8 +1728,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="57"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
@@ -1744,8 +1744,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="58"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
@@ -1760,7 +1760,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="66" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="59" t="s">
@@ -1780,8 +1780,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="57"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1796,8 +1796,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="57"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
@@ -1812,8 +1812,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="57"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
@@ -1828,8 +1828,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="57"/>
-      <c r="B19" s="60"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1844,8 +1844,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="57"/>
-      <c r="B20" s="61" t="s">
+      <c r="A20" s="67"/>
+      <c r="B20" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1862,8 +1862,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="57"/>
-      <c r="B21" s="61"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
@@ -1878,8 +1878,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="57"/>
-      <c r="B22" s="61"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
@@ -1894,8 +1894,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="57"/>
-      <c r="B23" s="61"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
@@ -1910,7 +1910,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="66" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="59" t="s">
@@ -1930,8 +1930,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="57"/>
-      <c r="B25" s="60"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1946,8 +1946,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="57"/>
-      <c r="B26" s="61" t="s">
+      <c r="A26" s="67"/>
+      <c r="B26" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1964,8 +1964,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="57"/>
-      <c r="B27" s="61"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="60"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
@@ -1980,8 +1980,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="57"/>
-      <c r="B28" s="61"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
@@ -1996,8 +1996,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="57"/>
-      <c r="B29" s="61"/>
+      <c r="A29" s="67"/>
+      <c r="B29" s="60"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
@@ -2012,8 +2012,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="57"/>
-      <c r="B30" s="61"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
@@ -2028,8 +2028,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="57"/>
-      <c r="B31" s="61"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="60"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
@@ -2044,8 +2044,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="57"/>
-      <c r="B32" s="61"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
@@ -2060,8 +2060,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="57"/>
-      <c r="B33" s="61"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
@@ -2076,8 +2076,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="58"/>
-      <c r="B34" s="62"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="56" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="59" t="s">
@@ -2112,8 +2112,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="64"/>
-      <c r="B36" s="61"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2128,8 +2128,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="65"/>
-      <c r="B37" s="62"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="61"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
@@ -2144,14 +2144,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="67" t="s">
+      <c r="A38" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="67"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="67"/>
-      <c r="F38" s="67"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2174,7 +2174,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="63" t="s">
+      <c r="A40" s="56" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="59" t="s">
@@ -2194,8 +2194,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="64"/>
-      <c r="B41" s="61"/>
+      <c r="A41" s="57"/>
+      <c r="B41" s="60"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
@@ -2210,8 +2210,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="65"/>
-      <c r="B42" s="62"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="61"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
@@ -2226,7 +2226,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="66" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="59" t="s">
@@ -2246,8 +2246,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="57"/>
-      <c r="B44" s="61"/>
+      <c r="A44" s="67"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
@@ -2262,8 +2262,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="57"/>
-      <c r="B45" s="61"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="60"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
@@ -2278,8 +2278,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="62"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="61"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
@@ -2374,7 +2374,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="63" t="s">
+      <c r="A51" s="56" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="59" t="s">
@@ -2394,8 +2394,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="64"/>
-      <c r="B52" s="60"/>
+      <c r="A52" s="57"/>
+      <c r="B52" s="63"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2410,7 +2410,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="64"/>
+      <c r="A53" s="57"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2428,17 +2428,17 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="67" t="s">
+      <c r="A54" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="68"/>
-      <c r="C54" s="67"/>
-      <c r="D54" s="68"/>
-      <c r="E54" s="67"/>
-      <c r="F54" s="67"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="62"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="56" t="s">
+      <c r="A55" s="66" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="59" t="s">
@@ -2458,8 +2458,8 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="57"/>
-      <c r="B56" s="61"/>
+      <c r="A56" s="67"/>
+      <c r="B56" s="60"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
@@ -2474,8 +2474,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="57"/>
-      <c r="B57" s="61"/>
+      <c r="A57" s="67"/>
+      <c r="B57" s="60"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2490,8 +2490,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="57"/>
-      <c r="B58" s="61"/>
+      <c r="A58" s="67"/>
+      <c r="B58" s="60"/>
       <c r="C58" s="7" t="s">
         <v>185</v>
       </c>
@@ -2506,8 +2506,8 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="57"/>
-      <c r="B59" s="61"/>
+      <c r="A59" s="67"/>
+      <c r="B59" s="60"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
@@ -2522,8 +2522,8 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="57"/>
-      <c r="B60" s="61"/>
+      <c r="A60" s="67"/>
+      <c r="B60" s="60"/>
       <c r="C60" s="7" t="s">
         <v>218</v>
       </c>
@@ -2536,8 +2536,8 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="57"/>
-      <c r="B61" s="61"/>
+      <c r="A61" s="67"/>
+      <c r="B61" s="60"/>
       <c r="C61" s="7" t="s">
         <v>220</v>
       </c>
@@ -2550,8 +2550,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="57"/>
-      <c r="B62" s="66" t="s">
+      <c r="A62" s="67"/>
+      <c r="B62" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="40" t="s">
@@ -2568,8 +2568,8 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="57"/>
-      <c r="B63" s="61"/>
+      <c r="A63" s="67"/>
+      <c r="B63" s="60"/>
       <c r="C63" s="7" t="s">
         <v>131</v>
       </c>
@@ -2584,8 +2584,8 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A64" s="57"/>
-      <c r="B64" s="61"/>
+      <c r="A64" s="67"/>
+      <c r="B64" s="60"/>
       <c r="C64" s="7" t="s">
         <v>132</v>
       </c>
@@ -2600,8 +2600,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="58"/>
-      <c r="B65" s="62"/>
+      <c r="A65" s="68"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="7" t="s">
         <v>133</v>
       </c>
@@ -2616,7 +2616,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="63" t="s">
+      <c r="A66" s="56" t="s">
         <v>188</v>
       </c>
       <c r="B66" s="59" t="s">
@@ -2636,8 +2636,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="64"/>
-      <c r="B67" s="60"/>
+      <c r="A67" s="57"/>
+      <c r="B67" s="63"/>
       <c r="C67" s="7" t="s">
         <v>194</v>
       </c>
@@ -2652,8 +2652,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="64"/>
-      <c r="B68" s="66" t="s">
+      <c r="A68" s="57"/>
+      <c r="B68" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="40" t="s">
@@ -2670,8 +2670,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="64"/>
-      <c r="B69" s="61"/>
+      <c r="A69" s="57"/>
+      <c r="B69" s="60"/>
       <c r="C69" s="7" t="s">
         <v>196</v>
       </c>
@@ -2686,8 +2686,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="65"/>
-      <c r="B70" s="62"/>
+      <c r="A70" s="58"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="7" t="s">
         <v>197</v>
       </c>
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="63" t="s">
+      <c r="A71" s="56" t="s">
         <v>183</v>
       </c>
       <c r="B71" s="59" t="s">
@@ -2722,8 +2722,8 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="64"/>
-      <c r="B72" s="61"/>
+      <c r="A72" s="57"/>
+      <c r="B72" s="60"/>
       <c r="C72" s="7" t="s">
         <v>191</v>
       </c>
@@ -2738,8 +2738,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="65"/>
-      <c r="B73" s="62"/>
+      <c r="A73" s="58"/>
+      <c r="B73" s="61"/>
       <c r="C73" s="10" t="s">
         <v>192</v>
       </c>
@@ -2754,7 +2754,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="63" t="s">
+      <c r="A74" s="56" t="s">
         <v>106</v>
       </c>
       <c r="B74" s="59" t="s">
@@ -2774,8 +2774,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="64"/>
-      <c r="B75" s="61"/>
+      <c r="A75" s="57"/>
+      <c r="B75" s="60"/>
       <c r="C75" s="7" t="s">
         <v>184</v>
       </c>
@@ -2790,8 +2790,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="65"/>
-      <c r="B76" s="62"/>
+      <c r="A76" s="58"/>
+      <c r="B76" s="61"/>
       <c r="C76" s="10" t="s">
         <v>139</v>
       </c>
@@ -2806,14 +2806,14 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="67" t="s">
+      <c r="A77" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="67"/>
-      <c r="C77" s="67"/>
-      <c r="D77" s="67"/>
-      <c r="E77" s="67"/>
-      <c r="F77" s="67"/>
+      <c r="B77" s="62"/>
+      <c r="C77" s="62"/>
+      <c r="D77" s="62"/>
+      <c r="E77" s="62"/>
+      <c r="F77" s="62"/>
     </row>
     <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="13" t="s">
@@ -2856,7 +2856,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="63" t="s">
+      <c r="A80" s="56" t="s">
         <v>152</v>
       </c>
       <c r="B80" s="59" t="s">
@@ -2876,8 +2876,8 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="64"/>
-      <c r="B81" s="61"/>
+      <c r="A81" s="57"/>
+      <c r="B81" s="60"/>
       <c r="C81" s="7" t="s">
         <v>154</v>
       </c>
@@ -2892,8 +2892,8 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="64"/>
-      <c r="B82" s="61"/>
+      <c r="A82" s="57"/>
+      <c r="B82" s="60"/>
       <c r="C82" s="7" t="s">
         <v>155</v>
       </c>
@@ -2908,8 +2908,8 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A83" s="64"/>
-      <c r="B83" s="60"/>
+      <c r="A83" s="57"/>
+      <c r="B83" s="63"/>
       <c r="C83" s="7" t="s">
         <v>156</v>
       </c>
@@ -2924,8 +2924,8 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A84" s="64"/>
-      <c r="B84" s="66" t="s">
+      <c r="A84" s="57"/>
+      <c r="B84" s="64" t="s">
         <v>15</v>
       </c>
       <c r="C84" s="40" t="s">
@@ -2945,8 +2945,8 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="64"/>
-      <c r="B85" s="61"/>
+      <c r="A85" s="57"/>
+      <c r="B85" s="60"/>
       <c r="C85" s="7" t="s">
         <v>124</v>
       </c>
@@ -2961,8 +2961,8 @@
       </c>
     </row>
     <row r="86" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A86" s="65"/>
-      <c r="B86" s="62"/>
+      <c r="A86" s="58"/>
+      <c r="B86" s="61"/>
       <c r="C86" s="10" t="s">
         <v>157</v>
       </c>
@@ -2977,7 +2977,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="63" t="s">
+      <c r="A87" s="56" t="s">
         <v>158</v>
       </c>
       <c r="B87" s="59" t="s">
@@ -2997,8 +2997,8 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A88" s="64"/>
-      <c r="B88" s="61"/>
+      <c r="A88" s="57"/>
+      <c r="B88" s="60"/>
       <c r="C88" s="7" t="s">
         <v>210</v>
       </c>
@@ -3013,8 +3013,8 @@
       </c>
     </row>
     <row r="89" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="64"/>
-      <c r="B89" s="60"/>
+      <c r="A89" s="57"/>
+      <c r="B89" s="63"/>
       <c r="C89" s="7" t="s">
         <v>166</v>
       </c>
@@ -3029,7 +3029,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="65"/>
+      <c r="A90" s="58"/>
       <c r="B90" s="41" t="s">
         <v>15</v>
       </c>
@@ -3047,14 +3047,14 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="67" t="s">
+      <c r="A91" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="B91" s="67"/>
-      <c r="C91" s="67"/>
-      <c r="D91" s="67"/>
-      <c r="E91" s="67"/>
-      <c r="F91" s="67"/>
+      <c r="B91" s="62"/>
+      <c r="C91" s="62"/>
+      <c r="D91" s="62"/>
+      <c r="E91" s="62"/>
+      <c r="F91" s="62"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="15" t="s">
@@ -3089,17 +3089,20 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A80:A86"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="A77:F77"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B34"/>
+    <mergeCell ref="A66:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="B55:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="A55:A65"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A40:A42"/>
@@ -3116,20 +3119,17 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A66:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B55:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A55:A65"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="A77:F77"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="B87:B89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished commenting on new subspace code
Still needs to be unit tested
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9030EEB4-D729-4F5F-A8A9-7FBF4284CF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BF24B2-A451-4609-B098-885F35850284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="224">
   <si>
     <t>Class</t>
   </si>
@@ -686,9 +686,6 @@
     <t>Creates an expression that denormalizes an input variable.</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Incomplete</t>
   </si>
   <si>
@@ -705,6 +702,12 @@
   </si>
   <si>
     <t>Creates unique bins for the space remaining points of a particular subspace being assessed.</t>
+  </si>
+  <si>
+    <t>Consolidates regret or windfall data into the subspace being assessed and then sums the averages within the subspace.</t>
+  </si>
+  <si>
+    <t>Calculates the fraction of a (sub)space's remaining design space size relative to its original size.</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1178,25 +1181,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1527,8 +1515,8 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1563,20 +1551,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="58" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1594,8 +1582,8 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="61"/>
-      <c r="B4" s="65"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="7" t="s">
         <v>212</v>
       </c>
@@ -1611,8 +1599,8 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="62"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="10" t="s">
         <v>213</v>
       </c>
@@ -1648,10 +1636,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1668,8 +1656,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="69"/>
-      <c r="B8" s="66"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
       </c>
@@ -1684,20 +1672,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1714,8 +1702,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="61"/>
-      <c r="B11" s="65"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
       </c>
@@ -1730,8 +1718,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="61"/>
-      <c r="B12" s="65"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1746,8 +1734,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="61"/>
-      <c r="B13" s="65"/>
+      <c r="A13" s="56"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
       </c>
@@ -1762,8 +1750,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="62"/>
-      <c r="B14" s="65"/>
+      <c r="A14" s="57"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
       </c>
@@ -1778,10 +1766,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="58" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1798,8 +1786,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="61"/>
-      <c r="B16" s="65"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
       </c>
@@ -1814,8 +1802,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="61"/>
-      <c r="B17" s="65"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
       </c>
@@ -1830,8 +1818,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="61"/>
-      <c r="B18" s="65"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
       </c>
@@ -1846,8 +1834,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="61"/>
-      <c r="B19" s="64"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1862,8 +1850,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="61"/>
-      <c r="B20" s="65" t="s">
+      <c r="A20" s="56"/>
+      <c r="B20" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1880,8 +1868,8 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
       </c>
@@ -1896,8 +1884,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="61"/>
-      <c r="B22" s="65"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
@@ -1912,8 +1900,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="61"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="60"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
       </c>
@@ -1928,10 +1916,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="58" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="35" t="s">
@@ -1948,8 +1936,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="61"/>
-      <c r="B25" s="64"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1964,8 +1952,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="65" t="s">
+      <c r="A26" s="56"/>
+      <c r="B26" s="60" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -1982,8 +1970,8 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="65"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="60"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
       </c>
@@ -1998,8 +1986,8 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="61"/>
-      <c r="B28" s="65"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
       </c>
@@ -2014,8 +2002,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="61"/>
-      <c r="B29" s="65"/>
+      <c r="A29" s="56"/>
+      <c r="B29" s="60"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
       </c>
@@ -2030,8 +2018,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="61"/>
-      <c r="B30" s="65"/>
+      <c r="A30" s="56"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
       </c>
@@ -2046,8 +2034,8 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="61"/>
-      <c r="B31" s="65"/>
+      <c r="A31" s="56"/>
+      <c r="B31" s="60"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
       </c>
@@ -2062,8 +2050,8 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="61"/>
-      <c r="B32" s="65"/>
+      <c r="A32" s="56"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
@@ -2078,8 +2066,8 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="61"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="56"/>
+      <c r="B33" s="60"/>
       <c r="C33" s="36" t="s">
         <v>115</v>
       </c>
@@ -2094,8 +2082,8 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="62"/>
-      <c r="B34" s="66"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="10" t="s">
         <v>116</v>
       </c>
@@ -2110,10 +2098,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="58" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2130,8 +2118,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="68"/>
-      <c r="B36" s="65"/>
+      <c r="A36" s="63"/>
+      <c r="B36" s="60"/>
       <c r="C36" s="7" t="s">
         <v>70</v>
       </c>
@@ -2146,8 +2134,8 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="69"/>
-      <c r="B37" s="66"/>
+      <c r="A37" s="64"/>
+      <c r="B37" s="61"/>
       <c r="C37" s="7" t="s">
         <v>71</v>
       </c>
@@ -2162,14 +2150,14 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="71" t="s">
+      <c r="A38" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="71"/>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
-      <c r="F38" s="71"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
@@ -2192,10 +2180,10 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2212,8 +2200,8 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="68"/>
-      <c r="B41" s="65"/>
+      <c r="A41" s="63"/>
+      <c r="B41" s="60"/>
       <c r="C41" s="7" t="s">
         <v>17</v>
       </c>
@@ -2228,8 +2216,8 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="69"/>
-      <c r="B42" s="66"/>
+      <c r="A42" s="64"/>
+      <c r="B42" s="61"/>
       <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
@@ -2244,10 +2232,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2264,8 +2252,8 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="61"/>
-      <c r="B44" s="65"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="60"/>
       <c r="C44" s="7" t="s">
         <v>23</v>
       </c>
@@ -2280,8 +2268,8 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="61"/>
-      <c r="B45" s="65"/>
+      <c r="A45" s="56"/>
+      <c r="B45" s="60"/>
       <c r="C45" s="7" t="s">
         <v>24</v>
       </c>
@@ -2296,8 +2284,8 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="62"/>
-      <c r="B46" s="66"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="61"/>
       <c r="C46" s="7" t="s">
         <v>102</v>
       </c>
@@ -2392,10 +2380,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="67" t="s">
+      <c r="A51" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="63" t="s">
+      <c r="B51" s="58" t="s">
         <v>43</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2412,8 +2400,8 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="68"/>
-      <c r="B52" s="64"/>
+      <c r="A52" s="63"/>
+      <c r="B52" s="59"/>
       <c r="C52" s="24" t="s">
         <v>45</v>
       </c>
@@ -2428,7 +2416,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="68"/>
+      <c r="A53" s="63"/>
       <c r="B53" s="34" t="s">
         <v>15</v>
       </c>
@@ -2446,20 +2434,20 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="71" t="s">
+      <c r="A54" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="72"/>
-      <c r="C54" s="71"/>
-      <c r="D54" s="72"/>
-      <c r="E54" s="71"/>
-      <c r="F54" s="71"/>
+      <c r="B54" s="67"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="60" t="s">
+      <c r="A55" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="63" t="s">
+      <c r="B55" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -2468,16 +2456,16 @@
       <c r="D55" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="54" t="s">
-        <v>56</v>
+      <c r="E55" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="61"/>
-      <c r="B56" s="65"/>
+      <c r="A56" s="56"/>
+      <c r="B56" s="60"/>
       <c r="C56" s="7" t="s">
         <v>135</v>
       </c>
@@ -2492,8 +2480,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="61"/>
-      <c r="B57" s="65"/>
+      <c r="A57" s="56"/>
+      <c r="B57" s="60"/>
       <c r="C57" s="7" t="s">
         <v>136</v>
       </c>
@@ -2508,8 +2496,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="61"/>
-      <c r="B58" s="65"/>
+      <c r="A58" s="56"/>
+      <c r="B58" s="60"/>
       <c r="C58" s="7" t="s">
         <v>185</v>
       </c>
@@ -2524,54 +2512,56 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="61"/>
-      <c r="B59" s="65"/>
+      <c r="A59" s="56"/>
+      <c r="B59" s="60"/>
       <c r="C59" s="7" t="s">
         <v>137</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="E59" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="61"/>
-      <c r="B60" s="65"/>
+      <c r="E59" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="56"/>
+      <c r="B60" s="60"/>
       <c r="C60" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D60" s="9"/>
-      <c r="E60" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="F60" s="54" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="61" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="61"/>
-      <c r="B61" s="65"/>
+      <c r="A61" s="56"/>
+      <c r="B61" s="60"/>
       <c r="C61" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E61" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="F61" s="54" t="s">
-        <v>217</v>
+      <c r="F61" s="51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="61"/>
-      <c r="B62" s="70" t="s">
+      <c r="A62" s="56"/>
+      <c r="B62" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C62" s="40" t="s">
@@ -2588,40 +2578,40 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="61"/>
-      <c r="B63" s="65"/>
+      <c r="A63" s="56"/>
+      <c r="B63" s="60"/>
       <c r="C63" s="7" t="s">
         <v>131</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E63" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="54" t="s">
-        <v>56</v>
+      <c r="E63" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A64" s="61"/>
-      <c r="B64" s="65"/>
+      <c r="A64" s="56"/>
+      <c r="B64" s="60"/>
       <c r="C64" s="7" t="s">
         <v>132</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="E64" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="54" t="s">
-        <v>56</v>
+        <v>218</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="62"/>
-      <c r="B65" s="66"/>
+      <c r="A65" s="57"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="7" t="s">
         <v>133</v>
       </c>
@@ -2636,10 +2626,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="67" t="s">
+      <c r="A66" s="62" t="s">
         <v>188</v>
       </c>
-      <c r="B66" s="63" t="s">
+      <c r="B66" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -2656,8 +2646,8 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="68"/>
-      <c r="B67" s="64"/>
+      <c r="A67" s="63"/>
+      <c r="B67" s="59"/>
       <c r="C67" s="7" t="s">
         <v>194</v>
       </c>
@@ -2672,8 +2662,8 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="68"/>
-      <c r="B68" s="70" t="s">
+      <c r="A68" s="63"/>
+      <c r="B68" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C68" s="40" t="s">
@@ -2690,8 +2680,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="68"/>
-      <c r="B69" s="65"/>
+      <c r="A69" s="63"/>
+      <c r="B69" s="60"/>
       <c r="C69" s="7" t="s">
         <v>196</v>
       </c>
@@ -2706,8 +2696,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="69"/>
-      <c r="B70" s="66"/>
+      <c r="A70" s="64"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="7" t="s">
         <v>197</v>
       </c>
@@ -2722,10 +2712,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="67" t="s">
+      <c r="A71" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="B71" s="63" t="s">
+      <c r="B71" s="58" t="s">
         <v>189</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -2734,7 +2724,7 @@
       <c r="D71" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="E71" s="51" t="s">
+      <c r="E71" s="28" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="28" t="s">
@@ -2742,15 +2732,15 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="68"/>
-      <c r="B72" s="65"/>
+      <c r="A72" s="63"/>
+      <c r="B72" s="60"/>
       <c r="C72" s="7" t="s">
         <v>191</v>
       </c>
       <c r="D72" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="E72" s="52" t="s">
+      <c r="E72" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F72" s="29" t="s">
@@ -2758,15 +2748,15 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="69"/>
-      <c r="B73" s="66"/>
+      <c r="A73" s="64"/>
+      <c r="B73" s="61"/>
       <c r="C73" s="10" t="s">
         <v>192</v>
       </c>
       <c r="D73" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="E73" s="53" t="s">
+      <c r="E73" s="32" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="32" t="s">
@@ -2774,10 +2764,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="67" t="s">
+      <c r="A74" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="B74" s="63" t="s">
+      <c r="B74" s="58" t="s">
         <v>138</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -2786,32 +2776,32 @@
       <c r="D74" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E74" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="56" t="s">
-        <v>56</v>
+      <c r="E74" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="52" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="68"/>
-      <c r="B75" s="65"/>
+      <c r="A75" s="63"/>
+      <c r="B75" s="60"/>
       <c r="C75" s="7" t="s">
         <v>184</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="E75" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="54" t="s">
-        <v>56</v>
+      <c r="E75" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="68"/>
-      <c r="B76" s="65"/>
+      <c r="A76" s="63"/>
+      <c r="B76" s="60"/>
       <c r="C76" s="7" t="s">
         <v>139</v>
       </c>
@@ -2825,31 +2815,33 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="69"/>
-      <c r="B77" s="59" t="s">
+    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="64"/>
+      <c r="B77" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="D77" s="23"/>
-      <c r="E77" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="D77" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E77" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="F77" s="58" t="s">
-        <v>217</v>
-      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="71" t="s">
+      <c r="A78" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="B78" s="71"/>
-      <c r="C78" s="71"/>
-      <c r="D78" s="71"/>
-      <c r="E78" s="71"/>
-      <c r="F78" s="71"/>
+      <c r="B78" s="66"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
     </row>
     <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
@@ -2892,10 +2884,10 @@
       </c>
     </row>
     <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="67" t="s">
+      <c r="A81" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="B81" s="63" t="s">
+      <c r="B81" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C81" s="7" t="s">
@@ -2912,8 +2904,8 @@
       </c>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="68"/>
-      <c r="B82" s="65"/>
+      <c r="A82" s="63"/>
+      <c r="B82" s="60"/>
       <c r="C82" s="7" t="s">
         <v>154</v>
       </c>
@@ -2928,8 +2920,8 @@
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="68"/>
-      <c r="B83" s="65"/>
+      <c r="A83" s="63"/>
+      <c r="B83" s="60"/>
       <c r="C83" s="7" t="s">
         <v>155</v>
       </c>
@@ -2944,8 +2936,8 @@
       </c>
     </row>
     <row r="84" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="68"/>
-      <c r="B84" s="64"/>
+      <c r="A84" s="63"/>
+      <c r="B84" s="59"/>
       <c r="C84" s="7" t="s">
         <v>156</v>
       </c>
@@ -2960,8 +2952,8 @@
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="68"/>
-      <c r="B85" s="70" t="s">
+      <c r="A85" s="63"/>
+      <c r="B85" s="65" t="s">
         <v>15</v>
       </c>
       <c r="C85" s="40" t="s">
@@ -2981,8 +2973,8 @@
       </c>
     </row>
     <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="68"/>
-      <c r="B86" s="65"/>
+      <c r="A86" s="63"/>
+      <c r="B86" s="60"/>
       <c r="C86" s="7" t="s">
         <v>124</v>
       </c>
@@ -2997,8 +2989,8 @@
       </c>
     </row>
     <row r="87" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A87" s="69"/>
-      <c r="B87" s="66"/>
+      <c r="A87" s="64"/>
+      <c r="B87" s="61"/>
       <c r="C87" s="10" t="s">
         <v>157</v>
       </c>
@@ -3013,10 +3005,10 @@
       </c>
     </row>
     <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="67" t="s">
+      <c r="A88" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="B88" s="63" t="s">
+      <c r="B88" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -3033,8 +3025,8 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="68"/>
-      <c r="B89" s="65"/>
+      <c r="A89" s="63"/>
+      <c r="B89" s="60"/>
       <c r="C89" s="7" t="s">
         <v>210</v>
       </c>
@@ -3049,8 +3041,8 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="68"/>
-      <c r="B90" s="64"/>
+      <c r="A90" s="63"/>
+      <c r="B90" s="59"/>
       <c r="C90" s="7" t="s">
         <v>166</v>
       </c>
@@ -3065,7 +3057,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="69"/>
+      <c r="A91" s="64"/>
       <c r="B91" s="41" t="s">
         <v>15</v>
       </c>
@@ -3083,14 +3075,14 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A92" s="71" t="s">
+      <c r="A92" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="B92" s="71"/>
-      <c r="C92" s="71"/>
-      <c r="D92" s="71"/>
-      <c r="E92" s="71"/>
-      <c r="F92" s="71"/>
+      <c r="B92" s="66"/>
+      <c r="C92" s="66"/>
+      <c r="D92" s="66"/>
+      <c r="E92" s="66"/>
+      <c r="F92" s="66"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="15" t="s">

</xml_diff>

<commit_message>
Organizing script file for interdependenies
Everything seems set up, now I need to write the code with GPy to form a MOGP
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BF24B2-A451-4609-B098-885F35850284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C522E474-22E1-49D7-A7C7-C24BB06F92DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1515,8 +1515,8 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I78" sqref="I78"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Working through interdependency code
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C522E474-22E1-49D7-A7C7-C24BB06F92DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EDB4F8-611A-484D-964C-07DDCE8EA397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="227">
   <si>
     <t>Class</t>
   </si>
@@ -708,6 +708,15 @@
   </si>
   <si>
     <t>Calculates the fraction of a (sub)space's remaining design space size relative to its original size.</t>
+  </si>
+  <si>
+    <t>connect_perceptions</t>
+  </si>
+  <si>
+    <t>connectPerceptions</t>
+  </si>
+  <si>
+    <t>normalizePredictions</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1193,6 +1202,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1202,35 +1244,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1512,11 +1533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I92" sqref="I92"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1551,20 +1572,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1582,7 +1603,7 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="56"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="60"/>
       <c r="C4" s="7" t="s">
         <v>212</v>
@@ -1599,7 +1620,7 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="57"/>
+      <c r="A5" s="68"/>
       <c r="B5" s="61"/>
       <c r="C5" s="10" t="s">
         <v>213</v>
@@ -1636,10 +1657,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1656,7 +1677,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="64"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="61"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
@@ -1672,20 +1693,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1702,7 +1723,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="56"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="60"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
@@ -1718,7 +1739,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="56"/>
+      <c r="A12" s="67"/>
       <c r="B12" s="60"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
@@ -1734,7 +1755,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="56"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="60"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
@@ -1750,7 +1771,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="57"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="60"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
@@ -1766,10 +1787,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="59" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1786,7 +1807,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="56"/>
+      <c r="A16" s="67"/>
       <c r="B16" s="60"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
@@ -1802,7 +1823,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="56"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="60"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
@@ -1818,7 +1839,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="56"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="60"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
@@ -1834,8 +1855,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="56"/>
-      <c r="B19" s="59"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="63"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1850,7 +1871,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
+      <c r="A20" s="67"/>
       <c r="B20" s="60" t="s">
         <v>15</v>
       </c>
@@ -1868,7 +1889,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="56"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="60"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
@@ -1884,7 +1905,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="56"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="60"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
@@ -1900,7 +1921,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="56"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="60"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
@@ -1916,10 +1937,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="59" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="35" t="s">
@@ -1936,8 +1957,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="56"/>
-      <c r="B25" s="59"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1952,7 +1973,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="56"/>
+      <c r="A26" s="67"/>
       <c r="B26" s="60" t="s">
         <v>15</v>
       </c>
@@ -1965,12 +1986,12 @@
       <c r="E26" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="31" t="s">
-        <v>56</v>
+      <c r="F26" s="51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="56"/>
+      <c r="A27" s="67"/>
       <c r="B27" s="60"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
@@ -1986,7 +2007,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="56"/>
+      <c r="A28" s="67"/>
       <c r="B28" s="60"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
@@ -2002,7 +2023,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="56"/>
+      <c r="A29" s="67"/>
       <c r="B29" s="60"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
@@ -2018,7 +2039,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="56"/>
+      <c r="A30" s="67"/>
       <c r="B30" s="60"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
@@ -2034,7 +2055,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="56"/>
+      <c r="A31" s="67"/>
       <c r="B31" s="60"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
@@ -2049,884 +2070,828 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="56"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="67"/>
       <c r="B32" s="60"/>
       <c r="C32" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="31" t="s">
-        <v>56</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="51"/>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="56"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="60"/>
       <c r="C33" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="67"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D34" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E33" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="57"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="10" t="s">
+      <c r="E34" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="68"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D35" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="E34" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="62" t="s">
+      <c r="E35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="55" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="51"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="55"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="51"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="55"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="51"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="55"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="51"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="55"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="70"/>
+      <c r="F40" s="51"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="55"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="51"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B42" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E35" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="63"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="7" t="s">
+      <c r="E42" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="57"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D43" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="64"/>
-      <c r="B37" s="61"/>
-      <c r="C37" s="7" t="s">
+      <c r="E43" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="58"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D44" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="66" t="s">
+      <c r="E44" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="66"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B46" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="62" t="s">
+      <c r="E46" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="B47" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="63"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="7" t="s">
+      <c r="E47" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="57"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D48" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="64"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="7" t="s">
+      <c r="E48" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="58"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D49" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="55" t="s">
+      <c r="E49" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B50" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="30" t="s">
+      <c r="E50" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="56"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="7" t="s">
+    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="67"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D51" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="31" t="s">
+      <c r="E51" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="56"/>
-      <c r="B45" s="60"/>
-      <c r="C45" s="7" t="s">
+    <row r="52" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="67"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D52" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="31" t="s">
+      <c r="E52" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="57"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="7" t="s">
+    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="68"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D53" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E46" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="31" t="s">
+      <c r="E53" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="14" t="s">
+    <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B54" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D54" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="s">
+      <c r="E54" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D55" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E48" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="14" t="s">
+      <c r="E55" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="s">
+      <c r="E56" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="62" t="s">
+      <c r="E57" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B58" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D58" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E51" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="63"/>
-      <c r="B52" s="59"/>
-      <c r="C52" s="24" t="s">
+      <c r="E58" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="57"/>
+      <c r="B59" s="63"/>
+      <c r="C59" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="D59" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E52" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="63"/>
-      <c r="B53" s="34" t="s">
+      <c r="E59" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A60" s="57"/>
+      <c r="B60" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C60" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D60" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E53" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="66" t="s">
+      <c r="E60" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="67"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="67"/>
-      <c r="E54" s="66"/>
-      <c r="F54" s="66"/>
-    </row>
-    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="55" t="s">
+      <c r="B61" s="65"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="62"/>
+    </row>
+    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="58" t="s">
+      <c r="B62" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C62" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D62" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E55" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="51" t="s">
+      <c r="E62" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="51" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="56"/>
-      <c r="B56" s="60"/>
-      <c r="C56" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="E56" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="56"/>
-      <c r="B57" s="60"/>
-      <c r="C57" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E57" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="56"/>
-      <c r="B58" s="60"/>
-      <c r="C58" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E58" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="56"/>
-      <c r="B59" s="60"/>
-      <c r="C59" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="E59" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="56"/>
-      <c r="B60" s="60"/>
-      <c r="C60" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="E60" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="56"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D61" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="E61" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="56"/>
-      <c r="B62" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="D62" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="56"/>
+      <c r="A63" s="67"/>
       <c r="B63" s="60"/>
       <c r="C63" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="E63" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F63" s="51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A64" s="56"/>
+      <c r="F63" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="67"/>
       <c r="B64" s="60"/>
       <c r="C64" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="67"/>
+      <c r="B65" s="60"/>
+      <c r="C65" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="67"/>
+      <c r="B66" s="60"/>
+      <c r="C66" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A67" s="67"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E67" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="67"/>
+      <c r="B68" s="60"/>
+      <c r="C68" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E68" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A69" s="67"/>
+      <c r="B69" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="67"/>
+      <c r="B70" s="60"/>
+      <c r="C70" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A71" s="67"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D71" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="E64" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="51" t="s">
+      <c r="E71" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="51" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="57"/>
-      <c r="B65" s="61"/>
-      <c r="C65" s="7" t="s">
+    <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="68"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D72" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E65" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="31" t="s">
+      <c r="E72" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="62" t="s">
+    <row r="73" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="56" t="s">
         <v>188</v>
       </c>
-      <c r="B66" s="58" t="s">
+      <c r="B73" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D66" s="46" t="s">
+      <c r="D73" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="E66" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="28" t="s">
+      <c r="E73" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="63"/>
-      <c r="B67" s="59"/>
-      <c r="C67" s="7" t="s">
+    <row r="74" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="57"/>
+      <c r="B74" s="63"/>
+      <c r="C74" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D67" s="44" t="s">
+      <c r="D74" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="E67" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F67" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="63"/>
-      <c r="B68" s="65" t="s">
+      <c r="E74" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="57"/>
+      <c r="B75" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C68" s="40" t="s">
+      <c r="C75" s="40" t="s">
         <v>195</v>
       </c>
-      <c r="D68" s="48" t="s">
+      <c r="D75" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="E68" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="63"/>
-      <c r="B69" s="60"/>
-      <c r="C69" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D69" s="44" t="s">
-        <v>201</v>
-      </c>
-      <c r="E69" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="64"/>
-      <c r="B70" s="61"/>
-      <c r="C70" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D70" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="E70" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="62" t="s">
-        <v>183</v>
-      </c>
-      <c r="B71" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D71" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="E71" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F71" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="63"/>
-      <c r="B72" s="60"/>
-      <c r="C72" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D72" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E72" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="64"/>
-      <c r="B73" s="61"/>
-      <c r="C73" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="D73" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="E73" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="62" t="s">
-        <v>106</v>
-      </c>
-      <c r="B74" s="58" t="s">
-        <v>138</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E74" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="52" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="63"/>
-      <c r="B75" s="60"/>
-      <c r="C75" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>187</v>
-      </c>
       <c r="E75" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F75" s="51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="63"/>
+      <c r="F75" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="57"/>
       <c r="B76" s="60"/>
       <c r="C76" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>145</v>
+        <v>196</v>
+      </c>
+      <c r="D76" s="44" t="s">
+        <v>201</v>
       </c>
       <c r="E76" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F76" s="31" t="s">
+      <c r="F76" s="29" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="64"/>
-      <c r="B77" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="D77" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="E77" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="53" t="s">
+      <c r="A77" s="58"/>
+      <c r="B77" s="61"/>
+      <c r="C77" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D77" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="E77" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="B78" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D78" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="E78" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="57"/>
+      <c r="B79" s="60"/>
+      <c r="C79" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D79" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="E79" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="58"/>
+      <c r="B80" s="61"/>
+      <c r="C80" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D80" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="E80" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="B81" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E81" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="52" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="B78" s="66"/>
-      <c r="C78" s="66"/>
-      <c r="D78" s="66"/>
-      <c r="E78" s="66"/>
-      <c r="F78" s="66"/>
-    </row>
-    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D79" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F79" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="E80" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="62" t="s">
-        <v>152</v>
-      </c>
-      <c r="B81" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E81" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="63"/>
+    <row r="82" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="57"/>
       <c r="B82" s="60"/>
       <c r="C82" s="7" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="E82" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F82" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="63"/>
+      <c r="F82" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="57"/>
       <c r="B83" s="60"/>
       <c r="C83" s="7" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="E83" s="29" t="s">
         <v>9</v>
@@ -2935,203 +2900,326 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="63"/>
-      <c r="B84" s="59"/>
-      <c r="C84" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E84" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="63"/>
-      <c r="B85" s="65" t="s">
+    <row r="84" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="58"/>
+      <c r="B84" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C85" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="D85" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="E85" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F85" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="J85" s="7" t="s">
-        <v>180</v>
-      </c>
+      <c r="C84" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D84" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E84" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="53" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A85" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" s="62"/>
+      <c r="C85" s="62"/>
+      <c r="D85" s="62"/>
+      <c r="E85" s="62"/>
+      <c r="F85" s="62"/>
     </row>
     <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="63"/>
-      <c r="B86" s="60"/>
-      <c r="C86" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E86" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A87" s="64"/>
-      <c r="B87" s="61"/>
-      <c r="C87" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="D87" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="E87" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F87" s="33" t="s">
-        <v>56</v>
+      <c r="A86" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E86" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E87" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="27" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="62" t="s">
-        <v>158</v>
-      </c>
-      <c r="B88" s="58" t="s">
+      <c r="A88" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="B88" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E88" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F88" s="30" t="s">
+      <c r="C88" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="63"/>
+    <row r="89" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A89" s="57"/>
       <c r="B89" s="60"/>
       <c r="C89" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E89" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A90" s="57"/>
+      <c r="B90" s="60"/>
+      <c r="C90" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="57"/>
+      <c r="B91" s="63"/>
+      <c r="C91" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E91" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A92" s="57"/>
+      <c r="B92" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D92" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="E92" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J92" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A93" s="57"/>
+      <c r="B93" s="60"/>
+      <c r="C93" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E93" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A94" s="58"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D94" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E94" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A95" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="B95" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E95" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A96" s="57"/>
+      <c r="B96" s="60"/>
+      <c r="C96" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="D89" s="9" t="s">
+      <c r="D96" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="E89" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F89" s="31" t="s">
+      <c r="E96" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="63"/>
-      <c r="B90" s="59"/>
-      <c r="C90" s="7" t="s">
+    <row r="97" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="57"/>
+      <c r="B97" s="63"/>
+      <c r="C97" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D90" s="9" t="s">
+      <c r="D97" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="E90" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F90" s="31" t="s">
+      <c r="E97" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="64"/>
-      <c r="B91" s="41" t="s">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" s="58"/>
+      <c r="B98" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C91" s="42" t="s">
+      <c r="C98" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="D91" s="43" t="s">
+      <c r="D98" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="E91" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="33" t="s">
+      <c r="E98" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="33" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A92" s="66" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="B92" s="66"/>
-      <c r="C92" s="66"/>
-      <c r="D92" s="66"/>
-      <c r="E92" s="66"/>
-      <c r="F92" s="66"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A93" s="15" t="s">
+      <c r="B99" s="62"/>
+      <c r="C99" s="62"/>
+      <c r="D99" s="62"/>
+      <c r="E99" s="62"/>
+      <c r="F99" s="62"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="B100" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C100" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C94" s="7" t="s">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C101" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C95" s="7" t="s">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C102" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C96" s="7" t="s">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C103" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C97" s="7" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C104" s="7" t="s">
         <v>178</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A71:A73"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="A92:F92"/>
-    <mergeCell ref="A81:A87"/>
-    <mergeCell ref="B81:B84"/>
-    <mergeCell ref="B85:B87"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="A24:A35"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="A73:A77"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B62:B68"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="A62:A72"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A58:A60"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B10:B14"/>
@@ -3140,24 +3228,21 @@
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A23"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B42:B44"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B34"/>
-    <mergeCell ref="A66:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B55:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="A55:A65"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="A99:F99"/>
+    <mergeCell ref="A88:A94"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="A81:A84"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B81:B83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished commenting extended code
Still need to unit test first two extensions, and code up the last extension involving objective space changes.
</commit_message>
<xml_diff>
--- a/Python Code/File_Tracker.xlsx
+++ b/Python Code/File_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeyvan\Documents\GitHub\DesignSpace_Fragility\Python Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EDB4F8-611A-484D-964C-07DDCE8EA397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA3D3D9-CCCD-4451-BFBD-52B4B691A5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="233">
   <si>
     <t>Class</t>
   </si>
@@ -717,6 +717,24 @@
   </si>
   <si>
     <t>normalizePredictions</t>
+  </si>
+  <si>
+    <t>organizeData</t>
+  </si>
+  <si>
+    <t>prepareData</t>
+  </si>
+  <si>
+    <t>Normalizes the mean of the pass-fail predictions between -1 and +1 and scales the standard deviations of the predictions accordingly.</t>
+  </si>
+  <si>
+    <t>Takes explored points from each discipline and organizes it into a combined numpy array used to train a combined Gaussian process regressor.</t>
+  </si>
+  <si>
+    <t>Prepares the space remaining data in each discipline to be test points for the trained GPR that considers interdependencies.</t>
+  </si>
+  <si>
+    <t>Predicts pass-fail amounts in each discipline's remaining design space with a GPR that is trained with combined exploration data from each discipline.</t>
   </si>
 </sst>
 </file>
@@ -771,7 +789,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1034,11 +1052,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1202,9 +1233,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1214,44 +1263,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1533,11 +1555,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1572,20 +1594,20 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1603,7 +1625,7 @@
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="67"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="60"/>
       <c r="C4" s="7" t="s">
         <v>212</v>
@@ -1620,7 +1642,7 @@
       <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="61"/>
       <c r="C5" s="10" t="s">
         <v>213</v>
@@ -1657,10 +1679,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1677,7 +1699,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="58"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="61"/>
       <c r="C8" s="10" t="s">
         <v>61</v>
@@ -1693,20 +1715,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="67" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1723,7 +1745,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="67"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="60"/>
       <c r="C11" s="7" t="s">
         <v>75</v>
@@ -1739,7 +1761,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="67"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="60"/>
       <c r="C12" s="7" t="s">
         <v>76</v>
@@ -1755,7 +1777,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="67"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="60"/>
       <c r="C13" s="7" t="s">
         <v>77</v>
@@ -1771,7 +1793,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="68"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="60"/>
       <c r="C14" s="7" t="s">
         <v>78</v>
@@ -1787,10 +1809,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="58" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1807,7 +1829,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="67"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="60"/>
       <c r="C16" s="7" t="s">
         <v>65</v>
@@ -1823,7 +1845,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="67"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="60"/>
       <c r="C17" s="7" t="s">
         <v>87</v>
@@ -1839,7 +1861,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="67"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="60"/>
       <c r="C18" s="7" t="s">
         <v>95</v>
@@ -1855,8 +1877,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="67"/>
-      <c r="B19" s="63"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="24" t="s">
         <v>86</v>
       </c>
@@ -1871,7 +1893,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="67"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="60" t="s">
         <v>15</v>
       </c>
@@ -1889,7 +1911,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="67"/>
+      <c r="A21" s="56"/>
       <c r="B21" s="60"/>
       <c r="C21" s="7" t="s">
         <v>91</v>
@@ -1905,7 +1927,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="67"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="60"/>
       <c r="C22" s="7" t="s">
         <v>66</v>
@@ -1921,7 +1943,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="67"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="60"/>
       <c r="C23" s="7" t="s">
         <v>93</v>
@@ -1937,10 +1959,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="58" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="35" t="s">
@@ -1957,8 +1979,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="67"/>
-      <c r="B25" s="63"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="38" t="s">
         <v>110</v>
       </c>
@@ -1973,7 +1995,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="67"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="60" t="s">
         <v>15</v>
       </c>
@@ -1991,7 +2013,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="67"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="60"/>
       <c r="C27" s="36" t="s">
         <v>127</v>
@@ -2007,7 +2029,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="67"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="60"/>
       <c r="C28" s="36" t="s">
         <v>111</v>
@@ -2023,7 +2045,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="67"/>
+      <c r="A29" s="56"/>
       <c r="B29" s="60"/>
       <c r="C29" s="36" t="s">
         <v>124</v>
@@ -2039,7 +2061,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="67"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="60"/>
       <c r="C30" s="36" t="s">
         <v>112</v>
@@ -2055,7 +2077,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="67"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="60"/>
       <c r="C31" s="36" t="s">
         <v>113</v>
@@ -2070,18 +2092,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="67"/>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="56"/>
       <c r="B32" s="60"/>
       <c r="C32" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="51"/>
+      <c r="D32" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="51" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="67"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="60"/>
       <c r="C33" s="36" t="s">
         <v>114</v>
@@ -2097,7 +2125,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="67"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="60"/>
       <c r="C34" s="36" t="s">
         <v>115</v>
@@ -2113,7 +2141,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="68"/>
+      <c r="A35" s="57"/>
       <c r="B35" s="61"/>
       <c r="C35" s="10" t="s">
         <v>116</v>
@@ -2128,274 +2156,334 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="55" t="s">
         <v>224</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="51"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="55"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="51"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="55"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="51"/>
+      <c r="D36" s="68" t="s">
+        <v>232</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="56"/>
+      <c r="B37" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="40" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="57"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="53" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="55"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="51"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="55"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="51"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="55"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="51"/>
+      <c r="A39" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="63"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="64"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="59" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="57"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="58"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="62" t="s">
+      <c r="A42" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="13" t="s">
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C43" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="27" t="s">
+      <c r="E43" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="63"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="64"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" s="59" t="s">
+      <c r="A47" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="58" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>9</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="57"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="60"/>
       <c r="C48" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E48" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="58"/>
-      <c r="B49" s="61"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="56"/>
+      <c r="B49" s="60"/>
       <c r="C49" s="7" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F49" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" s="59" t="s">
+      <c r="A50" s="57"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="67"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="67"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="68"/>
-      <c r="B53" s="61"/>
-      <c r="C53" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="31" t="s">
-        <v>55</v>
+      <c r="C53" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>9</v>
@@ -2405,17 +2493,17 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>33</v>
+      <c r="A55" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="58" t="s">
+        <v>43</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E55" s="28" t="s">
         <v>9</v>
@@ -2424,202 +2512,192 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="3" t="s">
+    <row r="56" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="63"/>
+      <c r="B56" s="59"/>
+      <c r="C56" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A57" s="63"/>
+      <c r="B57" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E56" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="66" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="67"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+    </row>
+    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E57" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A58" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E58" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="57"/>
-      <c r="B59" s="63"/>
-      <c r="C59" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>47</v>
+      <c r="C59" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="E59" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F59" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A60" s="57"/>
-      <c r="B60" s="34" t="s">
-        <v>15</v>
-      </c>
+      <c r="F59" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="56"/>
+      <c r="B60" s="60"/>
       <c r="C60" s="7" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>48</v>
+        <v>206</v>
       </c>
       <c r="E60" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F60" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="65"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="65"/>
-      <c r="E61" s="62"/>
-      <c r="F61" s="62"/>
-    </row>
-    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="B62" s="59" t="s">
-        <v>15</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="56"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="56"/>
+      <c r="B62" s="60"/>
       <c r="C62" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>141</v>
+        <v>185</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="E62" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="51" t="s">
-        <v>216</v>
+      <c r="F62" s="31" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="67"/>
+      <c r="A63" s="56"/>
       <c r="B63" s="60"/>
       <c r="C63" s="7" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E63" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F63" s="31" t="s">
-        <v>55</v>
+      <c r="F63" s="51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="67"/>
+      <c r="A64" s="56"/>
       <c r="B64" s="60"/>
       <c r="C64" s="7" t="s">
-        <v>136</v>
+        <v>217</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>142</v>
+        <v>222</v>
       </c>
       <c r="E64" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F64" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" s="67"/>
+      <c r="F64" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="56"/>
       <c r="B65" s="60"/>
       <c r="C65" s="7" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="E65" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A66" s="67"/>
-      <c r="B66" s="60"/>
-      <c r="C66" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>207</v>
+        <v>221</v>
+      </c>
+      <c r="E65" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="56"/>
+      <c r="B66" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="D66" s="37" t="s">
+        <v>208</v>
       </c>
       <c r="E66" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F66" s="51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="67"/>
+      <c r="F66" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="56"/>
       <c r="B67" s="60"/>
       <c r="C67" s="7" t="s">
-        <v>217</v>
+        <v>131</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>222</v>
+        <v>140</v>
       </c>
       <c r="E67" s="29" t="s">
         <v>9</v>
@@ -2628,16 +2706,16 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="67"/>
+    <row r="68" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A68" s="56"/>
       <c r="B68" s="60"/>
       <c r="C68" s="7" t="s">
-        <v>219</v>
+        <v>132</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="E68" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="E68" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F68" s="51" t="s">
@@ -2645,357 +2723,357 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="67"/>
-      <c r="B69" s="64" t="s">
+      <c r="A69" s="57"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="62" t="s">
+        <v>188</v>
+      </c>
+      <c r="B70" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C69" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="D69" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="E69" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F69" s="31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A70" s="67"/>
-      <c r="B70" s="60"/>
-      <c r="C70" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E70" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A71" s="67"/>
-      <c r="B71" s="60"/>
+      <c r="C70" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D70" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="63"/>
+      <c r="B71" s="59"/>
       <c r="C71" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>218</v>
+        <v>194</v>
+      </c>
+      <c r="D71" s="44" t="s">
+        <v>209</v>
       </c>
       <c r="E71" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F71" s="51" t="s">
-        <v>216</v>
+      <c r="F71" s="29" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="68"/>
-      <c r="B72" s="61"/>
-      <c r="C72" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>143</v>
+      <c r="A72" s="63"/>
+      <c r="B72" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="D72" s="48" t="s">
+        <v>202</v>
       </c>
       <c r="E72" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F72" s="31" t="s">
+      <c r="F72" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A73" s="63"/>
+      <c r="B73" s="60"/>
+      <c r="C73" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D73" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="E73" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A74" s="64"/>
+      <c r="B74" s="61"/>
+      <c r="C74" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D74" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="E74" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="62" t="s">
+        <v>183</v>
+      </c>
+      <c r="B75" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="28" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="56" t="s">
-        <v>188</v>
-      </c>
-      <c r="B73" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D73" s="46" t="s">
-        <v>204</v>
-      </c>
-      <c r="E73" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A74" s="57"/>
-      <c r="B74" s="63"/>
-      <c r="C74" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="D74" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="E74" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F74" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="57"/>
-      <c r="B75" s="64" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="D75" s="48" t="s">
-        <v>202</v>
-      </c>
-      <c r="E75" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F75" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="57"/>
+      <c r="A76" s="63"/>
       <c r="B76" s="60"/>
       <c r="C76" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D76" s="44" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E76" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F76" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="58"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="64"/>
       <c r="B77" s="61"/>
-      <c r="C77" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D77" s="44" t="s">
-        <v>203</v>
-      </c>
-      <c r="E77" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F77" s="29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="56" t="s">
-        <v>183</v>
-      </c>
-      <c r="B78" s="59" t="s">
-        <v>189</v>
+      <c r="C77" s="10" t="s